<commit_message>
merge code from main to HieuNghiav1
</commit_message>
<xml_diff>
--- a/client/public/templates/environmentvocab.xlsx
+++ b/client/public/templates/environmentvocab.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ki2Nam3\CongNghePhanMemHuongDoiTuong\project\StudyToeicWeb\client\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F6623E-A1B9-4C28-8406-6AD5F94AB103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DBBC2-77A7-4B86-875D-104C834BE135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
   <si>
     <t>content</t>
   </si>
@@ -418,9 +418,6 @@
     <t>https://file.hstatic.net/200000898205/article/he-sinh-thai-la-gi_5438090e3e5a42178c92f81c0b401f0b.jpg</t>
   </si>
   <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMQDxUQERIVFRUVFRAVEBAVDw8VFRUVFRUWFhUVFRUYHSggGBolHRUVITEhJSkrLi4uFx8zODMsNygtLisBCgoKDg0OGhAQGi0dHyUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS8tLS0tLSstLS0tLS0tLS0tLf/AABEIAKgBKwMBIgACEQEDEQH/xAAbAAAABwEAAAAAAAAAAAAAAAAAAQIDBAUGB//EADwQAAEDAwMCBAQDBgUEAwAAAAEAAhEDBCEFEjFBURMiYXEGMoGRobHBFDNCstHhB1JiY/Byc4PCFSMk/8QAGQEAAwEBAQAAAAAAAAAAAAAAAAECAwQF/8QAJBEAAgIDAQABAwUAAAAAAAAAAAECEQMSITETBEFRIjIzcYH/2gAMAwEAAhEDEQA/AIL3Jhzk/UCY2LykegEEvejDcJpyAFuqJG9JSCnQE23rKY25VQHJ1j1LiNMsXVZSHNBUXcnKdRTQWHthK8WEp5BCjuKa6BY29YHlXVoyBKydInctNp1QgBZzVDTLdlwQJlRzduLspwM3Jynbg4hZcKH/AAw4SodVjflVzQtMQqjVLNzJIHPGEosCk1lo2EN+qxb7Q7lrbikWyTxGVVO2k4GV1Y5UZyVkXT7w0nfmrinrw4Jjsqm6oSMKkrgtK0UFMlycTZN1RsepRNvxPb1WNoXJBUttzuSeGgWQ21jqWeZAV/bV21BgzIXNrWuWnnlafRazpmfdYzx0XGVl/UtQRwq7xCx0dFNr3nrmOFRXd2ROfZRGxs0tGuCIlVuqu8oEc9VQHWS08kKxt9Za/DjPqVpFNdJfRlEVKFIPw36KLUaWmDytk7MmqElIKMlJTJAilBEmApBEggBh9NMVWwpLqii13SsEdLGSUhyDiiVkiSiS4ShSTsBACc24RtEJb3YSsBlzkQqJmpUykhyqhWTPHCj139lHLkYMo1oTZZaaQSJWotGiAsdav2lX1jcl0ALHIi4s1NuVbWVpJkcqm09vUrQ6S8Lm+5UnSLqwtQ0Seeik1qTXja4Ag9CE3RqjiU654Akle1g0WOl/p58m3KzlnxZY+DVcyfKCNvscifus++ycGTIWy+OwCS/qfyAhYdl+Yh3A9153revlnavFZXVw5p5UC5YYkq9NQEGPyVLe1InC2gyZIrQ5KFYtUR9TKQ+rK6tTCy0pXknlXmm6vtEHKxe4hPNrHuoliTHHI0bq41cOMzH1UZ2ptcQDn1WRZWMqULnaFn8KRfyGjvalMweUwyqZERBVGb3cVJpXBhHx0h72bPSapke6lanUDnCOeqoNE1EbxuK0tS2FQFw+ix8l0p9XCrlEUp7SOUiVqZgKJBBMQYRoBBICqFdIc/Ki70oPUam1kglGFH3pxr0UOyQwBB74TYKRUCmhgdUTNSsgQmHgq0iGwi+UEBTKEKyRBkI2uSgyUo0UWgoVTervSq4byqAYKmsJiVnONlRZs7fUhwrTTrgnjhYexJK12ncLknGjZOzQP1IsGVDra44qtvLkmR0VXVvwMKUmKkTdXqGoFm69oQchXgqkhM3RjlaRdBRWU7KRPHdUmv2mzMzKuK9yQMKh1S5LhBW+O9iJ1Rm6pykBKr8ppegjjY8GpYYk03J1tRJjQujQJSqlJBl0W8KPXuieqmm2VyhwNhL8eAoYuCm31ZVak7Fnb3XmELd6TqHlALhJ6T+i5tRqgZU6hdZDpIhZZcWxcJ0dFvnAxH391EUDS9cZTpncZJiBBKsKWotrwIgng/1XP2PGjVq+hIBB7S3kQgHKyBQCNECjlIDMSlNSQnGhNloMNTrWI6bVMoUZWblRaQinSlG+irW3twlVbaeFlv0uiiNJDwJVwLRNm3kqtxalabPCTSspV2bbCepW3ol8gaoz7baE0+llaT9kyotxYZQsgOJRut54Uy1ticKxtrAg8KztrGP0RLICiQrS0Lei0en0u6bp0xERlT7WmAueUrLSIF/amZVLcWg3Ste+lOOiiVtLwiMhMo7dhDcKJqjHEBaOpY7WY57Kpubc8kqk+gZ9tAuwqjU7WMLY0rbkqLqOj7mbgO5K2jkpkONo5xcW5CjFsK7vqRByMKkrgyvQhKzlkqADCU1MCUpaEC6jlHe6U45G6jiUIGMhEl7EktTJDBUijXAwoiNqGgTLelUkd+391baXWeKgAwZwVm7VxBwthoNs5+yptmCubLxG+Ppf3r52g8xJPuowUm8qbjA4H5poBYx4ipehBGlQhCYjMsCkU6aRSap1KmpkzVIOlTVhaU8qPTYrC1bCxkzRIm0qadFFHTEp+mFiUNi2kJmpakdFa0mJTwiwKNzIT1uE/Xo9U1SbCoQ94KdFsCk0xKl06ccpBZH/AGcBOU6UuTrgnKFJJhYoUoTzWwE9TpjqnmNBUhYi2MpdYQmq3k4SXXAIyihDRJUG5tC4Kwc4ASolS76JJMoj0rWOVIdTaBATbapzKktpbuFYjJa1ogMkDvhYPVNMc0/Kuz1LfEELOappoLjI9itsWZxIlBSOVizcDkJRsT2Wk1LTSPMJ9MKToluHnZUbmOy6/m5Zj8faMj+yGeEmsyBkLpNTSKYE4lZ7WNEO+WCWnhEc1vonjrwotPtQ85Ctq2gNc3yj8OFa6JpG0iR6rV29sG4A/BZ5M1PhccfOnLLzQi3gYjmFQ16ZaYXcrukwt2kDM4hc+1zQnGdjZAnI5CvF9RbqRM8POGStXwV03QbpjqA2gAwA4T19ly+o0sdBxHK0/wAKt8Qu2k7htgTiD1Wn1EbjZGJ06NaWwUIT1QZ/590lc9liIQhKKJAGfpBWVu1RKNJWltThRNm8UOU2KVSCFOnKX4cLFsom0FIYFDolSqSgZMYUYISGhNvfCErE2LrgQo4ACbfVzhIK0USHIkirCU26UMMSw1VqhWyU6uDhWVDAwqikMqb48BRKP4GmLuK5GAioXjmjuoxdKEp6qgssf2sO5TD2ieVFlBgk/wB0tQslPpmE0aEZTpuA0Z+yj1rou4wElFjbGXVCr6xpAMlZ8q/sq4DACeAE5rhKJDQDyFFr2DXA/mpDajTkH8Ue5ZFHP/iPTy2WnjnBymtE0whwduJkQJkn7rVa7aB3n68JugGU6QftMcE9vb0laKbqkNpelV4cEg9OUpzGnkcJLnSZSZW9WZDzHAGeg6BShXnjPp/VVpTttV2lJxGmSrqmXYH3VZfO8JpIEzIj9Va0qkiUmqzd+azqjSzj2rUi6oXlsAk59VYfDrvBqNeDIJ2kzwrfWtGh7g504c/HAmT91V/CNMvrFkSyHb/YcY91277QOfWpG2cM9/Xv6pKU4/2SSshiSiRlEgCPQYprGJplNS6TFztnQOUmKQ2l3RUmpRcCJBkZ/BQOx2mAnWmFAFRIdXlUokORamsFGrVZ4UPxUYeqUaE5WPBKCZ3ow5USSAUcpgORhyAHtyMOTUowUDHQ5K3JkFCUAO7kNyblEgBwuRbkhBAgy5DekoIALcRwVc6bdF+D/DySqYqTZXWyR3iFM1aGvS2voLMqDTcG0CH8cA95/upV2JYR9fsqa4qF9PIHldAI4IIkH8FjBWzR+EREjRFdJjQSBRFEmFB7z3QFU90lESgBjWHQC6NxIhg6Z7/ZZn4VtwK7/MQ5oMt4kH+61lXzMLfTCyfwy0C8qDs10feP1VQ4mhy7RpyklLKQUrJCKJGSilMQWlXniDa+GvmodnXYHeU5zwWqza2FiP8ADKu57Xbj8jS1oxJBdM9wBEes9YWubfh1Z1Ha4FoncW+UjAwfcn7LPJDWTRrGVpMleLAJ7Aqj+H7kl3hwQJuXPBcXZNUbIPUFpwfTrlWN5dCk0vdMDkgEx6mOn9Vl7C/8K5cxtJjCWPeykzdL3FoyXxtIljh169lUIWmTKXTW3CZCj2F2arM/M07XnEFwAkiOmVIYQQCDIIBB7goqhCgUsFJCMIAWClApASgkAsFKBSEYKQxwFHKblGCgByUqU1KOUgHJQlN7kNyBjkoSm9yLcgByUJTe5DcgBZKSSk7kklAFnp9WWuaT7D0VbTqk0oOIeRzzjqkm8FEGo4w1oJeYJhoGcBVuka1SuGubScXbXbnSxzcO45GeCkoO7oeyqixlJKIuSS5UQGSkkpJKKUwFSiJSSUklMBxjoMrK6E5ovqzQ4H95HmBmHBaaVz34bbGox2dXA46By1xxtS/oiUqo6CSkEoEpJKgoBKKURKTKBHPPhv4gNu7axhc55dudJJO6MgHkjPToO5V3d66+jc0rlzW7ajSyo4CAZezzHJyGtAn8+vPqRJMDEwJ3R+PQK4t9SLXsa53ilu0M8xLGEEQ1rT5f4YnjK7Z4ldmUcjqjpWtalUYG1LdoqBsuqM4lhO0GT0mftOVl6mueJUNZjWNcweem4CD53U3APx5Zc2Y/zHlKuKlSg2lWDn1hUH7t5p7RvaSQY6ZwCAI9Vjra6LHiOm2ByJ3A5GJ44KzxYlQ5z6bSxuHUaVek87CfNSaMwH1CNzsy7O1pGDHEqf8AAmompTexxbDXNbTAJJwzIzmIbM+6w9S8Fao1x8hwKhaMO2uB8rYgZEwn9Kv/AAfEFIvLyHeAAWjYTy93SQAMiOOycsdp/kSn06Vp2qCrWr0zDfBexgJcM7gOnvKDtaYaQqMyHOcwGQBuAMZ45gfX0K5Rp+ovp1/Fkudume7sw4+oJnPUK2qfEz4ApkNim9r27TkuLiT3mSHf8Kh/T94Ush0H4d1E17cVHTjqWnIaIJ4yZB4VqwyARwQCPquaaRr7qdKqGSZYNrnOJ2Ma2HQDHXdx1jC3DtTFGg11SAYYXNJPlY4mM8TA4noeVjkxtMuLTRahGFnavxBvurenRBc15qF7iCAWgbZn0O7B6gdwrl18wVfCJ820O+hIH6rNxaLVEpGCoOr34oU93lknawOMAnnJ9gfeIWb+B9VfUrVKJa0CHVHnzz4hdBLZJlvHsmoNxchN9o2SOVQ69qbqVxasbw+qQ474BAaWlrh6bp92hXylqkmUgSilGoNhcl9Wswg+R7QJHdoOO44M+qQE2UJQQSHQUoSm61UMALurmtn1cYE/X80smExAlFKiaZditTD/AFIPlLZ6yAeAQQVKQ+ARNZzbVh/tVf5Ssj/h0fNX9qX5vWu1YTb1R/t1P5Ssd/h5+8q/9DPzK3h/FIyl+9G3JRFGUlY2a0EiRlEU7FQRSSjJRIsKCC5/opjU/wDy3A/B62+pXYo0y8z0AgT5nGG47SQucaJef/ubUdA3VXuPMDdu4+8fVdOFXGRjk9R00pJSaFYPY17eHAEexEo3ugSsTQBRJq2uW1GB7Tgj7dwfUcJyUAcSaY7fVK8TvmBA9Mz/AFTaC9U4ic3Un+GKc4bOwEcTM578fYKK18GTKQECUqQ7HfEzhOOunGPQESBByoyMORQWLa+DynajofnP+af09IUYlKDzETjBj1HH5lFAWVjRBBeTgBxaPNucePLHOYkeqk3OrVHhwNV3nBDhuce4gk8iC7GfmVbZ3bmOa4Rg/bvnol6hXFSoXhjW/wCYNOD3I9/RRr3pV8NV8OXNSrcPrVGS1rd5eWO2N24Y0AEN5g8H5cZR63rB8VxETt3jaZGYcZ6OE9scnkKo+GtYbblznU/EB3NFMuwA4ZPqYBHHVQ7+53uj+HzBsiMEzn657ZKy+P8AX4Xv+k3lXUHXVrSqMDntB8OvTiW7toLX7sOBEjMxyCsxaat4NY1wfMyoTsH8QLiX9cyJHSJHZRdE1R1uHPaCR8rwHHbDuPKOogn6wourVA5+4Gd438gw4kzP2CUcdNr7Dc7Vlrql74906rRBY0xVp7yAd0TvAcYy4dOwWq0T4qAtaW+XEU3l7sDaGPDRM/6Q7ucD1XPNOuvDM4zg9xxkfZSLC4Y1lTc3eYlsk7eIMgDnIz6EdU54k1X4CM6dnV9S1JmyntfHjR4XRtQOGW7uW4IM46ZVAwVKbmkw0S3xXt8oLWS8DcTtzscJ9cRgLPO1km3pAw9rA9mxxa2WBrWwzGCRJ65hSL/WaJLaex2wM3MD3yCcgNIbyIAzgjKwWJrho5pnQLq/DX02DLnkS3qGGZd7Ax903R1Rpr1KJMFmwjBAh20QSeskfcd1iBrIfc0az6wMl25rS5ophrTFOHc7skEZy4dcFrHxCXQ4QC7aKr2h0tDXu2wJGCNsif4e6j4H4V8iNN8RuLnhr4DWbajXzxtMndg4gHBxLRzkJepauZ8JhIcZcIbu3MaRIGMkgOMRwQspea+6qA55bM+G5wMHaYI3t4d82RBiOclP/t7vAc1j9ppvDHszLmlrtrmnq30AHy8lP4mkrFuvsXdG+fSDncUyWVCSY2jd5w1vaP7c40Jrt3Bs5cHEewifzC5Q3WHik+iHTuLSSCSGhocSGmcSYMRGCr34c1EmvT+YgMFOmHPYJbua3c6Dz0AMTg9k8mF1YRyLw2mp5oVR/t1P5SsX8Afv3/8Ab/8AYLZahmjUH+ip/KVzHSrp7Kh8N20luI67SHEHtx+CWFbQkgyOpJnUq9ZrBLiAJAz3JAH4kKHb3BNeozloDCHScGILeIHAP1We+JtRNRjPDA3EdXAQDseCSTwdpHuDlQNC1gC6YHeUP3hzXEGHQGggwI3Az9+6lYnrY3NXRuyURUJ2p05c0OBLWhxAI4PAH3H3Cct7xlQwx0xBx2IBH5/msqZY+UzW8zHBpyQ4Ahww7I5zBBVf8SViLZ210bgQHAkfwkgbhxJH6LMafqpa3w6hcwFxe1zIBnzF25p+YOEZMZWsMbasmUknRd16tR1PY8gua8Nc0NncNsSZAzuyI7jCw2nR+1NbwPE2xO3qRE9Ff2AqU9wcYDog1GOO4CILXcAwAOeeoWaBi43dqk5M8OzuPX3XViVWjCb8Og/Dl0X+IIIpt2eFudJ2xBycxiZPcqVqVz/9BfTqNEGA4wWkztLTgxnHCz9pXDKbngiXB7fB3u3BpdtaBE5MHnv6FK/+SpstQDIfuJDAZAIhsOEjEAHPPPosXDtmilwl/DV43a5hcAN5DGAO8pmC0E/NJMiOiv4WI0i9DCKtQOeS4kMAbta6QCQe8RgBbhTlVMcHaOIIIIL0jjAggggAIIIIACCCCAFz6IbkEEAOW79pnH1AP4J2q6QD2xHWMo0FL9GIa+Bz2QqVN0eggY6T/dBBOgEtKG6ESCAJVO4DWiB5gQZJ/ADiOOULm4DnS1oYMQ3npnPuT90EEq6OyOXKS67Owt7xuycxJAI+v4BBBFCsSbkxHPaTPKn3F+HtpuaNhptZ5hlz3CPmJ4gTGMcIIKWkNMrHVvMXdySc9TyptC5aGuHm3QPD2uja7dMun9EEE2gTNu74tpOaykHmDSqNe9wHzBg2mT67vfCwtC6DXyRIIIIwDHv0Psggs4YoxuipTchqvdudALiQ35J6CSePck/VE25IIdJkcZ4I4jsOEEFpSIstdK1XwiXnO4gNEzluwkGcxER7IWetvbULpDZa4EgcnPUn1P3QQU6JlbMk6lr3it8MggQY7AHMR0M9eRkKuqV2HyOkEOjEYECAJ9QPzygglGCXg3Jss7nWSKVOkxxdtaS4GI3EzHrH/IVIKsVw8iPPJEHHmmEEE4xSCTbLW0qUvCd4hkvqE085aM7jPQjoe6hW9ztp7cHcfO0kkEGZkdxjM9kaCWoWSdPuxSaCGtcJALiRzPTjuMcJ2prVSoS+dsn5d5Ed8IIJaq7HbP/Z</t>
-  </si>
-  <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcSDB3si_ehaq4GvPOKv1sCY5_QLyv7jjIg6o9PdNgO_Y7xw6mdVOVVizPxbqe0nm3tsy5Q&amp;usqp=CAU</t>
   </si>
   <si>
@@ -430,64 +427,46 @@
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRS6p8Ex-T0G7QcHdbhvoL0MafS_BT3bd54Y1pQe6sACHOb_a4BCXmRqgo8yYTUnJ7KRNI&amp;usqp=CAU</t>
   </si>
   <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUSEhIVFRUWFxUVFxUVGBcVFRYVFRUXFxUVFRUYHSggGBolHRUVITEhJSkrLi4uFx8zODMsNyguLisBCgoKDg0OGxAQGy0lHyUtLi0tLS8tLS0vLS0tLS0tLS0tLS8tLS8tLS0tLS0tLS0tLS0tLS0tLS0tLS0rLS0tLf/AABEIAKgBKwMBIgACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAAEBQIDBgABB//EAEAQAAIBAgQEBAMGBAMHBQAAAAECEQADBBIhMQUiQVETYXGRBjKBFEJSobHRI3KSwWLh8AcVFjNTgvFDY6Ky0v/EABoBAAMBAQEBAAAAAAAAAAAAAAIDBAEFAAb/xAAxEQACAgEEAQIDBgYDAAAAAAAAAQIDEQQSITFBE1EiYYEFMnGRofAUI0JSsfEVweH/2gAMAwEAAhEDEQA/AF+KuGld1jTi5hyagODM1fM1NRM7FCgmi7OGmm1rgBH3qmuDKGDTJWrwZJNdgSYGoXMERTm2lSuWtKBWismaeyausLrR1+xVdq3rVUJZQUQvDa0dbWqsPaijbduhkxqRFVqyp5DXoSpbJDYonaWjbNqaHtJTOwulTSkMUTlwwqYw9XJViipLGGolAt1aiVdkqdu3UcrHkLBSLdRa1R4t1xsis9RnsCt7FC3MIafLYq+1hx2q7TTmC0ZYYFu1etg2Fa02QaHu4IdK6nqTSyDhGSayag9o1osRg6W3bVTy1mXhm7RBibRpbeBrS37M0pv4Uk1Zp9Qn2LlETMtVEmnP2DvUbnCWIkKfaq1qIdZAcRUlwijLeI86HvWCu4rywNaXbiSyKaHeGuedHLepbhloquDd94NF1y9UbbSaoY1ZYNZEIa4ajwaV2LlGC7QyYaMrhcPJpitqvMElGC1VHqCK+ihbVQv4WRRZWKi7aUXqIOXKE4tRXlyrr1wTQt19J6d+lejZlkbBr9UWF1rsQCdiRqNo6HbUbVbhkP1roVtJBwHGEw80f9nMaRPSdp86p4VmIkxHQZSpkSCSCdjGnl3pvh8MBJH3jJ1J1gDQHbQDagsmkPigIYX1Pt/aothT2p5bw9XLYFQXajA+CEtjCHtTC3Z0pgLAr0WqStRnsaBC1XoWijbrzJQWc9GohbSaJSzUrS0SooIUZ5Z5vBT4deZaIivMlZLT+wO8qVatUV6q1MCrKINAuRCvCKmRUWp7lhGA91aT4m3Ti4aW3a5N08SGoU3Fqp7EwAKnxbErbUsSB2nq3QaedZv/AH7dR3J0LJCDlyKdOY9iJO/cVVp901lCbbYweGbXCcNVRqAW79vSi/Dr5ufifEK4IeSNWP3YX8Q66SP/ACK1HC/ilRaZrxzNm0ywJDRoPTfXWqpqyKyBDUQlx0MuI8MS6OZde/X/ADrMf7jZGI/PvX0BFBEjY60PjMODBqeWuxB4GygmZizw2BXtzBkU9NqqXSudLVOT4PbEZ+5aoJ7mUxT3E26zvE0NUaezc8MXJYC7F+jRiKzmHxBG9MlvCN6rnXkxSR7hr8GnVm4GGlZhGouzeI2NS8xJIWbR5cIpXjb/AGqq5fPelONvu3/KhgpOfVgenKhCMM2pOxiACNdHaemy+e2IxSc3hEzdB2MjXbyMH85q+7j3Nvw4QKTJhFBY8u5H8q7RsJnSpWcIj2l8JPDYCBakFmRQBmGUQXB1YCJmRroQCelW2UWaeWE+H+oEoyg/kSWi8Op0gayN+gnU+cdqEt0xwVuI1J8zvvRKWEeiNrDZQDlLGVEKBOpALanYTJ6wDEnQt8LcDTDAwcpggw0AwY2MEaedLMMaaYdqitsHxGFpaIVKostVd578xbgQQSSNGWTyzOh21/0UKG99pfiUJjHLUWWrJqrEYhEEuwUEgCTEsdlHcnsNazYpcILJWyVEJQDcaU4lMOIh7Vy4GJhsyOilMhE7PM/4TpTJDRyqlW9s1gJFtpauFUo1XCqoJbeAJHoFemuFe0SWEARqQNRipgVtUXk8ziKg1SNRNbbg8ge6s0rx7hAWYhQNydBThxWF+OuJAnwFMxBeJnTWNN/p5dq5yq9SeGFOzZHIm43j/HCtkKqjM2vUTyn9NjSgXPEGxADBSZykODoC31Ega9NtKtvXsoGY7qJPzKoy6lo1g14pXqpyICfDCawDoSoED8wQw161064bY8L8Dlzk5PLKL7TAV1HkROoIMSdtvPWD5GvD3HKkHw9wWymSWQDL9DzCeuvUkUwsvbcEEaEagypUHQfwyBlGnWdu01cbKnnVJKjRNQwiNAROmg19BR+oo/C0CjS8D+JRZt27V4FjJGcEZVQARJMa776wK112vk6MSIMgRIDagRBAMnv2/Ktt8H4lriXAZMMGzEkg5xss7QVOnSelcnX6f4HKPfkv09257WOis1MYcdamiVMmudRFdssYBibK9qz/ABjAaStaO+aDurNdemCfIuSyYkWNavFqjcRYhyK9FqqkTYwJga9FyhmuVU1ypVDJGGPfoU3iFyqYWSYGgk76VQ9ypXcVb8NUS2QQSSxMyTuBpMCBEk7tpVNVeIv4sfL3NT4fJ32lxBRyrqcymSAGHfKQYOxA3EitBYe1jFz6W7kw2ohGgtkunNzMeaMs6LrB0rKUVYDg50PNBBBAKurCCjg7rtI0mKroksbJdD6LY/cn0ObuAe2YcEefQ+lEYcRRPw5xa3ircKG1yqVMwugjoW1BJBbUCNqkbGVvIgEejCQD5waK/TuKyug7aNnK6CbBo201A4XSQZ0+8QADOukdtvpRVs6amT32/KubbTg9EZWLtGfagBqY6ep7DufKk6uem50HqdqW8Z4ithZLwWBCzpcLmJRfEEa5tOi5dp3PS6P1Vl9FMItjviPHkthiGAyAM5MSikMQ5UkQum5P0NKMCb+KueKoNq0MwF5s3i3RLCEVvltbHSFaZjpQHDcA+IIvYqcobNasliQARo978TEQCslTlB6mdQmJ6VS7Iaf4aVz7/v8A0G8dIyXGPh29am4t13toReVQzKEdOaSmaCdN/poDW24fjFvW0up8rqGHlPQ+Y2+lUswIIIBB0IOoIO4IqVmFACgADYAAAegG1T6jUu+KU18S8/I2KwGZ6vttQdppNEzSYZXJrRfnqwGaFzVYrUyNjzyLcS8V7NDF4qwPNPrsXQLiTY1E12avJqa+XJ5Irv3AqlmMAAkk7ADUmvk905rrfe1YzmnWT1Gh6fUHaK+jfEuIK4e6V+bKY6naSQOpABMeVfMsTdYWzky5iswcwkgBiuboYH717TLcm15eCfU+EVvkYh8oBBHMAZhZOgI2jLoN8x23qnDKbzM5AIBOUqQpMNoh3P3ZIPSNd6U4gYi4CwsFZKZSrc2ZTpnUEMLYMTGuh661dYxLqmZrZSSuZlHiHIh6jNnB1kSNNdTXV9HEfhfPXuSNcB6NykMozQZ2JUQADMmJ12Pfsats35JysdoIYgZSN4jUTPUafWlOa5dk23CKVVv4i5mLD5TmGkbxy6adKu+y27bk+M3iBQBKjw1GgkwFbLIOk6wSZgx6VSxh9/UzAR4jsWa2hYKSrC3lBPLEsD2IJiQdeopr8L8WuYa4y7ho3JKQZKqCOw29fZXhbuZFKNoSZYAyzZssKoggTAkdz6iAW3c57bgrmMksbiqdxCr8oEb7GPrS5wUk4yXH77NTaeUfbkNU39Kq4Y/8K3zBuRdRsdOlW4txArj+lHGH4OsmCXBVJWrswpdxDGgCF1PerakkgZSwK8YZcmuWqC8mrA1GoEzZk81QJqjxKmrUnbgjL8Lgbl0kIsxqTIAA8yTFTtcKuMYC/mB+ppzwoAWjZLAF18WdoXUAefy//KhvHyW7IU87YgqIUBii3mlf5RbBBPqd669OgjKCcm8sphQnFNkU+HLu/J6SZ/So8S4betWbjhJKqYC8xnYELInUzE1oLmM1HTf8q44jxLZG6kEe4g01aKtc8jlpoJgHwziFKC1b5MoBZVJJYZkV3uFmAHMtwHKSIk6QKnwbi63z4GuY5gvyrlVizW2QKCplVkDXRZPzcw+GxCqbioWOREK25kq2YocqT8sXIjScp1OhBHwotpb126QVZFIVIKAZlVScpAMqqhRI2edSZqnCZQ/OTS4TAKig3mDMN8vKvr37aT71meP/ABn4N0YdLIQNtdzLmIJMFUUbEA6kyO1KfjHjlwW0UEoXYkRvkUCTPT5h7+VIcbjE/h4i6ouC6twIoMQ1sMAD2g3AY/cGm10wjykhD44R9AwXG7DjnVgQSJk7iNZG4n8x5Up4pgkxRK2lMowZSsSpZdyp5XErbMHtI1FNfh3H2cTh0cWY0KRGqsrRpvodxvQFq+cIzrEli2vlKlVHmAw1+lHmMuAsSisltz4iRFXxZ8Qkq1tASQ6sUeA0ErmVoMagTV+A4zbutAlTMANAJPvWSIa9jrx+dl8MlJIynIANfVTqP71LG4LwroR7eR3OdSCTly8xM9Boag/4ujD5efxM3P2Poa3jEgzpIO+ncRvXl12YrlcoAWzDKpLCBl5jMKNexOu1L+B2mXNKhQ3NA0GYk5iB59/KmmWuNev4ayVfD+g5PPITgngxPlNHzShTFHWMQDvvUqGBQq5TVAYVVcxAG1LctrPNZL7tyqvtEUI2K71RfxPathPLyewMHx58q8XFTSXxqmuJpOprnN9nlgzvxTxdmvlBnyKSBoYzAQZjpI07yO8Vk7r5lKjluKQklhDyOZQdwTzbjQEajU05+MbLLdW5BZbhAEAcr6wGMj1B6CdRGuFxoU3dHIJykFhnBUT/ABA25AOaPQ8wr6DRaePpxcfY5lqbm8jriOPNsqqgAiRyOWUbldtVMbGDqOu5FPxApKkLmj78Dp+HMCFgidRMjXXWg8Gz2HYogfMAMxWGADAyCVykmR6RrTJuGvduSbNlGBblYkZgZguIImQNoiZHWqnCuP3l9ciXFeQXE8QIuBXVhmZWYpmKqGGmTKDPKJid223irFOyHKmHWCcudwCXB5QSG0WZAmd51MaHYey7FsqWE1IZgeZQZ8QPl1YckTMmJGmouPC7mQqLlu1b0Ui2hyFiSeVfEnNLRBJ6AVrnCOF+/wBP8G5S4FP2o4a2ii2wDQviM4ZNwcoyMwWRIglfTWAwwAW74lxbh1BKodQ1tTGaAJAJDAROkDpFK+IfDLZSwPispOYCSVAgiFJBkwdI19as4TiYRchlF1eSqxrzFYhpMQJzEDvGuzjGUcxfPn9s80vB9x+DLQXB2lD5wAeeCA3MdQD0ojiN0HQdKCwGOAsW1tqFUIAAJ2jSM2setDX8RXy1s/Vsaj7nRTxFI9vXPOgbr1z3agK6VNSiuREmQipTXjVHPVW1MXkwq3Kvt3aEW2ZphhMGTOkwGaPJVLHfyFTuOeETJNjDE8XCCymUs5lU1jQIwZu0LPXvpVeEw153W5kXKtplEE8rsQZDEAGYAPoN+kbK6lRIKk6wJObmgeWobUGJBnpXvMzO1wltzLGToQD1nYsB6CPLsQbbSi8fI6eySSbOTjdy2ypfsssZgXI5djHMNJLCImo4q/eaUtowGXOACNATALDcVbwW1N22NY8QSxIynMwAB6H18yO0ncYsZNVtw2UZmBytLMhFskZQCpa8YnXU9RFKll8I3ascsU8CxDW0d73zsZgnQLynvvOU/WreLY9lEr85GcDrCfPPkVb9KnjrQ8J2YgMoIJ1IzAkBf5jDHXcODpGk8Nw65dTE3JUC34dkAiXZ3bNdW33dbazlETpJEaClLOMBScUs5+RmvibihxTW3UQFVVA+pLH84+gpPk1106j1Ij9P0rR/BvA/tONNgnMnhlyCPDmBpO5Bk6jaR21N3xNwZcNimskQDlYCc3KRJ166hqLe1Lbj6+BfDZp/9md5Vw+TqrEH8iPpBFMPjawctx00KlbnURCCRI6e/odqV/C2ENp8yxlv21dF2E2lRB6ZpRterGmWOxhvWLrIdSjKDouuUgnXYAa1HqptbZL3WQ8tYMt8HWbj4x3IibVojXdlgMDHYFae/F+Jzvbs5CbuW64HTKoUk3CDt0Hck0t4AhsPaaWKthnzHqtwNZIU/wCIgNp3FMsAqXr9y/dbmORQNABaTKWE9ROZjVrkkt3sBz0NU4qtpLaXSfE8NMwAAhsgLDoO+g7UdhMYlwShnvIIIn1/tWQxqFrilwRm59dx4xDhY3kEgZfI/UvhKxc0P3gFEzrmykjy5THrXBnoITjvbeX58DopPyaJ8WksMwlQCw3IBmNPoRVges4+BcWUa2gzEqxyHw2IOXSZEBc1zrsBudKdZ+8TpMaCesCpdTpoVJJS58r2MUueA/PXmeh0erM1c2UQ9xzNVFyrm0oa69bXwz2Sm4p6VQbhFEZqruJNXVSz2AynGWvFttbkDMCNRmGumq9ayzf7OvFztcuBXMZDbHKOYlsykDQzsCInyFbbC2qYIlXV3OHERLim8sx+G+DcPbspZZTcCmcx5CSTP3IgT/5q3GcDtNZuWUtogcRygDmA5WPeCBvWquW6BxFrtTFdJvlmbUj5Nw5b7MmGiVNxZLEgKVJ8RFPmJ2/D320x+FbqXCLLKbLiP4hLtb2Ec05xqxAIPaRvV9jClccTrlZmuDtItBdPqx271qLTDuKLWaiUGtiXKM2RfZ84tfDfEg4KWkB1BuNcUZspgMFQ8oIgxruZ6CtFwb4EVHW/iLpuvAZ0KoUNwwTLlZdQR2EwPStrZwzESFMaaxproNaPt8FutuAvqf2mufbqNZettcPyX/bPKuC7E146UvYzWqufDlw/eT8/2of/AIUufjT8/wBqXpvs/Uw7g/0NlJGaNdNaP/hG5/1E9jS7iPAMRaE5Q690lo9ViavenugsuLFsUu1U568dqhXoSYtiDCYeTNNLWDZxkQHMdoBJ3B0jXpuK2WF+FsPYAzFrrefKv9I/uTTexhgBCqEHZRH5CqadHOOG3hh16aXbeDL4HgF7IiMEQcw5ogKRBIAkzqwgkaGjeD8Hwq+L9oynI7C2X5VyumUuATENzCJO0a05u4RwZCux2GhygaTp9B7Uu4hw+6ysotHKdCCPukax+1WqvDTxnBbGtbWnI+d2btxMWoRC9srmZwgYWwmY+ITGgPynNoQRGwFaXFPHiKzN4g5kBGlxQuYtMn8LSRBOUTpAo638LFY0VFAghiWaJmADOXUDfsN4qrEcLt5kuQDdQZA2ZgAmUpEAQxys2/fyp8k3BroBRxJPszGN4bacXDaBRCt1lRiSwyiysMdZzG25EeY6V1nibrh8HbylxadcRKECbuS5by3DPVGYmT5GBpTHGcDDtn8a4GnSCDGsgCegO1Vf7huCMt46bBl66R8pG0D2pLdrjjHP4iZZ9jOYniVu1jDftG6qOcrKuZSAUdjrOaCysNtAN9qH4jxC3fv23lsoCowYkkwx5VO/ymBWiv8AwxfENlF2JkAnMdIGhMFj15vOlWL4UBCNaIMAS0oxY6ll0308+gjsDlixSnkBPDyzScPzCxg7ogWlZLajchBZdDJO5zW1qq3avOSMwIJYLABBK/8AMg982afOhGzrZNkElQ4cKQA0hZy5s3LOknXfz1J4M/hKS9nxFa47hRGjXCHJGbpmIifKgtlB9MprujHs48MueIALssYzKXJUZpbmUkjKQpMHQx5V7xO0lm6qNJBUFQO6g5g46iRGXqDBEVRczm4XtWltIiratBSxYhGQrnfNzQqEeQOXaZt4liOUKQBqAp0AB0BUeZ118iOtKVsUpJM2V8Zcvwe3r7XLoukHlWHAMTy5TsJZoJ/qmmeGtIJa0BJzOdQQGAIbb5TO8RqBtFZ63bzAIdRJ6TM5Zn86YYO2llboicyhZEQsZtx69Km3cxUW1j8vw+gn1sy6wv8Awd3cQwAD/NEsIiC3NEfUfWarXE1RZVsULj2wc6fMkMQdPut00GxjbegbTmpL6pObm+m+PwCUhyt+aJtzQOAtk02tWSaSql5PZJFZFB4hYpmlmqb2Hms9KPgJMWKJoq3brlswavc5ULn5V30J/T+9HXU5PCNbwj1YWJ6mKW4r4lspI6zA1EGdiDtqMx+lL74t3DnJJIIM7RvH05jXi4W2NUAHmAAT5z1qmMIrsnlY/BTjOO3iA6jKrZtGGSN8vzETH4tdttdUd/4puLI+ZjrvsT/i8oj0Udqb4jAhz39j+tDf7rt9p9QDpTY2RX9ItykwB/i1RaUAc6kEFvl0AGs6nqdtZPelB4riXAVBoN+c9wYkRoNf9bP7nCLZ0CBok7aAqSDFSt4BBMIO0gCdIB89JFOWoX9pj3MhgOLyo+0PeVtmOYMhgyIETpvtPnTWx8RASVvXzOph3AM9YmJ1pTfwqgiATmPnmIH4B56+1GWuA4i5GS3kTu8oI6aak9pgfWhUJzfDf0Z7DHfDfjR0ACeI6783NuddTr1H9Qpvh/8AaGkEtaYwSJXXUEDb6is5a+GrgicQoj7qqYiSYkttqRt2q1fh5J5rznbSABpr03qqFeoh03+YaizbYL4rs3RKnyynQyDBmmFniKnWfpWN4fwrDqZJYnvMH/XrTQYN97bhh2PK37fpVsHNr4uyiEVjkZ8S4PhsRJYZHP30gE/zDZvrr50gb4OadL6EdJBB+o1plh1uyZRoG8g/l39aLBcaC2fY0qdMJPLieeni/J5iHy7iP1qNnHkmEH1rxsJm1cmO3X36VVevZRlQZR5U1RfY5yXQf9sK6l58qCxfFmNKcTcNKcZiiNzXpWbegVBNh2N4ix0zUsu4lu9BvjRVa4oGpZzz5KYwwHJijVy4+KDtxXrFaxTfuecF7DFOKR1r2/xBGENr6iRWfxLjvFLr2LbaZrXa/PIPoxZpLvC7NzVXKGCNDAggg6DyNDrwXEDRbyMJmTyncsBsRoTOwpPhsaR1o9OKkbGh/ly7QmWlXgjcwGLXMPDkTIKlTzGJgH/uiZjNsdq8uYK9IzWbjfLqFkDKCYYnue3lVtzj5Ubkb7Ed6jhfi0lkDbMwBGuxPka96VQt6V+5K1hLxygWtcxB1VSdzsW0nTfXSmacIKkeO4GUHkQaEkg5ix9PzPemtniVtgVKx/iDMWH9RM+lYb4p+IihZJ+UlSR1IMad610V1/Nmw06zz0aS5xVbRFuwvMxgKm5P96PxHDTAuXOW4wk6qyMY1EjZvXcz61884Rj2tqbrGHbQd8vRfetbwtcRcGa8SqyCE+9p37frS9TKGz+Z9F7D7I1qPt/k0HD7FObWHpZgjBp3argSmuiOJWbVVlKKYVQ5qeU3B5DFly2M0aydlXcn+w86S4vi9y3cNm8sDpMFGXyI0PSmPHsDdb+JYcBwuXKdmGbNoeh6VguI8QuXA1q6Crr91pBVhsRX0OgshKvMfvefmUVxjg0tzh6OQ1lgjAg5TqrDXlnfrPXpQN7AX7bANbJAB1DCN+UgZpn1HbTUxluCfETI5VyZGhH9x3HnX0jCY+34QdxnLCYJ5QDtp1MVV6ULHysMVZp13Eyji6YHhXQToIRoWYHNG3X2JmvTZxUsVtOTrAIAEGdyem2hEgjemfGPiYW3VVkSJPMzddIzEx1oKx8TM+pJ38vPvWehVF4bAWlfuWWuFYqB8ijT5mkga7gdZJO/WOxq2xwEADxb2YgzygKJy5faKHPFzt/eg8Tj52NexXEYtKvJpbGItWzyxPcAT9TVlzi3nWKXGtO9HYe7O7UUbX1HgcqIo0D8RmqLmNJoa2VqZArznL3CVcfYsTEtR+Fx7Kd6SteArkxorIzw+zXHg3GD4sw6zTReMaaj/XvXz/C4vXlNM1vtFVRtbRPKpDy7jh3pdiMaBSjE46OtJcZxTeDQTvwFGpscY/igE1lOJcXLHegsfjyetKDLGpJWOQ9RURg2Oq6xjTS0WDR2Gw1JYxDexjTFSOKoe3h6jdsEVm5oPBHGI7/IwB89qVXMFiplfDP1bX6RpR7MRV9jERTISi+xUoszuJx2Isgtcs8ojVTPl1Ar3D8ftt82Zf5gf12rT4kBlgxGhPXYyB7gUtxuGRtMoknoKa4V4ATkmDfbLLDS4n9Q7zULLIrqxu2xBBEsu4+tUNwu0vQUNft212UT0ga0tJJ8M1yflGou/E1tFIBDsfwEkfUx+k0iSyXY3bupJLR5kyT61RhbGoJHou//AJNMLeEuXWCW1Lk6Qon9Onc7UUpqPLYL5I4PCviHyqwVQfmM5QegJGoHnrX1DhFhxaQXDLAamZ9NeukUj4b8G3lAlgnpB/Sa1qYbw1CgkwAJO5jqa5H2hrasRhB5eecciNQ04pJntkQaa2H0pQbsVKzjYNSOvetyJFLA7NUXKoXGioXMQKlnBsZuPXevkfxPgsQl1r1xgxJIKglmCgkAnoBtAnbtX1G5erK8U4KzsxW5oxJytGk7ie31rsfZ2K8qXkbRNZabwYC5YFwBgYboe9NuFfEQRBau6MugJ+WOknp60Pj+GXLDkMIB1kaqfMEdfKgMZYzevQ9D/lXUU032U9coYcSvLdZWFy2YEcrg6VTZdF+Zl9xSdLaEwy69J19jRS8NtHZQKySz2wlL2Rfe4xZT78x25v0oW1xxrrFbNp2I76b0wwXDLaH5QQZ38/8AOm2EsqrFlUCQoIGmgmD+Zoo1w8mOUhIlnFt/6aAdi5n/AOtMsHZvLq5WOykn3kCjb2IjSgzcJNDOUF0jYp+RiMRFTbGGN6AS2TVxw5ik7mPSB8TjTQhxxq7E4el1ywa1AsbYPihU71obXG9BWDdCKuTFmKYptCmk+x5jMd50qu4gmoEljA1pvg+FBOa4MzdE6D+f/wDPvHVEpqKyzLLYwWWA4Ph2eGuEqnpLN/KP77VqMHbwQAUW3HmQD7wf7UH4JOp/15AdB5ValqonrHu4OdLVzbzHoZnhGHf5CD6b+29UvwIDaqbYom3iHHWfXWqY6lPtDIa/H3kL7vD3XahnLDcVolxJ6gGvfs63Nhr2pqlCXTLq9TXPpmUukHcUNctdRTvG8PgmFPtQGZVMPtXtuCjhixsWwG1BvjCx10HU1oL1nDv8twk9QBHu50FCPwZJmZjZVIAH1J/PWi344bETcU+xI10togI/xNqfoKmmBCauQs6y258wNWP0BrR4fg7H5StvzHO/0Ow+kHzom18LJMtcJkyTGp+pNLd8F5Fu2vzIR8Ds27l4IxKIZHiMNCegidB5mPSvrOBwlu0MttFUeQAnzMbmsuvw/Y0hmXy0J9/8q1Fq8K4f2vqI2bVB++RV04yxtYYTQt81Nrwoa7crkVRbkJYNeoB3Iou/cpNisWM1dyjK4EyQxt4jzq77R51nXx3nUreNmnOGQDRm7pQl27QNnHAbmvXxA702EGEQxd3SDqOxrMcasqqZwN2+RQJjqw1+nSe+lOsVepLe4nZB/iBzG2XL/ciunXX8PQ7T2KM/ieEKThVuCFYMT906NP8AKQCfpI86rVWt7gkDpsw+v70RfxuGZj/DuKv/AGuT3P3Y9NavXF2jA8Qkf+6pkeSspJH6eVFKufsVq2p9SBBitJUkjqDuKMs48kbVIYSw5kXFQ9OdW/TX6ZaOw+DsKea6q9SBDD8jK+hoPiSGRcW+wW2C2tE21Aoi61oaIQfMVZYwmbcGl4KFggj9hV9vDO1OcPglVczaDuai3EEX5B9a14j2xU7oR7YJa4MTvRCcAtAS5AHcmB7mqr3Ebh2MfmfzpbeYsZYknuTP6171F4IrNcv6UM7uHwQ01f8AlE/mYFJ73B8KWJVrqg9MoMfnVyCp5K1Nsm/i7Ge4LhvhfKCX6vB08k/ei7eFP4T7GvK6prqd3klsnKyWZMuGGb8J9jUWtH8J9jXV1Tfwab7PIrKt+E+xq62p7H2NdXVRHSpLsFok09j7VUSw6N7GurqyWlT8mpHPibo6sekHMV9joPUa0sx6597RnyzR7f511dTq6Jf3Mo9ayPUmBpZI0CEDsAatVWH3W9jXV1E9FF9sDvlhdm64+63saKF9/wAJ9jXV1JloY+7CRNMQ/Y+xoq1j3HQ+xrq6ky+zK35CyHpiyRsfY14149jXV1BHQVw6GpgmKxBA2Psaz+JVyZyt7Gurqpho4+4EmDG234W9jV1tWH3W9jXV1PWjS8gI5mf8LexqBdx91vY11dToaZLyeyB4t7hHyv7Gkl6xcJ+R/wCk/tXV1W11pAtFP2W5/wBN/wClv2r0Ya5/03/pb9q6upu0zaWDC3PwP/Sf2oizhnH3G/pP7V1dQSgewNcCMupsk+mZf7H8qcW+J3tlUoP8Iafq2/tFdXVLKleGN9ezGNxK5duuZfO3rJj0qORvwn2NdXVNLTpvsW+eWSCN2PsaibLdj7GurqNUL3B2nC234T7GpQ34T7GurqYqkZtP/9k=</t>
-  </si>
-  <si>
     <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUSEhISFhUXFhgXGBgXGBgYGBgYFRgWGhcZGBYYHiggGhsmGxYVITEiJSkrLi4uGB8zODMtNygtLi0BCgoKDg0OGxAQGy0lICYwLy0tLS8tLS8vLS0rLS0tLS0tKy8tLS0tLy0vLS0tLS8tLS0vLS0tLS0tLS0tLS0tLf/AABEIAL4BCgMBEQACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAAAgMEBQYBB//EAD8QAAICAAQEBAQEBQEIAgMBAAECAxEABBIhBRMiMQZBUWEUIzJxgZGhsQczQlLwwRUkcoKy0eHxYqJDU4MW/8QAGgEAAgMBAQAAAAAAAAAAAAAAAAIBAwUEBv/EADoRAAIBAgQDBgUDBAAGAwAAAAABAgMRBBIhMRNBUQVhcYGh8CKRsdHhFDLBI0JS8SQ0Q1NysgYVM//aAAwDAQACEQMRAD8AYyeWG19vX0+/tjRk7GfGJf5DhpvSdr3B+24P3B/THLUq2eTm9jpp09M3LmaBOFWLqifL0PmPz/fGb/8AYxcoy6prwa9+p1/prXXRr5MXHwoALt9Kk/iAwH6nFNHtGLUL8otv6e/Esnh9ZW5tL+SpzvCj2/En0HqPc+X3xo0MTmUY/wBzV33JnLUo2u+S08WUWeytE0O2329vv/n274TT2OSUWtyjzEOHKmipzUWHTKpIp8wlHDFS0ZAmwjRfAj6h6jEFtmdwEBgA4GB7HAS00dwEHUFmrA9z2H5YAOYAAHAAYADAAYADABwMPXATZnSfcfmMAWYYCDqtXp+QP74AOpXnfY9vWtvwvAAnAAYADAAYADAAYADAB7VwnKN3HUPbv/6++OatNxV0r9x0UopuzdjY8Oyg0gfl6g+3t7Y8pjMXn+CDuuXKUWv496NGvCGTVrX0aLqHLYrhhpVHeW718xZTtsLbLbYeWCVtBVV1IGby2xGEhVlSk1Juz3a3fcunvwLNJW7tuniZfi3D63YhR6XX69z9h+ePTYes2lmWVclz8zPq01f4der5GWz8HoD+I0j8F740E7nFJFBnEw5Uykza4dFEyw8CcSaDPwaUifmyRwMJF1AJLLGGKixTbbHfz2xVWjeJ04aVpWPS87Kmal4zlpVghjy8MSLIsVsiyLIzuQN2YeQFdh98caWVRZ3u2plYv4S/PzEcmbIihaFVZIWd3M9VaKekKWFncVZOkA4tdfRaFXAXUpPDvh8QcdiyU2iURzkHbpcCMuhKm/8A4mt/TfDylenmQsYWnY3Xi7gk3EWggkiysKtnsxFHmY+uQJEuaKxvBpXuIRZ5ndQaxTCShd9xfKKkrFBkv4TxuZL4grLG6QkwwmUid2oowVzpC6ku+1knSBh3Xa5FXAXUTwn+EbSK3MzehzPLBGFhZ1JhL9bsG6A3Lbv22FkkDBKvbZAqKGuH/wAKxJFGzZ0LLLl5Jli5JIHJMYcGTXRAMii6B3sDY4HX12BUVbctPEnhOPNcPy2YWZY3g4THPyxHfMCxhmLOCACarzNm/vEZuM2u8Z07pIreIfwo5ce2cDTIcvzU5RCquZk0Aq5bq09Rrz0/02MSq/cJwV1G5P4VMGlQZxSY83Fld4tIPNigkL/zDVCYgLvZUbi9p4/cTwF1FyfwuQ5yLKxZ9GLCUyhoyssYhNauSWtlc/SxoVuCwIxCr6XsHAV9zNeO/Cv+z2i0ymWOeLmIWjaJx6q8bbg7r3o7kUKxZTqZ0JOnlaPW/E2QZzkomGRTJOcpzdSFp2k5oKoqrty3IjQk9tTE7DHLFpXetzpJGYGTWfic/Oy4fLwwxm8oxGVX5rixfzixYk6a+hQe2DWyDQwWd/hKyZcMmZuYJAzo0bCP57aKWbsxUhidroCwLGLv1CvsU8HTcnZH+G+VgzkCvnUnCziGeJoipLtDzFAGo2ptBfYau+xGIdVuOxKpJMxHjTLQ5biE6ZZ1ZFkcVy9KxkswaIK96tHbV2PcYuptuKuU1ElLQz2HKwwAGAAwAGAAwAGAD37gkIsdDA+oAH/ScZWN/a/hl4x3NHDX/wAl5myyaff8e+PMRvOs3K/mrPzO6bstLeWxZRLjdoU0ckmOMuOiUFYW5DzK4xcZFJXR0U3czXGCRuoUH17n88dnZidvhjHxzXfp+CMS1b4m/C1kYbidk9Rv8/8AU49FG/MypGfzYxYUspM6MMiiYxwnNrDmYJmBKxTRSMBVkRurECyBdD1ws1dNFlGVpJmqfx1ludxZ+XPWeSNYulLUojqeZ17C2Ha8c/Cdorod3FjqXj/xQyUkua1rnoopjAyvEVSUGGtaEq/SG0gWpshm7bHCcGStsTxYmHy3iaKPiy8QWOYxLNqCO5kl0aNG7uxLPW9Fva63xc4NwylamlO5tW/iVw9JIeVFnNEedmzTlhGS3PizIYKNYqpMwKB8gd7708GXMt40Sq8K+OspDHm4p/jUWfONmlbLsEfSWU8pmDgrYQA6T2Y7jY4edOTs10IVaJO4b/EfJcnlSrxFAmYmmQQzMDKkhkKJLNzRISOYCeruqmyNsK6Mr3VgVWNrCOGfxKysYyuqLM3Dk8xA9BGt52y7KVZpLZRyWsmjuNjvgdGTuCrRI4/iDlfg/h+XmNX+y/gr0pp5vL06vrvRfnV+2J4TzX77hxok/iv8UMo8TPHDmOfL8MJFbRy1GWk1nSwNkm2AsenbEKjK4OrE5xv+I3DpRKqwZtxLmocw4bQg+WkKEIyPqUgQqR/8vMA7RGjJcyXViSm/itkknyzLFmpEjEwaWXRzlWUgqidXWBSgliDSKbY2cCoSsyOLG6MD4741BmmiGXObZY4tBkzUrSSSMatqZ2CDYfTQJJ2FDF1OLitSupNN6Gk494x4XmJcpmeTnRmcscqASIgnLgmWRxQcksRrrtuRdYrjTmk1dWLOLDciZzxvl3PGCEm/39YhFap0mNHU8zr2+oVWrzw3Ddo9xHFjqXHGP4lZSWNZFTPGcLAvKMpTLqYZNbtSPTlga6lN6U2G+EVGSdtCXViNcU8d8MOajzkOVnaY5lJ5ZHWIOiJEsRjiIbf6QaJqy2++wqU7WbJdWJiPGXEMvmM3LPlVmVJWMhEunVzHJL1pJAWztvi6CaVmc9Rpu6KXDiCnIvYUPS7/AFwAcFYAOYADAAYADAB73wKrA1kn0Xc/jXbGXjIqUbXk+6JoYaTTvaK72bPJsB/7v9seWUeDWytW7r3fmd8viV73LOJ8bVGsrHLKI4z46Z1VYVIhZqTbGNjKt1Y6KcTNcZlFfSrfar/Ju+O/s+hopZIyXVfyn+Ba87aZmn0f4MRxJ1s7UfQqR+2PQQWmhlTepn82cWooZSZ04dFEyrmxDGgQ2wh0I5gAMABgAMABgAMABgAMAHSMAHMABgAMABgAMABgAMABgAMABgAMABgAMABgA9m4bn62FAe2w/8AP3OKKsHJWvYupySd2rmu4XngQCTt5e/v9sebxuDik5RVorbrKXLvt7XdrUqub4W7v0S+5dw5rGdmq0m4yW1k/Fq9h3FS1XMdOZ3r/NsWcepJ5YrXVea1YvDS1K3O54L59+xHrizDYaVSUZN2v+2S5Nbp+/5Q0pKKfO267uplOL5oMTvpb2+lh/n+DHpMPRUdbWlzts/fzM6tVb0vdd/Iy2dnPY/l/nbHekcTZS5p8MiqTKbNNvh0UN3ZXTHCsugiKcKWhgAMABgAMABgA6cAHMABgAMABgAMABgAMABgAMABgAMABgAXHKVujVgg/Y9xgJEYCAwAGAAwAej5TMV3/L1+/tiGrhGRfZbiddz9/wDP8/bFMqabUny2LozaVlzLvKcWrSCfMX9ybP6CvwxwSwSeW/8AlmfidaxO/hZCn42RRvsQf2vCRwKSut1PN78hnibu3WNiHxPiFllvY/ofL9Nvwx208PGN1bR6+ZzSrN2fNGczWdJ2O/8Anf2OOpI55SKnMz4dFTZH4dIvPTWgdbNqWRb6WrdyFJBohWIDEBfPBJfCLFrMkyVm+BZW2ZsylXIdUbxBGKtKOVHGWLI1IjWbWmof0lq+JJLYuVGDd7kZPDuSkLVmyAA2zPFZoQtrB2BCiVgV2JMbG1F6VdSS5e9SyNKBV8G4HBLl1leXS5kdeXzIkL6YmZFTVdFmXTqagLACmxcym07ExhFot28M5J10rmYxy13cSRWxM0xIcWQxEahdSkDYEagQMJxJX2HcItGd+FyvMzHXLyoktKaPXI4lij2Naap3ehZpfucWXlZCZY3ZoX8NZOFnJnSSoZCFMsVI3KzADEijL8xI9IQAgsCSRWqvPJ8veg2SKDMeGMmrEiZWB5pVVni09EuX0mzvo5csp06i1QnquwBVJdCXTiQ87wDJoGfn2o5jDTJFUmmKeTRGLZ0KtHHGWe9RkBHkGlTl0B04mc4pl1jmljR9aJI6q+x1KrEK1jbcAHb1xbF3RRJJPQjYkUMABgAMABgAMABgAMABgAMABgAMABgA7Yqq3vv/AKV/nfABzAAYADABscvmMMVpk6DM4UbMTYs8fXff9v8A3iLDZgkz37D9sGUnMJnztgb+Vf8Ab9bwWFciBLMTiSCLy2a8K6iiCg5FPmnIJB7jyxbyujnad7MsYOFwSZRpTIqyLHI+nUosq1AMGJJJHYAC773pDUym1Kx106cXC5zg/AspMEV8wyyGHmt1RhR80ppW/wCpVXmEEiwf6RbYWc5LkWwhGyLE8GyOYZEWSOEKD2ZNbgQ5A2zHZiGlzLeV6WFgAlVzSV375j5YuyIuW8M5RqDTkWICJObAIysh+dKEvUFQkLpJBB7+YEupLoRw4jfEeBZaGDMssgkkVUCgvGeWxkyhIoU0jFXnGoADSjWLsKKbbXvqDhFJjw8O5SRInMxivLxyOBokBEcEL5hwqWyH+ctN3l0gdzRnkm0M6cWQuAZDKNlnmm1Fhz1K8yMadMcTRFFI1F2LSANuOhtsTNyukhIRja4jxHwGDLxK8WYWYmRkNFaIVpBYUbrWhfMg6wdhWqYTbdmiJwSV0Z3FhSGAAwEm34twfKSM0nMhi+XfLjeCoBUxBkKswzFssajRTFXQkWQGojKS9+7HQ4xe4yvh3IM5Rc0RTOLaWGnCPmEVVYL0lzFEwY2AJhsdiZzz6EZIEHJ8Dy7y5hDPSxyKqNrhWkbmapm1GpFTSgKobOvatgWc3ZOxCpxuyxymSyMuecHQsMRy2hebEqMgaETGR2HzNi5NEE74VuSiMlFyIGY4HlPhWnjzFvpRhGZIiyaliJVxsXJLSi1quXuDZqVOV7NCuEbXRN4TwvIa4HllU9MLunMQJenJh0YNZstPKx3FclxX9sSlLVL3uMowOQeH8lMz1mQgV4QWMsCqea0Rk0RgDpVHfe9jEdjuFM8lyIyReoxl+BZKSFJlncFtfy3lgV9SrLURLActiUjIcgipaqwNUuck7WBQgMtkMo+azKl9KfGCGERyRqvLkfMdetgRy1EcY1DbrHtc3korwIyxbZbw+H8hGZQ08UgK9LNNFSHXEVXSrB2cpqOsUtEirukc5Pl71GUIr34DOa8NZKMP/vCsQjmzNEyp8nMaTSANKebGlBa+pdmH1CqSfL3oGSIzP4dyS2DmiCWKKObA9CpykzMm3Lblx9GxGsWTakznl0IdOHUyAxcc4YADABdQ5isWHKm0TI81iGh8w+uaxFiVIUc1iLE5hBzWJsK5WJsK2AR2OOac7F8VcUSI2Bb6GNE+St5E+xxRNucWluvUthaL12GfFmQXSjx0XNg6SDYUD0898VYHEycpQlsuveW4qhGyktzGM141DkSsbPhPA4Z8tlFICaxIZZQqagVlzNAu0tg6Ej6REdqN7455SakzrUYuKEZHw3lBOInlkkdESRgOWsZuWJWWy10FaRm86G3beXUla4qhFOxFy/h7Ly51IVmIikQvq6LSndCDvRrTq230ke7Cc7UbkOCciRkfC+WLIGnJZdHMj+WC7MkDlIyWGy82TVe9RNW+FdSVthuFE5wjhuWLZx2ZwiSSpoRlCGLRO8ZNkF6kii0i61BLvyJSlZBGMbsjca8NwQ5czR5nmHWAF6dg3ZGo7OFKt6EHt54aNRt2aFlTSjczOLSgMABgA45oE4CUruxt5v4esrSDnSVHd3lzq6ZXQnlrIXoqjOhAbWAR0mrpVa/Iv4K6gP4fm6M0opnU/wC7ksdFUERZCZGKnVS3pCtqIYacHG7g4K6le3hQLPloWlk0zqzahCVNqD0pG7BntgFBIW7BF4niaN9COErocz/hqFRr5zxoscZdWiGpZDHkdVgy9i2c1GyNOhhRoYFUe1vepLpIczPgZ1upWOksGDQlGCquYPNK6z8kmBQr31czyqmjjdwcFdR3i/g6OCJlMrGZTK9mPSCsUTvormGgVTUGonrAIUg0RqNsHTVrEfLeF4ny0cnMkDy6CjGP5YbTnC8Ybmbi4EtqtenbqoS6jUmugRpxcRGZ8H6c3FlRM7a1YlxCRQTVbIruoljpdQdW3F0LFGVU0uK6aTSHs34MSMW88opTZ5AKs6JmpJFRjKL0jKsvrqdbryVVb8huCuopPA1tp5715OuXZ0oy8sJauTz6IkMQBpOrVQwcXuDgrqOjwUkSyPPJKAIif5QFPbgGMiYrMU5ZDCwAXTc3eDi32J4cUrsY4h4KWBGkkzR0orMxSBmB0uEqNy6o7Wd1sFSK37gVW/IjhLqVviXw62UIp2kWt35TogJLadLNYdGCkqwPUAdhWHhPMVzhl2KPDlYYAJSS4a5S4jwmxNxMg4JsTcXKzvP98GgZWJ52C4ZC78NZoMTEe/df9R/r+eOHGKyzo7MP/iar/ZYlUow2YUf+498Y88Xw3mXI7lSzKxnDkFysiZeWVS7KXutKgWQosnuaY/p9+xYl4iDqQjotPuRClGnJRkyn8UcPVJNUdEFQzUbFktZ2+wx04Ks5w+LrYTFU1Gfw9LifDvBI8wk7ySGPlKrXSkEU7NYJB+mM0e19/IHqnJq1imEbplzmPCWUVzGcxKp1ALqERFPLLEhYhh/Yrmv6WGK1Vla9h3TjcZl8JQhHYZgkrDLIt8sLIY1jYSKwc6Ym1sAWo2lXZIE8V9A4SJHEfCeWhE0TTNzA9JqCB15aZ4nWoYjlyGCMg/Vuu2/VCqSethuHGwznPCmUjkVGzhpnhjVwq6bmM45pth8qolax/fV7WZVST5CcOPUovEHChl5SqkslgAmgdWiN2UjvY5g3oX+YDwlmQk45Ssw5WGAAwAcIwEo2fG/CZlkeaM0smt0MutpJX+ezmQCJeQ3yXBDDSGU0Su4pjUsrHTKDbumMf/4Ji5RZ4GKl9fS4pYmnRzbKAabLyADz6e14ON3C8N9SJw7woZZZYRJGGSZItW5RtaZhhQC2SxhUCyN2qiSKZ1LK5Cp35i/DvhX4iPns+mMGUEaW1DRDI4YdJ1AOFBAs713xE6ltAjTvuPSeB5IxrM0YVbdmRJSyAMgQ6VTUHOtDpoEDVv0NRxV0J4b6ljmPDEuYd0zOZjOYUBUVUbQpbNtF1aIwCGkMrEgXvqPphc6jstPwM4OW7IuR8Bnmxc2WPQzRBxHqZwZTHSjSpAsSDrPSPyuXW0dhVS2uyo4X4ZabLjMa0RCX1Wr7COKaUvsOoVA42veh608qlnYjht8yVxXwp8Ll5ZZHBdXUIEB06OZNGWJK1ZMNhQbAq+9BVUzSSRLpu253N+DGVJXE+XYxyNCQSY+uMoHXVKFUACRDZNfVuK3lVe4jhu25JbwhNIsTy5mAfLjAFl9CO6JCAYwQwJlG4NDfc4XiJN2RLpt7sQ3gnTGZDNGKDMGVZGDBXii06AmoU8jdVnZew74OLqHD03FZjwE6FqnhoNL/AEuGKQczmOI61E3Cw0jv0m6Oxxl0B0n1KPxDklgzM0KElUcqCe5A9dhiyDurlU1Z2RX4YQ6DgAUHxNyLCubguRlDm4LhlOGXBcMpN4Lm4o5Vkl5pCkEcsi7Hrfce1jHPiYVJ03GFtepdScYyvI9c4FxvJzAFJVBPk/Qb9OrY/gceLx+GxlK7cG13a/TU16NSjL+756GB8dwmaaWZdwraf+ROmx+IJ/E49J2T/Sw8IS3au/F6/jyM/FfHUk1t9iP4dzEcg0uyqw/uIAYe1/ti7FqcNYptdxZhcktG0io41kRHI+gdAYgHvX446sPUc6act7HPXhknJR2K6sXlIFR6YAuxyaVnZnYlmZizE7ksxskn1JN4ErA22IrAAAYCAwAGAAwAcY0CcBKV2aPjnCc1AX1zlgziBrkbUV1TLGJRZGk8iXbUwGn3BNcZRfIulGS5juf4FNl4pJZJnEiWw0s1GnyRVramBvOO24BBX3OIUlJ6L3r9iXBrmP5fwzmdOtcwROzOXAkI00uXI5kljr05prrV6Xuah1I9NP8Af2BQfXUjpwDOQoGGZSOKuaXEzoiqTGI32AJ164qKg9xemtpzxfIhU5LZjrcAza6WGbUaWPXzZAkbyrl2AD/UJHOZW6Wu5LEXRnj0Jyy6jS+Gs6mqpVVhGdaiVtSroSQxMFFklZQ1CxQYkgAnBxIdCOHJczmS4PmpYYZMvOzNyXPK5jCRVEssYWNfNWMSKFB3dgK88S5JNponLKysxPDPD2cl50MUqhYpOW45rCMuxK0ABRsqRZoH1OBzirNoVQlqrjg8L5yRBUqPGxZ9pHZToEmuTTp6qMUinSC1r2ogmOJHoTw5dRcPhnMASiXMKi6XaSpGYFk52hpQAQyk5eaiNR6brcWOa5L37ZKpvmxjM+Hs7EjI0g+SHZohKSY1USyatI6QG5DEUbvTdWMGeG5HDltcfi8L57UAsqg1KCRI+ldMghcMwFC2ddvINbaRvgzw6Bkl1M83EJvOaW9Qbd2+tQAG7/UAAL70BiyyK3KXUYkkLEsxJJNkk2SfUk98SK3cTgIDAAYADAAYADAAYALjw1mAJOW3Z+3/ABeX59vyxzYmLy5lyLaVm7M3uW4dYojbzGMKribGlTo3MT4q4ZHlJEjj1aqLkk3sTSKPLam98a2AxM8TBzltt9zjxVKNJqK33LDhDQTpTsgvZlJAP4X+hxViXVpSvFN99jpw0aVRWk0u65lZ4ChFjv2xqRknsZjTW41iSAwAGAAwAGAAwAGAAOAk0k/BuJyNTa3fWhr4iJm1iR0RiBJYIlkkXUfpZmBonFalBFzjPqMH4/N8wGQyBLV9U0QTzcgFnCsKy2q1sVCD2AOD4IkWnK+pOyuQ4kSsbyzRqiuN5VYoiWp+WH1csvCqB602qgHYDCycLXGUZ9TiZLi8PLS5o9ICRgzRqPmFgI1t6ZrRvl7sunsMTemwtUXMcyWS4qyQvFJOXp0RRIF0xKMuAQxYCizRKB3uNa3AqM0AUZ23ImQ+KTMJl5czPA0wjUFSsrVKESPWokGnoCdzqAC7dsM1Fq6REcylZsnZXJ5yNYvg5XnjWSTRGwWPRIj6BJyeadlkfWGvSrUWqyMK3F/uHtJbEbg0WfhXMZWHLIzrpdydPMjbSeU0b6wpYAlkrUbtl88TLI7NsWKkron57gOfyyKuXzMkoTXKyxOgWOuYrVUpLFjHP0heoKxq9SqqlB7oZxkloyl4lBno45HmlOnXypB8RG7FvmEoyK5NjmS2K21tdWcOsjdkVtTXMnSQ8QSKWabMyoIGLAc1JCZpGKOhCydLDmvrBtlEhtes4j4L2S3GtJLVklMlxS4j8S5ZpGUhZ0dlEvwzFyFcl7OYQkAErpBNWDiLw10JUZ23MnnclJEVEq6WZFkA1Kx0uNSk6SdJIINGjRG2+LU09iiSa3I+JFDAAYADAAYADAAYADABJ4fmhE4cxpJXk1199j3+94rq03UjlTa8CynNRd2rno/AvF0Mo643Q9jXWB+VH9MeXxnZNeP/AOck/R/b1NjD46k/3Jr1/PoUPiqD4l5JE3o9Huqiq/EC/vjU7O/4ejCEt+fi9fTY5MUuLUlKPl5GRy8xRgw/L1xryjdWOCLs7mtljhny7FWUtpsLY1A+W3fGSp1aVZJp2vvyNRxpTotpq9tr6mRmiKmiN8ayaaujKaa3EYkgMABgAMABgAMAACBuQCPMG6I8waINfYjAStzb8d4zxGScRLC6c1yoRokk50iSjdTJCuwKRKBpFCNSdyxNMYwtc6JSleyRQ5p88uuSRJlE8j62aLSHkZZo3FlaDFZZ1oV3at12dZXp0K7zV2TI87xSRiqpOz0VNZddekvIChYR6tHMWXputattqXaHGn7Y16nQUuZ4rIOYIZXDaZA4yiG2UFklDCL+ZTMRIOogk2cRaHthep0HcjmeKTS8lQbQrE6tBEI4hNJGo5kfKIC6ljP0mtNjzwNU0rkpzbsV2blz9LJJE6/DmLSxy6JytJ1xgkIKFyhqOxLqTdrhll5cxW5k/kcRgSOSJ2bVFzqjhkbTHLyswxdnhEbC+XqCswFFTtYK3g3ZjtTQjJ5HiZaVlgdeYpLh8uoRuXHI6gRmMqGIjcKVUbmrGrEtw2Fip6jWdzvEERnkJKtaSaoVIjdZJjofXHUcwMkjitwsy7i6AlB6IHnWo3xH/aEuqOWCQmRtZHwqKzOBZbojB103URubAa8CyLVfUhubJnFsrxM5YvMj8t2d3QQaG6SpaaXTEBZIW2Lajps7C8RFwzaDPO4jMub4pFUjJPHyQBqMCrpvkgFyY92+TALaz0qD33m0GRmqJFJnc/JKEDkERoI0AVECoCTQCADuzGzubw6ilsVSk3uRsSKGAAwAGAAwAGAAwAGAAwAT+C5rlyi/palP49j+B/1xTXhmg7bltGVpanoWWyePPVcQblLDmT8aZaOJkSNAt6nYgdyx239qbb3xp9mVZ1Yucn3LyODtGEaclCK735lNwvOcpwT9Pn/3x31qeeNjiozyyuzRcdykc0QkiKswO9EGgQbuvesZuFq1IVXCaaVjSxVKnOkpU2m78nsZJlINHuMa6dzJascwEC4YmYhVBJPkMRKSirsaMXJ2QvM5SSM06Mt9rGxr0PY4WFWE/wBruNUpTp/uVhnDlYYAOMLGAlOzNBxDjeaeRJniCvBKZr0Ps8jpJT6ydK6tJCjSOsnuxJrUY7dS1yl0Dis2aKLA2XVdcSPpjRzIYYeYsSsCzEKg1DtdBdRNA4IqK1Gk5vSxPzXiXiMUxWZQ7wOXIeMsoZFWLmWtULRiGBALSSHfWcKoQaugc5rRorzxLNA84RrUiRydKswCQJPk0vc6RXNG53IBw2WNrA5z3OZDjOZWZpFiV3bldJjc0cuU5TAKQbDRD2NNY9BxjawqlK+wNxvNNl1y2glGVUSlkBIVYlpQrBXsRxXYb1FXgyRTuDnJq1iTleO5qMI4ykZKwiMSGKazHCqxk3roUsWlitf1XiHCL5k55b2Iz8WzXz9UIJlchyY3tHkikhIWiKYpKwpr8qGJyR0BTnroLmzebzCyQtCPmu8xtHB1QRHWI9R0ghIyCANR+m96wJRWt/bC8pK1iVH4rzuoMsEerVpU8uQnWFVWFliWcqqA6iSAqgUBWI4ceoZ5dCHlfEOZy6heWgsSaWdGDAS8wPpYEWCXbY2LVTVqMTkiyOJJbobzHiaVo5YwkSLKzOwTmL1yaeY1cyjq0rYYECukLiVTRDqtlLhyoMABgA7WAArAAVgAKwAFYACsABWAB7KZl4m1oaYedA/uMJUpxqLLLYeFRwd4mx4D4qkbaREYj06TXr5j9sYmL7Jg9YSa9V/Br4XtOW0op+gjjOX+JZ2qtX035UKH7fqcW4T/AIanGHTf+RMQv1FSUuuxjXiYXYIo0fY+n32ONhST2Mpxa3Ljw3nDG+lgdDedbD7+2ObF0HUheO50YTEwpztJ6MsPEvB9WmSFQQQbIP2r/XHLgMRLWnV0a6nV2hRhaNSlqnzWpW8N8PSSHq6V9e5P2GOyvXVNaas4cPTVV72Ra/7PGVNagdgSao+e3c32xzQlLFRulzsdNRwwksrlyvsVPGppJmXoIVRQ3F79z+35Y6sPhXRT6s5cTj4VmuiIEHD5XOlUYn7bD7nsMWVKkaavN2EowdZ2hr75ljxLhMUEXVNqnJHQv0qPOz3/AG+2OKhiq1arpC0Or3fh7fiaOIwlChR+Kd6j5LZePteBTLsb/wA/TfGgZiZsMx4/mLq6Qxrp1UpZmUkgBdQ21BaHf0xSqKL+MVz+JmMwl5e3IbLleZISUfWSeaTq1W92b7D74bh/DYjja3JbeOJisqtGh5vMN2bUyNO1Am+kDMSLp9K3G9xwUHGIvDfFMkMKwiNSEVgp1MN2bMElwpqQVmHGk7bD1YGZU7u4KtZE6Lx/mRs0cJU3qpdJbUlHqHYmRpZTsbaZ/I1iHRQcYrc14lllzKZh1vQKCam07qVJF3RPc+RI3BG2JVO0bEOrd3LGTx1NrDrGFbma/wCY9V8Q+Y01ew1uwJ810jywvB9+ViXWG8r42mQJ8sFkWNQ2txsiwKSyg0zn4dCHO6350tS6KDjDmd8aMYwsUQQskyv1PpXmtm65S3SkLmQdW240gBdjCo66jOsuQjM+OJ3RlEaKWM3UpII5/Ps+uoHMSENf4dyZ4SF4xA454hbNIiyRLqRaDBj3qJWbT23WJRRv28gGjDK9BZVMysUlYcrCsABWAArABKMWGsU5jZPmMhIzxNHFGrRZVTOnc6ZMpzOWtUj6TmNbAGwg2+rVTlmtfH+Tqz09vA5l+FcN6S7gHXGHQT6kGo0yo4UFhRVi3YdQ1Ar1Q3Pl9AtT9sq+HZLKHaWtRnK/zaRY1AOrVpOqyCoNqN7sdw8s3LoJHJz6lwmR4dGk6rJG1mUK7MrMNPxHKVV0GgU5BLi+pyNiopPjbRYnTSeojOcL4cgflyKSFcg8wPVwShQikU5Myr6EalPTscCc3uD4auIk4VwwGuYd20jTLqAQlwsxPLHXQBMflt2ugXqEWpdSvyOSyr5Ql3AmVJSotV6rGkEAanJqhuavsASyu82bTYROGTV9S98McIywSN7RpXjZXRpAK+bAwIJW42CLL5eg3uzTiNIvPoupZh5xbShrLoauDg+UGnrJFC7ajVnU+ynqAqk77n0s4M68Ovr8/wDRvQpVOnv3zIXEshlWiZCoFCN9WoBtfKl1aRp6vmFFK+e2+1jv7Kle8l3L6X8N38jP7YVkoS739beO3qMJwTJI7FDrAjYLrYUbSYB6rd75PSaILE16a+abWvvYxFCknddPv+NCDwuIqulu2M3tPCTm1UorU1Ox8bGCdKu9Ovv3/Lk8BU9A7/lhcAliKfxvVaNcxu082Fq/01o9U+XeV03DGY2xJONmChTjaKsjz9RVass0ndioeBDu5oeg7nGdiO0nm4eGhnl6Lz9rvNXCdjrLxcXPJDp/c/L/AG+5Dk4ZV5cShF8/U4KfZ0ZVONiHmly6L38u4mt2tUhSdDCxyR5vm/t6vvKWbhZPdbxqWiYuaoncgzcIHoRiMiHWJmtyHLw1h23wrgy6OJi9yM0FdxhbFynfY5ysRYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMxYnLYa4mVmsznCci+qQFhpi5jCJ0K9KwKqkBPltJJI60bI0WRvihSmtPfM6ZQpvX6eRF4RksnyQZfqYaHPMUMpOYy9FEKkrUXMOrewGHns0nK+nvRiwjDLrv+UcbhuTjkyjJJrHMjM2sxlKtC9oOpQDrHUKIAIvzFKTTuDhBNWfiTZuFZOQs0siIdagCOXLfRaA9MUarfUxBAP0G+26KU0tF9R3GnJ6v1Qxw/J5Fo11Lp5gVWuZGkjY5kAkAx2umGmJqmFjajhm53096CxVO2unn3jJ4PFKuWkPSzkLMqlFoLpUMqgVHa7kt3bUarfDq6bXyKJSi1FrzLyHwvkwxqQ6RfZ1JvVsL09tHmLF3RNYhVJpbBKhTk9ZaeP46FnDwbKukf/wCPSq9mUtbS/MLdALnQTR3rSBQ7GHKd2t/9DRo07JrS3frvry6EoZGNYyQza77a1cAdO17Fu5Njt28sZGOwVGSz5beGnobXZ+MrR+DNfuevruRmy4PfHHSqLDpKHI761L9Q258xcOQU9sb1LFU6tsr1te3TxPO1cFUpXzLS9r9fAkLwz2xdmKcgjM8OKjUBddx7YycZTnRn+qo7r9y6r39/HawNSnXp/pK+z/a+j97fLZiYeHO+5GkennirhYnHa1nkp/4rd+P5+XMu4uF7P0oLPU/yey8Px8+Q83DPbGvRhClFQgrIxK06labnUd2WfB4YY0ZZADqeM0V1CkZTv+BfbEVMzehNJRimn3egDJZDp1RDbTqrm0eltXn61X4Yi9Xr9CctHS6+oiHK5FKkCKGGiv5hOoEatidxpuzVeQ9SN1HoCjRXxW+pX5jJcMFVADvv/N7GZL8/KLXW/wB8OnV6/Tp9yp08P/j9ev2Mhx7hMTSuYlAjJ6QNRA2F1qF1d96xfCTyrNuclSms7cNEUOZ4E6jUBtipYijKpwoyWboX/psRClxpxeT/AC8SCcoR3GLbiKN9jnw2C5OVkzhXBWnZkU0wRmAr6iCoC2SKst3wspqKuNGk5OxPHhCXlFy0YOoADXHp00S7tIXoKO217g9q3Tiq9h/08rXGF8LZg6aVOoIV+ZHTc0uEVTqpmJjcUPT3GG4kReDIW/hSZFlaTSgjQsOpSXIEZIUA2RUqEnysDv2jirSxPAlrcjr4dmK6gE/lGauYmvlquotovV9Nnt5HE51e3kLwpWv5k5vBs1IAUMjPoKao6V7lGkvrrV8ptq72PuvFQ/6eVl1I58LzBbOi6RiNaUqusr3IxbooRNsf3oGeJEjgS9+f2Gc34cniQu6qFFdnQmiSoYAEkqSNm7GxiVUi3ZEOjJK7IHw2HuJlYfDYLhlZcnLYS5fYvpuE5VV2lJ1IuwlRgH05gkmksi0g2IU/MO/pVml0LMkeojP8Py2qGNGAS3DOGVmpmqOR6UUKpihFgWPfEpy1YOMdEOPwbJdeiZj0FlLOiHVT0pQr1bxm6PaRNjuRGafNBkhyYQ8KybMw+bQkdR81N0V4VVv5X9SvK3/88TeYrUF/v8EyHgMCPFpbUCvWSVbffyApQfIGz615spSsxJQi5LXQmZjhKBvl/R5dQY9huaArv2PviVN21FlTSehIg4d7YHIlQJ0PD/bCuQ6gdlaJNmYE+g3P/jCVItwd02h6ckqitJJ9708yqkm9MeQqycZNP10Pa0YKUU1r4aiY5nAJUkX6Y2ew8qzOXPReX3/gxO31L4VD+3V+f2t6jUsjnu7H8Tj0qSXI8rml1DMcJmFHQzWqt0gtQfddVDYn0xEasetvwM6Uul/yNy8BzAomJlu6sHuEVwDXYkMAB3JsdxiVXg+fvYOBNcve5C+HzQ1aVzAKmm0iTpJ7Bq7H74fNT529BctTlf1JeWHEtLOqzEKQKaMksSSKUFbatJuu1b4SX6e6Tt8x4qvZtX07vwPxcczKrqmyblQAxYI6AKdgxJBFH12GEdGm3aMvVDxqz/ui/kyZlOO5WXbXyz6SDT/9vp/XFcqNSPK5ZGpCRYSZAEWNx64pzDuBCm4d7YZSFcCFJkyNq2xlY3sxVpOrSdp79348UbGA7VdCCo1o5qe3er/XwKnOcJVuw/z2w2Ex1Rf0sSrPr9/utBMb2dSf9bBu8Xy+32eq9Cmn4cV8tsapkp30Yvh6OjjlsVYkLYq9yPX3rCuzWo6unoT58lmwVgJJ5gIVbTdWJ70ekHc7n19DhU47jtS/aScxw7PsVDsLVkK9cStqUtyyKIJOpzR9X98QpQ5EuM3v/Ambh+a0P1x6GUsV+ShI+UDpQfTZMY6a1UL8sCcQcZWOpwnORaw5EY5LA6uW2pY4paRQTuaSRTW4BPkdzNFkZZL5e0djTOsiSxyl9Ss5A5eoFWzC7p3ckLIdRFktW5rB8F7P3sT8drp+9TmUy2akZlaVF0Poa+UeorP0le0i1zRRtQGPkNhuKWwJSbs371/JHz+QznLaSUkpsCdSkEFg6kUd11MCCNt6xKcb2RDjO12U/wANiy5XYPhsFwsXPw2EuWWD4bBcLB8NguFh7L8OLfbEit2LjLcOA8sGYTKWUGQ9sLmHUSwhyXthXIdRI+b4lFF0jrb0HYfdsWQpSlrsiudWMNN2VWYz0knc0P7V2H4+v446I04xOSdWUtxCRYlsQd5O2ODH0lUp5mr2+hpdmYh06uVO1/r+RGiu2PPutCkrJ2sel4cqrvLW4qHKlzSizV/5eNan25h2kpN356aHnsV2RVo3ktr6dX/os/8AaeYiH8pPpRbpztHWns9DsPQfnjphXwlZ2jU/jfxRy5q1Nft6enmVcnGZNCrUdKUa+qyYxEFJOr0hTtXnjvVGN768/W/3KOPLLbTl6W+yGE8QSo0jBIfmMGIpqBX+0BtrHn33O++JeHi0k29CViJJtpLX31GX8U5gSczTCTd0VegQZzsNdg3mH/JfTdlhoONtfdu7u+pDxVRO+nu/f3/QiZ3xVPJHJGUhAkVVYqHB6FKg/XV6TXatu14aOFhFpq+nh9iHipyTTtr4/coEhLGlF9h+ZofqcPUqwpq8nb8aiRTew/k+KTZZiIpDsSCvdLB3Gk7d/MfniuOSvFSto9updFuGxruEeKhMrB4SHUd1+hj+O6n23xk9o16eCim3dvZc/wDXeavZ+EqYyVoqyW75L89w1Pm3c7mh6DbHlK/aGIrPWVl0Wn5fmeuw/ZmGoLSN31ev4XkM45M0t7nbljtYSyg98aOE7VrUNH8Uej/hmXjexqGIV4rLLqv5XtkWTIlSHTyN/YjHqqNeFeCnB6M8jXoVMPUdOotV7uTo8tK8aTc0hldlQVGoBHLJLMWXvr/tb6dzidE7WI1auByWaB7ohWyBqiSuUxY0o2ADoewqxgvELSHZMjmAWQSBqDabEZDKtB7YnooKh0nzo7EXiLx3JtLYi6cyyNJYKvrBNRgnSjtIaq9Whntu51VZvDfCnYj4mrkvh+TnSgzKoiDOoLRXqV3VT9QJCysxFmgQTv5rJpkxTRFy/C8zGSigAsarVGSSqk6ls3QV26h5Md++GcoshRkiPnFlFxSH6SBRCkjSFAAarApV7GjV4lW3RDvsyH8Nhri2D4bBcLF58LhLllg+FwXCw7Bw+/tguKy1gyPtiHIhRJ8OTwrkMoj85jhQvIwVR5n9gPM+2CKcnaJMrRV2ZXifHnmtY7SP/wCzfcjsPYfrjup0FDV6s4amIctFoiFCmLGygmxJhGBMSPy3J81UWw9LHZfxIxnVO0acbpfN6J+D5+SZfDDye/59+JZQ5MabKm/Qn9yP/OMLEdsV5Nxg0l3L7/ZGhRwdNNOV/fgVOby0i2ShA9twPxGMJp31PX0KtGaSUlf5E/w/F0M/qaH2X/yT+WGgjg7Wl8ah0X1LJhhzJaIkuUQnURv9zjojiasY5U9Cpwi3exHzGRjb6kU/hv8Anh6eMxFP9k2vMrnTg90Qp+DQt/T+R9PIX2HsKx0U+1cVDaXv+fMqlRg+RXyeG4fVx7g/9xjsX/yDFL/F+X5RQ8LTEp4fiXcaiaI3I7nzFAUR6jFdbtrEVVZ2S7l6at3Q0aMY7Hc/BG5KugPYg9jf3G+M6jjq2Hl/Tk19PlsbuG7HjiqEKidtXm8E3t38unPxYhhCKFUUBjnr1515upUd2z1FChToQVOmrJHZHCgsSAB3JxXClOpJQgrt8iydSMIuU3ZLmSeEouZQtCyvp+pRs49CVO9HyONSp2RiaUfij6mVHtfDTlaMvS3vzGnSsZUlY1YyuPZE22k+e34+WNPsnEulWycpfXl9jK7awqq0M63jr5c/v5E9o5EFIQACW+lSQTVkEixekX9sepaTPIxbWhFklfUGLC6I3C1TXYqqN6j+eKp1aVOym0r9WX06NWpdwTdumvodWSQENq3BJBoGi1WRY2Ow39sWLK1oVtST1Ewl1GlSALutKm9mXexuKZhR23OJdmQroVzJNWvUdXrt/fzP+vfEWWwaijNLt1Dbt0rtsFobbAqACOx88FkF2MSQlu9fgAPO+wHviSBHwuJuFg+FwXCxe/Ce2K7llhUeRs4LkNFhFk/bEZiMpE4xmjFpRPrNHtdC6G3mTjK7Qx7otU6f7n727zW7NwEa151f2r36Eifia5bLrLmNnNgINmZgTsB9qs9saGCjVrQWffn3GfjpUaM5ZP28u/QwfEOJyZl9ch2/pUfSo9B7+p88bcKcaatEw51JVHeR2EYGQToRhGBbZXJMfqJUeimmP/E3cD2GPLY/tKEpZYWl3vZeC5vvfloaNCg0rvT6lrBGFFKAB6DGHUnKcs0ndnaopKyJCDCFiHlGAaxxhgBjLYBWNPiUVsYfEiMZbAIMviRGMtiRWVeaPUcUVP3HtOx/+Th5/wDsxl3ABJ7AWaF9vYd8EE5yUVu9DRnJRi5PZalIOKRysBICqXsbsH2kHb3vy/XHrI9lVsHSc6TvK2vVf+L+q5+h4XtHtKeLlaOkFsv5ff8AQlHhxhdZss7Ruu+xJDDzFG+/puPbFdDtaprCssyflb6e+ZlwqtMvDmxOdVKGO5C9rrcgHcWd6Pa/PGNi0p1HJK3v18T2nZVeUsPHNv8AxfQTl4zzE/41/wCoY5aSaqw8V9UadZqVGd+j+ho+LTJCN92PZfP7n0GPUYrHQw8ddXyXvZHksH2fUxMtNFzfvdmcVHlbYWfbsB/pjzknXxtXq/RL35s9RGOHwNLovVv+S1ymRIQAjfufxx6PAUuDh4we+78XqeZ7QrKtiJTW2y8EP/Ce2Oy5xWD4T2wXCwfCe2C4WD4T2wXCwfCe2C4WD4T2wXCxf/B4quWWH48pXliMxFh5MviLk2M5xo8jNCVlLKAGAFb0pAAJ2vVjAr3j2lGUttPla3o9TaovNgZQjvr9b+ux57xTiUuZlMsp37BfJB/aB/l497ShGEEobdeveeIqylObc9+nQIcSyEWGSjLsFHn/AJeOXFYiOHpOpLl69w8IucsqNLlssq1QF+vnjxOJx9fEN5paPlyNOnShDZExccReh5DiB0PIcA6HQ2Aa5xmwENjTHAKxlsSIxlzgEYy2JEYxK1ev4YZK4jKPMzZmWM8sLGSzLuGLBdRAY9tB0gNuD3G2NKnTwtKqlVbasnpa217d+unLxKpOTWhT53LZiGMOJCf7wQtqzbk3vqBJP5jGph32fiqzhKmr/wBr11S07rO38ltPH4yhBRp1GkuVl480VjcUm/8A2H8l/wC2NJ9i4B/9P1l9yyPbOP8A+4/lH7ECSQkkmrPsB+g2xowgoRUVsu9v1epxubnJye78F6LQsOF8QkWt7T+0/svoN+3bbGTj+z6U1eKtLr9+vu50UcPGo7y/2aJAslSISp8j57bbjzx5aXEoSdOevd9jdo1smha8LkkkddEdyg9vKx2b7djvitRfFXC1e6/PgaznB0W6jtF+/UtOPcHMMIkdi8rSDW3kOlth7WBv+3bFuLwvCpZ5PNJvV+T29+mhRgcXxa+SKywSdl5rf38yT4Qy4aJz566P20iv1LY6+yLKnJ87+ll+Tk7bu6sVyt631/gt2yeNbMY1g+DxNwsHweC4WD4PBcLB8HguFg+DwXCwfB4LhYveUMVXHsd5YwXCwmeREVnchVUFmJ7AAWSfwwJNuyBtJXZ4v4h8VPmcwZASIltY0P8Ab/cw/uNA+2w8t9b9BTlTUZrXe/R93vUzP11SNTNF6dOq7yqknDNeOqlS4ccpy16yqTzDsb4dopuaPhxWGIyvtdeVmv6QB6nHke1ak8XiVh6WuX68/lt8zQw6UIZnzEHPSyG9RjXyUVq/5m8j9v1x3YbsajTj/U+J+ny+5XPEyf7SVlmYMG1uT23Jr03H+uLa/Z2H4Ukopc7rciGInmWpfKceMNZMdVsQNcWGwE3OFsAXEM2AW42zYki5muK8ZfWyRFQFIBerNj6lAOx9L+/pj0XZ3Y8asFUq315d3J9Thr4nK7ITk+O30y0D5MNgT6Ef0+W/bv2xGO7EdJZ6Oq5rmvuLTxKlpLQnZ9SyOqkgkEWp0sLHkfJt9vwxi0Wo1IyktO9XX+updIz0DTxaY1aNYgSAzKC3bswRzXrfuLIxt1Y4WvmqNNz6J6eKcor5fJHP8a05FLJpJmd0Z6I0kMzKrEV37Dv5g1Vb+epGMoQpRpNJ63ukm14b+NvHwW927kGdgWJAABo0DdWNx+d/5vjUoZlC03drn17/AJe+QmnIjti0sRxJSDi5xjWjZnVSqOJccM4mIzbNS+Y9L2B/OseZ7RwDqq0V8S2fXuNFV4Rjmlq+S6lt8bJHKk8TaZIzY76WU/Ujgd1I/I0R2xk4OoqF48nv9/L8GLV7Tq1Kmeb06cl79T1bKzxcRytjYMNx5o6+R+x/Mexx11qca1Nx5M18Hisso1Ye+qK3guUaCQgj2Yeo/wA3H/nGdhoyoT+psYuca9P1RquWDjXuYtg5I9MTciwckemC4WDkj0wXCwckemC4WDkj0wXCwckemC4WHMQSGADzb+KfHiayUZ9GmI/NE/Zj/wAvvjSwNL/qPy+5xYubfwLzPO1hONNSM6VNjqwnE5kVOmyblcuzEKO52xVWqwpQc5bIaNNt2RpM7w1mSNV30EdzWwUi69e3648hgcbCGKnWqKylfv3dzunTbgooiIhBIPcGj+GPUU6sakFOOzOOUGnZkuIkdu/lhK1ONSDhLZkwvF3RfQ3Qv0GPCVadpyS2uzYi7pDwxXlGuKxOVjXCsRlYXEEYMrIuUed4tqDpErHpYaxtWxGoedD19sbGG7JneM6rSV1o+eu3mc0661SKHk0NKjsPLfyvHrlKKRmOLbGUWiGK2ti7Fit7seewPn5YqxLcoOEJWdn3O/LXl8hoQ1u0OR8VYaw8coRt0VXOtfTqJBoj3I9MZFTshyjGUJRclo9FZ+S5ryfU6FV11QvhvC8u0bOEOzE6nFv5GwY6o2L233xzYzFYunVVNtLRaR258pX9dAjCNiDPBrLISusyS6i7GwFAK9IoUQtaq2r1xfCcqajNJ5VGNklpdvXXXZva+pOUb4hwZ6BGouFFpppQFAsKb37+94uwvacFNp2yt/uvrrtdW09LEZSjMWN65KixpoTguWqI2qEEGga8j2wk4qUXHYdq6sWvBpXJZGs+YJN0PSzvXbGD2nhIU4xqR05Pv7zixVFJKSNn4K4wcrPTH5UhCt6A9lb/AEPt9sZ9CpZ2YuCqOlPK9n9T1holJ1VjrcE3c3VNpWHMMKGAAwAGAAwAGAAwAGACNxHNcqKSWr0IzV60LrDQjmkkQ3ZHi88ZkdpHNszFmPqSbONqLyqyOKUbu7BcoMTmFcEOplBgzCOCLXgOUHMJ9FP7jGV2xNugo9X9xqcEncV8RMb61G5GyjyPveK6XZmHcU2n8xnJoUmXP1MbLEkn7UO2O+ko01w4rRFco31ZOyeQ173Q/XHNjMbwPhSu38hoUcxNy2aV3KAG1vv7d8YNTByhTVRtWZ1KSbsTBHjmyDihHgyABjwZAOGPBkAbMQ9sTluLYYTJIptVUH2AGLalSpUWWcm13sXKlqkVPiFL5cX97XfoFodvP6hju7Mp5Zyq/wCK9/QrqK6sPNwWPp+rUoChgSDS3Xb7nFX6yreVrWk22rXWpHDRV8ZdVTkRgrRCnuNtIbYg3dVuffHTgsO6tXi1HfmFimj4ehIU/SSAa77n3xvVJuNNuO6RGU0MPCmj+h7GkDS9kagKBB/pBHlvjy9WrCrrKNnfddH1XP3ciyMvnMoDI9UBrbb8f/ePR4RtUYp9CxR0I7ZIY6cw6iho5EYXMPYfyOU0sGB7EX7gkCsc+MSnScX5eKVyupFONmXj5QY82omfkR6T4QzrSZcBtyh0E+tVR/IjHdTleJqUJuUNS7w5aGAAwAGAAwAGAAwAf//Z</t>
   </si>
   <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUTEhIVFhUXFxgXFxcXFxcXFxcVFxgXFxcYFRUYHSggGB0lHRUVITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGRAQGy0fHSU3LTIvLS0uNy0tLS81LzctLS4yLTAuLy0tKy0tLS0vLS0tLS0tLS0tNy0tLS0tLSstLf/AABEIAKgBLAMBIgACEQEDEQH/xAAbAAACAgMBAAAAAAAAAAAAAAAAAQUGAgMEB//EAEkQAAEEAQIDBQMIBgcFCQAAAAEAAgMRBBIhBTFBBhNRYXEigZEUIzJicqGxwQczQlKCkiRDVIOi0fAWRGNzkxU0U1WUo7PD4f/EABkBAQADAQEAAAAAAAAAAAAAAAABAgQDBf/EAC0RAQEAAgEDAgIKAwEAAAAAAAABAhEDEiExQVEE8BMiMmGBkbHR4fEjccEU/9oADAMBAAIRAxEAPwD2AhCEigKQEEpoBIpopAkgnSSDIoCChAJFNJAUmknSBFJZEJEIEnSVJhAJkITKBFIhNJA0FCKQIpFZEJKABNJpTUgCE0kCQEFMIBKk0qQASTSUBpJ0hSGhCECQhNAIRaSAtCAgIGUIQgEICECVSz5C/MfG/IkjFsDA0uouLW7UOXNW1V7JwchuTJNFHG4O01rPKg3cC7BsLP8AES2TXu5cstkcWfmvxshrDI9zBGGmyTdg+1Xjdb+SXDc17fkz3yOILJtVuJBLNZ3vn0XZk8Ilmkc6RrRqh02DYEgcCNudbLRk8DmOLEwNHeMc+xqH0X6r3+Cy3HkltkuvT8446z3bHLgzy95iapHnXbiC47jUQLHhQXDBmva0OZPKZtdaPaLS3od9jv0VlyeFv7/GLACyJoDjY6eXMrhwuAzxhsjQ0StkJrVs6MgAgn4/FVvFyb13+ZEXDIsrvnjIn757DE8taxp9n2aux71oy+MPbM+3O0vhAoE01zogQWjp7X4ld2Tw7J+ejY1ndzO1FxO7bqx93gnldn3vdNsKMbBGbH02ADcdLoj3q2WHJfs73/abjn6b+doyfic0YgLXuNw2QSSCS57bPieXwCwOa/uYdUz2gySB7g5xOkaPDc1Z2U1w7hEjZIXPa3S2EsduD7WpxG3XmFxu4JOI4g1rC5kj3kEjTRLS2/HkdlW8fLrff50joz+fwYcVa6HHY+PIkfrka4EkjbQ8ja+R228lliSvynTlsr2DTG4UTsQ06mgWKFrsy8PJlYwSRxjRKxwDDtoAcHcz5jZbeEcIdDJPsNDx7G489iOlWun0eVzmpen+Kt025fc1dkY3ub3z5Xuu26XEkCiN9zz/AM1YVF9nMJ8MOiQDVqJ2N7GuqlVq4MenjkrvxzWMCEBAXZc0kimgRQgJoCkJJlAiUIQgEIKYQFItAQgRTQhAkJpIABCaEAEIQgElkVigAuLi/F4MVgkyJmRMJ0hz3VZ8B4nnyXFxvtE2F/cRMM+U4WyBhF10dK7lEz6zvcDyVL47jtkxM2aeZk+aAMQ6Q7uMV05YwxY97E1INT/pHka5IPTgfDkhJjA0Bo5AAD0GwTQAQuPifFoMZuqeaOIHlrcAT5NHNx9FW5v0i4t6YY8iY8vZjEYPo6dzL9yItkXFCpcnbTIP0MAf3mQ1p/wMcso+28grvMCTz7qWJ9e55YSrdGXsjrx91ySUBhdssORwYZDE8mg2droiT4Nc/wBl38JKsAVVgVjJIGguJ2AJPoNysly8UdUEpPSN5+DSUEf2b7SwZzC6LW0gNcY5G6Hhjxqjfp6tcNwRt7wplUbhfBnOweH5GO5rMyLEhDNWzZo+7YXwSjmWnmDzad/G7J2f49HlBzQDHNGdM0D9pInfWHVp5hw2I5IJVNCAgElkkgVJhJCBpWmhAqTQhAgFksaTpAITQgxJQgoHogLTWITQCaSKQNCE0CIWEjdTSLIsEWDRF7W09CtiwleGglxAABJJ6ACyUFQ4lA3CY3D4e3Tk5Rd84be9oH63Jme72n6QdrO7nNCx7VcLjxeGxwximMyMSyd3OJyoi57z1c4kknxK6uxsZnMvEJB7WTQhB5sw2E9yPLXbpD9seCsz2g8wCPA78t/yQZPfVkkADck8gBzJPSl5v2h7fSTO7nh1Bt6TkEAl3T+jtdtX13beAPNcv6RO0ZyJHYcTvmYzU7h/WSD+pv8Adb+14nboVWooHOBLRddBV+5vNc8s++o48nJrtEgeDBlzSvc6X9qRzi95Hhrdub5dALXREGTuadVVdMoatvrDpypRU2W5zWtJNDzJs3dldOJiubpkBPMfRbqIHW/BTM5ctYzt6s1u/KY4pjue2mEg340CP9UtmC14YBIbdv8ADpuuhC39E6upDCWNrgWuaHNOxDgCCPMHYrkhzZsJuvEfcYIvHeS6EiwD3fWE/Z2+qV1ZAcWkMrV0vkoV+Z3TXR0DuQ2jyBu7+K582Uk7/mtMrj4eldmO08Oa06LZKz9ZC/6bL6/Waejht6HZHbjKMfD8t459xIB9pzS1u3qQvJDlvaWSRERyxnUyQDe+ofv7THci3kfcF6v2X45FxHG1OY3U0hk0TqcGyCnDY82nZzT4eYKy45StXHn1RjxvgTn4sIhpuRjBj8dx2+cY0NLHfVe22EeB8lv4O7HzBDnNiqXQ5lnaSPfTJE+uelwIo3RFhTVqr439E4i6PlDmgys8G5cYHet8tbA1/mWOVnRaU0gEICkFNCBJBMpIBAKSZQNJFoQMJpUmgEk0IFSVp0gIEgrJKkGIWQQkFAaaSApDIVa7cuMkUWGw+1lyCF1dIAC+d3/Ta5vq8Kyqs457/isrju3EgZE3ylyT3kn/ALbIv5kFjYwNAa0AAAADoANgAoPttxo4mI+Rld66o4R/xX7NJHg0W4+TSp6l5j+lTM1ZUEF7RxumcPrSExsPuayX4qMrqbVyupapuPFoaGizXMnmSdy4nqSbJPmt7ZHbAX15c7O3TmpXB4OHNDnuIuiAPDzK68HDEb30NjQabBrbf03VMfh87q3tthLB4S1lOd7TvCth/wDvmpBjABQAA8AmUL0MMMcZqBoQUFWGvIcQxxbuQCR6qryvdLJvQcSBsD6cuatirGXnOL3FpoE1t1A2CyfF+Ju/gnU9UlNwtjWbDeqLr3Gx3A6G6Wns/wAROHktyL+bcWw5FfRcxx9mWuhY52/kXqHfkEEHnvfwXTPxJj2FrmXqBa5vSiCDuuePJx5TxpfGzG7j3FQPbXCdJiufELmgc3Ih8TJCdWkfabqZ6PKx7A8SORgQPcSXtaYnk8y+JxjLj66L96sBRsaOH5jZoo5ozbJGNe0/VcAR+K6FWOwY7pmRh/2XIkY3/kyVPD8Gy6f4VZ1IaSEwgSSaAgVIKyASpBiE0wkoDQEIUhoKAhAimEihA0kwUBAikmilAaVppFSGFWewftx5GR1yMvIeD9RjzBGB5aYR8VP5k3dxvf8Ausc74NJ/JQ/YGHRw3DB5nHjcfV7Q8373FBPAryvtJiDIz8w3RjMMTTzFNhZIQR6yuXqi8ykP9Mz/AB+U/wD0QUr4YzK6rlzfZRc/eRhvee1G393qRs3VfRSEkYIa+9O12KHPoT4Loe0EEHcHYqA40Q3TG1ziALIJv0+5Xz/xS3zGROxnbxWYVQgyHMILSdvhXh6KxcO4gJbGnSRvV3snF8Rjn28UdqaSa0CB47kOD9AcQ3SLHjzUQp3jmC5x7xu9Dcdduo+Krsr+gXl/ETLruzTCR1lYIQuS70r9D8xOPks56MkkeQfFE78dR96vi89/Q4PYzD076Me8Qsv8QvQ1px8NePiKzjju+LyjkMjEjf6vx5HMP+GVnwVmVc4wNPEsB/70eVGfMFsTx98f3qxqyxgJBNHNAkAoKEAUAITQIpJlCAQhMBAkykmUCQghMBAApWgIQACAik0AglAQgpUmTI2Hi+O9z5HRCWSKyXOMORCZGNHUgPErQPqgdFLP4mzCwoC8Oc7u4o44mj5yWXQA2NjfE17gCTyXJlZLMfijpHuDWPwHOe47AfJpr1H+Gc/BHZzDfky/9o5LS1xaW4sTv6iB37ZHSWQUSeYBDfFBPcJdOYWHJDBMRbmx3obZJDQSSSQKBPUgkVyVF47B3XEZx0mjinb5uaO5kA9BHGf4l6KFUv0i4ZEceY0b4xJkrmcd4Al/lpkn92VbC6ylUzm8bEIqvxaMiV19TY9D/qvcrQCPW+RXLxDCEra5Ecj+R8l25+O549vLEqqyY8g2CQfJOWMtcWnmNisCvL7xCY4ZxOQvDHe0Cautx57KcKr/AAGRoL3c9gB+f5KRlnLvIeH+a9P4e3o3atI2z5PRvx/yXA7GYdyxvwC2oC62S+VnDxaG47A3FG+tKDVpdyVdwOGuyshmMyx3rjqI/YhG8j/L2dh5uasHPhrPt6rSdWnqH6LMHu8BryKM73zn7LqbGf8ApsjPvUxx3jBxXQuewfJ3u7uSWzcT3kCJzhy0E20noS3palIYgxoY0U1oDQB0AAAA9ywzMRksb4pGhzHtLXNPItcKIV2tCccF8Q4cOt5J9whA/MLV2TJyJsnOJ9mR/cQb7dxjuc0uH25e9d6Bqr0uUYcadstvzsBrsbHkJNvZl6GY0hHJxcAxpPjG7zV84PgNx4IoGfRijawfwtAv31aDsQEIQJMJUmEAhJFoCkITCBJpBZIEEqQmgVJpIQMIpJJzgBZ2A69PegYTXOzNjJAEjCTyAcCfhayiymOJa17XEcwHAke4KOqe6NxupIrAZDC7Tqbq8LF/DmkchgBJe2mmnHUNj4E9Cm4bR3G+zePluifOwuMROkBxaHAlriyRo+m22MOk7eyFKrXJksaRb2i+VuAv0WRkANahdXVi68a8E3E7ZpOFiiLB59QR5rU3JYap7Td1RBuudeNLNkgN0Qa2NG6PgU3DbzHjGE7h0oiIvGeax3nkw/2d56V+weo25jfWcs+AXpnEMKOeN0UzA+N4pzXCwR+Xr0XnXGezGRiWYg/Jx/L2siIeDm/1zR+832vEHmu+HJ6Vwz4t94qfFZSZXeo/ALnxoy97R59fDmU82Zr3lzHBwPh0I2II6EVyO6meH4mgb7k14beNFZsePr5K4606WsAFAADyWQQilvAhC0MmdJJ3OOx00vVjOTPOV/0Yx67+AKi2TymS3weTkBjbNmyGtaBbnOOzWsaN3OJ6K79gey3yON0soHyiatfURsFlsLT5WST1PkAn2V7IiBwyMhwlya2q+7hB5thB3voXnc+Q2VqWbOzK7acMOkBNaMvMjiAMjw0E7X19FobxiAtc4St0tqz4E3X4Fc7njO1q1yk9XLxTszjzzxZEgd3kWmtLiGv0O1xiVvJ4a72h4FTC44eLQvaXiVukGiT7IBPK9VUts+ZGy9T2ghuoixenxrnSdePnZ1T3bkyuB/GMcVcrRqFjnuLIvl5FbcfiMTyAyRriQSK8BsSo+kx8biOqe7qQtePOyRupjg4dCDtt5rNXl2saEiUBABMJItA00ggIFSaVJoMShNJAguLjv/d5v+W78F3LTm4/eRvZdamlt1dWKulXObxsRlNyqxwbFjMDpO5LHsYdMhLvaJa72mjklwnhrAzGmbII36nXZ/We1Qa3fwFe9SeFwKRgDTkvdGAQWaaBBBFfSNc1rwezWh7C6Zz2sOpjKoA899z9wFrDOHL6v1f0/PszTjvbsihhMGNFOB86ZgS6ze73CvuXBxCdzXZLa9mR7gftNfqH+vNWWLs8QQDO4xNfrEddbsWb/JZT9nQ9krS/eSTvGnT9E72KvfmfBUy+H5LO01/X/VbxZWdppwHBZKcp8gssYwN+r81YI+Cjclkj3RaLLvk7Afsm2m/KnKxZXAHOc4sncwPa1sjQ29WkBu2+2w+9dUHB2slDw40IhEG10HXVf5K9+Hyy7a1/a14rfRXIzow4ZmkB8cjtPmHOII+77lZOB4PcwtafpH2n/adufhsPcuaLgGlsLDJbYnOdWmtTibF77UplduDiuN3faT93Tjwsu6EWhYyPDQSSABzJIAA8STyWp2Q3G+yeHlnVNCO85d6wmOT+dlE+hsKCn/R88X3Oc8eAmiZLXlbNBPvJV1x5mvaHsc1zXC2uaQ5pB5EEbELYAktnhFkvl55/sPmj/ecY+fcyj7u9KyZ2Eyz9LMgaPq473H/FMvQkBW68vdHRj7Kbjfo8hu8jInm+rqETP5YgCR5FxVn4fw+LHYI4I2RsHJrGho9aHM+a61y8Ty+5jdJ3ckmmjoibqeRYB0tsXQN1zoKLdpk03lZBRfB+P42VYhma5w+kw22Vvk+J1Ob7wpNQlXe19/MU0OPebNPInagfXklxPFAZjgxMYXzR62tAq99jXPmfipXinC2ThoeXDSbBaQDfvBXO3s/GGOaXSGyCCXWWlt0WmtuZWTPiyueV1504ZYW5X70BxrQDlCPTpqH6NVYIBqtvFb+Obzykf2YfiFMY/Z2FrXtJe4SVqLiLsEkEEDnZSx+zkTGvbqeS9ukuJBIbts3aug+C5Xg5L6ef5/dT6LK/P+0HxPHb8ghfpGrYaute2avwUh2kxgwQiABjy5zGhoq2vFO/EfFScvBY3QNgJdobRBsatr5mq6lb5cBrpWSkklgIaLGkXzNVzXT/AM91Z7yfyt9Ff0Z4OKIo2xt5NFep6n42tyySWuSSajRJpimQik1IVoCKQoDpMJJqQIQhAiEBBTQCVJpUgEUkmgSAnSdIBJNJAAJgJBNBQsDi+dlSugkyYMCUF1QdwZJSwGg6OWV4jlsUba0gXuEsXF4dLMYsvLkyJ2uI7rNcY22CRceMQyNzdrBDXequHF+EQ5TO7njD28x0c13RzHjdjh4ggqscSjfiM05zRm4PWWSNsk0A/wCO2vnWD/xAA4dQeaC4xMAaA0ANAoBoAAHQADoswqvF2MxCA/Fknxw4BzTjZEjWEEbFsZJjqq/ZpbP9n8xv6vi2R/eQ4sn3920/egstoVcdwriH/mbf/Rx3/wDIsBwHNd9Pi01eEePjM+BLHFBZlwcT4vj441TzxRD672tv0BNlRB7HMf8Ar8zOm8Q7IdG3+WAMC7OGdlsLHOqHFia/98t1ye+R9uPLxQRkkmDxKVrfkkstA1k9y+JrK5aMg6XkmttFqH4plSY0hh4fn5GTM3/dXRty2tPQSz210I83yX6qx8QwcrKldG95x8Ru3zT/AJ/I23t4/Ux9Kb7R8QpfhnDIcaMRQRMiYP2WivefE+Z3QbcUvLGGQAP0gvDTbQ6vaDSeYBvdbCsqWNKABNILKlIEIRSBFACLTCASTASpAkJlKlAYCEBCkNCEIEUIQgYQEIQJFoQgaChCAQhCBJoQgEihCBBMFNCAQhCAKVIQgE6QhAJWhCBhCEIAIQhAkIQgYQhCBEoQhA0BCEH/2Q==</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxITEhUTExMWFhUXFyAbGRgYGB4fHhwiIh8eICEgIB4eIiggGCAmGyAZITIiJSkrLi4yHh8zODMtNygtLisBCgoKDg0OGxAQGy0lICUtLS4tLy0tLS01LS01NS0tLS0tNS0tLS0tLy8vLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAKgBLAMBIgACEQEDEQH/xAAbAAACAgMBAAAAAAAAAAAAAAAEBQMGAAECB//EAEIQAAIBAwMDAgQDBgQDCAIDAAECEQMSIQAEMQUiQRNRBjJhcUKBkRQjUqGxwTNi0fAV4fEWQ3JzgpKisiTiU8LS/8QAGAEAAwEBAAAAAAAAAAAAAAAAAAECAwT/xAAuEQACAgEDAgQFBAMBAAAAAAAAAQIRIQMSMUHwEyJRYTJxgbHBBJHR4WKh8UL/2gAMAwEAAhEDEQA/ADOt9TpHa091cYULTuVirEcW4ENaQT3QZAgaW/BTCrUYEF6ZvZrhIgkxLFo5nCqMyZ41F0KozdPlqFSqq1h8pmRKSbB85JgCZzHtqu9F6rUoMkNbTJI5AYLJOG5iTJzBjM8aw3ZTJaPYNk2zUCo57kwQpLDkAEBRnAXxx+Y0+3m09UAh2XHK4xz9xpB8M7pGlKItKgQ1W25+YhYDFbc3D3HOrLQNS395bd/lmP58a6ExxWCrdcTcqFU0r8MRVpytgzAjuLEQDJ/5jz7frXBo1KwvaTYDGQVH+WeTi6T4yQdenfF/WG29K5CQ3jtkHBgE+MjMSdUTqbVXHqBkJCggSAJLZiCcFiAZiLTIBnWWrwEa3UNem7tqFUpuXIqVHFgBJI78KxUBjhxyB4HA1bF3VOnTpvc0Cjm2WzFPHmDnXim163UZ76hao4EBmAYiQeAf82fuSeTr1jpW+qmnTEZgiShti0YxiMAnMnONLT1LdCK8nU2roi1VZAD2kjFTDlYYYwYx5ke2rZuNm/puih6gluXgDHBiCZ/t+Wk1QVWRSyWAAAREMIqGSc28e36eHC1P3VR/VIw0qB8uOfbJjDH7aqOGyv8AyLdqjUadA06RvYSeGJIUiWBbIgYODx+Y3VTUtpLTpdzPUYQ8GR6nGCASALeIn20SrVyKQUqWCkqGlZEDF2RJwIC88caN/YmY0vwsTUntBUi5ubsTB/T9NVh136EtPNG/hndMFYWNE0yQVKkE2iIImefMe2NR9SeoXqBzlVuRmUfikFCff7DnzjU6bunRvLE3zTYKViRImAMHEceSvuNd/EIJpH06iusghahBGTCkGeOMHEe0aUmqZSi8FDr9TehUaqgaWMdpuIkEWqxWAARgZn6kwTentSpQ5R6RqsjBi2UDEE+IzB5ECI9obbPZv6tValNajWSrwFQS2AGUsZGcT/D9TocdMrrTVqlS+oDStE2KpujyDcLpPiZyJGqhSyc8oybFFXcbggtTqtdntuYycKFTBWS1xgTcI98T/CnTzctMEmxCytTaI7gxkMCItmcDJjtidWfeUHIVUo99Qr6jd2IDTECcgD9QfqIPhrppV6guKhKTWgW4EJggf3g88TqNSWcGulpepBW2KekoWrUrQbwtyMywokWmAYAI8kSDI80vpnW1ULM3yMhVIsZRzhnXtDR2wI85GrMux9Jc2oAJZqksGJD9qiYSROTyf5qdrSqJtqhVadn/AHqMASZUKI5Ig5wJ9iTwrngGo0yJd7QqqtQu22SSCIUBiTBj+MEiInGD4Onvw2RFGoKtJbLJWSoIKgZhoY8SDdHMDgoKFCtV2oV5il6jSxWJkN23mVtMr+ZGM6h+Feng1JrBGjhTANsAgkEguMKAonBHvrSM5X8/6MpRVd+5bfi7bE0w1TcpVF5BVQO3DSP0geOBob4d6LTv9Fg7FMCbmgkFiSA1v2b/ANOY0w+Ia6MFprTCBR2kBQQAoEc4yeI8j7Bxs9izSUJR0ZgKgtn5mGAVPkCQfYe2rXxN995HJXFV33RXPiXYK6AyIpEA0qlqnmAFYFSnk5Hggar3T6Ipbmsy3BR3AlqgtuEAkEw/fKgZksZtGr/8RVGSiRUZHmFjMlpWYzgZ4P1zqrbfqSD1ae6h6ynC5JDEQBce1wcjmBEZnVSatMz2FV/Z96te5RfODeojksMEQSJDRyJPjV1oU6dPZ1A7WS5AKgggyp7FXIHJjMRxjWuhVPUB9RypWoSDJlrLBnm3IPBJx58Mts1M7cLVpuwdvwq0/hJ7k+XEjxOsk/Mq9H+DfZ5Xft+SudA6c1Gm9tVXLsDSYJBPc6gEmIkxgZX6aSdZ21ekCtQU6ga4gLc2Ra1pZAq4AumT+L66v23ri1WisMDmGM+sgDKCT7/Q4yND/E20BAuFY9xNilwT2sZhWFgExyJzjjWcYXZc6wVzoFBKu1FWtTth1CsJErCqAAOAGYYg/rzd6SkVqQNWpUMsRasLAjPkTnjkTgDGuNhQAo0BJtC0wE/huekIn6FTz+Y0elIiuhVy5tfuYYyBAkcjtOtYwoV8E2/qVfVb0ghZaaxdPBLzxme1fYaQUqz1ErEpYvqhshgT8pPdPBy3jBGrFDlqxS0NcqgtMQEDcDnLHGNVwUKnp1izBmau64wB22i1c+YzPtq3iLZMrc0gDY0ltqswuYqgEgYvtWYHt/zMZ0wfbB6Lt59FFWf4qhqffJuXP21m7ppNYBRHqKsREWIag4/zBdG7enhU961JR/6KSP8A1U6w0oqM8dL/ANtmmpco57pIG6r0+kK1zA4sgzwJZjxJGKQj7nVRq/DVKszVKjMsmFyxlRgHj6H3+/gXnqIFzk8LewP/AIURP6u+qr1mq1Nkp3E20knIEEiSOfc6rX1/DqXNfn/jM9L9MtS48Z7+5S/hvrdGlt2oNSN71KbeoG8IytEfMmBggHJ0s6NWVGN9AVhEgO5AXPJK8+JHnRL9XovtRSIKNN5tp07YPIBLXrBuOB/l40u2NNmqWpcw+gyVEkwPcqDg/XB1zFy4Z658PdI24aGZqa2LUFEstmQZYMSzROC0+QOI16BsFV6YKlIjBQ3LH0PnVH+B9w/phaFqAEE0ql6sB3CQZhjI5HPnPN42G3g3+szDwPwjXRHjARFfXqJMoatJVcQBUSe7/wBwn3j6aoHxNVW1gwpVCQe6kwtiCVkD6FlgR45nV/3NLasjmw1CJMqAWdszaREn6A/prz34j6dY17ir6lQEywkBcAA9sySzcnwRmAdZ6r8pcV5kUzpDrTa6olylSChlTBESDGPBnPjnx7H8Ps7UqYpm1A2CSGOVfwMKOMD3OvJHpXtThjVVkItngLIjA7MiIEn6a9I6DuKZdaNOm1Jg6GokgTJYCA3z24U/Y+xGo0nTEGtTqRTWDFgh1Iz2VMFTx+vE8aa7QsNrVZipFr5H2Iz/AMtQ0rI26+RSEgf+XV59v9+2pKNU/sI7QQwYGSBySMz832Gtryy6pAfTq5LUyE8NAwAWjOcycDJg6rPV+qqlWkS6yKjllJUlJY/hglWtDDkAyMjzZdwudurJk/K1isPkH0wfHmAT+VM69T9SuWvm28gekW/H7+xDEgkYIg8jWOo3jv0F39xt1jfI81lYdipmmzWysypIBB/D/KCdP1RkajTjskQfxNDKcDAEAZFv8OfGqj1Gg1EwgSqD3SpwptYWSSSsm8wZi38tNt91iWCQKbIoYgEOByZugA+YEtEfcaaeHYuGWgRUepCsVwCoGeBOMR7aUfEhYKtIgwxQTdb2hxN8yeSAIn31x0TrCLUYu/ppCAMSLWJBjiRcQPYSTqHrvV/UdCjLDsACTKgK9Mz4MkxIz+UE618RUS1Y02X7QLAQG7Me6qSwkEYMAjxx9dAdPoim99rFqlNgTJ8WKCRmIGJwJ/LTLp+6YglFKkU/cMSSwk4OOT78cHjSXprOziCHNjMwfgC4cexgT+nvqtSmTp2g/cbaj+zvWFNsUPxfVXEgZmT76q/UdsV25ZGVauJUtN4YDlWgcGZH8OPfV43tONrUAUR+zpxjm4ar+/2NJ9uGKEtTCgPAP4UBBEcCZk+0zoat0vQJLy/Uqm9NWrt6cRaapJtX5QCCSDiYPMCABBmNACo6+jXajFMr3XyQ4ACywCm0EkQQJzk+dXCrsVWiwUhlRazBVuULBAE2i1xIJEiDjiNDjow9BQULqwBVQzLiVbC8XWsPac8RqYxbk8+hE/gX1Fh6wjX1E4VIt8CQsARxEQcAGJnOLtv+psuzRlm56kSFbkm4gxxnHtOPfXm+72NSlRrg33kgAvk/KwAE/YgT7CJwSbueu1Ttq1CwMBUeCbSApaIiSSBOZiJiDmIjq1OW7vgqarTVd8j74m6jQdWpUnCGaRZlBtTOZgQDJBjGMjnVSp7gJWrFyHSRLI5UvlcjgFSOfudd9PpOiG6CigQLRbnumMAnAwI8eda6Ft6qu9SxWolR/iSAYXkRMGQJHPtOslr+LImKqJd/hbe0fRZhVILeoxTEyI9hgH5oGNWLolCKFMSwuPv7DxPHy6qHw1u42u5X08AVAH/MSOOfpA/rq3UN/Tp0VBcAqXkfYP8A8tb6byn/AI9/Y3apNe5BtkgqJwFoCT9y35ca31GmPU/dZLBix5kyixOYgxwBGiUVbjdAAqKpJ4haROpmSnICRACRH+Z//wBRrbTeP3I1IX/oUfs37umCWIY7cEHPDFjn7aarRiuIAACrECPFX2+w0Ntoso/+bT/lTX+50xL/AL4n2Kr+iVD/AP20rHtRDs1Zr2UwPVeccwbefy/lpHT2kMiyT6jhzPmShk+5gHVi6W37lW/il/8A3Et/fSCnP7RSnhNsjfmVqg//AFXUzlUf2HGC3Cqk9/7U0z3vieD+7Qfbtu1ZNmgNRB7PXb/2t6Q/kdUPoe8YLuTzLLGMG0kxMAES48z/AC1a9h1MLTatyFoBgZGS7VHP/wBRrDQlbz6L8murS474JN8ZpsP47QD/AObVcn/4hdLK20p16tZzbioVEj2A0q6T1pzSQk9odbcE5SnPETAP35/ULa/FQol0sDd+WB5wB/bSerBzTlx3/Jm9yha77orHSumV3pGmVNvqR3KmHNojuBcYMmQVgfU6r9aiKRZWJBHaQDPyn3Vo4mDkc/fXuPRk/fbhViP2qmw88ij/AP51Rd90Y195WQooN+5b+IAA0ipsGcFwPbJ9idVtE1hgXwJ1RKVZqlZ3AiAwAlcj5i3bnH1Ptxr2bolHgFLvIqBvmngYi6B7x7xnPj25+HxtRcUWqyq15SuQsA2Q6ra4iQZBg+RE69J+Et+m3T0mYFyLiiqAbjMQQBcCB8x5PME5uGMGadMK+IOrqsKNsrBTAJIkQ0SqLJbwQBnVDrdWq7oVCKVlBHibTgi0CW8GAJUj8ziPQN9UqVlNT0GpEAyWcBh2z4OMgZEx+WvOOuesN49rs9BbgCpFgJzDR8zT/FkEwONTq8Fxb3IYv0pGeiEW6/Zs4umL0TkDie5flPjjJ1Y+nuKtJ19R49RTcLcS/E3SsiDAGlGwemtbYTCg7erMr2i5afcWB9wSci2PE63079zTFZiReg9RgO4WWHEiXFkZJwQftqbz9C3x9Qv4cFvow9xZEgWANBWvAJCk5yT7zIjTfo9Yf8PoEgFipIJjBvI/3EnnVM+DOrBa1EBCzFVGScyaoBgnOCuR/Dxq49EAPS6bXEQMwYx6hn6/XVwaffyEngWdQ31SnRp1BDEylrEpMqZhhmfHj6c6rm66iaNwVUJZSrESWyygXiO8yIH3E8aZfEe4FPY03D5DmRzMqwg3SMxH29p1W64Dri1SzBQzZJg0uM8gETwI95J1jJu8en8Fde/cd9V2lJ5apUYI0nvAB4bjtEDtGDByZJ1H1nZk1qoDSsqyk0ohQrmAFIl8Ag+5/LQ3WjuVFdlqSA5ZmP2gWgsTBJIA8g5jXW73FZ6KMwuLmoQy3F1EIhEmDAJI9jMRjJuWcEuLx8vwQbF2ctTFFGWVWCrEp3MkhpJUkmIM8nGI0/rbOwAoKSAOlwWZBJVsAsQBNpxgifc6C+Fi1NHNoUyouz2iWOSBBgA8wZz7nUHWNw4BYm71CzqQoBKgdvcOMMMD21lqaqjp31EoedfT7D991WWtKBbTTk1HUgGG5+c2gn+GeZjUHRd1JRmTBpEKRaVEWrMkg5I8Xf6KOuddIdER1AKBJBYkklSZnuu8SY440s+Ht1U9SiiMVljPdkqGWRHBGCYz9taS/UJukPTgz1DqNS3asJmaFMZyTl8Y5Oqh8RdV/dimiNapUk4IPYABIN0mCIz59tBv1KsylCzhVS0A8xm3xxJWI/6qtptgzwxyWyTcTEknHkg2+D/LUy/Ub8R+Q1Ebbbq7NSam5tlaix7AsGgHkjtxMeeY09+H9xWqGnBNjJkMAfKjsKuAoEcnJ9tUmvXksBEKpgjyPf8AUnUY39YWhnICCCAZ82gYieIycROlDXcXbyE4eX9/wWPqlGm71ElB3AfKIBAqQOeScDzMfTW+ibWlWoOpCdryWiYOCWMZBksPw4B51W9vWLUzMmaqSSZnuJPP3P66K+DxPrBmtDfKcz+LjxGRP9caXjW3fWx6sUorv1Lb030Gq01S9pY5AVRITwDxOD9p841vpm6SmlWapNrM3cPlLAwBHIwMk4n20iNK0qNs0N3Eg90QOYzPkSPpxpP1SvBb2WbcmPlGT75zB4PtpaerJf1x0JgsFj6PWVdrWVGEsEwRBILWkjPEj7663lG9izVEEO4RRi+STnyxzg/bVb6XumkjgWqIxm1rh4xgnA/tp6aKeojlkKFQSDBKszfiI9vMQfzJ1UJ7n9F+TTUWF8/4HfUN9U9NStk+sSbzy3pkRJ5gZ9+NHbTqrCVYcGmLn7YAa7A/FAYDA8HSpKKlKUqZqMzFhTUx8wW5m5ABA8wCM+3G8oFTVFwqAuq+wPyEDswQBMSQc84x1KTiu/Q55W5WPOnb1PS25M88AE5D018T4OiNx1mmtRwpub1C0ewFEZPtkEQdJqW29NKXaSVC5F3d++XxOOPB85Og+tglWWmplmeamLpN6x4kSgBiZn9TfJRtmr5ouzP6dAL5Wl/Rf+WkPV9wFrMBmNuVwf4c59sMRBjUI3xqUKs+o3p02W6oCCDbEEDz4MxkGOdBdX3M/tDtkmmLYuEXKT3TzhV/XU6zuGO+R6Ttle6LUb9mqlWUA1BK+brUYt+hj8tR7jqbPR9JYIsRbQcmaQEAAEGGfkwZ86H2FRzQroCf8btH/oH58Bdd1OnFKQqE1A1R4AAhO0nP0+UwCAftrki5W67wa6iWO+otSoQn8N1XFsTgQJ8AZP8AppVUqhiWgEkkkz7kn7cRxqau7ABsEIsyOQWlgJB5tUjOceI1m/LUqjU6hQssDwQIAEC3GI/rp7HRLp4LJ0T42Sne5TvatSaPELfdBiPCD6zpT074oYbhqxW64VcSRF4p/wDuj01wec6qG2qff/Z1vbbiCsmPp9xq5SnWHwZWP9l8V1NtX3FX0wwrzK3GMtd4gmIIiRg+eNOukfHdJFWNtY03LbbF0+TAMEGD5OcidVP9pgg2qYM5gj9CNBVNwIWF/wDl9Mx7Zzpw1W17mTXoeyb/AOPdtWWojVWRAhhgncxIg2juIEZyZz9tUPrFP0XCrUMSFCq1ymA1xMQBypGPOlXRupTUdmQSwtEKgAmJEMhAlbhP19pmapaRTuPyqF9zCmASZycaNTVqrHG2T0+uVFr0TcR6dQ2te3yHBQDhBzmPJnTup8R1lpmirD04JAjOQQc8R5/LjVK3AymIIY5/MadUGK908iOPv41GrJx4fdmqzZrZ7w03pnEqVP0NtxBMHP5/66fL8VVU2goAkKpbI5Hc/nxz/vzWRA7WWD7xnMn+4zqOtw0zycD8zqLl075DaN+o9SZ0ekWJUVCQCcef08fpoff9RICopIAXmfe1h9MYP5TzoYMoIJHzNJn7N9/JH5gaD6gYc/8AhEfov9tPTduim+pZN1uy6SzMxZXZp7biFAMxCkzLSRJ55Oi991QWj0xaSlSbSQAWqBjb/CLQoxqtUqjNYoP4HEfUzH84Ou1qQFuMzdIn6jz50eZXkeH37IY9P6u+AxaIIcmTcMnIJjGY9vpptV3aPTpojs1txE8CVEweQLhETH38Iejl5YKViBIJAkZ4n76ZVxawGB9voOf9/wA9cOvqPft9v7BLqC1qRL0pM2sBMn6GPy+mjuibtUrJBgWEZJP4gYjycRMf8lm6rFGBMiB4nOI8niI0NtdyfVSJyWGD4g8nz41t+n3NWxrA2q7wwBao7l4xyf7kyfbxGiK+5N6oQMleeDgEieAJjEYnSrcbuEAjIZGn2g/8wfy+p1re9QLkEhWMr9PwKsH6Qo/nogvL9RILXcKSZwPTP5mGIP8ALn6D6yQNjdTqMpRQHVSAvEu3Edo4DY8cYkaTbvcsFICiYj3H2xjjRadRNNaip2yRnM9pbxMEZ8g8DTuqY5Pv9goAKlogj1Lpk+FX6HHP6jQ/TdwaRIEWggqSBOR/p4/pqSnXU0zE+f5qAeMwMfroQ1RKHECIH2H/ACH89R4lqmKTTGm13zU7KqDLEgnJ7WLLPP1kH7e2oq9EOqlR3drH8wJMfl+QzoHfbkfuv/DIHtDOP6zrna7szM8Y/Iow+/nT8yiEfhCaVYk2+DcM/wDltx+erDtVajAJDobWN2MkSoExMSZ/6aqtLccH6ZPHMDn89OE6srYkkwTyDFtIqOTrTSdUmU8l36FUDrtlY5WhMTPmlnP05H0P30LvNyislFHAu3CKY9lKCfODbifp4max0z4ianF2WKsvb7kJ7EcWLpNtOqEnJJ71F2SZu5zxkfz1tqfqPLcVZillF86h18UqdJQbmb03C2sMeoSVnicc/TUi9QptTW51BfcTgk49UHLHMWs2R/PXm/Ueps+SCWUhf0bA+mNYN4f3YUkHtAImRxx7cajxtRLj2NHVlk63vmL1VDhQxAMTaRiCfmPiZ/T6it1VhQZDyqoTkkk8GSecEfqdddO2ijLn1BdI8yfBJ5OYxpDvDH7RmQWC/wDyQfr51EJSdkwwOOldQJVqjHLblcLzwgwDMYJgZ1rddVNSwEjtptVm1QMIw+pZpfkx9hqtVq9tOmB5Zj+kf6a3tSTImAaZAYnGW9/sB+o1q7Sv1Nm09vsGLWBgDuS5SZ5MKBnP+dozOdQ9bYVazuQcn3ONZToGwtb23ASeJmB+RtAn8tbrsymDaCcxJ/01M5TukRgrFGrBP5/1nUiV4dD4BH9I0dS6UOZyRx+mpF6TAmROPf8AtjXTKcGYASm9yoI8HIPsfYe/9dGDbIUBeoEYD5YkH+cj9NFL00cD3njn+/HjR1Loy8kkfnn9PH5xrDxI9CopMg+HOmI1QkVEMHHOfpkY4OY9tH9Q6etNX7hhyFHvkH6TM8/fWVKBUBRgeB7n3J9/y0RS2NQDNQ2HmxseOY8Y5+2ONRLLtmqh7Cja9OaoSQGKAm8r+GPyOfIEZz7YK3m1RCVNVhgwthLGO6SAe0AZMnj9dNqFYf4YVWiQMRj2gypM5JIJ48DQFfpDurP3s0kkVTjMgiWxHPICw3GtE1LJWwAfp/pF73wCckGFkk5ImPtHvk+OHojutdIjEsJYkcx+AeM5x4mBZ9t0ZaxNSEdsDtcMJRY7gMsCZOA2D4k6mpfBhC9tizJa0GCIyBTUE4IOJ4H6U8oHCynUaRmeYI4zHOuN+Lm8nHj7L/r/AE16J0/odFBm5Y8hSYtYyTiT4x7zkxqUfCdFriLbgVAjAIPm0ceIE5H5alfFYvDZQdttAG7bjaoIgjmT/fUm72/cuDz44HynH6H9dXTbfDlJj2kMQJJVB9MDPdEjEx+c6MHwu05UK3if6YmPynP0zrKUp8pC8No85pIZJ+vH9/56LetIJAPAzjjOdXPcfD8Atf2kcsI++Rgjjz+WtL0xAoIRySeVAOfqbgojPn89RTcroFCXoUWqjlrgMRHHn/f9dSUtowZSFYgcMAY/FP08jV1fpy+oLZW2SbhAnPmYyfuProet0xwsekUPLckcwIM5n3jH66uO5dA2O8lS3O1cgwjTI8ZPyz/f9NQJtKs/IRkZjmB/rq7HpDCCyKp8/U84HtEcDUdPYuymYBnKoGmMT4B+v2jSTdVQbSq1qLGFtIyLhGhd0c1JHcFIz7/7nV6p9NYuReo892JB+uY5H6ah3OyeY7W4gUzcc+ftxzAg6M3wCiVDaubDCxP6ASOPPgZ++oaVQwoAkxn8iNXP/h3dAZWOQyCwx7xByeDbg/25r/DpEEqoyFkELkxHzceNEs8xDaVHeNHpggYpH+bOdCivA416DuPhYuP8IHEResgc8mBmeRPP6B/9lo7qlJQM8OD/ACuExH8R/ONWmmuGCiynMSTGIs9/qmu9ly2OKZ4PuCP76s7/AAyFqmUYqRgrnE5HMcx5/wBNYvQASRTEsVyoiYuHkwCQIkAznQpJNIdCBKZByINsj6TjW6dqoGtEl5B/M6e/8AJuDdpH8WM+xHPk+I0LX6GCsioIBkBQ3seMR54Gs8J0wUXYnpuLRdGTyR/CJ4+yxqbZ2rUpgE4Ue3sSfvyNE0+hmr2B5A8loAPcCM4BEEfnrqn0plqL3LdE5MzxBnj21Tqg2NhJ3oXwQWP+pMYP+zpLUqFlYE4NQf8A2ZufvpiOkVAQGDMROQZmMYiZyP56Wp051UjMl5Ig4wefbVR2pBsaBqtND6YJwAeB7sf7ffTLa1kUMLQQcWkYOB9PfwZ4Ghd3sXW02z2qAfExJ/OZ/TQ/ouDwcT/T/ppum1kTQxp9RiklOAggzj5s3A/XmdAb3cXN/iDAjBP9h7ajo06kDGQBHmB4H9tcWVPc5M+B/LVuuURRZdvsJHYQ5jkMMe+SLT9pnTH/AIa6BbiAGwtsNJj6H2niT4jI1ztKwdHdQ1vcCRVklrZCCZkETAEEknPELtt1oVf2ao9NjUDfukEsFi03k3QX8kEZxGOMfBT5NVpxXIwp7IkXCSZNwIIgDkkcqDxMYhvbW62yqgygJu4CAkeB+IfXnWtz14Cr/wDkVQgkQqLcpxwHtWREkCROZwdO9z1pQEsrMaRktDUwwJP4pyCcwFwZw2ns2cI1jGIJU6VIlhAjP39pPjxiffTDbdFp2ksogrdJEgT7TAP541m2CVHDPt6asSIZgG+zXBg44P8ALRPqqVlzSZ5wA5kQeYEIDEfy86dLkKOqG2pqwWiVmYlVUyTMyT4zNonOo6tGmWHqKyBcLIM4xIGY7vPH6yeAsAhXLA4Pzkj6ytwMiYED+2lPqUyFAqEfhi0AzODKzYYPsPeJyG3Q6GzCnct0GeFxe/1CkGe0e/idJ+s1qzKyUFW+7MOAwnLFSR2xIEwT7eIKo7xEEUi+B2kpXtAgZJgLHJy0RBnOhalKo1OBWqq3ixfTBE47SxY4HmceNUl6ifsZ0XYbwAKt1pJwW5yD+KQSD5gR3DPJaLWrh/SsftUerWckwCflTt/esGiSCoxpZ03brSrGu9GvUqrNlRywALWqRJ5AyTJP5aspqqNqjVCis7FiWMz4+YcmI/TxqlRORdW669MFVdDaohV+YhsLgGckTMgSeDOu/W3BvrUqLI9xA9QiAPzi0nkSfIHnBdDcIEe3BZbpCkSffPygie4nk8+NDdJ3JAY0ZYYB77lkQO5zPdAHlhA8DGgYdWFWoZqoqKcfMxJ85j5fHtxnUP7BUpXGLuMqMx9e7PnIEyMDUD7uoQ59VQvNtJTkcyDdDzn2H2g6l6ZuyKc1LWbkOyEFgRIuQC7Hu0AAzJzpNKxqyahvCWDMF5gXOF5/gvhgT7fX6al39BfUUeoFX3uAwIJ8yAR/TPInmpv1crSVqhJ7sUnYR7SUIBBPH8tcTUpm8mZgs4KkY5k2T2wT9PHMaVDsPosbWIWfqcL+fmOfHtrN1QqRIULIEMCRH3kAxPgGdQUqofFKvTAaGUKeZ5JAyQx9oGffkDdNUC2t6Yq3HhynGGA8AkHwRIyfbQ0qyF+gbUDL3EqeBcycz9j3ePrj31LSEp4tt8k+xj7Z8+P10nbb1G5ZlIgyWNkAzwrEheRzxIjXVTatCtejAG4i4opicgv3cEwQdKgD9xtwctkEj/PnA+UZA/1k62+xQmaaqMmJLH+YMtjP6+06BrhR6ZYr3OTcGuEgTGWk4nERjjOCtslJGj1GqM3uHwfYBVIGZ8fn50UOzupQqUwAFhYgQDwPbyPt9NQ1dxUpNHpsVMdsL2nA+nj+nvjRO8oIGNyMV+klDjMFbjB9mxzGo9tTimq06jhROA4+vaAGER4AP+mltafJLVisbNIVZskTbM/QwC2MGGmZ/LQW86XTUkqHqtbatOAgAkA5unBJMxm3zmXdU1CbFLt/FTUUyZmZ+YH+R99cFXSL6ZGSQXIUn3JAQgiPpA+/Ct9oHHAAemuiA5ELzkn9JjOfPt7SRlWs1MuaT+0H/qAZzgg+fedOqjKygWGOJug+MyBn/kdR1KagkVEKgTb+8JugEkiYkQC3tEnnS2x7slwwJaOzNpVzbZHJYFcZgrHAI/2dD77ohrZeFI5hgCJmQMyAcGD7++mlFFqCaIpMFie4sRPvnI/9WpaPR2ZZqLTAMESZJHt9Pbgf30VXUFFlXp0FptYDWnkdsjGCsic88/TnRFeracrErm6JEfWZP5ab0OlUKbN2MWMLein2mLjIMr7cmcedRNtqY+QJOTa2WA4OAUkTHvqLi8IJpoUqkmSQfIkEDJx5zBPOpNtSqVHaJIxdBJGJPOZJEfpre+3Ppl0Aa4yACBMjJW0KJxk5MEc+NA0eqMyH1FV15DSQwJknuNxHzcRiNNRvNkNp5G9baj04bcAIkXAUg8Z8xlTxnGlG9o7O8g1N1Ix2GnH82nUI3+JXvOe1oAP3YL4j21ISjQTUKHyoYkc+LYH99aJPoS2+hJ0nqrGrQRlZEKLTdWiBUDuyvj/PaMfhY8Z0raqb/QpUmLmVVoDNkyAC5CqpJBjk4MicT9Ipbxovo0qXk1GX0SIJGGRXgx7gEEmJ50y2/RqVKstX1yowR6dcnvByVX0e6TmRHP1OtWqZonaEKdIr1FalY6FZVab2gDuBJtLQpweDHdIGTL3pPSTQppIUTENSR3MecqAgE8m7yM8aa0q9O8mP31RixttJngntQEHAIPbwMYxPTumWovAPa7MzH6/OCxIIGBPMSYERKV4BKmckqgDVTNMgiXcA3GQYQCTOSD3HGtVKquqwnqIs/wDdTkcEyRg+wST7jGsRWuvUuVAN5i4qYk2jDSDAieRAHGu6W2G5ADCoUBBKqYKjOGYspB8lvcxmNSo9EUn6ktLbspQBAJwqCiXxgFipqKqmTjE+eNPKHQ2+ao1kLGGtkYyVnt+vdOoqXUqG3BSlSVMZbH835PHOf5RpL1b4toWkJXo+pP4nDBT9FB+YH8TTHgCdbrTiucmbkNq+y29OKtSq7nlYhZniAOSRwfPgzGqj1L4jqGpbt0sUAnCzUf8AMy0eIiTPGlVLqm9q1DSprRrBgZaGJIIJIL9pQ/cxnnTja7GhTWKlKkSOTDLJGbkYhnrBSWE8AT4mFKilZL01WdfVrKnqEiBWQlgpBM3SAAACfeBBjA093dSvVYW1UpUlLU3VhkqsAsDkEzGMAT+KCCLtVQIopt6jVDeGZytqyD+INiJNsAEBQD50Bv69L1KVOqxEBmWpCFRc8nk3ZeP/AGkkEAHRFUhSds5anWeofUqypYmFtW0GQIuDqT5i0ExkDRNfapcBQFQsFBNp9MGcg3JF3H5fQHTdul0LVdHqusYFIzdcBzkk+D9J40DtkNFLUSoFQtat4YOZ4tIAUmZnxB+sp+5S9gqg1VljFVuSpED73i02jAnu4icTqGlRplSpgmJLU5KGccEG/mB7+2ku+3u6UkVaqUywEUmVGU+6sy2s0AROYjJGmfT+tvay1dnRDqCE9OpaGtx6c83QFgZEFc5GosojosgX8dEMWi08AEAnAhZJgA+x5ONMKvxEqfPVHMdy3E+JcYCrlc48AT4rfUPiJZtfZblBECmVlfMiVaCMzFn150dsastU9LZ7q1wCzBAMjJAlBcCSCeTzA0CLF0/cpUM0rG75ZSSvsAYtLSMAGIxIbMa63TGsjUlatSqi60yGtjJhsrIEfMZgxIJ0PU6F2hqYclcgwyMp8gKSAM5nPnmdd2bhe41mZiJhHCg8AGP6mSTiNP2GF1d4wZEJKgiLWIkQABDSQwJ8lSf6E4VyrIFKkti2yGbE9pkAmPJPjxoDb1KlP5UqMjsBJwtMW5MGCc8RdOh6O8Y3GhuKjESGDJxAI/8A41IYOFEScTxo3BRJXo7Rrx3z8tQyzwf86Fi0d3MkR5Glu2o5Y0t1Tq0yZUq6ixTEACnyBjxH1BE6MoblwzVC9TAWQ1MecAByqsWJjGftobpvVkrVFpna1S9KYZqdLnIJB5E+SFEiSRGlaY3gj3W0dLjdUpqeCrvkCTjuwMzmBmJzoZabESz109iwvnjntY/7wcaP6dVSuEFTZui3EDmIHNysBjERBE8Rid1dtt3qGodqVg2gyguAgA21IgTwBBx+Wou+oyKj1EpbJUqwJDVKVoGeIOJ9j9D9zqpu1Znio5bwiG8D/wAJtWwwDwffxB0XtOiUKjNBS+MrLK8d3IyGFxj2kHOIHW02dM1qiI5vpYdVBkE5yc3ETm1uSJydVUhWiCluHCXX1eJJYGTxxDc/7M8GGpu0BYBG9SoxIPbTMWjkuqvwPYyTk+Q3rbSittOo9MLE2n920mBOWEeMAf6arfU9iqszB2HcMgKwMe7LlQZ4+/21Lk4rIOgpt2YZ3dWlv8JoAVYBPc2andgk8TjUS7yWY02T0yMIYknOZgnwfMHA8TpV1KhVKAK/ppBhh5PgHyBwYn9ONB0aJCh+xRMCxixggFTcVDAyLs4EjUbk1yO84LMu6UgGq03eL7WOG8SRyVPbHIzpfu9uoUWlT3QpixfOSJyfEHmMnGg/20oQqUCbi3crCZkEyrREXAjP04nWUepeoRazOxBmk0I7gQY7SwYDk5mMD21cfkRJ5Ot9VSlTIZqQdoEMVwsiYOGHcvaM5nEY0B0yx1NtWmYUza8FBxwQJHiMR/LRW62wYhnZQvlnIjAOCCvGAMGBPnkr6+1oVJHqhGQQDRSIyB2BrQB3eImcnnVra1kzZql0cu37v06gJ+alWTH5MQff250U2wq04UuR5go08n+Ekf00Oekuq3NZXv8Ax1Kao4Ue83ycA5AHnRCdUUSqu6AYhXqgH6wtRV4j5RH1POhRiuCYxS4Ot3VQBmYiJlkaiVZTm352DQZPfg4H0knYVoX1D6dbIBJuBBE5BDEAA8kY7hj2Y0/h+sRaolQrKWZLXysCGItJDGRMjA+2ku92BLBanpUjIVQr3OTC4KKGuLEGcyJkYEEawaMdUt+lNMr6AIlS2AT4yhE8n8PEzzOpOmboVABUdqowVNMupJPuCSIMmIx/LSDa2UqOaCsDgvFVeAT3VE7gY91jgnBnR9Le0twDQq0zTam0oWQG8E5HqKbGJMEGR/XVbUF30GwehRQFqQ5hVYiowHvDKAngkkqPf6quu9c2m6toG30wSpq3mPqEC5qZ/EQfcZPbwdntkJWpcCrdsXNAOGwEJQgyLWJ+hB0PvumdOSD6bkqO0qr4BJx3LA4jnHH10KVclON8CrfJX3D+nshVWhTz6t7ln+xMyoXAAxj30yTYPSpoKjFrSYassnutAg5PII/iBMQcSw6d1alQamKaEQS8kAspLRaVVyGPbjOAR9idW6tTVyW3HpI4LWtcoImSSQSaYggjjmTPl7idoN0SnTZdxW7CzU4ViCogQXBx24kH7H3xXCqPcLrbiIBBF5hZqMo+VPKoLbjGRPdaOnUnr7oCrUpnaKhY2sS1UjgVJUMygkkAYMcZI1XlC1ae6q0yCC1wuBZiQ4hQCYPgz8oGfDHT90A92Yt9fcNTCVahRUFxZlUWBbgCFlZHBMQcmNVmhT9Uu4Sa4MiTzHaokSFETJET+ebZ8F7V22yVHawhGqMrCSx5nOf9NU7oXUt1QanTpisVAxRZ2n7EiEQYYyZiDjwKawSnks3TttVpkvTq00aS1RQLgwJgFj+IhiwLScAjxOhX+Izd6VAPWcCECcC7g+Lifrn64Gjh0QLTLt/+RJBX9oqkKTgAWothyYiDkecR1tOpeg9ZqW1IJm9gpDELOQC5a2JItwP5aztI0pg56AQDXq0PUqgFnRVDZAz2qSAxwCfoIB4Nn2YpbZEr7s06dZxaEmQhJJMTkkyJn6DyZ10/csf39NFZoyFeSLo8SVnA9v66B6jsP22UrUYCyO5lAE8kKZYNbcQbcAnSTTBqhH8RbajX3ixVFMopZskXMw7eJkACe7OPAM6b01o7b/FQE1QbYZqhI8R2cHuPmCE5JkCnoTBLNtTSrTE/vLxeSoZSZtK33YDSBjEQNH09nO2o/wCGDRIpMX7iq/MBCEgGIiQYkHHOj2ALp7lSyxSr01Em654OJkrJvHIMiQZx79dRrMrqtdFZHa1WvipmCCrATAPbaeYGZMaDpfCm3RwaYF0ANezdpNygW4uYgwZ57WwI1PtkpPVE59UtCsCJQQQGmSSqls4xIyMamqZXQj2+zWit9HcMUn0+4lWmcq5/owGfAjRG16uElGUrbjsiJPiME+OPpzOpE2tEftFGit1QVRUemWCsCwBuUkFTKnEysggxrmtsNwhvFUMpwQEAYiecAm4DBEw0cDTaEgXqjUah9P1fSdYForGTdIIKq13AME8wedLG6fXWlU/euVWneO9g1wj2hwPEHAHOca1vuu1KDn0NmagwZapnkAgKAHuAyRMCDwcaKo/FTsoNREoEGH9SmxBA57riVMTyG+sSNKlQ7bDdtXaptVqU2NwA9SnVdoMfNDOCU8ER/lGJnQFGiSrPUpikQSS5k4/8NwZVIhpuHH6sq+/FNFNRlCE2phVkcgST3DxA98jmBt8zVKBehY6gSJYQfAUwwhTHzCQLW4PErGBtXk10wVKJ7TSzawZLgpDHAkzg4xmfoZ1Em3R6jVKRqU3uLOikQ4cyzQUPqdxypPaZ+p0uobk9jgBhTUQEuyCxJIhiAC3vHP4uCZT6y6KQ+3plQAVa2JBtgXKbgZAmAYtiJxqlIlqg+t1Z6YAhngy0BmSMDCtP6AtGTgTrQ6j6oLKm1eDxYbkAImRMGDbwczoLd7gVA9WKm2aZYqBUUjw0YMH65A8cwLR6BVdRWp1EqmO0iEbEnAMd5xyZgmYwdJizfAZvOliraanYVMKiXT2nA48RAwIn7HUG76E4BLq5yRKAXDxkoYaYYREj3zo6hXqMYrUy4ZcuFOR7N+FiIGRPgzqal1BRBLuh4IqU2Voxm7giAv8ACD+Q0tscsaVMr2+2AeqhU0lKthyhlWYycGRk4kiRaYkTpN1alUAVSGQfxwSsiDhJiJEg8nB86vnUdjapqOpJ5FikODAEgrIP3wfrpYG26EhdwQ2R6bosmZmCzKMzPMj20o7k+QaKp1PZJUtqs5o1BF98KrxBvDSJPvgz7zMi9S6cadNTHqEGTGLWJIwTEmLc+x86te46PRWy8D1DNoemCDJzE9obAgk5B840Fvvhr1bHNRFloCEmfqJERJPAYz2+JGhPiyXBvIhodV3AUB4C22+JxxmRd3ef76l23xcQIqU6TkEw0hZHiYdZP1jOjN58MVgtSr6fqpeT7FQuTdEH3McnxnlfT2zkStAwc8EfyYgx/udXGviYiznqPq0bKoscyQxCVgZyVCEgqZyDkgah6d0eJl6l0gKWY0lGAMqrRbjg/lpbu9+QlIbZ6IYgl2uUEqBBAYC4rddkZ7feTobdNvT6YptVNwAhRDKcE9qTIIyYAMiJ4iuox91WoKJkAEqZJ7+ZwYETmSCZH8tLN+a72CnSRUghxBWWjB4Aqe1o/Ef8oOgtpT9RnuqM75USzEKRFxJY4juknyIjli/6B61MO1BnK9qsGDMoA/hDfMYHMcR99CY6wcV6NNK71dy1Sy1Yie+5FnkwM2rOYgRzrvaUqdRQdvTakbZucwWUgybbgAJj8Jkn35M6yisiVXoqrqVVQLnBXuYFadMyzBpi4D5gQRGk2932AoqNSI7SVHBiSvmDPKhj7SdDY0iTpnRlZmqNe7x+7uMIsxDBTIAiALuRcSsQGMq7CjUcFERmCoXdbnYEyDJYqpm4QRMktAzpanTKzCFZ6ykQl/qqAIgi5VhTE5IAjwTnTmnthTX9lpBTJNV4DhjyIuzcASABH1jGnZKRW+qJWNSpTo0rkAMqJcMPNoUAEkcKZODHGX/TKCttitVBYBBWoACSB5NSb4PsSBMHIxP1OvS2xpX1lpMoUBZliScA4iORNwAxxnUtFTUABrbckkXAVGk5JIHYScQ0zEjiOSmM2+4RCTCEiBSFpIAUZZiOJJwmZzmASOGJamVVhabSaiWXloEKS5hciAqyM+PGqnw6iNUYuGauLIRyCYM4kyCQoUQfrxAC7qTGmUPpuKQsWmGAzLRcSZk90jyF5Ps6FYb0vqLWsrgqoLBe68qFtBLraPOe3HHMjQNXqq0HSqK6hyQyW1BDgjmCpb0zBAEZxxEiT0nvFc0y7XOq20+7uiYGbisAeBkE+NHf9hFeuz1b3C1DaWqAs2cuRb2nEDnnSVIHbB6depVUuawFAFVNKiCoN7AXRTBLNP0nyfYMuobXcSKW1o0UoAEOWAuxhiQRzFsE3fXRR2gHyghbgCtM2Dn8TjvI4FswIGI1J1mrWJoUqLhZqEGFm4QvyqAQqZzNuPvqcSyVlYJujijUHoVf3rPJlq16zHy5JAFpIGB5wDoHc/F1Cm1Sj6YUqTKNhsQBA8gf0t1Ps+i7f1GIE1A4MHOBHHvieZiR99Sdcp0nf96gqOgLQZynlokAkYmefp4SkNoE2vxCNzQqPTogmicI8SSZBAkwsLcCTkZGAcm0+lbioy/tL0xSUC1EOQ0FQZCqICllgc/1io9dpIsAQJgBYQBoGI+WTkwTnmDzobd/ELqgsD3MRI7Zgm2QQwMTAx/EPrD3LgVFiO6p0FN/vOJYge5n5B9PynVe6n19CA61C8AkQjOBmMssgfYn76UV+qOq21VWm99qlg9UCYIKoVVWYe4BE4mRGhT8NtWc3b+q1QqCVLMjA5OApC8QbbRGfyMt5YcLCHXS+sjcMEIV1EjNwKMAJB+hUzzx9VOj621oVQGanTZqZgEwYJyojt+kCeVYYOSlXYGiCKrVHple41ajsBDYIl2DEicCIAhibpBu+qGrTq0GRlLUwwAYdtrASuDAnI5+bjgCW8ldCbYgIuEkNkoGuGO3KVCxBwMhvMRiTwOpWGGFEq2GIey2RwFYtLCFhViDcYGk+ydahlqr3Ag3sFte0HBywouAMmMwYAJMR7zot5mogVbjEtaQSS0ZT8TEn5VnyxJ07EWIiiAQSthkMDSSYxMsrkGft5HtqFPUdXQba+m0hK4KQhj5lRQx7TOJPEYwNI/+zbE9tRhkMQGtYAT5m0xIgniSI0+WpVQUlSHsIv8AVIDj68qSWMw38Uj3Oi0woApU3pyAFZlBCryQMiCgIyB3ET5ngRoja0SypSpIiqKSmsxwL8Fpj5WEDIMyfEHSzqfWGBan6s1VIlrQbeGA+ZiMec/Mv1GldXpdfcKS9clQQDVi2wmDGAC2JgAyS30EqMUgv0LzsNzTpqxuVyO497ETHMZsF3gTz5Oke239RnLvVpVJbNJVIAE8hWgkxiQAZjJ8x0diBRSmga0ZvqHLHgM4I+mFAMKfudDUyDTJVVURl6hU3GSIxKKcnkTxnIGiw9yxt1cysMnoNAYM9j05wSA4EqOfqBwPKrqdNU3LIdv6VNflrIVsIgFSy3CoPqVM84963ut3uA1yCo7ASHFTHGYQrIyDwck4HOnb9dLU6L1Sb1Bp1cTAntvUgSCOfIMjOJVxE5UzBQr01LK0qfx0WAGMD5bQJyf0GcDXX7RXSmZqBmklPVC/nDWgk4iDBxzgAxHa01cFGVWYm1gYmREAjg4+VoOOPBBehVLMTWjGQxUxAxiMmZ/l9dS5UOTonTrBp1CXtBYZNJyJHiUYMvIwQeZyJ1xW31NnctXcm7yoEfT5CD9xz951y7MwUVFNQDywkkDibYjPsdLKuxWYFJcY/GP1tMaaa9CboIobugHdadEK6pghZCqYgTNhzasCR/Ync7S1RUe9Bw7LcMXcxcI/KTgxrvfPt0IaSrvJampFg8zcRdgE4BKgcjxpLvd5SawBha0OwkKanBBwblnEdufYE6022F0WlU26f4jGkCwYUxBquTk3SCaYJA+XOJnQm86pXqL6e2pClTwLg63tJzmHZVyJ7QxnjOA9nQBqC1DTuUmbBU8ybmn1PpBwcatHw0lO4LSUNTHe1dshlABhRMrJk93mT50cAskPxWUFGmrKson7yy7xm1rTcqmTMnwQZmCuFVOyqLWpQRm5SSRaAoAtMERgyOfY6k3dMNUqVP2kIGecguQR7qD+8v7hbEYHkYjG/ooTZSlrO9qxtAXJLekDnuABD2nHA1Cyi2R/tRrMgl6NL0PUa1iRk2WgTJfnJ5An2Axt7vKikUKT0aUkFqgFOobSkE1HPDKWyPKnmNFdQ6hRFT0zuK23ZsEhVRbhFwUAkjme84kaTbnplMUNwxfdsQo7qwlWJIiwhiri26ftyMa1SohsYt0ShuKoqestKuy94SorhyAAWW0mCDMgTMcA6mqdCop2BUrEKubzTIlQScrOSSckwCOONVPoNN2INW4AEemCImGxxDAA8iCTiWUa9LApXkNUEsB2sSRx5pHPjjj8zlTbToIpPJWdps6pUmghVcqYqIQBkEq1NSLj7tOPEnBvQehelcNwSqYaHaSrRmAkRwGgi3JxnEm/6mKNAqRSoUmJWEpWl2Oe2Dn6nn6SRI+y9WoEajt6tTMLUZlSbe0zd3gTOVVSPLZjQmDQ56l11qaFKFNy1vELK/Wz65PGk/Vk6hXsagPTvkslUlXpliZAkEFZyCO4A5AidPqnR64UEkU2I7loBLeeO5ZYkeZ5J9tBVd1+GrXAeCMOQxziQSAIB4UjjUuUr4KpeoR8IfDj7aizbit+9qEwZJVboAABAuIge3n3OmdTqNCl6g9Qu1MSwgTwMkARkQfbP31Str1mqVNNRVRqckhpmqvItDgrcYa79QOYrnTfiapW3DK9IM1UFfUVnRyR30x2EAElUXEHI4GC6bd0LckqLF1/42qVIXaq7WsO7tmZ9ybQIxjOdBrS31SrSrU6hpVFYN6FQggYhgrAsWU+xC8iCTyR0DaUq4astKFpkK6sVqUjMGEg/u4J4AgXSBBGm+82aObybVKgYVYBBi7wxx7iOY0nJRCrVtnOx+H6QrNWWsUWovy/NyZsKEEGGkLz+EAYgm7rqu3WoEeq1SSUIRp7hItgZ4MEDGIx+IcdQqU6Aao4v5W8AFVzc3kqWFwBBiMn30i3vUFp1AY9NiRDUjBbIEGBkCYJxnGYnSU23Q6SLHuH2tMgJ2gmbbuI5OR2niPIzgaxd7tKb3kNdBuImfzaJbH+YfyxSOo0EcU/WYpawtKkKTdJtC9yxlVViPwTkHI3oVa5/wAb04hhT7gLeP4bjBEZPjVk2eh1etU0/wAKi9RgCQigufuSLj/P+euemZJR0NNvTckkELDKwImBbBCvB4BY6p3w50LdVifR3FT0rjebmVF/Mr3nnjI8+CWoFKjVgV3qik3fUqsIuxjzAImOJBxPzaUl1HGQdS2lWtcK20dXAXvJi8e55BZZJHJiRzhmnW3pU1e6oqgOMtaSVYTCyptW73B5MRI1W97va9Vv3VWykV7kllkmeCDAHGAyjHJzLBqCHbv6iksYLsSO7Ki4gAgnCxySTzJOoZSJV6ztgCiO5RB/3SmQRzccZHPGPrJ1zT3lN0qQlZhyVKuxIutChIDE/QHgA+2tbBP3gHpn5WEzALEGCI4YsRkcx7DM+2rqqE0StMEGHUDBGItYQGJ+8xJJiNCSsLwG7HptEy1QNTJGA9MKWnP/AHlxInxzOtV6lBVhVdoVgtqEoB7S62CccZPudKNv13bJWvqVDdeVgXMTkiJHy2+wiBMeNddR6WEf1QzM5PaVchWuzcFkKxiJXB9/mB1VYFgn/wCJjBYi2DAP4ccC3BiVBj3Gk++31VTFPahgCGmAwVZFw8gAkT75I501rJR+QkZi3M/xAqMQTDAzM8ng5zcU4FjgA1aaHlchWcgQSCxMhvOFk8jWfUpq0KE6k5cl6SAEgywYhTyYFwBMwf8ApqDcbmojzTWl5JQUQLfJJc+4kZAMn89OaezQzTbm3CpUWlaZGLSyFe0x8qj6ZGhd10wwSqBQEUsZQfKSYKyJY9xJjOYmTqOFUTKcGo9+4kXqz94UgEqWa1UpkYMyyKCD5kmc++hqW9dnDw4RVgFrXuP0kDEkn3ABzkac/sQuUIaZRjyWBBMmZb5XXzgyf4cyN9R2VoJc0yWU2W3SFHHaAFBAjE/lxpyFOPvwLWemwAZVBAMt4EkwcEDGZ/LOs6kO4MKuGUMLTAAyAMcwABJzoPcbVyFMG0d0QO3OcAGMgQcA6j/YCmP3nubFZh+qFhPuJkaFZi1J8oH3HrVmAanUHqcRTYyOfdVkiCTdgADOdN+k9NsrBGYLVUREgPJm1WCBqdVT29rHEnJzrWs11Jm1Dn06b07qReizBal9FWdGIwC1NSXUqfClgB/DI02FdtrtiFVf3xIp2kIsMZ4e2wknhvbnnWtZqJ4oIvJXHSmgFIkgk3MlJmkZj5kUyIuGSJJOudt1TbVXs7jSpqar9pF6rkAzmC1qhOO4nwIzWaNOK+wPCSAdqlXcPfUpglyXKujNkkm4Ad05JBGYAHtLrp609uoppVNI1KpgMFDkRbIRPltLMe8Y8++t6zRubbQ/hjYHvviOnTLmlRMzBMJTYEgDJUMchQJUjEY0j/7T7pnikqovqKFFMG4sSDBYy7nmQSJ/TWazVwiupnvd0X3f7Abx3ajUpu9NxTZA0YAUvYRwZLY8n8QmNWE72nSColNh6aixRCjH5yBBIM8/XWazSlFJmsXaFu76lNEmoQal0hR832wePvPB5515bvq24qVFvRqaVWhZgO8mBajEEiSMx551ms04u3RMlgOrH0FSht6tZTTYs1SmRBbM3AHIXAAOIzq17HZ06oWulorgAgstsgCWUWtkgi7MwLhMEEZrNRJsuKTCaW1Kr6W3gUpuKo6j5pIkBSwif6c8a6rdHMi8U7f4jgxHNx5I4HafEW5Os1mofuVWKA95t0QksRVJAZP38NdMnALdsRJHdyBOiVp02BcEDyCBUPIETIFsGPPge51ms1KljA9uTVTZUnJYrbUK2s5SUa3ki55ByZAwfyOut5stvFM1Ha5T2AqPJLTDYIzE5HA8xres092QrASu9dqYoBXCBcsqwYk9o7jjESrGfMaAr0Xannbs5XlApgRPyq1oJxMzPIk8nNZqxcg+y2VRVZfTekQsiALDPkFu+QfwsQMcxozqu5J27NWC0wLFJFveASebRgsFUiCBJiYOs1mirdCukC7Xceqf3isipSZxTQ4+QEiCIJkxc2ca5/bhUb06ZYXPABNoUTnuiSBJM4I5PE6zWamTKRylOi7sK9KmVYG5+MmJZQRaQWFpYeF9iInpddMvTrU/UpN3IBZ+75GGmYC8gjhiMzGs1mkrG8HG16pRqvUpUh6FT1JWak3geVLrCkmPEjER4i+It7taKUjWaqlR6VxURfkki5yTawBtB5wMjWazW2npx3GM9R0A0fiNKaqBTYkmfUcipULcAsABHOQFnOtf8arMbKlVRDC5QqjPNxkn+fvxrNZpdR9Bv8P0U3FPcBLf2kAKrzEwDAgSFE+BxzydBbzcIXSmECx/iHklgflYxNMkC3PcPbWazWbjbaY3TQJQ3yenN9jEwCzKpGSIMuPYyABzwZyDX3CkyGX7j0jP1kSDnGPb3nWazROO1JnNPVaimf/Z</t>
-  </si>
-  <si>
-    <t>data:image/png;base64,iVBORw0KGgoAAAANSUhEUgAAASkAAACqCAMAAADGFElyAAABHVBMVEX///8QUS9tvU4AAABtvk5qvEr//v8ATCYQUC8ASCAATSlou0dkukEQUi8ARh34+PiQkJAAOwDPz8/09PQAQhXn5+es1Zyvr6+9vb2KiooAQBDg4OCXl5dqamru7u58fHynp6fHx8fV1dWfn59ftzqPyXhfX19nZ2ebtEpHR0dycnJVVVWWzYKJx3F9w2CuvrU7OzsoKCjP58X3+/R1v1fI4rvt9unY69Lc5eDM1dGBxGej05JvinosXUG/zMRggG0ALwCJoJKktKri8Nu/37JDalNZtS2VqZxNcVqz2KSLoZVbfGgwOBdqfDNBSx+o1JYcHBwAJwAAGwBPrxx8k4YpMBRYZiomIy0SEBhKVSR8jzsyMjKgu0wZFSBdbSmCQu6rAAAW80lEQVR4nO1diX/iRpYuMLJuCZC4BC0OC3dsC+hGHOJ0A8KAmRnP7LCZmXR2//8/Y1+VDgTGSXYzbeiNvl+HcAhR+njH915VYYQiRIgQIUKECBEiRIgQIUKECBEiRIgQIUKECBEiRIgQIUKECBEiRIgQIUKECBEiRIgQIUKECBEiRPh2kK/h5lo59zAuG7oMN7kM3GTySvrco7k0yEW9JJN76eKHcqZQyBXzH5PpXOFTNY8U+cyjuyDkb3PKfaZWSsof85lKRb5DpfQnhKqVag49oLvICQOky/lasniXe8h/gAcldItuqh9y1RwAFcrVcw/vgiB/LaJ8/qFYVMqF5HU5XUUZHaVrui7fyLny/jhr1DEX5xvmJeBzPlmryDc5BR17Wr6wv9/meYoyuu86sktDtaa/8cp16H6HisfjCaP3HiM6IzIluZT/LQdaVm/RbwP6i5518AKfAKbiQvb1e/5fZEc5k4Tb2k36U+bhF9UR8ONkR/VmXDAwnhpPhkE1R87ehBrYpuL86PgT8pXMNxj4e0O+r+RrZaV8c1OQr++LJ4+x+s6o0aEEQcCBKBFPxPlEYtgXEhRF8YIw9CNT18BGxb8cvT0NafKbXsM7IHd/U3wo31cKxU9pJV+GnH8Mq72pU4Yh8FSCuJYLftMRqCe+adbhyQQl8I57dIOHF4328Uk+Z3LfuVGBMqrk7kEd1R7SyfxxMLEWjtkEMyJhmvzbM/XSrG/6vW7dezYhNLE4uLbi4Jau84VDWD7/vWvTPFQihUqtUHwVR6z2y5CEI0EwsM+Feeo0O0QJbDo8HzxJCQ7Og1a3S8JWd8gLm/AJ06XvmizlQclX9F8I45DmII53s2aTF3iPLGrY5TvAVNMY9oeURxTELsNPeddo0TEgmj0Fwkqv3KarhTc+4/tAsVDx73q6CBRA29lkRyMTMBq9ZDdOe9HDQf0FLj8OwYoChrBnNihKoPaWlogbvhFZlOuwHf/cf0UQAU8ni4tG8o0x99rZOklw2N1CwI87JnhVvyGAqdS77VGHN+ptA9MRjvO+OodXEjhBGn5hc3PpvZn8h/JrKVnMfa29PrTXNTvGE4lLmA3PTPZxHOzHaDrWYijEO3CMOaT4DlEIAXB6NPrkZH3DfZPg7D+g8pbGvwzk0pmaHM5oxULmoZg+1gI9p4EvNf7SXfR6fWdo7AN1GAmB2qANSKYE34VoL3Qao6zTxUodo98F9/QKGY9rPiTWqzff/Gp/D5KZm0KtVKne5FA+nS7dy7foIV9Ft2FLs5yGAXJSaPaRPl09r1o26o2Mk1QBVx2rHxc69Wx34YqAa90eTKctwHQgo57pik5HcL2xfR1UhdcP73rl/1uA9L7O3ZQLmfvarV6q1Sq36IMe/nKJNeHwCyl9sNZUiWXV1GR+3Y9Tp7mi+IWF7UYftJ53j0uG1QAqgaYtV57YsJoCRRn85tSYLhNVVEC3lZuPQFmtnK9UK+lw1w1o4gVSmySM/vWjxsXEWCxGaxNtUrTeoAr0eA9NHye0CqzSHBfbg4lxkvpou6ceNeuOdTSYy45UuADWqyiX+ZAr3pL45PnDYgORmfIVdluZsMATE2PZsT2XOG1q8YlXLLlWFUeZVJihMEQ69fgGIclk5Z2u+HdDLvn3iDYKpTjeREsa25OojuE6d0Calum+EaviwgitVPENqmLA9dT/nP5LfWj6pqVXSq/HdH7Iuk2gv+4LWW0zLhwYDGVYKxXsiRFVcpFjsBh6iYaH/pegEgKoAqhrQCZN3jKqmCjGNNcDkfnExw1IqW4+lC+lmvGTTGb6vBXVFEBLkVtJnGx386nLWa/bMAxqT1MiAZqIf7lm8CWK2oBM5q05EYxq0BVCXpfgm2a82223XyD5N1BLjcXeNCt6TUby8pTNZrubjen3QNOXoz/l6W6iqiyH7YN8vzj0iCJHs5KqTsayVReEA0PhDb6+gXw/0PDh0gqIekbIvdydJSR8mhIJfuiYvbohPOFSz1hcv21UAGJUsuDUm0ZDMJyO21wo3r5VHLw37DEDLImMm4iCb5xhPLfQ5n0j7HSCkXgBTW0/r/W5RI4E/1jCJRLauDVyWQKXo3iq3qZMk+fj2RGoUspEK+nA5bDTicFH0mMYzsIcQtk42hhxp+kOMHdzET1ie52iD/3h2DvosYWbJwk3iAvNzQIp03EsxaamK4lxr28M/jd1mVqiJhEQ3a5jjpz+E9XZPJltk7gkb+mp4GNolplMlsvJJCb5hsZCXmiP4llzYzoO9TL0xngRc80zjWaOnYA7pI6boDpP/IkyqJcFyszXrEoTZyE2xT4jewenGtOeTXVwGG83hVH3xWiCaW3aI9LVAzvrejEdPoAdT1vz+Wo+n7daE1eSxdQ5JD7eqdeFRqfdceLeIPPn7xErS+mYJriE5TjGhelTpwsDt8CNRhvp84kk0e7FqlMSp6Q5whrBZn0PggTJb+q80P67wb90R0YXBfHNRM/uYay0nEoSSHsWbidTlWVF1yBRz+jUnc3GeNo0TW+YmbNXNDpDv85E2Jn0SehpBsZf5ylhBCJ7m5Igwblxn6EfEQ4y0koGk5KXhL+YNugLuF8OusDsbkBD1fmhGeiKJvgovF+czHetCct50Ga7+Q6fN5YCykcCJfANxzGf+v5AK2ckCcO/uEOoA1AO44NXtBZ80T00n2h+QCFyMyYpM7BJdtYCi5oQWxHBVU0cu4fOhm9CxdsZdQTHavoZQejpWHzSM5xItmsIUhCq1o87GckT8uFwKlQHPQIi5Ol4quZ8GJ9wPeJMCKRR6BlGZK/baBqTXFvCdLAiCTU7CDsit36er1XOtcKU3XflFGoL8dGQHyHTaO/FqLGQiRLRVseDWZPgCGYKaA95nmqEZmqKNx/PGaqmqdc0ER7mg3FKPdA9oJhaKV82xFIDL8+BNtdjHLflJM5VF6LWQl6SNBv80NoYWTQCpho+U0IbLTkS9tfSOshog0lqrrPu6d1nrIMqWXlAJ+bJ3g/HIpABsSlivZn6G7MarFOxfVQH4yFyFB8Vo7cQyR5pLMBE1laWmmdOYozVpp758B20eGog5wmYegKm/CpIcNAWHJveotZ4b1b2bmfr5CyiZJ8aaqVyot36PoAaphWuVkUuBtYvqRJonPGcjHbKsAFVoAfUPW3K8xTpHC5jSMXXmsDbQM+r9E7pddy2Z91EvWEW9Ydd5AwXKFvvuJYGTD26TGEopJU3IPddphgSJRHu7GRHo6zTD2zrjJLq0KTW6piJDWw7sx+R/Ch5ih2cZX802JfMyOCNbtWjPdrIXu3G49kU3irwXoo7xoj3bcpnCggZ/+0L4D9Iee0y5UZJZJmGwPMGlMmCu6yqliufqaNw7ZVsHkAHZJAymUz3R2DGxliCx3AFPPWPZhjwj1YKZMHMJtlKpKX13FYsxZ4+jpFb9mCm8FQwVIbWApH/zICpLeHcbUbZg+lg4N5tSaL3PQCGAu5n9V6gguTJCphyHp1JU12jXUgHiAxOzi2OU+nH59UYV19osATalq4lTUK5kIZLiXFfcPfAT52cpGkq/KNj10M3HgFTQwehpwWy/m6hBR8wZbgRPYbD0aA1HeAOz2A6B7K8gpAkvxEwRHUW8W4WMybUQXtWzsMTZiqsONkVWISeEkkxJkkkiMiT1GQ+JcNnZ0rKU6gQzyfTFkQkMLm9VfrxTNNfeJ8pnL2wXfXAy6w9U6ASiBp4brWWmo/UrtXa0r6jox7WGfxiSBn9Ou70uCs7MmeKVHrY+USahpKCI9csuhU9LuM4z2jUgR/9GTq1HGwlkdu2dNT6su87uPdwbyrhMXUEjyneUtyTspIKysI/AXw9ntGKExkrsbiwAXui+AV+Gw9GhUo3Z1r1sjcIHJY5qPNYL9mTdhPCgSPwTXnt1YH0DrwGl8Wcmlo+tvxWjQ9p7s5tJk5EdMoLYLYW+yWInI7nshLCotMQho0sMVJ8unTp/p0p8tDaZ/3YZMLYijJlJu5Y3VYvGvhHgEP4XSt6hkthyT1Mx/nvgCp2RhwnnuhssntsMFyZRZkHH3yKKSmDQOUnOu1uv+P0G3gGkMLdl8y5Gp/zfSWj+mJPnpHajXXNXJd8ena2f5dJYRYnmB+Ohdptd1gPkU6Wq5vCqxPwrSvS+c1BJiHUgNbluH3UhNFYpEAU+HYzvsE2xZtvXsY7YMXuB6sOXMz8VpzbXQ+8sTUNmRda7pagOJk1B5WLnxz9l7coEU+8msVyySMioY/8VhQObhyrqhJu500mnIp7OQwp0BGEKH7UHwqdLA5Z+wUdZ8HznimR27lwlQ4OU9dgL0F21AZ+S1cEkxpoLAStlD3/omnr8TjcnsFM+ZN7PF5uxuPb0FqFBNWTNTeMMyAtpPWsNcgo+FuR9eL8UcVjwr4vw3uEhtPtvmDfM5xfu5hvipBNiTGkyDqyvRCC2/72F4hHPgmaPfMOxuaGO1QcfPGyTRTjNmRUDGRNsCmKN/jhyGnjFQhWr5/tBGQlhiSTQHpVpeVqIJMls1C1vGxI2aLPQJKRKLkArU8Bz3ycN5r9X7mUb4zWPsKIHBrYLWXlMkWcb5xq4XDkIqXsPKbgKgZjYGjX8s4iT8OBimGfe4YRr+Pl04rdeh5vH8ergYIWI7fISfBZNGMZkZW2UPlYfW/JLAlmhtHZ9JC+Vd180ht1yPLH5ujMPEH9q55gCl+2BiO1NaypfLWjBX09MKUxnqecT2yk7MbbJXMY0dXWwuyja3s+XoqqyrJMCmQTu52inknUg9GHwEandhmytCE0G+1mAWFkod0Xr6Kyeu12P7Q69vr0dXx7hGRNmCmGmyBcPMP/ZN8/NeTp5xg3aS3nu+0yRmsrHa/DOJrUAce9nm5jEJzJK/RuSmNZq0Kx1I/zwAWyWW2bQe2hcMiSBz6+QLPB0UjPRpEP9hRTIqnlxxJ+zlYDph5p/0iVk1hCkLpkvHbV/jziBM1pjRb9J+kJFiN4Rk+bDKy6wI/QHNy6HTfip/MjxKZe0F4JGOo5L+Yo27XeuJBvjsdA10BE38cpRkYzPCMu6UEISul4acaB8WD72t8NapKZvi9wRFFas4rtFYyc9ozMpzaaFa2G8AZNhKrhcSNq0XAFmXC2VVVkjsRnCgp6eQpMMWoLjckLqu2HcUaFkvjVFA5oIQnPQnGhKWA1E9IeMfZ5wNgD1c0LjKitUN3Ci16P3O6INqM/WPv+Z2NptVcZxrmo2vfmOO9rbEncxF6SnhQE70BU0o/yUUCCso9e7+at1mq3VNmg1BmjcG0DUl9ZtVIt1ns5hQnAqz33i2UxjpjiTUXTJrvWdLrapjLIDBvg01kc8Bq1AqOiH+cEay62pDnXm+jnfdXB6vODspbTlpDle4sFVkyZnb98LKXgqBQcxehTxNjzoGbEucIJra0SGvV63awfW1UHzyHilSNSag7EklfJWmNSC50H64ALWiI4qEzEoE8g0lu0lbyHEJ6lyQB1IcnjpdVxUAU6nohmRHV1YHocbTOMKu+1KTC1CBPVRT3LAhlw6IEJwfKMmd3iVddYyQqNkeO0qcSJpvP7ICiBSVtKPI5Ee+OIqTM09ucncMDZBJsUEpQxXMCLRLGOQ1GKe5wNtjQ93tm+GIOs2ggtLRJ6I7LZzzIPF6YJPbeGpieKhbeSJoR4H/X6zgYb1bk2lQ60w4Wpb0KEzDV3nYzTBtYQeMIhhvQIoHbpYqogWWoh38PV45gGLaV4NiVq8iIcdIApwsMrptoQFpgYy+iojqs+/gX1hniF/wuPC+wzwWZOTbefokpdy/oSWw6T6eEKJN4cNup4h0y93mjyDtp+mWZSEuuvChahWLYHkDO4tdsNhkuf+X3PgCk8CSj0TOrA//jRNcey6iNCIwN4avZQ16Dw05aA51XPBX2rvel0h2BjA7TSaMZGEDT6R9uILaRM0XT1PNs9rie0hlf3QWUzofFaRlc4MIwEFIdtxwDvE6DeO7apuGDZ490AWaYQ5zu431LHRJkvfR7HtvOhxam/tJ7QMymOo6UvOzTYHq6EztdOrBaQ7elsoqk0M2YgWrkTYZAVxv6Un0/IAhgGoPrBlhsgZYi/hn6Hj1Md8oXg9wl9p0md0fsI5hPSF3rLtvBaT3qyHs/mrSKq3pBZbzmTQRk5DY+qSkY/Nb+rTMdMihZF2q+D1Ix1uPo6aM91+71F3+T3lsXz5qiDD/aIwStseSe7qFNni+g+BrtJyl09FizuJDsPaEnTYttZaxCsuf6o3CvJpP4hX0kXcqXMTTp5U7qV7wvJE2dVpo8a6y1mwKr05XD7keAz1e4IfKOLN2sFoHiiTwUHz38Rm0rwBhoJzbNXyxDb548MVnssAdxTJXG5mw+O9h18KJRyyQ/JPEIPpZsiKlWTJbmQz6PywVHJB+9XATIz1ltJlMoc730ImIIwBJKpuXCMcMBKkB0UaNNeWF7G7CT4E7+n8M6oEptR7GkLR+XZat4a2CfXy5eVcq5U1G/xb0koH25ytUoJlTPlm4OdZR9CwUt+jmHXZncoe7SjLWCKZETQZc7iqHYGobnIUpt2YGzG2doJAcp6Lo9+y7qbXK1YTOdlOaN/DBxBVtKF8G425Q4VC1WUK7guq0O1I0q2JRwSlTAOmMLUDfvtTjiWgQmZ2U6vGay9Or9JoULmLpd2Y43+22ZqlZDJKZXDDaZ3OkoX9FzVn8m0l6njxBeO6HVv4itOCWav2xGCA5961/1NO9iGc7ZaJoxSuZr7mCkXrpP5wkelVPh9O1WKt8n73EO6fJO59yic670jk8JK0ju8HRgNuOBo0TbxbvgEhHDH6YycjV82Jc6e+DDKyeJdtVb4XPwo5/P5QvL3LlUCEZEvfFaqpbyfNJ2nw/YKROu+h8VeegIdAqTB9qgZj5uLrgEPBa9LQwkX8fNUNbn4gD7pDyh9X63mk/+eVSWZiv6wP5HDH+c+PPVCcKDRE2SFNRDogGzY7wDHHfaLQa2SS5fzmY9yofzvWVQJJwo9srL8YahKxE9PNyeALNzQofZE8YZ5/rT3juhlsS8lwlS9Am5NAEmd4bAZ58ksNJ4KrJ990u+9YW281PbG0gVeiDey7aD8thbdTTa8KvYPhf6IMqhTm7rBxTovb5FyAVXMGWCBDnB/lsrb9k32nz7F36Tpj0oUQa/70mjG3dTHx5v1l/YliKVLBDES/MNLi0Wv98cMQ/93XMoO9stC+et9IXlYYNauLmEH7cXh9gbJmf1vERVrMtKvLv03Sc6Cu0/3yTz6CvXzfQnVbnO5T2n56nJ+FOFyIF/VkF6Ur6q4dYqukjclIOzTOTfwXSqUzyRGfU3KmasbdHdfzKR17JER3oBeKlTwb8Dmbyq5KPNFiBAhQoQIESJEiBAhQoTfClkHRH3BX0X1/usV4PPH3/THgv64SH/CNP35T4SsiKu3kbwiRP3wA6Hq6ky/RfEdoOwT9cMP/0nu3p57RBeK0p6oyKp+CbWAqD/vqYpi1Qk8+ET9ePVj4IB/PfeoLhC1PVFXLlV/iozqJApAyz9+dIm6+ksQq6Kg/gqgpD4k//FjiCjigJ+jaZ9jYKIKyX9iov6Fo7rvgN/5HwD8Brj6DETd+fnvJy9WRUy9xtXV1yRJf3eFq59+unLD+s9/iph6hSsPd8lC4Z+BtIps6jXuAqKSH8i9n4Cov1x9jvovx0gGRN2HiLr6eO5xXR6KhJ+vhxZ1dXX+PwFxebh1qXKJ+tfPLlFfzz2qS0Txao8P//XfP2OiopV+J5HbE5Us/IMUyN/33739dkh6RN1DWP8Utad+CTlfKSTJtMOpHyeI4KLohvU7bFEPZ/vbD98Him7t96kQ8RQhQoQIEf7g+B9pAdLfQBNLFwAAAABJRU5ErkJggg==</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxAQEBAQEBIQDxUQEA8QEA8PEBAPDw8QFREWFhUVFRUYHSggGBolGxUVITEhJSkrLi4uFx8zODMsNygtLisBCgoKDg0OFxAQGi0dHR0tLS0rLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIALcBEwMBEQACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAACAwAFAQQGBwj/xABHEAACAQIEAwUDBwcJCQAAAAABAgADEQQSITEFBkETIlFhcYGRsRQjMkJyodEHU2KSorLBFRYkJWNzdKPSQ1JUgpOzwvDx/8QAGgEBAQEBAQEBAAAAAAAAAAAAAAECAwQFBv/EAC8RAQADAAIBAwMCBQQDAQAAAAABAhEDEiEEMUETFFEiYSMyM5GhBRVCgVJx4ST/2gAMAwEAAhEDEQA/APMAJ9V5xgSsyICVBhZQYWAwCVBAQkiCyoILAMLKM5YGQIQQWAQWAQWBnLAzlgZyyIzlgQDw9kK6bld+0uHtant4m5JN/GfI/wBQ4oiYmvy9/pbzMTE/DoWx9H6JIsdL9Lz5/wBvbPZ6fqV/LT41hlyklsoAJGmpNpyiMlufMPNsUbudb66ek90ezzyrcVvNwzLVYTTICsgGNGcsmrgbQIRIJaFS8ysJvHsseTQhnOW8bSifefPGBCDVZpBhYBhZUkwLAPLKggsAgsoILCCCwCywMhYRkLAILAILAyFkBBYGcsCZIG7gcY1K4ABDb339hnDl4Y5PMunHyzQQxF2uSVHXwHjpMWpFazK1nZHzFx8NTFGkftNvpba/jPj1pM22z6U2jMhyhnZhq4lZYZmCLCDAASGFsIQBEolpFxCJkwMuokKZSS8xMt1huClOU2dcGon6F8oYEoNVlQxVgMAlQYEAwJUEFgGFgZCxqDCwCCwM5YTGQsAgkAssgILAILAyEgZyQMlQBmY5VG5tf3CcuXlikfu3Sk2lRY3iN9Bf0/GeO/J2eitMa+HqXOunjPPLtBdaqST0HQSKQ7wpQa+8kpDEiplHWNXEyiQxg2kUDwkl2lTGVEkrEG02tMNw2A8zjWthVn6B8swLKDVZUMVYBhZUMCwDCyggsAgsiDCxoIJGggkAgsaM5Y1MEFjQQWTQQWDBBIBhJNGQkCl5iqvdV1sq+zUkzxc/8z08X8qiE88u0Q2KSTnMtxAKyWiJWYaxEupiLTmZlYqMU5ns1gHERJgDKywIUMgwwk0xi0kysQbSS5mW4htdkZnW+rZUT9C+QaqygwsoYqwgwsaGBY0wQWNBBYBhYQYWDBhYBBYBBZNMZyxpggsGCCxqDCwYMLIDCQCyQKTmWqAAmhvuNLiefnn4d+KHPos8My9MQ2cO052dKtzEYPMmcbbEeE5d8nHSaq04ea7M9RJh5mbNRVKgtJCzDXZZuJZwl1molmYDkjU6hKyauMqhMzMtRUYp9JNaxdcN4UWF7Tz8nLkusVW6cENhpOP1Zb6qNVn6x8LDFWUwxVl0MVZNDAsAwsGDCxpgwsamCCwYMLGgwsmmCCRoMJGmCySaYzkl1JgQSNMGEjQxUjQYT2Rpij4rx00qmVVUgaE7kzhblnfDrHHGeXPYjF9qxZiST1Nv4Tz3mZnZd65DCsLTjMOkSOkZzs3VtUuKZQV3BPunOeLfLfeGv8oBMk0mCLRJrMLaGYyXQlrHylRhrbCPJ4LNOXTEXDneTsvUh11moliYbeHo30nO0usRCywHCGbvWO85W5PhYh1WFRaSS8Xp5v5lm/JFYKbGG+0932lXm+5lySifXeAxVgNVZdDAsaGKsaDVZAarAMLBgwsaYMLBgwsGDCyGDCQYMLBggkGCCQYYtOVMGKcLjjOPcXzNYE924ItYTlazcVUmLxfaEGwFgBpOMy2BGmJahtUO8bTjacdaxp+IIQFbi/W2tpzr5nXSciGhrNzLmbQW5AmLS6Vrq5p4M2Atv1M8k3eqK+CMdhmBsBoOo6zVLwzarWpplN2mpnUiMb7U1IBG3snHZdMNrKuQAbzMTOritXCMxNhOvZjqKmjKw9Y9zMdjwyuezXNax+6Z44/UW9hVp9WlYiHzrzskWm8Yc6qz1a5mqsuhirGhqrAMLGmGBZNMGFjTDFWNMGFjVwarC4MJGphgSNMGqyBgSAapBgxTjTGSVW2YgX2v1mbcla+7VaTb2UfE+ZKQWrTpE5wCFfTKdbEjz8Jz+rM+zX04cHiqhZiTqSdT4mZmQtROcyuCAjQzORJjQM5knA1Ks5zDpErXhqqDmOttbTzcsz7PVxxHuu/laEqT9HTSeTpLvsNvFGm1MlbG2mm/lMRsT5WXO1qJfYT0xOOcwZhcG1xe9pm14WKrdeFue8R3QptOXZvC0FrhbC+8i4rcWhv6zrSWJhY4Ss5C32UACbraIsxas4t7XAM+pS21fOvXJDlmuydXOIs9LlhqrBhqrKYaqyLhgWUwarIYYqy6o1WNDFWTTDAkaYYqQYMLIYYEgwxUgwxUl0w5KR8JjvXc1rpObjX4jgRUQ6lSuoIAOk4c/HNp7R8O3DfI6vLcXTs5A6ExHs52jy1SkkymGpSnOZdIqFadzaXthFdls1MEwW5905fV2cdZ4ZiNapSb7OfU2nTmJlutXScFwaMjF+vdtY39bzzXny9VI8NyvgqaqMpzBRtf2zm20OH1WL5dwdx0El4jCqxq0wpFgJzbmG3gaAdvCwuBbeMRZliqOBpM4qtooq3uLlvujFV2MpAuNPdN1Zlc4XDAJYjz9J6KcE28uduSI8SYVtPfSMh4b5M+CyJplzqCerXHDVEauHKJNMNUQuDVY0wxVjTDFWTVwxVjTDFSNMMCxpg1SNXDVSTTDRTjTAVayIVV2Cl82UHTNYXNo1MaNTmPDIASWsQTfLsb7fH3TEcm/Dc0z5UDc1Fq6vm7JFOXcm636jrOU0ndj3dI5I9p9mxxznCkwy4YliRZnIdLfZBnRy7OMq1rm8MzIUeYtC1k7tbDScsddMw1fKb5cx8LTneN8OnHbPPu26TsbGp11CnSwnLr+HaLT8pjcOBZl2bbrLWZ9pS9Y94KoqLec1MpWFxwbMWAF7X9k4XdqwsONEBQul9zbpMROy3MKOlxTsyMoG/eJ1J9PCb+nrn9SIlbYLi1JmsdCxG+vrMTxzDcXrK74fSJbukEAbjUCWsTJbw3MUVPduNN7eMt6+Csq9KAzgk6f+6TnWmzjW43fkyZs1heeuvBEeXG3JIis9NYyPDzWnZKZZpjCiIHOIJ6NccOQRq4cqxq4cok0wxRGrhiiNMMAk1cMVY0wxVk0w1UjVw1UjTDUSTTFBzbxjsaWWjVRamYBgrg1VG47vn4ny8ZNSciHB4zHVaz9pUcs3j4enhNa5eSs7Hck+smtRslV1N7SazMeSg1pNE7SOwJakmrBqG5AHWYmW48tysuRVA3tc/wmI8u0+ILWoTEpEzJhfpeZxuJbGDAZwt7XM538RrrTJtjq+D08h8LneeWba9UVxjiyJUuNV/SGxkickzXG4+lkaw9k9VJ2Hk5a5PghVYW0Os1sMRWzreWGr00YqPpaa9BbecLXyfD00pOeV/RPaabX39Z1rloxJ8S3zRvYDpN9IYmwXpzXVNL20mo8MTGsMJ1c5gsxrOOcQTrrnhyiNXDlEmrhqiTVw1VjsuGqsavUxVk0w1VjTDFWNXDlWTTBM6rbMyrc2GYgXNr2F5NMchzjzAyslPDVSBlu70yCrG4ICuPDrb08ZqHO8/EOJxFdnYsxJLEkk7knrLMuIVaSJUYqW8pcg0tnkmUYJmZlTMJhHqnKis5sTlUXNhuZztbHSlO3s6bC8MwtOmFrqC2jNqVdbja46jwnCb2n2e2OGkR+pr4UYYMQidTZnY7TVotmyzSKbkNLFgZjpYX0F72E1X2YvmpQoX16ePhJa2FKb5ahuSbTew5ZMy2sJTysGYGwN/CcrzsY78dOs7Lf/lqodBawPXWcvpQ7fWlt4PiZqEIb67npOd6dfLtS/acMpYdKrENYZAba2uRHmI8GRpONwvZhGNyWa6kaBV8L+MsTqTGeXQYvChaaVAwW47vibjoRM2pmS1Fomcb/BAzAZgPIg3vO/C5ci3NO09GPN20h9pGsJKaSkhK6TcSxMeQZY1Mc0gm9c8PQSauHKI1cOUSasQaojVw1Fk1cMVY1cNVZdMOVZNMNVZNMeac7Y4VcUwWp2ioMgUCy02XRxrucwOvpN1ebknz4c6WMTZzwdKkWOug6n8BOdrxDrTjmyVAATlufMix903WfGsWjJyDMLga1cXpU3qAXuUFwLWvc9NxOduWI9268NreYhsjhDlMw1J2GZBY366zl9eNx6PtJ678sVOD1kALqQpNs4DFb+tvjEc0T7M/bWrPlbUsE2ERatjd9m2OU9PbMxf6k47/AE44Y1oY/HtVtmAFr2sLbzvx0ivs8/Jyzf3ad50lygDNIzJ+FxJS/UHQg6ic71124rzVf8vU1L52Xu2NyRcaDaebk/D28We5HFXUs2QjLfTyHlLWMZ5J/CqRSTYTczkOVazM46zg/AzlLjwvczxcnJNv+n0KUrT/ALV9Z6VOo2duv1TqbzpTZiMYvNaz5VGJxL1G7pdlH0b3sB6dJ6IiIjy8lpta36fZ1PD8NU7MGqO4EOS+4N+s89p+XrrDouXcSHRly5Shy+RE9XFaMeXmrOrRlM6axGFCjJCzZhlmmSWWAoiNXHNIJdYw5I1cPURq4csauGqJNXDVEauGqI06mqI0w5RJpin5s422Doo9NVZ3qBFz3KgAEsSAQTsB7Zqvly5LTWPDzXDYLEYp3NNaldvpOQbsbncky2vEeHCvHa3mHYcC5HLLmxK9lci1PNmYAb3INtfWcJ7T8vXSlIj2dKeUMAct6P0eoeoub7QUgGXrEQT77it4Ly5hKuKxdVkR1o1vk9OhlIpoVRbk3+kdfMbnrNfGOcREzM/LtUAAsAAPACw90a0X8gom96dM5jc90amZ6V/DXe0fJ1bDUmpNTdVNPLqtrCw10tLMV658Mxa278vMOY+MYcOUpI7pYgrVJygX7uX62wnOnDE+YnHXk55r4tGuXqVwdlA9J6Yrny8c3ifgkG8sswwVk1OpmFAzC+19R4zF58eHXjjz5XuJxI7MIoFMDXKDf23M88R58vbaY65CrJm3Ff8AKnCWxD6WFt/HWceTz+mHo4srHaXonyDs6DKoBspsGIGY779NZJ48rMH1O14l5LxGm1SszPZSza2GgE1xzEV8M8nHNrbK7wPY0aRLDNYDK+xJ0uGvtOUzNpeitYrH7N7hePq4oBEpNYD6Ruct/Ezc1+GIt47ezsOH4MUkAsL9Z3pXrDzclu0ntOmsFNGmFPGrhDxq4VJq45lI1nD0jWupyxq9TkjTDVjVw1Y1caHMXEmwuGesgVipQWe+U3YA7EeMseXPlt0rsLhDMzLphqmTTHIcw8MPEcaKKVUpjDUu/wDXcZ7HRdPFRqZqLzDhakXt7+zquC8Ho4RClEEBrFszFizAWuSf/kx2+XSKxEZCyEaYMS9kxScrH53iP+PqH/KpzUy5Ujzb/wBuhUzOumGrGpjjufOanwrLQomzOmZ2H0luSAAem01FZsk2innHmmIxRqMWYlixuSdSTO0Rjz2v2nSc01jGmUgLgnbr6TlbXWkRuy3vlNJAQEz5h42Kzj0tPvOPXPLx1jIjdbFHDJ9NRnAXvA92xI6emkzsx4letfeGo7naaYbPD8KarZfH7h1M58l+sa7cPH2ny9Q5R4EMKpa+Y1Auvl4DynPjvM22TlyP0wPmriCU0KVfovYCxOYt526Ry2mZ6wvBWIjs81xOP+f+atUGayrbTU+frvNVp+ny1fk/V+nytMThTWFHDBBSZ6t3Yd7LfceZGs50n9TfJWZrjveD4D5PRSlcOUFi9subXQkelp6KxjyWnWy01qYW0aYU5jsuFOZOy4Q5js1hRMdl6uaSTsYekauHJHZep6GOy4YpjsYYsdjFFz2f6DU+1S/fE1SfLz+pj+G6SmdB6CZmXeI8Gq0nYxzPAz/W/EP7ul+6k1af0w81P61nYK0569GGq0amGBo7Jih5Vb57if8Ajm/7azpafEOHHHm3/t0gmOzrjn+bea6eCTKhWpWa4CXv2fd0ZwOm2ml5ulZs53tFY8vKcVxCriXL1GLta5ZjsB8B5TvkUjw49p5JLqvSyLlLZ7964GW3lFIts77JeePrHX3a2adXE0UHsGytZtjbQzn9Su+7rHDfInPd0vAeTMTiUFYMgQnxLPobEWtvOFuaJ9nop6ea5NpXvOKYTDYWlhqT02qKxNQ09GI1IzW33PWYrG5LrNsid8OT5fwfyiuqX0szEeIUXt7ZOe/Smp6ane7ouWeBO+KJamwph2ZG1yd06Kb+6cLcnasRHu9XTpaZn/p6kmwuLabCbrbw8to8vPefK65i1S4J0WmG8rXOthoBOdJm95l6/wBNOPy5XlymHxCjbXQak36WnfmnKuHp8m2vVuFcNWitzdnfvMzam5Gw8JikZBy3m0/s3GM32c8LYydlwpjHZcKcydmsIcydlwhzHZrCrydlxzSNNadT0aOy4crSdlw5WjsYYrSd1wxWjsYoue2/oT/bpfvTrwztnl9ZH8N0VJ9B6D4TlNvL0xHg5Wk7L1c1wVv62x/93S/dSdrz/Dq8fHH8e7rlacOz1dTVaOydXmfO3MWNoY2rSp13RAKZRVCiwampOtr7kz18VazWJx83n5L1vMRLnMLzJjKTO1OvUU1Gz1DcHO9rXN+s6zWJcI5LR8u94hzbiMPwvC1GLVK2KWp88QqhAGOtlt3rEW9CT58IpE3mPiHr+rNaRM+Zl5tica1RmdyWZjcsxuSfWeqMiMh47Xm07LFVHVEc3C1M2U7Zspsfvk3ys7ERP5JznxMusn0a9t5mfLdbYtOEYhalVKb5yGIUZQCQSQoNiRfecOSsxH6Xs9PyxMzFvMR5eq844P5LwmsuGLUjTFJi1N2Vm+cQPdhqQQTOXD/NES16i0zEy8SNQnck+pJnsx4pmZ93c/kjTNj2zWITDVX1F/r01/8AKeX1MbV6PT2mLY9g7NNLKBY3HkZ4446vZ3t+WMRVyqzG5CqzEDcgC+nnOk+2Qx+7wPjfMBxNRnOexNwGtp7BtPVw8E0j93Ln9VF/aPC3/Jvi78QprlJulXXTu2Qm/wB1vbHNXK6xw8u2z8vXWqTy9nq6ltUjuRUpnk7tdSmeTs1FSneOzUVJepJ2WKkO8dmupReTsY5anUnXUiD0qSa1hy1ZnVw5asmnUxasadTBVk7L1UXPNT+hkeNSn/Gd/TTt3j9dGcX/AG6GhV7q/ZX4Tha3l66x4g5asz2Xq53g7/1pjj/Z0vgk9XJP8GrxcMf/AKLuqWrPL2e3qalWXsk1eU/lCq5sfV/RWiv+Wp/jPpen/pw+L6v+rLm52eZ23MVQNwXhp8Hdf1c4Pwnnp/Vs9PJ/Ro4meh5l5xmoPkXDV6ilimPtxTgfuzMe8t2/lqpJphIVu8FqBcTh2JsBXok+gqKTM29parOTD27nuqP5Oxl/zVvaWUD758/htvJD6PNH8OXgwn0Xzod3+SJ7Y5/0sLVUf9Skf4GeT1U5R7OCvl7Eong7vVhdcd1r+Bv7pIv5THzQRoPSfaiXzZrkRrpvyb1QvEKV/rJWUevZk/wM4+p/py6em/qw9davPldn1ehbYiOy9CnxEvZroS+Ijs1FCWryd16lPXk7r1JavJ2XqX28djq5KnXntxxiT0ryTDRpxQUFibAC5PgJnrMzkNTMVjZDT4vRP+1p+1gPjLPDf8Oceo4p/wCUCbjeHXeqnsOb4SfR5PwT6nhj/lBj8dw6qWNVDpeysGY+wayRwckzmLPqeGI3tCk5l4zSr4fLTcMRVQ5bMDlytrqPhPT6fhtS+y8PrPUcfJx5Wd8rqnzLhVCqaouAoNlci9h1AtPPPpuSZmceqvrOGIiJlsPzJhVsTWU3Nu7dj93SZj03LPw1Pq+GP+Su4XjUGMxWILAU6lFaivr9BX7Mm2/0kM78vHaOKlfl5uDlpPNyX3xi0pc14M3+dAsbd5XF/MabThPpuWPh6I9ZwT8sLzngr2zsNbZuze3r4zX2nKx99w7jz7j2NFfE1qo1Ducp8UGi/cBPpcdetIh8fmv35LW/MtCbc1piuKZ8Hh8N+Zq4hv8AlcIV+/tJiK5abfl0m+0iv41VzbmOpVZgoJuEXKo8FzFre9ifbACBmFSB6rznxYVOEI//ABIwwt+lpUYfsGfM4K5zzH419P1FongifzjywT6T50Or/J7ieyx+HN7BmNM+edSo/aK+6eP1X8kvpenrsPofhOEVxrPF6Xiry2yZxnnvNfZU84EUMPiHX6lGqR9rIbffaYvSK80Vid8unDPeHzViVsZ9mns8nPERbw2uXcX2OLw9TYLVUMfBW7rfcTM81e3HaP2cuK3XkrP7vYXqmfA7P0fSCHrGOy9SzVMur1LarGnUlqpjTqW1UywYU1UzS4X2pg6uHXiSj63j0M+x9KXxo9VT5k3+VUH1j06H8Jn6NmvvOOPkOI4qjU2UHVlItlO5FpqvDMWiWOT1dLccxE+ZUd56nzGIEkVIEgSBv4bHBUdTc5sO1IbWVjVz+7f3znauzE/iXXj5IrFo/MZ/loTo5JAxCJAyIGIElEkGYVIFlieLvUwtDCkWWg1RgbklixuNOlrt75zjjiLzf8uk8szStPwr1m2YWHD8RkYMDYqQQR0INwZw5K9n0fTckV93rWE5/rBC3YMABctlq5VFr6nLt5z4/wBveJyJfS+jwWjzZRc187VMRQalZQKhW7DNewYN19BO3B6ee+2+Dkpx8Ne1ZecV2uZ9asPic1tkgzbzOoHPGJsBlomwAuVe5sNz3p4Z9BxzO+X0Y/1K8REZBZ51xPhR/Uf/AFS/YcX7pP8AqXL+39v/AKA844r+y/Ub/VL9hxfun+5cv7f2LbmzFHrTHon4mWPRcRP+pc37f2I/nJi/zn7CfhN/acX4Y/3Dn/P+ICeYsVa3ae3Il/hL9rxfhPv+fP5v8QH+cGK/OfsU/wAI+14vwff+o/8AL/EJ/L+J/wB8fqJ+Efa8X4P9w9R/5f4hWT0vGkIl5BiUZgSRUgSBIEhEhUgYhEgZEDECSiSDMKkCQJANXImcbreYOTFuAVDMAdwGIB9RMzSHWOefyBqxPUyxWEtzWn5KLTWOM21iVEgSBIEgSBIEgSBJRiESQSUSBmRUgSBIEMCQJAxCJAyIGIElEkGYVIEgSBIDaVVRuit6lx8CJmYn8t1vWPeu/wB2KlQHZFX0Ln4mWIn8pa0T7Rn9y5WEEKkCQJAkCQJAkCQJKMQiSCSiQMyKkCQJAhgSBIGIRIGRAxAkokgzCpAkCQJAxCJAzAghUgSBIEgSBIEgSB//2Q==</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIREhUSEhIVFhUXFRcYGBgVFRUYGhgXGBgXFxcWFxcYHSggGB8lHRcXITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGy0lICUtLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4QMBEQACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAAABAIDBQEGB//EAEcQAAEDAgMEBwUFBQUIAwEAAAECAxEABBIhMQVBUWETIjJxgZGhBhRSscEzQmLR8BUjcpLhFiQ0gsJDU1SistLT8TVzowf/xAAbAQADAQEBAQEAAAAAAAAAAAAAAQIDBAUGB//EADcRAAICAQQAAwUHBAIBBQAAAAABAhEDBBIhMRNBUQUiMmFxFIGRobHR8CNSweEzQqIGFTRikv/aAAwDAQACEQMRAD8A8XX1hgFABQAUAFAHKLAKACgAoAKACaACgAmgAoAKACgAmgAmgAoAJoAKACaACgDtABQAUAFABQAUAFABQAUAFABQB6HY20n0WV2EPOpCPd8AS4sBOJ44sIB6s741rlyY4vNC0ub/AEGnwaVzbDpnl9K3P7LP7v8AeY//AI4D4MPPtaeVYRl/TSp/H35fEV5mf7VvOYWU+8S37va/ucbnVPu7ZxFBGAZ5yCTnW2mStuubfP3ks5td9xNjagXGFHQLxM43Bj/vL/WwAYCMhqZ6tGJJ5p8c339yG+jcS1F5s5IH+HfRaKMRKm0srnxW49/KeFc+7+nk+av83/ofmjJ99ebatCbpTrq3SpL6FvH9wShtTZccCVmXG1EojKAfvVttjKU6jSS6479a+ghraa1vjaSXHwMN42lJeU4UpSHLqEJwpUQOAAiphUHjaX/Xy+iDuyq82qLW5bSqFt9FYqUU5z0dsAlaAoDMY8QkDsjTOiGLxMba4dy/Ng3TMn2hU9+6DrnTphSmrglSlOtqIyUpRkYSCMBzSVKGkVvg28tKvVej/wB/mJmjtRRRZ24bKkuW3RqxJJSR76hb0hQ4dGgcsXOssXvZZXypX/48DfRr290p28Lbzi1tnZ7QIUtRA6Zi3bWsAnI/vCSd9YOKjhuK53fo2PzKPZ60Aas2nEdY36HVg55lFy2lJ4j+7BUfiqs07lOS/tr81+4JdCGytsKNu3c3K1ulu8AxKONaUuW7mIoKvhUErCdJQNK1yYvfcIcXH9GhJjdiq4Diwt8KIsbgs3eNyVoUpBCi7JUMJChB6yCVA7qiezaml/2Vx9OH5fP8wIuuJft7hJfbUtNvbJdfUXMKli6UodbAVqhBQnFhzjhnTpwnF06t0uPT6h2MkKQ2sN3CW1DZ1kA6lbqU/b5wpKccEZdka7qi05K1fvS4+5DI7Ifc6KzWbmEJXeOvIKnVG4bbWlbsICSl0lIVkog9bvp5FHdNbf7UuuG1x9ARkbQeWLC1CH8CC2/LIW4Cubt4ThAwKAHE7q1xpeLK1b45+4T6PO12EhQAUAFABQAUAFABQAUAFABQA3bX2Bl9rDPTdFnPZ6NePSM50rOULnGXpf5gNubal1bmDtWpt4xaTbC3xzHLFHhO+s1gqCjfnf52Oyvat+08Eno1pcS202T0iSghptLchGAEEhIPaqseOUG+eLb/ABBss/abKkW6XGVlTAwyHUhK09Mt0gpLZOYWU9rnU+FJOVPv9qCxu19q3A50juN2Lpu4QFOKhBSXcSEyDAUHAOAwDKplpVtqPHFfUe4ymL7Cyy0UyWXStKpjqqDeJuI+JsKnma2eO5OXqqFZfd7Xxi6GCPeH0vdrsQp1WHTP7XXLSpjipx5+FV+gWC9ry+090aT0bbKChWYUG2ktGcssQSTynlSWGoOF9tv8XYWVbSvULaQyyhaEIU4odIsOKKnAgHMJSAAG0wI4mqxwkpOUnbdfkDHdoe0a3veEqxdG6EBDZcJSz0akFBSDl2UFOQE4qiGnUdrXa8/Wwspf2ziU4oIjHat2/a0wJZTj0znotPxa5U1gpJX07/X9wscd9qll0vBsBXTsOgYsh0La0FGmisaiTuk1mtKtu2/Jr8XYbihvbLTQQhlg9GHS4tLzgXjlstYAQhOEBKlQYJkzuqnhlK3KXNVx9bCzv7bQhstNNKDfQvtjpHApWJ8t4lEhCRA6NMJA4mc6PAbe6T5tP8L/AHCzPtb7Ay+1hnpg2Jns9G4F6b5iK1lC5Rl6X+YrNFO3UFBbcaUUm2YYOBwJP7lfSBYJQoZnKI8ayeB3afNt/iqHZXb7cDarbA2cNu46YUoErQ6oYkEhIjqgpmPvaU5YN2633X5BZS9fNLt2mi25jaS4lCg4nDC3VujEkokxjjJQmKqOOUZuV91fHyoLM2thBQAUAFABQAUAFABQAUASQBnJjIxlMncNcu+om5KtqvnnmuPUaS8yNWIKVq6Ak0iSBITzVMDvgGpnLbG6b+S7HFW6IVYjtAHKALHmFIgLSUyAoSIkHQ91ZYs2PLfhyTp069V5FShKPxKjiFRMgGQRnORP3hB1HlVTi5VTrn+ISdeRGrEFAHUpJIAEkmABvJ0ApSkopt9IaTbpHXmlIUUqBCgYIOoqcWWGWCnB2n00EouLqXZCrETdbwkpMZcCCPAjI1EJqcVJefrwOSp0RqxBQAJSSQAJJyAG87hSlJRVvoEr4RJ1spJSoEEGCCIIPMVOPJHJFTg7T6aHKLi6fZGrESQRnIJyyziDIzOWeUiOdRJSbW11zz80NVzZGrEXWdot1WBABME5kDICTmaw1Opx6eG/J1aXV9/QvHjlke2JQDW5B2gAoAKALmnwlC04EqxRCiOsiDPVO6a58mBzyQmpNbb4XTv1NIzSi413+RTXQZhQBygC9d0stpaJ6iVFQEDU6561hHTY45nmS95pJ/RFvJJwUPJFNbkBQBLB1cUjWInPSZjhUb/f20+rvy+n1HXFkKsRNbilRKiqBAkkwBoBOg5VEMcIXtSV88eo3JvtgGlH7p8jVWTZIW6uHyo3ILR33ZXD1FLegs6LdYzAjmCPzpNxap9ApUDja1EqVJJzJJknmTNKChCKjGkkNyt2yBaV8J8jV2KyBFMZygDopN0rBF1yz0ThSFpUUkEKbVInIgpPL6Vz4Mq1OHc4tJ+Uu/vNJx8OdJ3XmitxwqJUokkmSSZJ7zW2PHHHFQgqS6SIlJydvsjViCgDlJMApgdoAKACgAoAKACgAoAuuHEEICUYSEwo4icSuMbq58OPLGU3OdpvhVVL0+Zc5RaSSr1+ZTXQQdSknQTQIZY2c4vQVEskY9mc80IdsZc2UUQVhWYkGIBGkg7xMjLhUxyqXQo5VLoEsJH3R8/nTtlWywCkI7QAopk8PvKO7MEkj5hX+WsHBl2QWwYMJ1BG74QPAzw41Lxy9AtEnbY5xpn8O8L+ppyxPyBSQFgzMb/w/h89PSm4O7FY5W5Jw0AQUwk/dFO2OypVkncSPWnuHuKF2ShpB9Ke4e4oWgjUEVVjLX3wpKAEJThTBKRmrPVXE1z4cDxznJzb3O6fS+SNZzUklVV+ZRXQZl9zdLcw4zOBAQnICEjQZa1hg02PBu2L4nb+pc8kp1flwU1uQcoA7QAUAFABQBJRECAQc5MzOZiBGWUDwqIqSbt8eXy/cbargjViLWrZSt0DnStCbHWbAawTGvAd/DxrmzavFh/5JJGmLBmzOscW/oiwQMgU+Ck+kGuaPtPSydbzsn7F18Y7pYnR6fZ+zn0JIKVNAgGVAhWnw676yy5YSlw7Pl82Oe6W5NGvsz2ULragrHhIJBySMWqcOIGJ0rny63Y7j2dmh07lNOV7T580tRJChEZHIiCMiCDvrT2drNTqJPfFbfX5n1ntn2dodJBeDNuT8rTVevRbXrnzYUAFABQAUAFABQAUAFAFRfTx47ju176jxEOmdDyZifQjjrllofKjxIhTOdOkjWRluJ1iN3MZc6PEiFMi5apPLu/KtFINzFXLVQ0z7vyq1IpSKKZRygCbrhUSpRkkySd5qYQjCKjFUkNtt2yNUIKACgCSCBMicjGcQdx591RNSdbXXPPHl6DTXmWM2ylchxNU2S2ONW6U7pPE1DdkN2MNNKUYSCTyFYZ9RiwR3ZZJL5l48M8rqCs1E7CWpI6RUAZhIxEnuG7yNfIa321oM+bbHG2+t3R9JoMeu0cd2OaXntfP8+49fsJlhllDtqy0jEn/ABFysKMxmUpSdJByxI00o8NQf7hl12bVv+rJy/8ArDr+fcx9Xtqw02Ap9LqxMltPaPIA4RuHa3V2afSZMyuHXqeVqv6U3GcdvyfZ5nbHt685IaHRj4lQVeA7I9a9XD7MhHmbs4pZm+jzzWzrh4lQbcWSZKiDmTqSo5etehuxwVKkYuV9mi17IXREqCED8ax/pmoeoh5CsmfZxpP2l6ynkIP+ofKjxm+osLD9mWCe1eqP8LZ+gNLfl/tDk57rsz/iHj/kP/jp7s3og5D3XZn/ABDw/wAh/wDHRuzeiDk6Nm7PV2bxY/ibP1SKN+Vf9Q5D+zzCvs75k8lQP9X0o8aS7iFldz7KvoTiCm1pkDqLzJJAAggZkkDxo+0w8+AszrnZFy327dwDiAFDzSSKtZYvofBkKYJEZ/e4fe1nOo8Nv8/zKs4u3JJPEboy7Wmf4vSk8TbsdnVMH5bhmAoKAMHl603jl/PqK0NVuSdoArdZSrUeO+mmNOhJ61I0zFUpFKRUFmCnKCQdBOUjXWM9KTgnLd/nj8C74ojViCgCTaCowBQKx1m1AzOZ9KhslyGakkKALra5U3mmJ4kTHcDlXHrNDi1a25br0XH4+Z06fVTwW4djC9sPR2z35f8AoV50f/TuhhJz2X6L+dnV/wC6Z5JRuvVhs/2YurjPBhTrLhwjPMkTn4gVzr2dvnvzOvkv0+R7k/8A1Fg0uBYdHDlL4n+vzNQbLsbf7a4Lih9xkZdxP9RXtw3KKjjjSPk8uWeWbnN232w/tE01/hrRtP4l9ZX5/wDNVeDKXxSM6E7r2lunNXikcEAJ9Rn61awwXkFGesOOZqxK5qJPqa0SS6C0cFsZjIHgSJ8qNy6CyXu3FSfOlvQWSNpGqgP1nRuQtxw2o+NO710o3oLBVpH3k+Jijcgsh7ucoKTOkEZ91G9eo7BKFoMpxJPFM/MU3TC0PW3tBdN6PKPJcL/6pNQ8MH5BSH/7TpcyubZpz8QGFQ7iZ9CKz8Br4WFB7ps9/wCzdWwr4Xc0+ZP+qjdlj2rDkWvvZm4bGIJDiPibOLLu18pq454vjoLMYitRljTClAlIkJEk7hGevHlSckuGK10V0xhQBQ9bBXI8apMaYi60U61Sdlp2V0xmuhASIArOzKyVIAoAKANyx9mnFJ6R9QYb4r18EnTxjuNYyzJOo8sVjH7VtLbK2Z6RY/2rvHika+WHxqfDnP43XyAyr/az9wYW4oj4Rkn+Ua+Naxxxj0g6KG7NR1yqrFuGEWiRrJpWLcXJQBoAKQiVAha5ZKiI/DnluWhW/kk1nOLb/nqUnwLe6LgjnOqY+yKPU/0rNY5VRW5Ek2qgrFEgKUQJH3nAs6900LG0G5A3aK6qSIAAkgg/cKTh5HeD4ULG+A3I6i2UFA5kT+HIS7x3dcc6Fjaf8+Ybk0ds7dSCJnSCerrhbGf8pGXCqhBqVv8AnQm00PVsQcUkHUTQMpXaJPLup2PcxdyyI0M+lOx7idjevsKhpS0knsjME/w6HyqZRjJcj4Z6guC4R/emGy5uUglKv80Z+Ex3Vy04v3HweZqfaUMfu4+X+SOvbOUtlYaTKQkgBMDcRkKFNKSs5dFHPl1CzT6V8v8Awjxa0kEgggjUEQQeBB0rtuz3jlABQBFSQcjQBT7mjnVbmPcxipEFAGjsjYrtyeqIQNVqySOPeeQ8YrOeWMBWah2ha2eVukPO73V9kH8MfTzNZ7J5Pi4XoBiXl27cKxOKKzu4DuGgraMYwXAdEmrL4j4D86dkuQ0hIGgipJslQAUAFABQAUAFABQAUAFABQAUAFABQBJLSiCoJUQOA38Bz08659TmeLG5RVv0N9NijlzRxyltvzNj2b2YXkOOoUk4DgME4cRgqwriFCMsuIrgj7UhkStV6mntf2RmxReKL7qr4dX5+n0Edo3CwShAwKBg4hnv3btefhXo40prdfB4+D2djw/Hy/n1+BiIedaXjClJX8QOZ7zv7jW+2LVHo3Zto2yxdAIvEYVaB5sQR/EP/Y5CsfDlDmD+4BHa2wHGR0iSHGjmHEZiPxAad+nOrhlUuHwwsya1GFABQACgD0VnsRthAfvThH3Wh2l943d3mRpXPLK5PbD8RX6GZ7Q7edfCUIHRtBUdGjLqgHWNTwGkxUvHsp+fmVFIzGLdZUCrEBJO/slTcacirI86HOQ7RfblwACFZBuctycRUo9+U1O6X6EtIvZWsJ605FGZ3gmT84PdVRk65E0r4Kitz8UYxnmIEonMZgEE+RrPdKh0jSFdVmR0CmA/bbFfc0bIHFXV+edZvLFeYxr9hpR9rcNp5DM+pHyqPFb+FAHRWKdXHV9wgeoHzovK/JAHvdkNLdZ/iUf+6jbkfmAftO23Wg8Vf0p+HP8AuAP2nbf8In+b+lHhz/uAPfLM626x/Cs/9wpbcnqAYLFX3nW+8SPkaP6q9GAfsZpf2VygncFdU/OfSjxZL4ogUXOwbhH3MQ4oOL019KpZoMCFpZCMTk66HqjLeon5cqUp80jj1GfJF7MUbk/wRN6+RkkAqTkFR1QUhQJSkc45d1Lw20LS6aePJ4uSVy6Pa2F+0ttPQpShoaISAMJ1MgaHOvnMmGWKW2R9H4ry+83bMj2wt2g0HFEBchKN2In7vPKTyiurQahwyKDfDM8mnlli3BW0r+48cROtfQHmCj1nvT5flVJlKRbsnbDtseqZT95tXZPHLceY9aieOM+yjUe2YzeJLlp1HBmtgwPFH6jurNTljdT69QPNuIKSUqBBBggiCDwIroTT6GcoA9QhprZyQpcOXREpTqlud5589TugZ1zXLK+OELswLm4cuFla1FSjvOgHAcByreMVFUg6GGrVI1AJ4kfKk+SWyzok/CPIUqQrDok/CPIUUgsOiT8I8hRSCxiz2ap0w23i4mBA7ychUycY9hyaf7Gtmf8AEOJKvgbAJ8TH5VlvcvhQERtZDR/uzKW8okkmdM40nLXOhYb5kwsUf2g872nFHkMh5JyrVQjHpCspRaqO6O+qsW5EnbcISVKVASCTAJyAk1LmkrEpW6REhEkSo4dYAgafmBU+Kh8nZb0685DSMzh6ue/rp8+RpeKgpgC2YHWEzEjWASd2URvp+KugqRzqZZqzJAMDcQknukgUvFQckm7bEkKByIkSIyOm+rjO1YnKnRxVqrhNVaHuRJi7da7K1p5SY8jlScYvtDs0U+0BWAl9tDo7oI5jd5RWXg1zF0MkLG2e+xcLavgc07gf6mjfOPxKwKA3cWasWGBod6Fd8f0NTkhi1Eaf+yoTcHaMvaLzlw6HHVyE9hAEJT659+vyrkxezFDLvbtLpHsS9rRjpfAxQpy4lK7v6BXqHiARSUk+htNdlTzIVrrxqkwToTGNpQUklKgZCh+vSm0mqZadnoW32toAIdhu5AhK9EuciOPLy3iudqWLlcoOhT+yF38Cf501X2mAWjISlTiiokkkypRzMn5mtuEgbofbbCRAqSG7J0CCgCbDKlqCUJKidwpNpcsDZGzmbcYrlWJeoaR/qP8A68ax3yn8H4jF7zbjixgRDSNAlGWXMj6RVRxJcvlgIt2yjy760slyQyi1SNc6myHJlwEaUhHaAIPN4klPEEedKStUNOnYqiww5hQMg9pIOoSDv3xmOdQsdFbwTYR94HLQpkZhAIMnMQiOOetLw/mG/wCR39npgA5mSSSkEqlKk58e1NPw0LezidngRmMlFQ6uclaVZmfwx3Gl4Y94xas4EJRlkIyEek1cVSomTt2W1QjhFAFS7ZJ3R3U7GpMWctVDTP8AXCqspSGbHbDrXVnEnQoXmI4DePlyqJYoyKHRa29zm1LS5AKD2Sdcju03eVcmbUSwyWPtvr6er+SNsePcnJ9L+UZztkponpUxGg+I7o5Vlm1e/ItNhfvPmT/tXr9X5I1x4koPNPryXq/29RRUnM769CG2PuR8jnlb95+ZytCCK0giDQBn3DBTmNOPCquzROxn9t3P+/c/nNT4cPQdF6EgCBQZEqACgDQ2ZspT0qJwNjtLOmWscaznkUePMZp214kHorVMJkY3IlShOZG/ie4GIrmzPbHdP7jXDj3yoesfZpKitLhKgSSlYPWHfx3d+fj58/aUlUo+XaO96JRTT+5mbd7EUwVAicOHrRkQrQjhnlXo4tVDKk15nl5McotpmhZ7FU8yFJ7YUrI7xp8x6mufJq/DzU/hpGscKnipfF/gqe2A8lCnCmAkTG/dOXLPyrWOsxykorzMpaeai5My66zEKAJJQToCfCgRMWy+HypWFokLRXLzosW5B7orl50WG5ETbL4eoosdogpsjUHyphZGgYUAFABQBz3YLy9eFcWv18NFi3y78l5t+h1aTTT1GTbHrzfoiJtMRAGTad/Hie88eFeJl1s9Di35Pe1GXpei8l9F+bPUx4Y6me2PGKHn6+r+8ZY2kFhxLiApr4lTiB0BnUn151rixPQY4wT3Z8jt/Xzb+UTPI1qZuXWOH8/FlG1NlkDpWldI0RqPugbiPr517mlSxx2S7836v1POyT3ysyq6zMKAOETrQBT7ongfM07HbL6QgoA1tnbMSE9PcHC3uG9fADl8+7OsZ5He2PYyraG0V3BCEjCgEBCBkOAnn6ChRjjTkwSt0h7Y1i4yrpSDAkKHLf35ZjurztVq8GVeFfL6OzTwyY5eJXC7PWsKggz5cNDXzUsu2W1ntz96Jn3vtCkEpSnpBoQTCTy0M16ej9maiVTlLb6ep5Oo1mKNxirK1+0AQhAaHWAIzmADnG4qzmuvS6DL7yzPi+Pmcmpzwcoyxccck7n2jccQEoREgYirSd8cq6MegjGVyZjl1Epx2mOizG8+VehZzbi9DKRoBSsVi95OJvtETBCcQyKkiZTw57sXCs59oqHmZ7aHcIH7zNsJmV4sSkoBOZgQVKM7inWo94v3ST3SFJVDgJTMAryX0RIEDTr+ExT5/n0Dj+fUm2hanIBWAMZKj0gBhbZAjSYxCOyRmNSKXLY+Ehcl7Cqcc9C5EdJ2uhYwxG/Fj8cW+j3v59we7/PvHrDFjUFYuzlOOPtHJiciIw56kRVQu+SJ1XA6tsHUCtTOyhdmNxj1p2UpC7jCk7vEU7KTRG3ZUtQQkSpRgCs82WOKDnLyNMcHOSihi7QWpbIhQ7VfMez9Pn1+rer1KpRdQj5X/r9T2dVlx6XAsGF8y5ky27LasKWcUYRixcd9RmxQ0OWWv1XM+oq7t/L5FY5y1MFpcPEfN/L9zNvm5ASnIA6cTxr1PY+myc6vUf8AJP8A8Y+SRy67UQTWDF8MfzfqL7P2g5bqlOn3knQ/1517k4KZwWPXez0PIL1tu7bW9P8ACPp5cKzjNxe2f4jMWtxBQAUAFAGvsywQlHvD/wBmOynes7suHz7tcZzbe2IxTaF+u4XJ7kpGiRy/OrhBQQmbHsls9CnhjIkAmDv4geE1ya7I44nS7LwVKfJ7hVsmI3T4gnd9O818u9Kmmj1vtNNMx9v2Tqh+7KQmOsJwlRHpoOO6u/2fiwxnvyK5eRyavPLZti+DybbZVoK+js8ux1q1A1zNTZDkMUhBQAUAFABQAUAFABQAUAFABQAUAVLYEyOqoaEcaUoqa2yVoqM5RdoSuG1Akqkzv1nxpwjGMdsVSLc3J2xg3DYZSlKSHJOJU5EboHlXj6j2T9p1azZuVHr9q+p6OLXeDgePH2+/3Eq9s84qeZCu/jTTGnQtbXC2FhSTCh5EcDxFOUVJUzRM1L21RcIL7AhQ+0b3z8Q4/XvmsoycHtkMw63EFAGnsbZ6Vy67k0jM/iPwj9ct9ZZJ17q7GU7Uv1PrmISMkJG4fnVQgoIVk7dnCOf6yobM27GGXShQUkwQZHhUSipJpiTo173bqjkgkSMyfOADz31yY9HFfET7zvcxcPvOj944rCe4T5Ct44scHaQNlqUgZAVZB2gAoAKAJttKVoCf1xpOSXY1FvoYRs9W8getZvKvItYn5kvdWxq55RS3y9B7Irth0bPxH1+gouYVjDAz8R9fyouYVAPdmzo55kU98l2g2RfTOK2edxB9KPFXmLwn5C7jCk6g/rnVqSZDi0V1QgoAKAOETQAncWsZp8qpMpMVplhQBW80FD5GmmNOhazulsOBSdRqNxHA8qcoqSpmiY/te0StIuWewrtp+BW/LhPz4Gs8cmnskMx62Eau271JhlrJpvL+JQ1PPf6mscUH8T7Y2UWjMZnX5Vo2ZyYxUkhQA1a205q8B+dJslsdqSAoAKALmLZS9NOJ/WdRKaRUYNjGFpvXrH9eFRc5F1GJBy/UdIAqljXmJ5H5FHWXxPrVUkZuXqTTaK5Dxo3Im0S9yVxHrRuDcHuR4j1o3BuIqtFcj4/nRuQbkQwqTxHd+Yp8MpP0LWr5Y1z7/wA6h40+jRZGW4mnNeqf14VNSiO4SKX7RSc9RxH1q4zTJlBoVKxxHnVWRQhfq6wIk9iMMnRwFzTISiRnrpWc+zSHQmUKgBJUCSDIxDCkpXiAnQBwiE8huqPoafULlCoCgCFlL2QkjEVpKcxkMpgncKtSaSv5gqt/cZ6kqjUwAgQZVJCwlRgGSMKAf8xNFPz+RfHkM2CSCud5y1iMbnE6xHhhrTHdsifSL7lnEOY/UVqmSnQbH2h0KyFCW1ZLTy0mOX50skNy47NTb/Y9n/vP/wBKw8TIHB5u0akydB866myJMfqCAoAZtGJ6x03c6TZMmPAVBA0rZykmXVhAH3UwVHvOie7M91cT1bm9uJWzo+yyXvZHS/NnH7oqAQkYU7gN/M8TWuLBte+btiyZbWyKpFjdslAxOeA/WtaOblxElQUeZCt/tZIISVBM6JHaPgM49KxzZsOnjuyyo6MGl1GqtYYt1/Oyu0WhxWELAOsGQSOIB1HdRg12DOrxSsnVaDUaZXkg0vXtGm3bJG6e+t7s4LZXfkhIhRT+8aGUaKcQkjMHcTUT4RUOXyZFrfuEIxLgkJI7PWJ93MdkZHpFZDzyyy3M22RJIunQhJU7BUltSckmcRQFkgAYokqgaSPAt+otsfJeoC7dMlK5CUpJzQQSVOpICgnrZhEKyyGYmRQpS8gcYrtfzg6q9dJWMXWCgAkKQD9s4kgSngkCaNzsNkaX88kPbIuCsKKlhRkaER2QZAAkTrnWmN2Z5FT4G3GEnUeVaWRYo7aEaZ/OqUitxWl4gYTJTlliUnQzkRmNKUoKRrGbiMG1bcEoAB4QB6bqzTceGW0pcoSU1BgpE91bKmZO0cwDgPIUUIMA4DyooLFbu1HaAHPL1qkVGQmAKos7QAneNfeHj+dUmXFilUUaraIAFZmTZKgC23axHlvpN0JszNp7dft3VMqZSSDKYxZt6jLPOMp3EHKvGza/LBtRSf7H02g9i6TUxjKeRxtU+uJHpvY3bLV0rChtaXQJJV1kpHEKG/hIBrjeuyZuHwvka672AvZ9Sck0+vX8B7a4HSYUHFAAyz62+vW0MNuO2j5vVz3ZKQJSlkSc1HQfr51u25ul0ZJKC57FFKUs55n5CtOIoybcnyeI2I8XXnHl5kx4AkmByAAFfA+2M8pzW71P1XT6eOn0ePHDz5Zo+0L2BCXEqhSVdUjUEgxHiBWfs7K45OGTHAs0J45K00ex2fcdK025EY0JVHAkAkV97jlugmflmoxeFllBeTaNS22epQBJgHziuXNrIwbiuWb4dFOaUnwhi72ekJJTMjnM1z4NZKU0pdM6M+ijGDcO0ZdepwzyuibLZUQkamoyTjCO5l44SyS2xHHdmkJmZVwA+VckNbGU6ql6nZPQyjC7t+ghXcjgZIqSUlK2yoHUpWpKvAg/KK49RHNdwfB26aWCqmufURb9obZsdGGbpQGhct31RnpiwzAGhz4515zzZYvmz3Iez4ZI9w//AEhpwsOJxFLjcgEEpUAZzj94EmeWtdOPW5F3z+Rx5PZqV7fyaZWNmqBBbcSTqAeor+VWtdUddjlxJUcktHki+C161UoQtBSob4y89DWkcsL912iJY5Ne8qYvZbKccVhjCBqo6D860yaiEI3ZnDBOcqKb51rGW2oIRAKtSpWpz04ZfnXm6DVZtVnnNP8AprhfN/sjv1ulhpsME178ufu/2L17J5Rn3TOEyND6cqpMtMoplHCJyoAW9yHE1W4e8aqRAKANNhrCI37++s5XXBnab5FLuyUtQVKcshlmBqc9+cV5i0uocf6klKX0pfJfQ7/tWKLqCaj9b+/6l9jZoZThQMIknLid5Naez9JPT4msjTbduuvoivaftGesyqbb4VKzXZQGk41do6CuqT3ukccVsVsU6ziuJPpWiqKMZS82aDLQSMql8mbZ4e52UbN9R/2Lp6h+FWZCFcNTB318d7c0MorfHo/SPY3tWGs06xS+OHl6r1RW/s5d24lhGSUwpxfwg5ADioiYFc3sXRSyycvI6tf7Tx6DA5S+KXEV/n6H0fZFilRCBklKQABwGQFfYZ8jxRSifm+GHj5HKf1f3npG2AIG4CK83Ym7Z6ydKkdLQpPGmxqTE7rZ6VZkZ8RVwy5MS4fBjkwY8rtrkS2c820VBeoMTBOWm7SuvLCeVKS6o48E8eFuMu77HztJn4v+VX5Vi9NN+R0/a8X936mZtR9tUYMzvMEfPWujTYpwbvo49VlxzS29mfXacRFaARB0NTKKapjjJxdo64VKXjK1zhw9qMpmcs5zrB6aB0rWZRe5tMaSkKKCfvIASoHjIHW/zSKxlok+mdWL2pKLW6N/IzkuX1vAQ+hwbukQE5cOplPhWb0E2u0zsXtDSzduDj9Hf6hdqu7ttaFBhJIyU2tSVAxkTibUFCeEd9ZZfZ8pLbOq+rN8Ot0sJKcdzryaX7iOwrFxhvo3CkkEmU4pJJJJVi1NelpMLw49nH3Hne1NXDVZ3khf3/L0NGuo84i4gKEGgDLWmDBqzQ5QMKACgBiybkzw+dJkyY/UkBQA1YsycR0T86zyS8kaY43yyu4dK1egFOMdqJnK3Y5bs4Rz30mzFuy2gQttGzS82ptcwYzESCCCCJ3gisc+KOWDhLpnTo9VPS5o5odojs2wQwFJRPWWVEmJJMcBuAAHdWel00NPj8OHRrr9fk1mRZMnpXHQ/bvKQZSc62yY4zVSOXHklB3EvvPabou0RPAIUVHONAeY14ivOzPDiXvM7FqpvyMe59vVgdVsaTKkq4AzAOmp10TO+q08cedXGylqZeZmXn/9BuM0gNjWeooEGTlBURMR411LQxfYnrGuhKx2/cuqIThUdTIgd5NdDjsRyqKmx1zb62iA82M9CgmD3TSi76CWKjSstrMu5JVB+FWR/I+FMzcGh6mQFAFtswVmB31jmzRxRtmuHDLLLajRRstMZk4uO7yrz3rp7uFwelHQQ28vkyLm3PZUCPD1r04ZFJXFnlyjKDpozUKLauY9a1aUkXGVcjF62CA4nQ6/r0qIOntZpNWtyE61MgoATvm/veB+lNMqLFKosKACgDTt0QkeZqGZt8llAjqRJgUmA7eKwJDY8f131lD3nuNZvatqDZlqpZkCTu+pp5cigrZlGEpvbE9XbWIRoM+J1NeJkyZMnb4PZxYcePpcid/s4k4k6ndp4zXRp9VsW2f4nNqdJvblD8DC2nZlxCmiSgmMxqIIP09a9FSU1aPKyY2ri+GUbMs/d2yFOFWZUVKyjIDechlRairbJhDaqM7aO2VKBDQIEHrSASMJIgagb+OmmIV4mq9oyn7uLr1OiMK7MpTagrNK5nevPtnf4nPiVndXmNNPmzQzNrP4EpnEJ06+/CgjLWMgr/KgV7nsTE5OUvoY5ZUjGSpSzAlSicgMyTX0dJLk5023we29ndmqZbOMALUZI1gDQE+fnXnZ8ilLjo9HBjcY89kdu7SZQkoXC1RkjWDuJP3fnTxYpydroWbLCKpnlGbo11SxnLHIeo2Lt5aQA4FKQcgozlyCt/dXn6mUsPvrlLtef1NlBT+R6xp0KAUkyDoa0x5Y5IqUHaMZRcXTPSbKYRgBAzIzO+eFebnblNqR6+mjGME4jxSKycUzoTZRcWyCMwD3/ThS96HMHQpRjPias8htFkSSncT4ia9vFJ7VZ4cqUml0V2DmqDof0f1yoyLzRrjf/VirreEkHdWidqyGqdEaYiLiJBFAIyiKs1CgCbCJUBzoYn0alQZhQA3s5uVYjoB+vrWeR8UaY1zZQ4orV3nL6VSVIiTt2bWz7jojIEiIiufNi8RDw5vDlZp/twfAfMVzfZJep1/bo+gHbg+A+Yo+yS9Q+3R9DKuXsaio5V1Ysaxw2nFmyvJNyPG7c2oXldGjsA7vvnj3cPOvA12seaWyHX6hGIm20ppSVrQYB9Yy7s8/CueOOeCSyTjwaJOPLLffEuKlxJVAhKU+s551r9qhlluyq/RIe9SdscbfTuYA78I+ldePXxj7sYUi1Jehlu7SDLuNLDSThIMakEjeAI04V7OCaz47t/eYuajK0kQufaZ5392y1C1ZAhWI94yAHedK1jgjHmTCWeUuIo8uo5mTOZzmZPGd/fXYmcbQxYW6nXEtp1Ud+7KSfAA0pyUY2xwi5SpHqdrOoSWrUT1QCYOkJhIPeJPlXjayWWGCeaFff6Ho3HdHGbGx7lKRA1PaGfmK872Vmxbdsfi81/k2z4t6PStggf0/i/L9RXrSps4oqUSyTz/l599TSKuRQ4ucp/UD8q1jBd0Zym3xZXVmZmOAoVluMj6Vp2jVPzGb9MhKxvEfr1rPHw2jXJylISrUyCgDOu0QrvzqkWuimmMZsE5k8B86TFIeqSAoAdT1WSd6j/T5A1i+Zmq4gV2KJM8Pr+jWkjCQ9UkBQAUAY/tLelCA2ntryy1j+unnUtXwzTHG+RXZ1ihASoiVjUydTqK+fni+z5bj9x1RilyaoDLiVAgQO1O7gZPdXoNPLjqa7NbjJHnbu6CZCI7wMvCs9N7O/wC2T8DmlLyRkPKUsxmokwBxJ3AV6sMWOC91JGfLOtbCfWqCgoG9SsgB3amr8WKH4UmXX10Q0tu0RDaEnpH9xgZhKvvKOkjju1pRXNz/AAHJ0qj+J5BJrrs5KPVWeyV2qW31H96VAJbOQIUCCCdZgzy51yZtRHbK+kuzojicKl5+g0WgVY1AFckyBx+m4V8dqtdkyOUU2ovy+h3Qxq7fZpbKR1p3AHXfOVV7KxSll3rpf5N5ukegs7wE4IE7tefPmPKvo45Ib9l8nFng630NlzkPWuhQ+Zy7iFWQFACl+jQ+H5fWqiXE7b9ZpSeGf1/Os5cTTN48waEq2MgoAUv05A+FNFRE6osesBke+pZEhmkSFADt/klCeXygfnWWPts1ycJIlYp6s8TVS7OeQxSJCgAoA8uXOlunFnMN5J9RPoo+NRLo6saov6WJ7vXdXPmwLIl8mXZRcXhKEogQk5/iA0B7pNdCjTsly4oHE27yNUsrHkfz+dTcov1K92S9DIZvWrZSlrSHCOyQqEg8cxM/oVo05dEJqPZj3+2Li+X0YWlCIJwlQQgAb1k9rUZZ91XGMYKzOUpTdDVxeIDSbYv9IAAkN2qICj+J1czJz6o1OlJd7q/EptVt/QQNiWllXZUggkJJIbVqE4t6hHmDwrTfZnso2rForAdcUpSzMFRJgSRlXzftTWT3Swx4j+pvjjfvMcNeBI64mtZdRvF3n8q+g0bWDSeI/r+w370qFWHilYXvBn86+fx6iUMyyt83f7nZLGpwcD1QNfexdq0fOtU6CmIKAKrpMpPnQuxrsp2YrrEcR8qWXo6MXYotMEjgYrRdGb7OUwKLwdQ+FNDj2Z9UaGhZdnxNSzN9l9IR1AkjvFJ9AuxvaZ6w7vqazxdGmXsutR1BTfZzvstoEFAEHl4UqVwBPkJpMa7PBbNvw24QswFDU7iNJ5ZmqcG48G+9RfJsMuodJCHEFWoGISRvioace0UmpdMzb+9bbJStUKGoznyFXGLfRMpJcMw73bafuJJ5qyHlr8qtY35kPIvIxx0lw4lAlS1GEgZZn0FN1FEq5M9Hsz2FdK/7wttKE5qCVysjhpCQeJrCWdeRvHC/Mburti3uUqt2kYUCDhgBRzkg8ROvKp5a5LdJ8Iv9o3rdLeFspK1ScKDiAKiCtalbzAwidxNEN1inVcCSdqpyS2hRMQBkB514WX2bNbsmWaS9SVk8kh5NeFLvg64DiXlFISdK1lqcksSxt8I6IRV2RFcUjqgemsFy2g8o8svpX3Ps+e/TQfyPA1UduaS+YxXac4UARcGR7jQNCNgeuPH5U8nwm+P4iN2Ourvpw+EU+yqqJK7jsnuoQLsy6s1NKz7A8fnUszfZdSETa7Q7x86T6Guy/aXb8B9ajF0Xl7GbfsjuofZzvssoEFAC+0PsnP4FfI0mVHs+YXtdGMMpP2d/xTXer/oVWmf/AI2Rg/5EN+3X2qP/AK/qaw03wm2o+I8qqtWZI1vZ/RfhXPlN8Q1cb/1wrE2F100SUmtUQzT2HovvFeJ7c6iPEaya+bZ2RGU6CpfR0xOisZHTA9Hsv7JPj8zX2nsn/wCJD+eZ4eu/55DdekcgUAcVpQCM+y7ae/6GnP4TeHxBe9tXf9BRD4Qn8RTVklb/AGT3GhAjMqzQ/9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxESEhUQExQWFhUWFSEaFhgWFxYYGBoVFxgaGBkZFhYeKCojGB8mGxcXIzEhJSorLi4uGh8zODMuNygtLisBCgoKDg0OGxAQGyslICY1LS0tLS0tMi8tLS0tLS0tLS0vLS03LS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAJ8BPgMBEQACEQEDEQH/xAAcAAEAAwADAQEAAAAAAAAAAAAAAwQFAQYHAgj/xABNEAACAQIDBAMMBQgIBQUAAAABAgADEQQSIQUTMVEGFEEHIjJSVGFxgZGj0dIjQpKToRUzNHJzgrGyFiRTYmN0tPBEs8HC4hdDg5TT/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAECAwQFBv/EADYRAAIBAgMFBgUFAAIDAQAAAAABAgMRBCExElFhkaEFExRBUrEycYHB8BUiQtHhkvEzQ7Ij/9oADAMBAAIRAxEAPwD3GAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAZPSjGVKNDPTNm3tNb2B0aqisLHmCR65DMMRNwhdb17mtJNzD2BtW+F3+IqKLVKgLtlUALVZVvwHAASDno1b09qb837l3Z22cPXJWjVRyBcgHW3O3LzyTSFaFT4XcydmdJaSq/WayK3WKqqDYHdpUKroOwAWufbIuYU8TFJ95Lzfuam0sR3tFkrpTD1UsbBxVVr/Rqb6FuxhykmtSWUWpJXa+vD6lCj0sw5xL4c1KYAChWzatUZmVk9IsvtgzWKpuo4XX+7i7i+kOEpOadSvTVhxBYd7+t4vrg0liKUXZyRW290ko4ZqKF0vUdQwLWy0mDfSei62gpXxMaTim1n7bzXwuJSogqU2DK2oYG4PoMG8ZKSutCWCwgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAdf6dIGwhU8DVpA2NtDWTtHCQzlxivTtxXuS/0Ww3+N/9jEfPJLeFhx/5P+zD2ZjBQ2dTORX/AKyyLvNUQtiHUVHJubLxvxkHNTmqdBZXztn89WWd9UO0cMr1aTsKVW+6RkspCkByXa9yLgacDBa8vERUmnk9Fb7s56H4jDqMWGZFbrVU1M5AumcgE3+rYEcrhvPCJwsqaU993f8ANxm4Yf1XCEC1M7TBpDh9CalQpYcrcPNaEY/+unbTby+V3Y3sPUVdpVgxALYemVBNs1nqA252JEeZ1JpYh33L3ZRqbTZ0xRU4ejTSo6Or02d3I0LMAy6vfQWJNxxkmcqjalbZSV1mrv3WpAzgYLZbsbKtWiWY8AN2wuT2C5AkLQo//FRe5r2O6qwIuNR5pJ6JzAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQCOtRVxldQwuDZgCLg3Bse0EA+qCGk8mfGMrsi5lptU11CFM1uffEA25Xv6YQZn0doYMruTkphr/RVU3Wa5Ja1NwM1ySSQCDeTZlbQts2y3FzC7OoU7bulTTLfLkRVtmtmtYaXsL87SBGnCOiR819kYZ7Z6FJrMWGamhszG7MLjiTqT2wQ6UHrFcizUw6NlDKpCkFbgGzDgRyI5wXcU9UZ+1K+DzKK5os6m6K4VnvzRNWv6BJtcrKMH8SR84dKNarveq6hdK1SkityygN9INL8VAkNEbEHLa2c99jQOEp5N1kXd2y5MoyZRwGXhbzQW2IuOzbLcc4bDpTUU6aKiDgqgKoubmwGg1JgmMVFWirEsEiAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAfFWoqgsxCqBckkAAcyTwgFJdtYc6rUDDmgZlPoZQQZNmRdHP5Xo+MfsP8IsLo+au1cOQQbsOW6qNf93LrFmLoyU2QlaqjU6HV6KMWZgu5qVmylVXKtmVAWzEtYkqota5k3sVtc46M7NWpSZnfEEjE11H9ZxI71MTVRRYPwCqB6pMmIq6KWzdkl8NhMVlbEHcDfUqtRn3gcIc67w5d4pXTMQCGYXFwYbzsQlkmb2Cx2FpjKlM0rfV3FSn7BlAPpFxK2ZdWLH5Xo+MfsP8IsLoflih4x+w/wAIsLljCY2lVBNN0cA2OVg1jyNuB80iwvcngkQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQDDFAVsZU3nfJQRN2h8EVHzFqhHBmsFAJ8Gxt4RltEVtdm5KlhAEAQDD6H/mH/wA3if8AV1paWvIrDTn7knQ/9Bwv7BP5RIlqI6I2JBYQBAMPpTRCU+tp3tWiQQw0LJmGam/jIykix4GxFiARZPyKy3m5KlhAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAIMVi0p2znKGNgSDa9idTwGgPGLEXK+I2hQKkb5V86uM3Zw9o9smzF0VM1HX+tVNL6BwT3ozNoB2D4QR9SHd4ZGd+suGYDMd4DcL4PZ/ek5jItUadNmyriahOugdfqmx7Ow8eUgk1pBIgCAYfQ/8AMP8A5vE/6utLS15FYac/ck6H/oOF/YJ/KJEtRHRGxILCAZuP3YcZq70ywuAGAFlsDxHnEkhlLH0MM6mlUxLlX0I3g1B74XIGgtreTmQ7byapulvfE1Ba1xnF9RmFhbXTlIH1JcNjaCXviM2tu/YG2UXNuGmoueEWJujTBvrIJOYAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIAMA6biOmSnLmooQ3C9QHmDoV5f9Z5Me1G9Idf8KKVzH213QUoNkOCUmw0LZSDfgQUuCLCdVLFyne8bW4mU6uy7WIj3QCGC/k5A5AGtQDRhqL5PVaU8et2XzLd5wOdodP0oglsDSLeZwbk/3snp9kmGNc9I9Q6lvIonuqimq1FwFMHWwFUA+exFPmf4zVYlt2t1N6cHNXWh37oj0i67hqddk3bPmumbPbK7IO+sL3Cg8O2bxltK5SMrq5vSxYQDD6H/AJh/83if9XWlpa8isNOfuSdD/wBBwv7BP5RIlqI6I2JBYyekm3kwVNarqzBnyWS17kM19SPFnXg8HLFTcItKyvmc+JxMaENqXyOs1e6Dg38LD1D+sKZ5+fzn2z0f0Osv5R6/0ee+2KPpfQ4XprgezCn7FL4yP0St6l1K/rVD0vp/Z9v04wR44Zj6Vpnstz5ACR+i1vUuo/W6HpfT+yKp09wI/wCGbl4FL4yy7Drv+S6/0WXbFF/xfQtbO7o2GqVadBaVVS7BQTksL87HhMq/Y9WjBzlJZfP+jpo9oU6slFJnc6bgi4nkHefUAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAOH4H0QD83YmtTam/0jMe+TLqMmumYnS5Ujwb+e08qFJx2ZKPF/QnZhZNZXf5Yt4KrhSu9YszroLnM2huGJa+tzx+MxqQrqWxbXM5vidy9ijTw9XJWUiqB34dgSS1iNRcaA3uDKOhVzVibZ2K9baVIs5RAwsLkC68frA3Gusu8NUhb8Yy+ZkbbIvTqBgqAHOLW1bwQB5jNqaX7opfL8/Mjuw8ZKnnxPWO5+UyKKeia29bEkn0m5nbhdrulta5+7OaGh6BOgsIBh9D/zD/5vE/6utLS15FYac/ck6H/oOF/YJ/KJEtRHRGxILHUu6RSzYemD/bD+R563Y8tmtJ8Pujyu147VKK4/ZnTcPs6kBcqPXPanXn5M8inQh5oB8IVD2TIeDaAH9XgWHnFxMO/qXybOrwkWvhRI2zKJFwBbs10mixFTec7wtPcZePwFMAm06qVaTeZzVaSirozdnIoxFJh44t7ZONalhZvgzfASkq8U957fsNiaYnw59YaUAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAPmpwPogH5u6ugWzlidclxcBidSb9nnHsnnxc5XtlvN3h1BxtK+j0az+pp4bAoyA0ypPaApubHS/Pje81hGrOTik2/n+fmhyVIqmrydjkbFCq7Mjli3euWtlFgALX4cePZaa4iOMS2nD9q1WTv9+S3nLTxFNtRTu/8Asg6mxsi2Khr96QRfLr69bcrzilOlK7lKz4/M6n3aVjsONSkU3takhZBZWJJBtYWPba54G4v7Z5C2nNxpNpP3+30PV8VT7pOrm8uv+HauhRp6GmAqG5AAsBcknTs1Jn0GCc+4j3ju8/d26HDVcHNunp+fc73OooIBh9D/AMw/+bxP+rrS0teRWGnP3JOh/wCg4X9gn8okS1EdEbEgsdR7pTWw9M3I+mHD9R563ZCvVl8vujyu13alF8fszybamLJZqFSoRTqKMocEm443y2svDQgk8hxndipqDtJ2Ry4RqavFJtFTA4FgWZmSsFbKQ2YEEWucrLoADxuOM5I4m1S1010O9wexe39nZsLiVpU1ps9MEcApFrHUT1YQfmeRWndtxTOpdL9tMHFMMApHEHnxuB/Ced2hUnGWxfL81Ozs6EZR22s+P2KnRbEVVxVJQwem1QWvoRcgmwPYOWvHjOKOMqwpSpfxa5fI9GWHpyqKp5rzP0jsD82J551GnAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAEAQDhhAPL8b3OVQ97VrN+tk4epZh3C3mlStOSsnb5f7c5wPRJ6LF0LAn9W1vRbWa0U6TvFmVZKurVEn09jVGzqviD2Tr8VI4X2fT3szK3RG98qlCTckG/HkDe05akYT1ijsgpRVm7rc7ELdDGNiS+nDl7JyvB0/LIiVNPTL6nZ+iux2oALrYX1PHUkn+M6KcFCKii0VZWO2y5YQDD6H/AKO554rEEecHF1iCPVLS1Kw05+5J0PP9Rw3moqD5iBYg+cEESJaiOhsSCxh9LdjHFUVQNlyvmva97KwtxHjTswWL8NNzte6trbcceNwniaahe2dzzjH9Ca5qpUSrlNPhenmB9V9JfGY7xNrxtbiZ4LALDRa2r34FKv0CxTu7nEsN4bsAhAJ5eFwnNGqk72O3ZKb9y+sf+II9FP8A8pu8Y9xXuuJDV7k9Vr3xDE3vrTH8LzKeIc9Qqdi1snuY1KNelW31xTcNlFOwJHnubTFyuaJWPaNjUiqAGVJNCAIAgCAIAgCAIAgCAIAgCAIAgCAIAgCAIBlHaj1Hanh6YcI2V6jtkphx4SoQCajL22AANxmuCBNt5W99CXJi/Hofd1PnjInM4NLF+PQ+7f54yGZxucV41D7t/njIZjc4rxqH3b/PGQzG5xXjUPu3+eMhmNzivGofdv8APGQzORSxfj0Pu3+eMhmc5MX49D7up88ZDMjq4HEVAVqVwqHiKCGm5HaN6WYgHmoVh2ERdEWbL+Gw6U0WmihURQqqosAoFgAOwWkFjP8AyU1NmfD1N3nYsyMu8pF2N2YLdSjE6nKwBJJIJJJm+8i24lyYvx6H3dT54yGY3eL8eh93U+eMhmfBw+J8ah92/wA8ZDMdXxPjUPu6nzxkMx1fE+NQ+7f54yGY6vifGofdv88ZDMdXxPjUPu3+eMhmfQp4vx6H3dT54yGZHiMbiKIz1KS1EGrGiW3gHMUSO+A496xbkpOkWTDbRo4eutRFqIwZGUMrA3BUi4IPaCJBJJAEAQBAEAQBAEAQBAEAQBAEAQBAEAQDG6ID+qp+vUPrNZyT7ZMtSsdDZkFhAEAQBAEAQBAEAQBAEAQBAEAQBAEAQBAMjooLYVB2AuB6BUcASZalY6GvILCAIAgCAIAgCAIAgCARYnELTGZjYegn8BAI/wAoUf7VOF/CXhrr+B9hk2ZF0cDaNHhvEvroWAOmh0MWF0SYXEpVUOjBlPAj/enokEp3JoBXxeHZ7Zar07eIKZv6c6t+EEGfiaBp2z4uuLmw72gey5valoLDidJP0I+pVweGpUkCJjnCAm3fYY6sSx1KcyTJ+gyXmaGzqdznGJqVQOKnc21FxfKgI0IPGQyV8zSkEiAR4isqKzsbKoJY8gBcmAQ09oUWvaouhI4geCSG0PIg6+aTYi6ODtOha+9S17XzC19Dx7eIizF0T0a6Pcqwa3GxB1tf+BEgkkgCAIAgCAIAgCAIBWxGPpU2VHYKzXy3vbTjrwHrixFz5/KVC4G8S5NhZgdeUmzF0feLw7PbLVenbxBTN/TnVvwkBlb8m1PKq/sw/wD+cm/AW4kOF2I1NQiYmuFF7C1A8SWOpp8yYvwItxLWGwTqwY16rjxWFGx9OVAfxi5Ni7IJK1XHU1cIzWY8wba3IGbheytpe+kmxFzj8o0P7Wnrw79fP8D7IsxdFlGBAINwRcEcCDykEnMAQBAEAQDI27ttMKpeocqKBc2ubtmsLXHiHt7Y0VzOdRQzZmv0nw1UZWdGB7Cq+kfXlktxh4ymcrtHCcRutR2IBoAQODdgJk2ZPiqZLhsThiTkFIX4kUwNL/rc9ZV3WpaFenJ5Finj6dIWTIB/dTTQAD63IAeqQnctKrGJNh9rZlZhZgt+zLqFzczpaWcbE06yqJtHFXauUlSRcGx7w8R+9PMqdqUIScXe6y0O6OEqSSasQVtoI9swVrG4vT7ftSq7Xw/HkS8FU4HxvaIsciaCw+i7BwHhcNZb9WocSPBT4E1DHKtythfjameA4DwuA10hdq0Hv5DwdRbiZdpkkC41NvA5/vS0e0qLaWeZDwtRK+RO+LbKpsBdSx4m1iosBpfVuPmndKSirswinJ2RC2MJFjYjtGT/AMpmq8C7ozRTIpAAbpLAWAFIWA5AZtJdVYvzM3BryK2Nx+HQF6lNbKC2tEaWGZiO+5C/qltuNtSqTbskR0elWHC7xNVcA5lpXDDsIOfWX2fK5m6tvJl/Y3SJcQ5VL6EBsyZeKsQRqb+Bw04xKGyTCqpu1mbsoaiAIAgCAIBS2njhRXMbABSxNr6AqLAadrDtmdWrGlBzloiG7GWnSemWCZu+IuBk7B+/McHjKWLm4Ur34oyq1o0leR91Nq024gHTtpnsN/G56z0/DT4HP4+lx5EPW6HiLwt+Z7BwHhR4ap+MeOpbnyJa/SNFAJPE2FqZ4n97zTlxUo4an3lR5aZZmlPFwqS2VfkWNnbaFVrDsIDArlIDXsRqb6icuGxtLEtqnfLgdNzXnWSU9q43coah4AEsbXsqqzmw7T3vC44y0Y7Tsik5qEXJ6I69S6c4ZuD+7PzTp8FU4czzJds4eOt+R8VelOEY5m1bhc0jfS9tc3Zc25XPOT4Krw5lP1vC8eRGvSTBDUKAR/g8uFu+jwVX8Y/W8Lx5Fin0ww6gKpsALACkdB9qPBVSf1zC8eRPszpbSr1dxTOZgASChUZS6odcx1GcG1pnUw86avI68NjqWI+C/wBUdlnOdogCAIB533YVU4YBjYGrS9tq/GZV3JQvEyqxUlZnnVHZ1FFFS1wDow3nC3mY29YE8nxdXb2U7P6f0vuUeGildq/58y7szamHS2WnUJ4i3WLa8ew/wmsq1e3xf/JmqdL0+5st0nppbMii/YazK3pyuotKwr15fzf/ABT9mWcaUf4rm/uiOpth6utPDkg/X6wMtudgQT6pWeLnDKVW3DZ/wsqMZ/DD67R2zoYtsPWuwY52vlDgD6L+8Tf1WnbgMRKtFuV9fO25bkjSFFUlZff73LO3tr0aGaq1mBqlLIATnubg8rWPGeRWot1pZLVvqexSl+1LM5wWIWsi1UFw3MWtY2I9s5J03GVrGyllmW6z0wg70X7f99spLYis0uZWMZueuRVpYhGNrW80yVSD8jZwkg2NpJVpUyQGdu9vfWxF9fXOijHanFwWjjfmZS+F3fkzbqOFRCxsBTbX96nPqsQ7U3c8mim5pI61jOlNBHy98VtqwUkA8rDU+kTyntPQ9qGDm43ZXxPStALqVI87HTWwuoBP4Xl4RmyJYaK+I896a9IK2IVQzKn1Fyn6lQsKlVqYuwAVAtiLkMedp1U6cjGpKlTVof8AR1RNoVAhoI7imrlqS38Hv8wZfTpcdhuZ6UYRkldZnlSnKLdtGesdx3a712qLUALoUJYaXzLX4rwFrdkrOCi8mUUrrQ9XlCwgCAIAgCAdf6Z26u9wD9GdCSBfeUrXI7LzKvLZpt7vqUmm1ZHlmwq9BH3letVD5jZVUAAXZPCIudO0Admk8qUq8aiqUYq/F7+Xkcdd01JqV7ZafjN1dsYZh9HWxCsB9bK68R4Qtrw5iW8XjqTzaduJioUZ5RTTM9tpUzUNSstSpqMoRmVNOBC8b+uMRWr1ZKUZxi/Pz66ERpON9qDaJtrYjBVAAqGiQb5lS97jtJ7Qe3s15zjUMS8ptSv5X/NTZumv4tcbW4mr3NWJeqWYsQ4A/VFRwptztbXj7Lz0cBZSaUUslovPj8jttFS/buXselz0y5jdLVvhqg506n/JeaUnaaZnWipQabss89x4TilZDcA5T6dCPxPP1ievTqbWR8/jMJCnL9sk0+N7cC3hdrhtG0P+/ZN1JM8apg3H4SdMehHE+jifZJujPw072SKuM2gT3i8+21/iJWU0kdFLCWf7jsXcyosMWSRa9K9vNv6NvbrPOxVWM42Xk/sz3uzobNT6fdHss889sQBAEA8z7t75cID/AI1L+XESlRXiZVNDyPB7ZFMDKGBHiuw9p5eaefUw/ea25GcajjoaP9IFq2z00OnFlDXtyJv+M51g3T+Fv6O3sXdba+JFnCbUw+bvadNCRo6quYHmNLTKeHqtZyb4XZeFSHkkiltDa+LQ2aoGB4MAOH/SaU8LQeajbgVlUqrV3PSO5NiXqYTEFzc71rejcCephYRhFqJMG2szM6QYQticRT3hCmu7gWXLmLEX53tznnVWlUlK1/I9akm4qN7EA2dUAAFd1AuBY5dD6PTOVyg3dxOpU57yWrRxTG5xNTXz29FlGn8JH/42tsId1PeU6mZaqlsUd63AEgHUG+UDQ8OEvCnBxaUFYpUk42UpfT81L2GwVR8RRqPUz2rIRckW79eCgWE0w86UGoxj5r3K1adRxbvkd06dU6rYBlogmoUGUC9/z1G/DzXntVrbD2tDy6MpRmnHU842bj9o01LVcIHprcM9Q5QuXwu+BHDtvecypq11I6Xi6mhYrY2ixK1sE11NmAxNwDmKkZSSNCCPNaXVRQ1a/OZyzxFWWpWrYrAiwTCVGOYBlCO5ynNcoV0Nsq+nNOiOIXDmYpOfq9yzUw+HUEvhggBJJYlPoxwIUnMCTawIHbrM6/aVKmrQ/dLd5c/6uZdxWcv3ZLe9eRt9ydqZxOIyFdShsvAC2IAF+3wT+Mzw06tROdTzOpxUYpI9WnSQIAgCAIAgHWunlHPhaqXtekef9pS5S9Oj3z7u9rmGJrKjTdRq9vL8v7HlFPZJqVNwlfd2UFiQzAg9oGYG9wdPTrMX2RJTabvbh5fnl1OGn2hSlBOUev8Aln8zVfucgrm6wrkdgouWvztvSeEiWClBZPodEa0ZaOX/AC+xIO5woois+IFMEaq1Krm1NtRvj+Ey8K9W+iN3N2+J8yjiuiqUHpZCtTO2Utkq96AMwaxcjLpx52HbJjgXU0l0S/05qmJcFq89M7/4dr7n+yXoVaueqKmYpYCmqWszcmP4zqeBWHW1e9y+GxNOq3GEbW43uejSp2GP0r/R6n7Op/yX9EvTTckkQ6aqfslo8jxyoC4IZVI/WYGwHLXlzne6NVFX2Nhr3ULfJtEuC6FVq43iVKSqTpmPfeuwIHtnLU7Up0ZbE07r88zhfYle+TVvr7F2j0BxCEMalM2PAFib+bQazOXbVFqyT6FsP2PWjUTk4289f6MnaGyMSjkHDkdgYtTUEDtuGtf4yFjI1Vk78Emeh4GEZ7Vs9/5kdm7nWEqriM7ZipQAarlua1I8Lk30OtucOUdL5mk6bjDasesyhkIAgCAYPSnotRx6bqsTkurWGYHMmexzAjsqHSCGrnWf/R7Z3J/t1PmkbKKd2jkdyDZ3J/t1PmkbMR3cT6Hci2fyb7VT5pHdxI7mJOO5dgrZe+I85c/90z8PTvfPmW2EbOwuidLCI9KibK5LG+YnOVyXuWOluyawioKyJUbEeI6HUXdqjHvmYsTZuLG5+toLykqMJXuiybTumfZ6JUfN7G+aYeAo7nzOrxtbec/0Upf3fst80eAo7nzJ8bW39A3ROieOX7J+aPA0ePMjxtbeuR8J0RpBg4axVgwsGGosQNG1GnD0zSOEoxzSKSxNWWrNg4RrIAwBVSCcp1uVNxrpqvn4zoaTVmYaHUq3cxwjhlZ6rK7FmU1KpBZ/CNs1hfT2SrhG9wWdmdzzB4fVFBN75nzu1734sxt6RKSowlqWjNx0tyNxdlECwYD0K3zS8YQjoiktqXxSZ8VNiBtGYH0qT/3StSlCorSRNNypu8W/l5citsLonQwlRqlFVXOQXCqRfKrAa35ux85J5y0IKCyJlJs7BLECAIAgCAIBS2ns8VlyE2BUgixNwSp7CLaqJpTqOnJSjqjKtRjWg4S0ZjUuhtBTcWv6GP8AFpvUxtWaszip9lYem7xT53LuG2CKYsre0NfjfU5tZl38rWN/B07tk2L2TvUNOoUZSLEFDqPtSneM1dCLVimvRemBYEAebPp6O/09UvCu4fClyMamCp1M5N8yfZ2wVotmUjUjNo1zlvbUsbamWq4mdVJS8icPgqWHblDz1Nic51lTaWD3yZCbAgg6HgylTaxFj33GWjJxd0E2ndHWx0Aw3M+1/m886PGVd5r39Tf0NDDdGEprkVtD5mPm8blOGvShXltz1LeJq2tc+F6KIP8A3G43+txFuPfeYTN4Wi/I4lRS83zIK3Qmi/huza3GbMbejvp0xtFWijp7ye8uYDo2tFg6tqABwPAMrc7X70ayihFO6NKmJqVIbEnl8jdljAQBAIy5gFbGbRWlbNfUE6AnwbX/AIwRcqt0hoC/fE25Kxva97cyLcOMmw2kWcLtOnUZlQ3KgE96wGpYDU8TdGiwTuWd4ZBI3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgDeGAN4YA3hgHIcwDK6QbR3eWmtelRdtSailzkGl0UEDjYa85STt5mNWdsk0vmYQ6V1C3Vt9RDhta+Vihp5QQRTvfPdrWvbQmU7zyuYeIlfYur7+Hy3nYNgbQ3isrVqdZ0OppqV70+CWUk2JIbhppNIu/mdFKd8m03wNHeGWNRvDAG8MApvg65JIr2F9BulNhyvfWDPZlv6Hw2z6541wf/AIk4HjA2Z+roRDYz/wBonC35inwPEQNiW/ofdPZdVfBrKPRRQefs9JgbMt/Q++o4jyj3S/GBsz9XQdRxHlHul+MDZn6ug6jiPKPdL8YGzP1dB1HEeUe6X4wNmfq6DqOI8o90vxgbM/V0HUcR5R7pfjA2Z+roOo4jyj3S/GBsz9XQdRxHlHul+MDZn6ug6jiPKPdL8YGzP1dB1HEeUe6X4wNmfq6DqOI8o90vxgbM/V0HUcR5R7pfjA2Z+roOo4jyj3S/GBsz9XQdRxHlHul+MDZn6ug6jiPKPdL8YGzP1dB1HEeUe6X4wNmfq6DqOI8o90vxgbM/V0HUcR5R7pfjA2Z+roOo4jyj3S/GBsz9XQdRxHlHul+MDZn6ug6jiPKPdL8YGzP1dB1HEeUe6X4wNmfq6DqOI8o90vxgbM/V0HUcR5R7pfjA2Z+roOo4jyj3S/GBsz9XQdRxHlHul+MDZn6ug6jiPKPdL8YGzP1dB1HEeUe6X4wNmfq6DqOI8o90vxgbM/V0Pung64IJr3AIuN2ouL6i99IJUZb+g2nspaxVsz06ighalNsrANa4PEMDYaEEaCVcbkTpqWej3oqno1Ry2DVRUzZt8HO9zkBSS3AiwAykZbAaSNhFe4jbzvv8/wA6FvZuy1ohrM7u/h1KjZnYgWF+wAdgAAkqNi8Kaj897I+o4jyj3S/GWI2Z+roOo4jyj3S/GBsz9XQdRxHlHul+MDZn6uh//9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxESEhUSEhIVFhUXFRcYGBUXFRYYGRkYGBYYFhkXGhYYHSggGBolHRgVITEhJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGxAQGy0mICUtLy0tLy0tLS0tLS0tLS0tLS8tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAMABBwMBEQACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAAAgMEBQYBB//EAEAQAAIBAgQDBQUFBQgCAwAAAAECEQADBBIhMQVBURMiYXGBBjKRobEUQlJywSNigpLRBxUzQ1Nj4fCi0pOy8f/EABsBAAIDAQEBAAAAAAAAAAAAAAADAQIEBQYH/8QANhEAAgIBAwIDBgQGAwADAAAAAAECEQMEEiExQQUTUSIyYXGBkRSh0fAVI0KxweEGUvEWJDP/2gAMAwEAAhEDEQA/ANpFd48vyEUByEVIchFAchFAchFQHIRUhyEVAchFAchFSHIRQHIRUByEUByEUByEUByEVIchFAchFAchFAcnKgORSISYUEnoJJqJSSVstGMpOkLvYd099WXzH61EckJe6y08WSHvJobirC+QigOSTgcA90wugG7GY/5NJy5441yPwaeeV8Fj/cSDe8Z8FrK9a/8Aqbl4au8mIHAxP+L3fynN8Kn8bx7vJX+G8+9wPjg1j8Vzzkf0pf4yfwH/AMPx11ZX8S4Y1qDmzKdj+hrXg1CycVyc/UaWWHm7RBitBl5CKkOQioDkIoDkdy1Wy+0XasFjA6TrpoNzNVlNRVsvDE5ukM2riNqjo42lGDCekqatb7qgnjcXTF3QqLnd0RSYBd1UExMDMd4qu+3tStl4YJSVoGChO0Z0VJADM6qCSJABJg6Ub/a21yRHBKStAQoTtGZFTTvswC67QSYM0b/a29wjglJNrsGWrWK2i2w7ASQQKqppukXeKSVtCMtWspQZaLCgCUWTtC8FVuzLpnicmdc8ETOWZiKrGe5WlwMnglBWwy1axVBlosNoXlVEzu6IswC7qoJiYEnU1Xfctq6jY4JSjuXQMtWsXtDLRZFDmFsZ3VJjMYn0n40vJk2RchuLFvmomnscKsr9wHxbU/OuZLPkl3OxDTYo9EKu4G0d7afAD6VCyzXRl3gxvrFDWGwiWsxQRO5JmB0BPKieWWSrIxYIYr29xd0hgVYBlPI1RScXaGSipKpDC4Ww3dNpR4jT50xZ8id2KemxNVtRWjBLZuzdH7KTDHUeGaNvWtcszyY6h1MEdOsWW5r2ez/UY43xjFi+1rCorqtgOAFJ1K3o7wMe8lsBeeY1GLDieNSyuua/sdVVXA2uLx4Zg9oZQ6LmW0xIQiTcABhpOmWZGvSoePT1w+3r39CStbiGPm5ZS2xZUdoytnAZ8RkbPm0PctAL0Y9Kf5On4m3++P8AYDtzE8SCm2qXCxOIBuG3sJum1kO2kWt/xDfWK+Xpt25tVxxfyu/zAdTF8QAy9gbiksR2ltjOg5E/s43A5kkVGzT3e6vk/wB2VlFSVSRa8Jwhe0xxVtbbBoDAG2CuVWmCSNyw9KVkzOMl5btfcz5NLhatqisdBJgyJ0PUda3Jtrk40oq+DmWpsrtDLRYbR3LVLGUR+OX2tYO8ye/cizb/ADXDln0EmoglPNFPouX9DTi9iDn9F9TLeyWEODxeIwZMjdTyJUAz6qf/ABrdqJ+dijlQifszeN9jQe1nDxfwF9IkpF1f4D3o/hLVkwZPL1EZevH3HQ5xSX1MxxJ3xfD8LhrerJbu3ro8LAyKPMiT8K140sOonkl6pL6hv34kodeW/oT+GXVxWH4dhG1/bM10fu2B3QfORSssXiyZci9KX1LYskZQivV8/Ql8Z47ewrL2y4Vu93rNp3N1F3kzpMfOqYMMcqe1y+bSopncMdWl8k+SPxK1iH4xbKi1JtDswWcL2cNBaBOeJ0GlTieOOjb568/P9BmRuWZY+1DuM9pXK3L1m1Z7C3cFsZ3YXrs7sg25gx0NENPUlCbe5q/gvmKlKDg5RXCddeWSuKcbuLiLVjD4dH7aylxS7MpBcN73IAZZqmLDuxynOVU64Vlp7IzjBRu1fUbfjl5r9zD27eHR7QAPbO4Nx/vBI0AmYnlFCwpY1kk20/RLj5hcN7gkrXq+pG4pZvHjKtato104ZBldiqg9nrJGpjpV8UorRvc2lufT5jMjvMoVfA9gfaYfZbuIvWh2lu4LYtqTlZyCRqZIAAM+VGTTy82OOD4au/gIi4KDySXR1XxJGA4q/wBp7DEraE2u1zWSzBAFLlHnZgAfl1qk4Lyt+O+tcl9ieTa+OL4M/wC2GPvYzBLc7K2mG+0xbEsbshHEt92CJ25itWkxxxZ3FtuW3n0K5cv8ndFVG/qbS2ug8h9KxtimhWWosijj258Oh6UWFF3wDE3XzB3DBYjTva8yRyrBqccY1tR1NHlnO9z6Fu1ZTaY3GcI4gwgXQQTezTdYghzcCoVIy5Qpt8pkH16EM+nXLXp29K/2BL4NgMVbcm7czJlIC5yQCGGSFjQZc21Jz5MUo+wuQLZxWQBaXQUKHWQRrtryNWi6dlZq4tFDiOCva7wJA6oxHxrpwzwycNfc409NkxK0+PgMDtRqL1yRtLE/I71dwxv+lC9+RcqTJNri2K2ARz1yGf8AxNJlp8XrX1NEdXn9E/odvcRxREMRbHghB+LURw4e3JE9RqGuePoQwHG164B+dv60/bD/AKozqU1/U/ucyA6sxb8zE/WpVLoiHb6tsdy0WFBlosKDLRYUPZapYyiFx3h/btYQgGwmZnExmcggCBrppr4mpwT2bpf1PhfItmW5Qj2XL+ZW472bFu9avYRFVVALLnjWTMZjzU0/HqXKEoZX8hOXBU4zxV8TSYcLJDe6wKt5EQaxztrjqacTUZc9Cg9kOBthbrtdAIIyAggypJzbbTpWrV51mglH5/Uz6PE8M25Pj/Bz2Y4C2Gv3XYgSjJbcEGJOjRyOgo1WfzcaS+pOlxPDkk2+OxBucAxBwzYfsrU9rna72gzPowHprzPpTVnx+ap2+lVXCFPFl8l46V3d31LbHYS8uKs4u0ivlsqhQuFghSpk9NeVZoSi8UsUnVu7o05HNZo5Y00lTV0Q+H8DbC3XNuzavKfcdmCsnnoT5xvG9NyZ/Nik24vv8RMMTwzdJST6c1RYYrh7vjrGIbKVS2quQeYDzAOsS1KhkUcEsa6t8DskW88MnFJUyH7Q8Nu4mVaxZzZu7iA8EJOisvPSmafJHFypOu6ruL1UZZeNq68Svt8iZhOGOmPtXywa2lpELkjMStvKSRvvSpZE9PKFctt/mOjFrURnfCSRV4b2adsPes3Cqs10XUMyJAYEGNpBrRLUpZIzj0SpmdYJSxThJ027RZ8Iwzrb+ztYtWkZGS46tLPmUqCFA0M66k0jM05b1Jtp2kPwyaWyUUuKbTKfE8DxRwowmW2US6XD5xLSG+6dh3jWiGfH5vm821VUZZYs3k+Uq4d3fX6GmRdB5CsrY+hWWiwoMtFhRU2w+GS1Nw9oXyZl0nMxImdxTZKOVvjgVFywpc89C0v8exNpGd8hVRJJXX5Gsy0uObpWanrc0FboX/e+JkNCEfhAIn1maj8Nj6clvxma74HX9pEAl7TjbZgRqY5xS/wTb4Y3+IpLmLG7/HixFtLYRmBgsZOm5A251aOjS9qTspPXyfsxVWRTxe/bZEJQlyQpKCdBJ2pv4XFJOS7CfxmaLUW1ySTev3D32n91Rp8BUKGOHQl5MuT3iThMAzuAysF3Jgj0mqZMyUfZfIzFp3KXtLguC2XuoAAPCue231OpGKiqQlrzAd6I5zEUL4EtWNqir7ttR6VZ5JPqxccUI9EOdr1UEeVV3MvtXoMYrhyOJtgK3TYfCtGLUOPvdDLm0sZcx4ZV38K6e8I8eXxrXHJGXQwzxSh1Q1lq9i6HctVsZQZaLCgy0WFBlosKDLRYUGWiwoMtFhQZaLCgy0WFBlosKDLRYUGWiwoMtFhQZaLCgK1DkkrYUQr+NA0UT48q4uq8YjD2cSt+vYdHBfUat3LrAtmVVHMxE9ANyfKucvEtXP2tyS+Q1YIibXE1UDtJJJgQVUeHKZpmDxfPTtbq5fyKvFjXUj4TiWbN26bXDk0B0+6R411JeMYIuKVu4ptrmvVfQzRxSd7vXgk3MSl252BAZGtljvuGAA+pro6fU4ssPMxyXUXOPt7JLih8h+2UrHYhHDajRgRGngAfnTuNvPWwp7+OlDGPti7c+zspyFA+Yad5XECfSrQbjHevl+RSaUpbH06isAbd8W75WGGcLqepU6c9FqJ3C4fImG2aU+53BKzIj37ffV26SAWI06d2onw2oMnGrSlNdDW4S/aZf2RWOg39RvXLnGaftHZxyxtewOlT41QaJNvehdQMhc9nsblRTfBAtKrzcuNnfQsxDAz3hodNNIrorU4bb29/ToBZ8D4dftF+1ulwwWO8zQwZ83vbAgoIH4azajLjnWxUBci2azABSNZjxOlSlZDaXUicQ4gjLkU5jzI2Hr1rThxST3MyZ80JLauSty1rsxUO5apZegy0WFBlosKDLRYUGWiwoMtFhQZaLCgy0WFBlosKDLRYUGWiwoMtFhQZaLCgIqHKlbCitxd7NoNvrXmtfrpZnsj7v9zTjx7eRm0qgy6k6SBsD5np5Vz4pRdyXyG/MjXTu2kanTbrpSmrZVulZX4crfRLmohs0DqJEGnYc8sCnGK95bX8jNDbqIRn6OxeKshyq5oIIeBzg/TWq6XUfh9/s3ui4/cvlxqbSvpyJa7+0CRupafUCoWlf4V6hP8Aq2/l1B5P5uyu1j32NxZe0Ljd8sZ6ZjJ0rqx8Wn+Ihla4SSavrSoW9L/KcE+vcfxDXT2cXCMjqxnnAI/Wq4PFJw3723a4+DstkwOW2uz5F3bjl7T5v8Mscsb5ljWKvh8bywhKM0m3XPQJ6dOSadUWNviKnRgR8xWrD4zilxNUDwsjnDk3XeR2WRYg6hhJY+G9dvHnx5YLY7MkscozbfQlYS0txFdbj5WAI7x2+NRL2XTSGQW6NpsVhnCM/ZXSGSM43G0iQd9KicVKtyJhLY24y6dReE45fuIHUIykaHKR9DVJaWCdOxkdZlatUMpx2/csG8pVVAY6LrCzO89Kt+FxxntZV6vLKG9dCBdxL9nauhnPasgMFtM/OnKEbcaXBnc5UpW+R/iWHZVBQG4wdQRvoSJOvhUY2nw+C2SLS45LRLYG1KsdtFZaLCh3LVbL0GWiwoMtFhQZaLJoMtFkUGWiwoMtFhQZaLCgy0WFBlosmgy0WRQZaLCgy1FhRX4/E/dHr/SuJ4lrL/lQ+o7HDuyKtsxnMQCBrzPSuQoutz6DRrHO7hiIzkELyA0geQFEpOTtlMu5xe3qUX2x8NasJcjMWAOs9wfqJHwqKMPnSwQxxn1b5+RYX8Wq3rdmB3wx8o2+MGo22aZZoxyxx+o0/Dn7ftc4yhMuWP8AvPWquPFFXhn5/mXxVDyEEBgZBEg+FKaaHxakrRIRpq6dlgIqQEkVADOJvoilnYKo3JMCrYsOTLLZjTb9EQ2l1M9iPbfDoctoXLrHSFEA+Gu/wr0ek/47rofzJTWNfF/tCJZYPjqW/AfaTEMpVsEbSBTkOcAzBIBQgH4V0Muo02JqM86lK+aXH36C9rUXtiSbGPKMGFuHvCbhJJ1VOmw6Vz83isnjyOFVBpR+NsrDGlJWve6nExFxOzS0QqKWkDkIMb761gXi88mHI8kvb420vuM8rbKKiuO5y5i7soFYAKxJAAAMqwiAOpmk4fGsscc1kbcmvZfHD+JMsNuO3ouo9guLXUL5grKWBUbQoVRA6ag1oyeOpKG1Xx7Xbn4EQxyTlfrx8ifwi/bz3WLmbjhsraRChYB57V08Pi+n1CjFOmuzKxxOLb9S5y1tsvQZamyKHctUsZQ3fuqglzAkCT1YwB8Yqs8kYK2MxYZ5XtgrfUjjilggEOCGIAIBgkgECY3MjTxpf4nHV2aP4fqLa28oas8asMocvllM8EGQN9fHwqsdVjau/iXn4ZqIycdt81wF7jNlY1JBZlLQYUqpYzpyymenOiWqxxrknH4ZnmnxzVpetuuBV7i1lQ5zglRsJJJ10HX3TttBqZanGk3fQpj8OzzlFbav98ncVxJEVCZl8kKN4ZlWT0AzCieojBJvuGHQZMs5RXSN2/l/4ITjFoqrA6sVGWRIzZdzt99T61C1UKTLvwzOpOLXRN38r/QLPGbLEjNHeCgmYaQpkfu94CdtaI6rG3VkZPDM8Ip12t/Dr+fBY5a0WYKK/G8Xs2zlJJPMLrHnXN1Pi2nwS2ydv4ck0JtcbsNzIPQqapDxrSy6N/YNoo4p7gPZrptmJFLy+ITyJrCuPUvHGQbVtdS7QByGpPly9TXKjFPmT/UvwRuI4vs7TOToinKPPb5mq23SYrNl8vG5ehzA4gXLaP8AiUH15j41FE4sinBS9QxL2wUDgSzQsjnBP/fOpIm4JxUu74G8Vg7U9s6jMgJzeA1+VBXJix35slyhIvi7Yz5soZCSfw6a/DWoDesmHcnVr7FZes3bKYe2ga4A8sQOX4fmfgKGk+plksmGOOEbfPI/fxmXFJaEwVM+Z2+n/lVNnFjZZ61Cx/AnYrDlvvlfIKRp4EGnYsqh1in9zU1ZWWsebVzJdcPbMlbqqYSPu3CJA8Gnzrfk0kc2LzMMWpLrFvr8Y/5RTdTplVxXh4xmMCPcPYpZDgKR3iWIOvw1ro6PVvw3w/zIR/mSk0210pC5R3zrsX2C4dZsiLVtV8QNT5nc15/Va3Ual3lm3/b7DoxUeg+axMkQaqAmBUVRAlhVWgEGqgdt2WchVBJPIURhKb2xQdSbguJGzmBlyDAGYZB4zBJ9DFb9N4ll0ycW2/hfBFIlWvaX8dv+U/oa6en8clPiWN/R/qTHE5e6afLXesihnF4RLqG24lW3ExznflVJwjOO2XQbgyzw5Fkh1RCXgNgZYUjKxYAMYksH+oHoIpP4XHwbH4nqHdtcqunwoE4DYAKgNBUKRmOoXb4bULTY0qIl4lnk03XDvp69RV3gdlmZmBJaZOY81ZPozf8ARQ9NBtt/vsRHxHPGKiqpfD42cbgVggrDAFi2jEQSCpI6SCQfOj8Njqiy8Sz7lLjpXT6isbwpGCkKSyKAozlQcpDKGI5ZlWpyYYyS+BTT63JCTTfEnzxdXw6+5HwPCsM6hlQjRFILGVNppCsOoIAPWBypcMGKStL0/Ifn1uqxz2tru+n/AG7r4D1ngVhCGUNK7EsSQMoWNeUKvwq8dNji7FZPEs84uMqp/D6/5K7jHFyZS0YHNhz8B4eNcPxHxWUrx4end/oc+ipw2GUyXbKBvzY+CjmfOuHjwxk25ul+bJS9Rdm6ySLZyyd4GaOmbcelXhOUE1Dj+5N10GR3SNYJmPHmarGMlyit06GuN41lsOObDKDz13PwmtWKcm6Zn1uRwwuu4WcuKwqq5ZTAmB95dBPhsaa5pOisYrU6dKTohcTJw9q1atZ2hwxMdIMaci3KpUlIz6i9PjhCFvmx7jVi/ee09sAKsESTofek6aDQCoWRdxmqx5cmSEodEX920txCrCQwgiflV1z0OhOCnHbIq+KYE28K1qwpPXWTG7HXcnoOtSY9RhcNO8eJEzhSuLKC4IYCD6aA6eEVU0afd5cVPqSCo359aBtLqcIqoDd62GBU7HQ8tOlWhklCSkuqBqzP47C2sPicPctqqdozWmCiAZWVMDnIFdrBmzazRZseR3sqSvr8RLShNNdy9NefY0SaqA2zbgakCY/75VWiG+tdSLgWc2wbghtZHrUTSvgXhlOUE5qmIt4sNce2N1A+e/w0qJrbFSZWGZSySh6D+Fi5GXWSR6gx9aVUnLaMhJTVonXMOFJVGaCIYg6N1/hmmTexuMHx0fx/0XfHQgYxVTSST000q2LSvJz0Q7Fp3NWQWaa6eLEscdqOhjxqCpHqGWvSWcqgy0WFBlosKDLRYUGWiwobvXUQS7BR4kCqTywgrk6CiOeKYf8A1k+NZ3r9Mv619wIGK4hatt21twwMC4i6kgbOB+JfmPIUmWtwRe+Mk/VI2YWs0fJl1/pf+Pk+3oyNjuKm6ITRT46kenKufq9fLMtkOF+ZkcWnTIy4bIVLrM6hSY8iRvH1rCsKxtOS+gVXUrbXERdxN22YOUCPMaMPSQPSpnHc9zMuPUKeaWP0/bJ2Huq2bL91ip8xvQopD4TjK67cEPG4N7l626uoFs6rHXf4jSr8GfLilPLGUX7pExONX7YLOmUplI5Zm739B61Ty12FTzp6pY+1V9S7XDihYjfSQ52SjlMa9dquoJFow3NIg/3uhUMAZIBykERKlhrEfdNG5UdT+FZd7i2qur690v8AIu3xG0QDJB0kQZBJAjbqw+NFx6iZeG51Kq+t/UE4payhiSsqWgg7DU7UbkTLwzOpuMUnTrh9zi8StzBMGSBoeUanTTeotBLw7MlaV/v8x+xeV1DKZB2NBkzYpYpuE+qIHEuNYewYuXAG/CJLfAbVu03hmq1KvFBtevRGWeWEOrKw+2eE6v8Ayf8ANbv/AI1rvRfcX+Kx+pm/aXjwxF212U5bZBEiCXJHL0A+Neh8K8Jek02VZquSafwVGXNn3zW3sbrHXCttnG6qWg+GpHwkV4TTYlkyrG+7r9DoSdKyAvHsM2XLdBLRCjfXr+H1rTPwjWR3boNJdX+nr9CnnQfRiER+3a7mXs8kaNOg1+MyfWsE1tW1rkzxjkWeWR+7RzhPEBcRix1DH+U6j5aelKypRaQaXUeZjcn2bFcMuC8hcABiSJjUdPkRSsqcZ0+hOCaywc1w2T/Z7hfZI4ds25HLU6Dz5H4032cm6T7L8y+kwPFBxbssYCgk7ATSYR3OjTGNujN3rpZix5ma7UY7UkjrxioqkNzUknrGWu9ZyqDLRYUGWiwoMtRYUQcdxS1aBlszfhXU+vSsmo12LCuXb9EQ3Rj8ffe8+d/QcgOgrymqy5NTPfP6L0Fvk42BKhS2k8vvR1jl61R6ZxScu/3ChdxUkZEywdycxPmNvSKvKME1sVV682Tx2HLl+40SYjYBVWPKBTJZcsur/IltvliVusSTMmdfPxo3zu2QnYza4dbVjdRO+QefPX6zrT07QlaeEJOcVyRPZvB3rZudqBDNMz94bnyM/Krsz6HFlxuW/uxrgWIuHE3syMA2uoPdI90HpK1JTSZJvPPcnT/f9jQ9ihbNlGbaY8dfmKk6OyLe6uTh7QHTIR/Ep/UGnJYmubT+5b2iFxDiYttbz5klwpBEqwbu++NAQYOsGAa2afRPLCe2nxfHVV8OouWXa18yUvC7QEZdNOZ5AqOfRiK5uxHTfiOobu/y+N/3RFGCts4CL3UPeeW1IIOUa94gqup2iPKu1N8Gt6zNjxt5HzJcKlwul/D/ACPHhVn8J2j3m2gjr0JFTsRm/ieo9V9kL+w282YAhtdQSDrE8/AUbUK/HZnDY3xx29Cj9qeIjCWctrR7hMHcjmz689fnXa8D8Njqs26fux6/F+hg8Q1s5e1J+0+PoROAezNpbfbYlc7sMxDahRvqDu3Mk1q8U8cyvI8Wme2MeOO/+jLi08VHfkLu3w7DlQRZtZSPwLqD6Vw34hqrvzJfdmhY8bXCRnOK8FbDv9pwYHdJzW4zR1gdPDlyr0Wh8Uhrsb0msdN9JdL/ANmTJi8t78Y7bxi4pUW9iLIWQzWllS3RGLHadxGtZZ6aWgc5YMM2+ik6aXxVd/QYprJW6S+Rb38bYtD37Y6CVFcCWPV5OkZyfyY9zhH0K9uM4dj3ryfHSlS8G8Sl7TxS+wt5sb7osMPYtsvdylWnbYzvqKwTjkhOp2mvUsscNtJcMlcO4clsQggEyTvVm3N3IMWGGNVEtHVZhRoNJ5nxNXybW6guF+Y7gp+N4z/LH8X6CtmlxV7TNmmx/wBTKYmtpsOTQQbfintTBK2AD++23oP1NK1XjSXs4VfxfT6HKc/QornFsSxk3n9DA+ArkS8Q1Unbmxe5jtjjGLAMXGIG8gNHqRpTIeI6tcqV/QlSZIvYvFOmZ3OWJ95BI/KDNaJanVZIXN8fT/0m3RHXDHLmlAIn31k/wzM0pYpbd3H3QULHZhd2LH0C/wDsasljUfV/2DgYw+NFxrg3KMATO+n/AOj0ofPLFQyqcpJdh+aKQw6WgE9BNTQN0rKb2av3CbodWEuW1B0J3X/60ySRz9BknJzUl3sn4biIbEvZ5KojzHvfUfCpSNENQpZ5Y/QtKk1CL10IrOdlBJ9BUorOShFyfYp/ZDHm4jqx7wct6OZ+s1Yw+HZ3ki0+qf8Ac0IqUdIZxuF7RShaFIgjKrSP4ga06fN5M1NLlfGik47lRCXB4m2nZq6XViAbhZHiI99QQT4wDWic9Jmk5SThfpyv8FYPLiaap16ikxxtKBes9kogZlIe2PMjVR4kR41T8HGf/wCEt3w6P7d/oTPUSlLdl6vuWFYWqLiTUVfQDAXXGO4goGttD6FEMk/xH6ivaqP8N8Ld+9L+7/RHK3efqPgjXcZtO9l1txmYR005/LT1rw5s1UZyxOMOo3wa1cSyi3AMwEb8twD48vSqyDSxnHEoz6oZ4Phrqdp2hBzOWEEnff02qJFNLjyQ3b+7s5xnhaXrTplXMRoxA0blrvXR8O8SyabPGcpNx7q+wzNiU4tJcmGvezeKUx2RPipB+hmvd4vG9DNWsiXz4OVLTZV2HMH7M4hzDL2Y/E39BqaTqv8AkOjwRuMtz9F+paGlySfKo2vs/wAL7FRaQlpJJJ0E8/IaV4HxHVy8R1HmbUu329TqYcWyO1F+tyVAEBfDn4nrXPeRuOxcL+46+KIGO4mlsEAy3Qcj4mnYtO5deg3HhcuvQzjuSSTud66SSR0VxwhJNSAktUqNlXJIZwfEmGjd4fP486xZ/D4S5hw/yM09NGXK4L7C3LLLOeWOyAQR4sTy8BNYpaPy43P6V/kyyxSj1H2uuVCSco+6NB5kDc+JpTnNx2Xx6FLfQaFql7CKIq4sdv2P7k+u8fCnLG1DcZ1nXn+V8CcxIBgSY26mrI0NtLgouA4e8l5yy6GQxkbnvA+Pp1rRNpo5Wix5Y5ZOS69SThOIzi3Se6RlHmmv/tRt9mx2LU7tVKHbp9i9WqnRFgVYChwfA7qYjtTcB1zTHvZpzLE6edMs5mLRZI5/MsvTiVDi2SJYEqJ3iJHzHzpywyeN5EuF1+p0t6Utp2/ZS6rW2mNmAMHr8Ko4tU33IyQjki4voRuEcEt2CWUksZE6xlJkCJ5daBGm0cMLtdS2FWNgsVIHakCr4hx3C25D3VJ5qO8fIgTW7T+HavK1LHB/PoIyajFHiTMZa45fW464MM1qe4hQtlB5AbqJnSa9RPwvTzxRlq6jOuWnVnMWpyKTWLldh/FJxW+uVlIU7gZEkdDrMUjF/B9LPcpW182Xn+LyKmi04DwN8NadpHbMunMLGoXxk71xPG/FFrJKOP3V+bOh4bp4YprzujfPwQ82MxGU92DOgAERq2vxC+hNee8w9D5Hh++lLivX6f7+R20cQJGpHfIJAMnM0DwEZY9alNlskNDKpcf09HVKlb/vYm925gEmJQ5oVYMjN58/6VDsMUdGuVXO5Vd36V6AtzEx3hGi6ADnlzEeI72nlUclHh0Cktsr69/nS+XTkRdS72KqA05SG2zTBj586hhielernOTVXx6V3/8ABthfhhGhzHx95oG/MFT6GqjP/o71O+eF8Oi56duUOn7VbcmCpYRqAYUl9QPLL461f2sfwtBs0PlqNri315d11fbvQrG41lGQGJ3/AKeFO02JP2mcrT4k3uf0Kya3GwSWqyi2VckhBanRxipZBBetEMJlnnSIVqsjN5MtVRkl3gMUSIOpHOuXqcaxu13MGoxqDtdyalwGs6aZnKkcEuDEdr2gic0x4+7E7Zedab9mjmrR5Fn8y/j/AK+xeMoG5ApTSXU6Z0IDsfhUpX0IKF+DJZZrxZoQZhrrmGpnqDTdzfBzXo44pPLfTn6lpwrFdraR+ZGvmNDVWqZt0+XzcakSrV5WLAHVTB8DAP0NSMjJNtLsPCrIuMuLWoKg9YQn6CteN56W1uvmUezuVNrE4jMblpC9lSNGkXGUiSFn3gCZE67iuxLBptix5ZbcjXbmKfx9L7mRZMl7oq4/mWfAset22cp91mUg6EAE5ZHLSKweIaWeny1JdUn8PiaNPlWSPBZCsKNBQcW9q7ds5LQ7W5tp7oPmPePgK7ui8Ey5lvyvbH49TDm10IPbHllNibOOxD21xLtat3CQABCgxIUqDueWauvjloNLjnLTxU5R6+vz/wDDJJZ8sksjpMvsB7J4W1unaHq+o/lGlcbU+O6rLxF7V8P1NuPQ4odefmXCIFEKAB0AAHwFcfJklN3Jt/M1qKiqRWcJ4mLzXh+B4H5dgfiDSjLp9QsrkvR/kSLuIty6k6ooZvAEE/pVZRT6jXkjyvTqUvs/izeR53Dkx+62o/UUmeL0Mmhz+bF31TH7mNy3ltT7yk+vL6NS1FqNoc86WVY/VEfG42LyWiZDAyD4+79D8arscouRWWqePURjF0/3Qoq1vaSvrK/1HzFId+p1ns1Kv3Z/ZS/R/kyewyrJuAsYhAJ0/ebYeWtNbcI25Jv0/V9jF0FtjUK5QgXaTqSfU7fCr/iYSVKNBuQziL0AsTP61eMXklReEd8qKO5ckknc11oQpUjpWoqkNlqfHGLlkEFq0QxGaeahBNaY40jLLK2FXFWRbdcpo7hPwGJNt0uLurBh6GYqFw7B8qjQ8UwZt3y4Ui1d76H8wDEekmsviOP2dxmzc4/kU3FMfku2hOgMt5HT6TXNxQuLZwdVqfLzQX3JPH8cyWcoPvEDxgamjDJylXYZr8zhipdWPYW7nti4Tusk+W/61mnje5pj8WRTxqfwHMBfzKtxef8A2KnbLHLgtiyLJBTQ/wAQti8hRpE818P0rQs3qgz4/NhtY3w3CLh7R7xIHeJO0gax0GlNvcUwYlp8bV/EpvZniBN9wx/xJb1Gv0n4VeS4OfoNRuzST78msFQjtCqlAM4pLmXLaKqY0YiY00gda16eeLfuzW16eovIp7agU/FcOuGVblhW7RdXI1zpPeNzrrz612tFllr5SxZ2tr934PsomPNFadKUOvf4rvZH4txR8U64fDGAwBdvSSJ6Dn1OladDoMehxy1OqXK6L9+vYVn1Es8lixfUvODcFs4cd0S/Nzv6fhHhXI13imbVvl1H0X75NuDSwxLjr6kjiF2ybbi77gHe0blrI038aTpYZ1lj5S5/f5DMsoOD39CkwHE8UhtdqoNm4wVXPvjN7maNJiOVdbU6HSZI5Hhl7cOWu3xox4s+aLjvXsvv3+pobwlSJiQRPTTevOM6ElaaRQcH4WuHdn7QkaiI3XQyehmaV5sTBpdJ5EnKym4dxUnFM/K4SIPT7v0FGRtRtGHTam9S2+kv2jSWsQF2QDUnTTUmT86yrVPujsxUY9EQ7nDEuXxe7Rgd8um4iI8N586dHNGapGWWkUs3m2OYvg1t7guGZ8+kR5RFDbSpFsmjhPJ5juyxJyKy5Yc6EnksbAcp5mqe5Fxrl/2NZBvEKJOgpEcTm6SCMXJ0itvYz8Iit+Lw6PWfJqjp4r3iLcvE7muli0sIe6i9xj7o0WrZDEJnmoTNaI40jLLK30CmUKsbu3wCFALO2i20BZ2Pgo1PntQ2kTGMpdDT8F9gsRfGfFucOh2tWyDdPTPc1VfyrPnVHJs1QwpdeTIrWGjdY6rVWgst8Txm9eW2HObsQTm55SVEt5aCfGjIvMjtZWlyvUYvcIOIYXFaQ5OaB7gA28a5G2WO410PO6rw6c8t31/IscXwcXEVWbvKsBuXKTl66UiL2u0Oy6RZYJSfKGuKWRYw5S3PeMAanf3vkDVordK2L1EVg07jDuNeyd0lWQ8jmHkdD8/rU5YW7KeGTbg4PsX/AGdL2HUo72U6ESOlWSohq+GNWsGisWCiWMk+MRp09KvZSOGEW2kSRUoYKFWJFigBN5lCsWiMpmekazT8G55IqPW+Cs6UW2Yv2OuAYmI95GH0b9K9r/yCDlo79Gv0OH4bJLNXqjdTXhzvjF/D59HMpp3RoD+bqPDbzrRjz+Urgva9fT5fqLnDfxLp6BjrVtkK3Pd08CCNiI1B6RRpsuWGTdj6/wB/WwyxhKNSKrDtiS7otzuhQUN22JaSRqVIIGm5E+FdLNDRrHCc4026e2XC+5khLO5OKfTpa6k9LQdO8NSIIiIOxBri6jDGM2ompLfHkgYfgNrtCQqiYOsBVy8xzrOt0/Zszw0WJTckv9EwpbVjoXHLUrr9YpO3HGTvlfY1cDWcBiwtpH4TmIHjqZml2lPcor5ch3FW+KENPcHkBp4wZ1p+PPkUr2/ZFlu9Au4pDLFweZ1k1d45TfTqTsk+xn8Zii7Ty5Curg0yhH4mqNQVIjFq2xxCp5Tk1ojjozSytnKZQlsRevKgzOwUdTUgrbpFvwP2WxmMhoOGsH/MuL+1YfuWj7v5n+Bqjn6GiGD/ALHo3s97M4XBA9infPvXXOa4/wCZzrHgIA6VQ0pVwi4oA8hwPELFu1aD2xcbvZgFWV/aXCGzHUtlZYG2m9UpBuEf3rbywUgkXO+tq2CGZlKsFJ5AOInTNIqKDcOJxexEdkwlApyhAQM1glQZ7wm27SdZfzNHAWT7nFVtsbNy09s6SCqgZmsdnmMMSNYaZNUypbehDZcC4obNlGWROie7muHL00DoJ55awLNifCj+QtyihlUBG4PrNYHja6oXwypxnF8Phx2aDMRplXYeZrraLwTUalbvdj6v9DBl1mHTrauX8CLY9qknv2iPFSD8jFdDL/xjIl7E0/nwJh4tBv2ol9gcVbvCbbA+HMeY5VwtRosunltyRo6WLNDKrg7DFMqaswHmQPrSFhnJ+ym/ki0pRj1Ym3cDCVII6gz9KpKEoOpKvmCkn0HAahMsQ8bxeza0ZpP4V1P/AB610dJ4ZqdT7kePV8IzZtXixe8zM8Z4894ZFGROeup8/Dwr1vhvgsNLLzJvdL8kcbVeISzLbHhf3Jfslw1s/bMIUAhZ5k6T5RNZf+Qa7H5f4eLtt8/Ch/hmnlu8x9OxrCwGprx7aXU7hDuY8/dX1P8ASs0tQ/6UV3BeN5YZ7ajkJ318JkVeWXUQjyqTIafVo6zFJabbExIViTAGnKI3586ZkzzUEnXHZP1BKm36j73VAnMp8BM/MCiU4pXaLCrmQqMmvMttr0g8hRJQaW3kOOxTY3iSjRNT15f81MNNu5Zox6dvmRU3sQzbkn/vStkMMV0RpUYQ6IZLVpjjKyyCSa0RxGaeU5NPjjM0stnKalQluztSQO8I4fiMYYwluUmDfeRZXyO9w+C6dSKq5V0HQwN8vg9C9nfYbD4ZhduTiL42uXAIU/7dvZPPfxpbdmqMVHhGqoLBQAUAeE5aihFnIoomzkUUFmoweDGNwpLMBdw6sAZBZ7YUkKVmdDoG8aKLrlGYxV13UBmJCjQE6Vv8LnjxT27Vb79zkeJ6eU4ual07EQCNq9E4Rl1R51Sa6M5lq5FhFAWdAjUVWUVJU0SpNdAbXU0Rio9EDk31O22K6qSPIx9KrkxY8nE4p/NExySj7rokjiV+CO1eD4/rvWP+F6Pdu8tWP/G56rcyJFb1wqM1lx7NrYzntYzaZM3uz/WuH45PVRxLyen9Vdf/AA6Phywuf8zr2vobB3AEkgeJrwvLPSxi3whq9fsRAcs3UiFHgBz86tPCq9WMeCddBGK4kkQ1wQPuqNPgoolCc1XYjypvsQLnE7Y2Vj8BUfhm+oxaWT6kd+Knkg9STVlpYjFpV3Y03En/AHR6f1q600C34aAxcxrkEFjB3G1OhgiuiLKEI8pEctWmOMrLIJJrRHEZ5ZTlPjjM0spympUKcrO1NFLE4fPdudjh7bXrvNU2XxuOe6g89egNQ5JDIYpTNtwP+ztdLmPcXm3FhZFlfzTrdP5tPClttmuGKMOhu7dsKAqgAAQABAA6ADaoGCqACgAoAKAMHiv7OuzOfBYl7ZG1u8O2T0Jhx8TQRtRleIcFxuGDdvhGccr1g9qo15oAHH8tFi3ClwQluW2C5LiPqZA94HaGG48jUrkpKLj1JOIUKw7MspCyZ0MnkI8KhEyq+CKyRzB0/wCirK07RR01TKe47oxEyAefSvX4JLLjUvVHmM2GMZuItMYPvAj51dxZneF9mSEdTsQaqJlFrqLigrYRRYWEUBYRQFhloCwC1DaStlo23SNPwjCXLuW0GJgSzMdEXmSeQFeA1Mo59RKUIpL98n0HR4Pw+BKTt/vgZxLKGIRsyyQrRE9NKzONPg2J8ENjJqaYAlssGIEhQCfAE5QfHXTSp2urItALLEZgpjva7DugFhJ5gEaeNWWNsq5pDRNMjiFyyCSa0RxmaWUTT44zNLKFNSSEuVnYqStjd2+FIWCztottAWdj4KNT57UNpFoxlLoafgnsFiL8PjGNi2f8i2w7Rh0uXRonkmv71LcmzVDBGPL5PQ+GcNs4e2LVi2ttB91RHqep8TrVR5LoAKACgAoAKACgAoAKAKjjPsxg8VrfsIzcrgGW4PK4sMPjQBlcd/Z7dRs+GxJaP8rEguI6C6veHqGqO1FdquzM8UwmKsFjicI6AnW5bHa2gOuZO8vmyirWLlB9iBes2rgBt3FuSPeQgwehitul1s8Py9DBq9HHI67+pXYjBlTBFegwamGZXFnDy4smF1JEVrNaLKKYtL7rznzqNqZVwhIkW8cv3gR86q4MVLA+zJNt1bYg1XoJlFx6oXlqCtnVtzS8uaGKO6bobhw5M0tsFbJNq0Brua85rfE55U4Y+F+bPU6DwqGFqeTmX5I0OM41a+zLYtKwaF7S5oM0SSp5sJJ6VypVt2o7SfNsjYbjIt27Shc5CkOCYA7173NNGi6O94AVZSSSVB1G24wxQowaCrgsHytL3O0zAhYB+6dNRVd98UWruOPx2dDaBBiRnI2a22VSB3V/Z6DlmNNUr7Cm6OPx8mf2cyDu+km3bQkqFg/4c6R7xpi5FSyJHW4+ZJyGCdZeSRF8QTl1E3tPBAKYoCpZ0UoFMSRmcmzsVJWxF+8qDM7BR1Jip6Ak3wi24J7L4zGQwBw1g/5lxf2rD/btH3fzP8DS3P0NMNP3kejez/szhcGD2Kd8+9dc5rj/AJnOseAgDpVDSklwi4oJCgAoAKACgAoAKACgAoAKACgAoAKAKHi/sfgcQc72Qtz/AFbc27n86QT6zQBleKewGKUlrGIW8JnJiBlc+HbII+KetWjOUeUxU8EJ+8ZTi+AewT9ow93DiPeYZ7RI/wB1JUA+MV0sPimSKSnycrUeERbbx8fmQRhcwzIQy9VMj410sfiOGXV0cueizR6KxlsE34TWj8ViSvchaxZbraw/u19xHxpP8SwXXP2NK0mWuw/Yw94bsI8daXk8RwL3bZX+GuXXg13C+D2Bh/tF+5sSRaVlDOo05mRJ+QrgZ5yzT3SO7pcMMGOo/wDpXcU4mb2UBFt20nIijQTvJ3YnrSXjHedYmxw244UjL3tpaNCLhBPQEWrnwquwYpNqzv8AdF793l97aTbgHoSL1s+RquwtuZ1+E3QJOTQSe97oAuHM2mgi1c+FQsZZyY9i+BXUL5YZFJ78xoCwMjlGUz5jrTYxQme45b4HdI5ZjkyrrLZy68xKxkOhFMTSFPHJkXEYFkXMxWMxUQ0klQCdOneX41ZOxUoOPUjmrCx3hGAxGMMYS3KTBxDyLK9YO9w+C6dSKo5+g+GBy5fB6D7O+w2HwxF26TiL4/zLgEKf9u3snnqfGlt31NcYqKpGqoLBQAUAFABQAUAFABQAUAFABQAUAFABQAUAFABQBwidDQBm+K+wuBvksLZsud7lg9mSepA7rfxA0ENJqmZniPsPjrcm1dt4pYgLd/ZXB5MvcY+YWrKVCpYUzOYy8bRC4q1cw7SBLoBbjwuCUY+tWUhMsT7/AJDpS33srlh9wge9/wAVbkS9ttX8jiYUzDd0xInTyqGyYwbtPgZirUU3Fnhbt3sFVCB+1Crr3icjkiWMKIuEQN83LnRpWaIzk4cAiYxYjOMsoBKSI0gg7/4MAn/T0OlHskp5RyzhsUQWNwiAe73STAXKANmn7Tt+8fKo4LLe+4lMPi2JVnZQ5IJzKQWuLmjQ65sg1G0edHBX+Z3Ig4neJntGnQzp+IvOg3zFjPietX2oU8svUjW712+/YWEa9cBJyIAFQtALO+i2xoN+mgqG0i0YTyGy4H/Z2ulzHuLrbiwsiyv5p1unz08KW5NmqGKMDd27YUBVAAAgACAB0AG1QMFUAFABQAUAFABQAUAFABQAUAFABQAUAFABQAUAFABQAUAFABQAi7bVgVYAg7ggEH0NAGV4l/Z7grhLWg+Gc/esNlWeptGUP8tSm0VlCMuqM5xH2Q4hall7PGLEDXsro6QpORj6jyqynQmeDdbvn4lHcxoRsl8PhrgUqFuIyFz0BPdbzBNSmugqcZ8tquO3ckYPEXFVgkRq2oBiVKNE6agj4Cryir5E48kknXYf/vS+VJOpzhg+VdNbhKnSCpNxtDtOlRsVjPPnV0dGJvuSEuA6TOVU/wBPbTSOyt/y1R0uGMUpytxIl7ijoynMHuXLhZbSJLtcylA4RBJMMfDrtU8IhOcqaLvg/sLiMRD41jYtwALFsjtWHS5dXRPJdf3qq5eg2OFdZcs9B4ZwyzhrYtWLa20H3VEep5k+J1qo8l0AFABQAUAFABQAUAFABQAUAFABQAUAFABQAUAFABQAUAFABQAUAFABQAUAFADOLwtu6pS4iup3VlDA+hoAyXEP7OcI2uHa5hm6Wzmt/wDxPKgflipUmhc8UJdUZ3H+zPE8OpUImIt82snJcMdbTmD6MatGSu2hOTDNw2RfAjhPszjMUZCNhLWzPcH7V+uS0fd6S3wNDmWhgrrx8Df+z/szhcGD2Kd9veuuc1x/zOdY8BAHSqD0klSLmgkKACgAoAKACgAoAKACgAoAKACgAoAKACgD/9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUTExIVFhUWFx0aGRgYFRkXGBoaFxgXFxgeGBgYHSggGhomGxgXITEiJSkrLi4uGB8zODMtNygtLisBCgoKDg0OGxAQGy0mICUwLS0tLy4vLS8rLS0vLS0tLS8tLy0vLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIANIA8AMBEQACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAAABAIDBQEGB//EAEgQAAEDAgMFBQMIBgkDBQAAAAECAxEAIQQSMQUGQVFhEyJxgZEyobEUI0JSksHR8DNTYnKT4QcVFkNUgrLC0jSi8RckRGNz/8QAGwEBAAMBAQEBAAAAAAAAAAAAAAECAwQFBgf/xAA9EQACAQIDBAgEBgAFBAMAAAAAAQIDEQQhMRJBUWEFE3GBkaHB8CIysdEGFBVCUuEjM0OS8VOi0uIWY4L/2gAMAwEAAhEDEQA/APfuanxr0loeFLUjQgKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAKAudEA2Mzrwrx8PWliMZ1lKtGVNRa2YvNPJ3et9NcrLRZtvsqwUKWzKLUr6vQqAr121FXehyJN5I5UkBQBQBQBQBQHm9+tvO4RlCmEoU4pSrLBIyNtLdWYBBmEjjxrOrNxWR0YelGpK0tP7saOK2/h2wz2jkF+C2kJUtSpAMwgExfU2qzmla+8zVKTvZaCOF3naQz2mIfbOZ5baS227BKVEAZSnNIESYjrzqqiSu2XdGTlaK3XEtnbyPK2QcaoILwQ4qMpyShxSBYGdAONQqj6vaLyoxVfq92RZsXeR3O83iuzIbabdzsoWbO6JUiVKzzy1HCkZu7UiKlGNk4b21nyGcVvK2pttxh5ABxKGVdo27Mk95GUJzIWRoVCKlzVrp7yqotNqS3X3DDW9WEU8GEvS4VqbjIsd9BIKSopgGQYvfhU9ZG9rlXQqKO1bIQ3l2ziW8QlnD9gP/AG7jxLqVEfNnSUqEAjjVZyknZGlKnBx2pX1Sy5l+C3vw5bYU6S0p5CFQUOFCS5YAuBOUSQYkipVRWVyssPJNpZ2Edob5/wDXIbQUrwyJQpSVkLIBK8wygIAIgSe9qLVDq/NbcXjh/kb3j2C3wwimitTwlAb7SELgKdACY7t0lVpEjrUqrG2pSWHmna3G3cPO7wYZKiku94PJYIyqPzqxKU2F5HHSxvVtuPoUVKbztuv3FA3qwkuAuKBaQVqCmnUnIkwVJBRK0g8UzUdZEnqZ5Zaj2E2qy6sobXmUEIcIyqjI4JQZIi44a1ZST0KyhKKuxypKBQBQBQBQBQBQBQGma/DYTlCSlBtNb1kz7JpNWYu6nLJTodRy6ivt+icdS6VnTo4zOpB7UX/K2qf1527b+RiqMsMpTpfK8muHNe/6Ur7s8QKAKAKAKAKA8rvNsR7FYpvKottNsOjtAEKlb0IKMqpN0AyY0NjNZTg5SOmlVjCD3u68jN2HszGMO4TEKw5WRhBhXEdo2FNZHJSuc0KSUgWBm58KrGMk07brGlSpTlGUU991zKcLsHFNHCvBjOpnE4klvOgEoxFkrzFUQImNbi1QoSVnbe/Ml1YSUo31S8h3Z2wsQjYqsIW/n8jiQnMm5U6tSe9MXBB1qyg+q2d5WdWLxG3uyFP6ixmHTiUYRtSEutMqGRaEkOJKUvpQSZStSZObTkZiq7Eo3UeRbrYTcXN6N+G4qb3dxOVUMLSDtBh4BbyXFhpKe8VLKzmUDrcnlIpsS4b0yeuhx/a1pvLsPu9iQpJLWm11Yj2kfoSAAv2vdr0qdiXnch1oPf8Ast3mxtzd8YnHMrda7TDpZUFSqBnzApBAIJtPSrShtSV9DKnV2KbSedzF302JjHlPNttLWyENfJ0odS20jIR2gW2VAKVa0iANLiqVISd0tMrGtCrTjZt55348hraux8SXNqJSyVIxbSC2sLQBmQjJlIJBBJJvpbW9WlGV5cysKkLU7v5Xn4kMZu0878qSW7OYFptEqTBdaEga2hQTfSodNu/YTGtGOznpJvuZDZO7WJGKZdcSAlU4h6VJOXETicqYBvAfTcT+j8KRpy2k329+YnWg4NLsXZl9ivYuw8Sp9DmMbcjsH233HH0LSSvihOaEN5TEADQyNCYjCV7y53JnVgotQ4prL3maH9GOEUnDrdUQS4pKEqGimsOgMtkTwJSsjxq1FZX95FMXK8tlbvq8z2NbHIFAFAFAFAFAFAFAadfhZ9mcIm1bYavKhVjVjrFp+BSpBTi4veIqXYCBI41+v0cLOOJnXdSTjK1o/tWSu+1vhZdp8tOqnTUNlXWr3ldd5gFAFAFAFAXIwyjwjxrN1oo6I4apLO1u044wocPSpjVjIieHnBXaKquYBQBQHYoScoQFAFAFAFAFAQxDKVpUhaQpKgUqB0IIgg9Io1clOzujrLSUpCUpCUpAAAEAAWAAGgpoG23dkqEBQBQBQBQBQBQBQGnX4WfZgTWuHoSr1Y0o6yaXiUnNQi5PcIKRYGRfhxr9gw+Mc8ROh1cko6Ss9l5K+fFM+WnStBT2ld6reiuu8wCgCgCgGsE3Nzw0rCvO3wo7cJTTe29w7XKegFAUDCpmfdwrXrpWsc6wsNpy8izs08h6VTblxNerhpZeBV8lTM8OVaddK1jH8rDavu4F4rE6VloLYpi0gX+Nb0ajvZnHiaCa2orMzcTim2/0i0o/eUE/GunajxOFU5vc/ARXvDhRq+nyk/AVXrYcS6w9R/tOI3iwp/v0+YUPiKdbDiS8PV4DmHxzTnsOoV0SoE+gNWUk9GZyhKOqGKkoFAFAFAFAFAFAFAFAFAFAadfhii5Oy1PsivEIUbD89K+06FwdHo2cMRjHacnswjvV8nJ+8lzdl5uN6ystimstW/QoOEV09a+66+J5P5SpyJHBnmKqsQuBd4KW5kcW6wymXVpSOalRPgOPlWTrSZ0RwtNLNXPP4verDjvNNvOpmJCClE6AZlXnpFT18rFfycNq+7gXM43GuiU4BDYOnaOwfSAR5iqqrPiaPD0mrWKlbcxTJyKw7Li9ezbeKnL/ALISSB1IqJz2nctSpKnGyNJreBQAL2ExDQ5hHapHiUSofZqhoamCxzbwzNOJWBrlMweRGoPQ0AbQxaWWnHlzkbQpaoucqElRgc4BoD57s7+kV4/JnnUMhnEPqZ7NIWHmykpAUFqOV5AzpzFKRBMa2qCbH0h1wJBKiABqSYA8Sakgznsc8uzDM/8A2PEto8kxnV6AHnQCi9hvO/p8Y4R9RkBlHgTdSh4mgKlbk4IiOzUD9btFz7yR7qAWVuypm7bbGISPoONIbcjo6lOUn95PnV9u25eBk6V3m34s7hcPgn8yBh0NvJ9ppbaUuDwgXHUHlpV4Ti3aSRnVpTSvCT8TKxe5ra+/hzz7pJKDBIICxJSZB1nTSrTpQ3MzpYio8mr80vfoL4LBvpUW2sQ406kXYfvbmlV0qT1CfSojf9svEmpsr54ZcV7uPr2zisP/ANVhjl/WN3Hncj1I8KlV2smVlg01eL8TV2dtdl/9G4Cfqmyvsm/mK3jOMtDlnSnD5kO1YyOpE2FG7ZslJt2QynBniaweIW5HYsFK2bKXmSnX1rSFRS0MKtGVPU4Glcj6VO3HiV6qdr2ZxKCbAVLkkrsrGEpOyRJbKhqKiM4y0ZedGcFeSK6sZD+EdkHnrXzzwv5XFxhRoxjBp3ktct3LPm7q/d7GGrdbTe1JuXAYrunCM1sySa5mydtDJxG8eGQ0Hi6nIZyxdSspIOVOuo10qxBmJxWOxf6JPyVk/TWMzqh+ynh7uiqAQ2hh8Lg3EhbSsTiHEylbygoFWYJAVmskSZzXiKEnptm7LykOOqDj8RmiEoB+i0n6CfeeNCDC2ftN/GOrZJUy0FLOdKVJW4jN3UhZEItqRc8OJoSeoweDbaTkbQEJ5AanmTqT1N6EF9ALYjANrVnKBnGix3VjwWmDHSYoCfYykoWc6SCDIFwRBCosfQUB5fA7gstral99xlhedlhaklttUlQIhOYwSSJPjNCbnrCgEgkXGnTw5UIJUAUAUAUB57e/Y630I7FCe1SqQ4VlCkgcEkaz7qAs3OwDzDHZPADKslMKBGVUHh+1m9aAlvXgkLZKyFhxvvNrbSVOJVwgJvBMTw42iaAytytuPPuvIfNwhEJy5YgqCjl5nMJ/C1CTK3oXs3tHLutFpQS68ywtTDTijYOqSMoMkaXnUzU3VimzK975cCxWMxmDjth8oYgEOpM906HN/wAteBraNWSWeaOaphoTfw5PyNLZ29bKsQ02m6XAQVEQUrPsDzII/wAw60q1FJWQw1Bwbcj19YHWcIpexDSep2hJwClyLK9wIonYlpNWYovB8jXSsRnmjglg8vhZ1ODj6XuqHXvuJjg2v3FO22njh1oYu4oZQSqIBsozziY6xWDd3c7YqyseX3Q3XdYfzPsIUI7qswVkUNCE9ecSLdagseF23tF3NtBx9/Ji28QlOHT2riH0AOj9E2FhJa7KwGUlRXmm14JPruC2el5tl3FMNl/sUZ8yQcqsuZQANhCiqpKmqBQHZoAoDxX9Km3nsLhELYJGd0IWtMZkpCVkhKiCErJTlkgxe00JQpuRtd07RxWD7Vx7DobStC3F9qpBKWrF2JVJWvX9XbjUA+gVJAUAUAUByaAJoDtAFAFAFAFAfK9pbh4kLxjbLTS04tzMMQp7IptHah4oU3kJUM4BOU3yp5RUE3PoeDwRw+FQy384WmUtpzGAooQEjNyBi9SQeB/sNjJn5oGZsuIOtoTbyoSfRGsQUNJViFISqAFme7m4xPPWKEHn9qbzrCylnLlH0iJzeF4AoC7B71pyfOpOefoCxHPvG3rQG1s7aCHk5kE2MEEQQetAN0AUBS1iUnoeVazpSiYU8TCfJl1ZG4UAviGG5Dim0FadFFIKh4KIkVaMdp2KVJ7EXI4rGJ4TWioSvmc7xkLZEG8ZzHpV5UFuZnDGP9y8DJa3iUXi2WsqQSM9yCc5SkAxBtlm9iqOBqsaSvZmk8Q0rpGptDEp7Fw5iISdDCpiwHWbVnKEovM3hVhNXTEWNntpw/yd0JeSr2kqSCm8Ejke9JFXhRctTKriow+XNiCsMnCtZcGy21nUBCBBJNgf2j4mBV5U1FZGNOvKpP4nZLPL1N3D44lIzJgwJ8YvUdRwLLGJOzXgY286WncudxLcAjvAEqBUhREExllCZtJiJAkF1MV8zH5mcvkiaOzNoAoELS5FswIJ1tMcYipdGMs4sqsTOGU16DS8ZyFFh1vYljH+1C2czMma32Vaxybcr7V8yTbpCgSSYqsoJxaRaFVqak3c0kqm4riaadmevGSkroi46lPtKA8SB8agkzMXt9pByiVkfViPUm/lQFTW8rRN0rT1gEe4zQDitssC3aj0UfeBQDDeMbKcwWkp5zp48qnZZVzitWZmK3iQn2ElfMzlHvF6ixZGWztx0KKiQqfonQeEaUBo5m8ajIs5FpMgA301Ei4igPHbYxmGZeeaQl944dGd8oUynIm05UuKCnCmROUQJEmlxY3sNsfCrZQ+nEK7NxIUkmASCJ0ImelATZ2ihlBRh0qBJkrXBJ8hagHcHvF7KXE30KgR65YtQG2cQmJzAzyv8KvGnKWiMp1oQ1ZkoXy93lH5/lXceQi0uk6kmOvGqqKWiLyqSlqzodMzJnxo4xtawVSae1fMk48VamkacY6E1K05/MyurGRXiH0oTmWoJA4n861DaWbLxUpO0RfB7UZdMIcBPKCD5BQE1VTjLRl5UqkM2vfcWYwSEp5rT/29/wD21MluIg9XwT+3qIYvbmR0tlowFoTnKoELSCSO7qL26TImjnZ2Cp3je4853nG+QCl+dkp9ylUeckI5QfcvX0LMW9kQteuVJMeAmpk7K5SEdqSXE+dvvKWoqUZUdT+eFcDbbuz2oxUVZFmAximlhaTpqOY4g1MZOLuitSCnHZZ7LauEecU2pp3KkBWZOZSc4Um3eSJSZjvcASYkCu2Sb0PJhKKTTR0Y0tISlzvOAQSDZUWzExYqjNHCYqkqmxk9TWnh+sd1kihrays3eAynlqPxrNV3fM6JYOOz8OpstOyAUkwb8q6PhkrnDecHZZMTxbTazKxJFs2bgNeOgNjyms5Qg9UbRqVY6P1MbeN9jC4dbxbUopgBOaJWogBJPDWT0qkoQir2NadWtOSjcxtlbXHyhlh9LaxiWEvMrazp9oLIQoLUZV82oSCLwCJkDKnst2aOittxjtRZ6z5CzyMSb5rQkXOugNvGt+qgcf5irx8i9LKMikAZAQJ0so8DfUW9RV9hbOysinWS21N5if8AU5+uPSseofE6fzq4EUbKnRY9DTqHxJeMS3F2G2YUrCs+hm2tWjRs7tlJ4vai0ked2tuk+XsUvDOshGLTke7ULKkDVfZ5TlVJg94SOBGtROjeV0yaWKUYKMkbDGxOzZZabWCltvKCqxNyom3MkmolR02SYYvXbAbMXMSmfE/hVepkafm4WvmdOyl80+p/CnUSI/N0+Zo7OYLYyqIkmYHAWFb04uKszkxFRVJXSJA9OECRpMixgiDlB6SJ1Aq5itDw+1tv4pzFYxlp0sDCsOODK0hztFNICyFqXdGZMxlBIibxXNUqyUmkehQw9NwUpZ3PV7ubUOKwzTxTlU4gyLgSlRQYOoBIkX0PGt4S2opnFVhsTceBqA6CPPhb33+6rmZ1WlHoTHU8tvmpWdsfRykjxm/uj1rmr3ujuwSWy+JgYZSgtJR7WYZfGbVir3yOyVmnfQ+iPp7yOi/9ix99dz1R40Xk+z1RbUlClI+cP7if9Sv5VH7i7+Rdr9Cb7QWlSDooEHwIipaurERk4tNHz/H4BbKsqx4K4HwP3Vwyg4vM9inUjNXRQwE5k5yQmRmI1ib+6qq18y0r2y1PpVegeJqQW0k6pB8QD8aq1F6ounOOj+pH5Mj6iPsimzHgiXOpxfmddWEiLCx5QANTEiwt61LyKJNu5QBw8BEyZAzQe9cx3jzFRYvff7+ndyFNqYFvEMqacGZC03AN+8oZCk5rEqAKTwiKq0mrFoylGV1r7+m8zdl7toaf+UOPuvuJTkQt0pIbQiQrKEkQLlPQqJ4mqwpKLua1MRKpG1ve77m6J042ETMHWD3r5U3P1q0Of37y37uBepJERw14k+vGpK34nYNzYW5fGpICOR6WjWgIAkAWmLEmxjnUFtSakmDB1HlUlVzAA26dBf8ACgyAHrfW3KfhQEcpExJOok2qCSSTMHiOR48akjQhlmTHnIjgZHDXnyNQmpZonQx9o7r4Z5RW4lwFSQleV1TYcSAIS4EkZgI43npFUlTjLNm0MROCtFmjhGg02hoZUhCQCUjKkZYmAokpEA2kwDraasslYzk9p3GmnQQIIuJFwZHAjmLj1q1yjViSqhkopxuDQ6nKsSOHMHmDSUVJWZMKkoO8TwTmGW04Eq7igRCjpr7QPEda4tlxdmeupxnG6zPohFdx4pVicShtJWtQSkak9bUbSV2WjFydkVM45lagEutqUQQAFpJMQdAeH31VSi3kyzhNLNMaqxmI7bwHbNFAMKBCkzpIkX8iapUjtRsbUKnVzueGeYKF5HARBGaIJAsTHAmK42rOzPVUtqN4n0XOAJkARqbCOGtdztY8ZJ3stRA7XRmiDExm++OVY9dG9jrWGns38hpnGIVJSqYubHTzrSM4y0ZhOnOGqtciSSesgRPEd4DXh7U8dKkruIzbibcyJCzbjbMfs0J9+H28zpPM8SZv9EQox/2x5ihHv39fIIPgbDwOvnlT9rxoMvfvf5FzCePPTXTh66+ccKlFZHVrExedY0mpCW8Am5M2jShG4ZGz3FN57pBFgdTPGs3UV7G0aMtnat/Yqrug2npxJ4zVzLVnFLgDNxtbr8KBLgdKCY1EHgdfGpFzpPjblF6EEiONvGgINqJ1tyHG1QiXZGUhZBkGK+CpVZ0pbVN2fL3merKKkrMfw2JzWNlfH+dfUdH9JrEf4dTKXk/75eHLhrUNjNaF60mDHH88L16xznQj3XFyT76A6kc9fT3UB2hBj7y4NtSA4slJQR3gMxgnSCQDr5VlVimrs6cNOSlsx3kN6kPOYU/J82ZRSe6rKrLqYM+Fp50qt7F0MOkqtpHkFbL2o6AlfaFOsLcTl1Goza2+POsNmpJHZt0Kb59hqbK3NWpOZ5zIoHREK0Ig5ptxtHLwq0KW0r3KVsU4O1vE9EyBhWwjMty5gqIkC1pjT8a1curVtTnjB15N5Iqd2qonugAcjespV5XyOiOEgl8Wpn7cYadT2s5FiM9iZBhNhxIJHlUScZq+/eTTU6T2dVuPRlCXUCRKVAEcOEjTSulpSWZwKUqcstSj+qmvqn7RqnUQNfzVTiDeGQgwgcRNzJI7wEzbgeRiKmMIx0KyqzmviZ2bazbmROc/vWzGw+rVivvw+3mMt4Zasxva5I5kAc40tHnRtJ5kJNq6RUtuIA6AeUkfZAm+ulTYhO/v3qcbTPhE8dCbDz9o8RpUIluwzVjMADIABJPKhKVzc2bsiIU5c8E8B48z0rlqVr5RPQoYW3xT8B/aHs+f41lDU6KvymFjMEFEKHtD310xlbU4akLrIz1SOH3X5VsctgJvF/HhQAkG8nw6UGRW+UhJUuEpBkkm1tDUO28m9tBXYe92FDqu1CkgRkWQVDrKUiQeWvlXPUm5ZI3w8qcXeYpXwx3gDUptO6BqYR/ML6jX8a+x6Nxv5mn8XzLX79/1PNrUth5aFrjgSCVEADUnSvQMkrkMNiUOewoKjWDOv5+NE0w01qfM3t8sSpvE4pLpScPiG0BgoR2Rbc7aM6iM+eWjMEAWjkON1pXPUjhKeyk/E9rvG/mwgVEZ8hg6iRmg1vWfwHJhVar4lqXQrCQFCQ2hKr+ySlBvysQfOqVJ7NFySvZaLUtTp3xKTyuxrZzgDSU5gVBExN4EifC1Xoz2qaemWm8zxELVZLn3COx8W2y0AtxIlZAk6nKkkCscJWUqe1JNZvU6MdQarWjnktBte1sMbFxBHW/3V0OcHq0cypVY5pMr+X4T6zXp/Kq3pci1sRzEtu4lpWHX2RSe8kHKI4yJ9DVajjsPZNKCqdYtu+/U1tkGWGv/AM0+5IFaw+VHPW/zJdrGVqjxOn54VYzSFotxNuRE5zfhbMdfq1U09+H28zV2Rs4OkkqEJV3oInNlFoGhyka9KzqVFHtNaNF1M9x6DENBLcJEAR8RXNFtyuzulFRhZGFjcHMkCeYrqjPczgqU/wB0RBCIHxPEnmY41qc7dyvF4pDSStaoA9/QDiahtLNkHi9q7wOOqBQS2lJBSAYMgyCSOM3jQe+uec3IsnbNG01/SPiQjKW2lK+uQoeZSDE+EVlso6ljJ20Ran+khfZBLrAUsfSSvKD4pymPI+lTFWYeKco2aMX+3WKC1KHZ5TogplKfAghXqfSrXMuukaH9o1J7P5SAVOjtCEgJDSbdla5JMFRkyAU110qbdJzeiMqlS00nqz0SHAYIKSDxBmxEiPdS5FhLaW0WmEFbigE3gWBJkzr8TaqykorMlJt2Wp4fH7dOKOYLSUA2SlUgeMaq6mueU9omUJRyaFaqVPbTXxJ652gJsPZVA+7pxrpwmIlh6qqLv5r35lKkNuNjTfaS4kpUJSoXHMa+lq+2jOFRfC76Px0PMzizH2ficK1iFYdC1IcSAnIonKqQFgpJmT3jxBlSrGoTipbJrKM3DbehzE7pYFb3brYSVlUnvKCFKnVSJykk9LnWqLqpLbXG3fe31J66rFbFw3xX8ykc3B/pVUV5r5b5692f2NMGntN8vseTecWlRU2YJQgKH0VhKUwFdRFjw8KwbZ3KKevFjOMxoWlhbSyhxtCkn6yTmMpUOIIItoRVnLJWKRhnJSWTfoRXi0uYfs1d11LwVAMEdwgLQeUjXhoai/wW5k7L62/L1NDZW3Vn5twgOAHIqQlK7XMkwFcSPSqGpqrxZ72VSbJ7nfTdXfnja+WgFNvvgsQFAkujQg/RUeHl61on8HeZNf4qfL1IrwbasM06492aQlKTKZRZawMwkWJVHhPO2yS2E2zjm2qrilc9CygKQCVpUMsZhBSUze5mQQBPhwra1zmbaZ5zbW8Iuhg8ZLkCZiO55WzctOdYzqbkRcxtm419tRLLi0qIJOVREhIJMjQ8da55yjFXl7vkWhKafwjTe8mNQhZTiHIJGbNC7nkVgxpwijnGM1He7+RdVKji3fIyv60flR7d0ZzKocUMxPODetDPafE29hbyrbRkcSpfBszebDKSeFxfh14WVdRunuz9+BGyxTbrzqnlBwyU6AeyB0HpXPSxKr041OJacHGTiZpNalBhGCdNw04fBCj8BQnZfAi5s942DLpPINqJ9IoTsvgNsbMDHzmLAEXSxIzuHhnA9hvnNzEAV0UMPKq8tOJE5Rpq8vD3uM3FvLdWt1V1E5lHgJIA8BcACunG1YU4xorf/wA/2c9JSnJ1Ga+7+0nW0FIPdmwImDxjp0rxcRi5UrRiXqTccjI3uwrjyc/echaStAMKUgTKUkC3SAecGL4wxm3lPXjuOjBYiMZ/HlzFX8UH8YvENsqYbU02ns1RZaG20EJASO6MpAMX1tOUdCqRW86MbiaSio3u+WY2DWkakZaM4I1Iy0Z7bDskBZJ1IgfH4CvjZyTaSPb3FQe+cy/WEeYIP41fZ+C4JvYZYWlUWEzfhb3/AIVWNSOy0LM0cE6M0TbKBe0mTpz/AJ16/QlRxqyUpKzW955aW7MzmxUU4qyPNbyEN4xl1uzqnEgwZKkABKwRNhlr0q9eca82nZJdtn2ceWVyaEdqlssvxe3m1/NoUZzkzGhSdPGxPkdYNeXTcqdFU03ZPau0u79z359pd07ycmtxRvFtVt7KEGSn2rERwj416FKM51515aSSS7F7v3mlGGxFIU2d3/m8ibmSogEgAAcQbW99XxWIjh6bqPuXFnXh6LrTUESwyT2qkdmiTYykHLHESI0vpxqtTF040Ov3Wy58vehaGHnKr1W/3mRylLwHZpJEpggQZm5t1B0+iOVWjiacqPXXytf+u3cVlQmqvVb72OY8FC4gAiSFAASFCOA01HrUYXERxFNTXeuDJxFB0ZuDM17eFaVEEqkH9nnm+JmugwL/AJYpxCZJjUAxawHDoBU3ysRZXuenwaGVYAJxBhqTmuROVzOAIvqOFdULOn8R51eUo1m46/1Y8u1tRxTCWQo9kiQm0KUkKOTPHSPTjWW02rGeIym/eZRUGJubsN3WrKomAkEJJHeN5OnL3143S83sximlveefLLU7MJHNsvf2GpKCgZYUonU6cJtyiuN9IKdSNR3yS/vebKjsxceIjj9kqKGUIQcyRClEpCSTKiZmYB0kV3YXGRdWcpyST0WeVsuFtOephUovZikszQwGBab7POSst37otnkmZVBIFuHwrnr14SlO0n8Stpu736bzeFO0VdaEcW+07fKUrVZSjeAYMWNxreJqtJqnGMIydk759nIvKCbb7jax2Lw+DwodwiEKUVBAWRmUCQVSsnvaA2tqLRX0+DjDESyeRw15dRC6WZ4x/bWJdMqxDvgFFI+ymB7q9CtKnQslC9/fM4IyqVM3JlKsa/oHnTJgDtFXJ86y/O0UruH0LdXVeSk/Fl+J2f2WIDaiSLGYJJ52H7QIrzf1qVfCSnTVnmtdOHk13m6wahVSb9/8j2EYytvJKJ7U+1mAhMEi3OSfdXg1cQ6k6ctrOPm+3sS8ztlBU4TdiCQEwnTgPKkpOTbZ4zcpZsTx+JIOUcQDPiVA/AVpTjfMpPKKfb6fcz63MQqQfUDs5HX18uVfK9ZI+y6tFiMMlNwItc+E6+pqNpyyJ2Uilx5kiC4n7QrpWExKzUH4FG4cSmGP1g+0Kt+WxX8H4EfBxMjF4BIxrToCltLZUjMm+RaTnkkaApt411Utt0XReU9pOzyunl5PMtsqxmbewLDTZWlOVwqBBCyL2kxxMCPM8zPrxwjUl8V1vTRFkX7v7tAozvqKM3spkJVHMz46Vx4vpRwnsUVe2r1XdYuo3NzD7FYROV1QnXvoPxTXm18ZVrpKpBO3KXozelOpSvsO1+RIbLZCs3bKzEROZvT7NZvESdNU3TWyne3xa/7i6r1lNzTz00X2LDsNGbPnczARMo0+xULFvq+qUFst3t8Wv+4r+Yq7fWXz0vZfYre2C05BUtao0Mo+5Na08ZVwrcYwUb6pqXqylWrOrbbd7dnoK/8Ap2y6VKHbGdYWmxjqmuylj8bVV4QTXvmZWQq3ue+0rs14Z1xA0caW2CRwlC+PnXp7eInDahaL4SXqn6EZD+0NzgcOofOpJSoI7RQhKlC1gOJiuOeNxtLOrBbK1tw5ZmUsPCU1O7ujzuJDiF4dkJ7JTjaMyVQrKoqUk+ydLCvTweOnVjJ3TSk0mlusvucE+iMO3eV7vmP7q4ZGJbUp0SUrgRYRlB++uLpTpOvRkoQtmuGfcXp9E0IO8XLxPUKQ22m5CEjmQlI+4V80turLK7b72eg1CCu8kIbUeT2YUhQUCCQoEKFhwIsb/CvS6Owm3OXWLTdpmcWNr7EFsPXeQwbjSm0KWrKTY3gSJHKwtNUr4StCclCLcV77yaOJpSpxc5WbL8XhGEwXFhE6FS0pn11rkpyqy+SN+xNnVJU4/M7GPtbBNtezmOmp53tA5V7eCpdbR256u9uW76nm4zEypTtDdrzHU7Kwyu52iu+PZzC/EcNQb+VclLEY3CS66MbW5Zd+eh1yeHrLq29TxO0MGtlxTatU6HgRwI6Gv0DD16WOw6qR0finvXaveR4FSnOhUcXqvM9XsbY+FeSlxtbgUkgkZkkpUOYKeehr4npLEYzCzdGtGNno7O0l4+K3Ht4anRqxU4N/Y2f6oQdVLUeZKZ9ya8R4iW5JLhnb6nb1SEXWUAwmSLgzF/CtYyk1mc1XZeSMDaWESrMiTBiDxBsQQeYOh6V6VKbaUjxpPqKvw7uO/l2bjy7WOLiyhyzjYyqi0lKlAkdND512xiksjXG4fqoxqU84y77XSaX18AL5SqFaZVHNwgRr1qxzqjGpTbp63S2eDd/J89HrxLmFEjMRE6DkOE9aGFZRjLYjnbfxf24eO89/hN7mHFhGR0TxISBYEnRc8I8682j0TOnUUqri4rVZ/ZH2MIym9mGrE8dtaM2ZSsizCekqzCeQgEcda7qWGpKqpQila78mvU7MbQUMOrLPK9uzMV7Qcx616R4my+B3OOY9aDZfAYwO1G0pcSVj6JNxHHS9zppXPOgpVoVP4p+ftm1NNJ3ENn45p7EZ3BBRHZoURlJnU3urTu6W1MVNanOothOyerWv/HHwNDT27jQ4sJCVAoEkmIOeIykG/skXivIp4OWGvtNO+luX/PM7MM73MyK1udJo7J2gGQ4CknOmLGI1/Gt6NZU78znr0XUcc9BjaG9rIlJQ6CRPdCSL9SocuVctPAuWI6+Ftm97O/2e/NHLKDp/C2Gy9soXGRfig2PCbfeK9LFYOniI/Es9z97uRROx6ndzeJjK4lZLakrghYEnupMjKSIvVejcBWo02mr57r8FyRnUr04O0pJdpsf2gw365Pofwr0fy9X+LM/zdD+a8TF3u2lh3sOUBec50kACdDN5GlaUaFVVI/DlfO/AwxOKpOlJRmr23M8JvGtPydJjK4hYhYFyCCMubUATPlW2LoKC2opJX0Ssc/RtdylsSbbs/qjc3OwJawwzCFLJWRyBACfcAfOvhelKyq4h20WX38z2kZO+rqu1Qj6ARP8AmJIPuHl516HROzChOe+9uzLLzPOxMHVxMKb0yduOeffb+szD3dcI7VObuhJtNsxt6wP+2vV21s7RxVMO3N04vThovenaa+0HLJTFp7saER8R/wCKpKbUkkTDDxdGcpNK1r8Vnw56fWxjbUcUvNnOiQEyeAFvAcfOpbjSXwrV7t7vn3jC0XXu5NZR3u1ssn2e3qh3YLsspCjI7UJTPICR5TI8qu2lbmZdS5bTWaXnZpfR35IZxjqu0FiFBI8jKoKec2rLavNxaytn5/U0rUVGhConnd2tq38PhbPvtbJ3PVbV2S3iEgOCFDRQ1HPxHSvnsB0nWwM3Kk8nqno/75nr18NCvG09eJ5lW6uJaVnYdBI0IJQrwg2jxNfUx/EeBxMOrxNNpPitpffyPKfR1elLapS9H9iSt4MYxZ9oEcynLPgpPd91VXQfRmM+LC1Lck727U/i8yzx2Jo5VY+nmsgXttoNhci0Zk/SjjAGpGvWK8mp0Ni4VJR2G0r5rS3vdqa069OdvitcnsTCl9hpajmUpAJKSITIHd4i0gHrPOuOvKWHm4tWW6+/n37i9bDRqzdt2V16mVsbd9t3aOOSScrQQBpq4kE8Ne4fWtauLnChTktXfyOyrhIzw8aV3Zegnvruz2SmA2vN2zwSlK+6NNVHSLwTAseNa4XG9apOStZXdjPC4N0ZStK6tllmu/f9+82tl7stpIOIxTSv2EKCU/aJzR+bVhWx82rU4vtZz0+iYp5rLvbfa8l4JdpS7sDGn6DSY0KEsNnQj2kJBi+kxXpPpTCvV+TPSi5Rd45E2tj7QCSnuR1LalCRf5xQzaydbTA0FV/UsH7TNOvrfyfiDGxtoImMt/rFtenLODHlT9SwftMdfW/k/EqGwdoZs1pkn9InKSc0d32QBI7oEHL1p+o4P2h19b+T8SOK3axjhzLQiYiR2aPUIABPXXTlVl0phVo/JmUtqTu9SWI3dxixBbZAme6hhs+qEgxfTSn6rhuL8GRZgvd/HFvs8rUZSkEhkqAMkwsjONTcKBHAi1P1XC8X4MWZHDbt4xGbK213jMKDTgGsBPahUa8I9wh+q4Xi/BizKzutjM2fs25mbqRlBzSSGx3COGUiB7i/VcLxfgxZk8Ruzi1mS22DEd3skD0QAJvrrT9Vw3F+DFmTf3dxixBbZEGe6lhs+raQY6aU/VcNxfgxZkcVu1jHAAtDZ/aPZFehF3IzmJtJtAjQU/VcLxfgxZnMLuvi25ytsmY9pLC9LfTSb8zqeM0/VMLx8mTmTb3cxgzANs94kklLBidcpKSUDomI4U/VMLx8mMzR2FuYltQW8UqI0Qkd2ReVGBmPlwuTXn4rpbaTjRVue/u4E24nrq8Ukx94WmlpyrnOAcpGokcelhIruwc60L7GjyfvicmInSjOLmruLTVvfIzMNh2EMKaCDKiCSTJJ5k8LcIrqlUryqbW1la1t3h6mFLEUofFsu975PjzJrUhSkZmxlRPdEibQJM34eNW6ysllPPnbfrb3luMoVaSi4Shk7actL8SjarKHzKk5dB3TBKRwPCYtMVNGpUpQ2U753z4jr47cpOOqce5jLiWcrKUNwGjOXhorU6nvGTzg86zjOvtScpa/8ZcMvTgadfSVPZUdVblk08+Of1fEGHUBwuqQCqEhIEgAgqJNz1HhFTUlVlHZ2tcnxa937d5WNenspOGaba4Z23d3/Bp4LauY5VgCdCJjwj764quGsrxN6OM2naZp1yHccWkEEEAg6giQfEVMZOLUouzW9akNJqzPm++uz0MukM2lGbLwBk28DGnD0r9C6HxmIxWCdSp80W0n/JJJ5/S/frc8KvSpUsSoLSVrrhnu+vloZO7G0F4cJcQZJSAQdCAIAI5D8TxNefjcRQq4VUJR2pZZ6bL5diy3J8z2qPR9R4h1W9mN3kt/Fvtfa9wlhttuHEvq7QpLypVlJSDknKLHSCa4JUIqlFWvb1PRpqKlbwF9qvgrbVmBIVJvJ1GvpV6UXZqxeo0mrbjQQtJ0IPgQaxaa1N009D7CHk/WT6ivCdGotYvwZ421HiSBHOqOLWqLXJRVboHIpcBQBUgKAKAKAKAKAKAKAKgFL+LbR7biE/vKA+JropYWvV/y4Sl2Jv6FJ1IQ+Zpd5nv7y4VP96D+6lSveBFejS6A6Qqf6du1pet/I5pY/Dx/d4ZmbiN7MMT+hWs8ylH3ma9Gl+F8ZbOpFdjb9Ecs+kcO38rfchRe9jXDCJ81JHwQa64/har+6v8A9r/8kYPpGlupLy+xX/axP+Eb+0P+FaL8Lf8A3vw/9iv6jD/pL33HRvYj/CI+0P8AhUP8LPdXf+3/ANif1GH/AEl77i5retj6WFjwyK+IFYT/AAviF8lZPtTXqy8ekKG+n9P6G0byYM6oI8Wh901yS/DnSK0kn/8Ap+qRssbhH+3/ALSX9pMGLhN+jVVX4c6ReTa/3E/nsIs7eRF7fNoaNuE9cqfvNa0vwpiJZyqRS5XfoiZ9KU4u2y788jKxm+LyhDaEt9fbV5EwPdXqUfwzhKC2683JLX9q8rvzOZ9I16slClGzfe/seW2hiiQpS1EkzcmSTFcuJxjrWpUls01oll4/b1PfweAjh11lR7VR6v0X39MjLYfUGwkAhQtwvc+gHhXLKKcrnZGTUbHTs0AXuRqfGL+AIOusmnWtsnqkkNjCJnTziOfvrPbZpsItaaj8/mKq3cslYYgV+h3Z+bWDKOVLsEkKI0JHh/KqySepZN6IuOIdTbO4P8yh99YqlQqK6jF9yZpKVWm7SbXeyQ2i8NHnf4ivxqrwOFetKH+1fYdfV/k/FlidsYgf37vmsn41k+i8E/8ARh/tRZYquv3vxLU7fxI/v1e4/EVk+hsA/wDSiXWNxH835ExvJiv1x+wg/wC2s30D0c/9Lzl9yfz+I/l5L7Fid6cUP7wHxQn7gKzf4c6Pf7H/ALpfcuuksQt/ki0b3Ynmg/5PwNZv8M4B7peJb9Tr8vAkN8MRya+yr/lVH+F8Fxl4r7E/qlfgvB/c6d8cR9Vr7Kv+dVX4WwX8p+K/8Sf1WtwXg/uLPbz4pX94E/upSPeQTXXT/D3R8P2X7W/vbyMpdI4iX7rdiRjv7fUsqCnnFZSAoysoSVSAFEd1MkHXka3pxwFGexCMU+UV9bEuli6kNt3a7fQ5Fenc4DtQSFATS0SJlPgVAH+XnFRcmx3uad6edo+zy6zTMZe/fqcU1A1T4BQn438ppcWOISDqoDyJPkB98VLIROEDUlX7tgPtCT4QPGozJyLcE6EKzSk8IUkn1gEDyn31y43C/maXVttdnrxXLI7ujcd+Sr9cknlbPXuavZ88yOKxGa0C3H148qw6P6Njg1lJvt03buOWp1dLdMy6QaThGNt6zlv38M9LaizjlogDmbyfU/CPdXj9L43rZ9TF/Cteb/r6nq9DYHqqfXTXxS05L+/oDjMJBPtKggck6g+fw8RXjXPa1OvMAIbIGoPqFkT4xA8qm+RCWZJ9sdmgxc5gfIj8TUE72SfA7Nsxrmn7VAtWLVBJaDr1163m/mB6V+iH5sFAb2xVISghSDmINzxmMpHGBe/WONeJ0jSrSndZx5bu497oytRhDZeUt99/eQxOLaggwqOGtc+HwmJ2k4/DzOnE4zC7LU7S5GM6QVEgQCTA87V9BTUowSk7uyufN1JRlNuKsm3bsOtsqNwLc+HhJ1PTWrNpFUm9CKkkWIIPW1SQcoCxLYi60g8r+8gWqL8ibLiRS3eCQPE8D01PkKm5Fji0xxB8DP8AMedEGi9jAurEobUoDiAYtrB4noKyniKVN2lJJmtPD1aivGLaFyIMHUcK1TvmjJq2TM9pbqcI9gQygpddS4H8xCgUkHvCYUISABAjMo3ma8KWArbeyllx95n0EekaOxtN58PeQ+kQAOVe6lZWPAbu7naEFuFYzrCAQJOpMCqVJ9XFya0L0qbqTUE7XGMds4tic6T00PkOIvXPh8Wqztsv0OnE4N0VfaT8n4CVdZxhQBQE2miohIiVWiY9SbVSpUjTi5y0RenTlUmoR1YzitluIMZSq2qUkjwrkodI0Ksb7SXJtJnXiOja9KVtly5pNorTgHTo2rzED1NqzxvSFOnRk6ck5aKzT7+7U1wPR9SrWiqkWo6u6a7u8A2hu6ila+CQZSP31cf3R518cfa6ijjhUSomSbk1BJfiP0bXgr/WqpIWrB79E34r+KaBahiP0bX+f/VQLVi1QSTzfn8mvqP16j/CXl9z5X/4/W/mvMvZcMWCY4ykGeN5Bq8emsNL5lJe+TM5dB4qPyuL9816la0dK9GhjKFb/Lkm+G/weZ5tfBV6GdSDS46rxV0TLxiITHLKLeB1nzrexz7RFCyNDHXj5HUeVS1chOx05lkC6lGwgSok2GlyaZJDNsbRgMSkqQll0FHtBLapHHvFI0i97Vm503m2s+ZooVFkk/AXewriUpcUhSUr9lRTCVRrFoqylFuyehVxkkm1kypKiDIMGrFU7HVuqNionxM/GlkhdsjQg9Hht6ylsIU0CU2BByg2AuItYDTrXkVeiVOe0pZPvZ7FLpZwhsuOa7kZO1NpKfUCoARMAcjzPE9a7sNhY4eNo79ThxOKliJXktNBKuk5goAoAoQFCQ4dfzxoAoAoCSGidBbnoPMmwpews2XO4l2RmUsECNSDHCawjhqKTtFZ56I6JYqu2ryeStq0LvOqVqonxJPxr5vpqUVVVOKSSW7i/wCvqfTdBxk6Lqzbbbyu75L+7iruISkgGZVYJAKlHwSkEmvKhTlP5UexOpGHzMk06lQCkkEHQiqyi4uzLRkpK6NDF44rbbR9QGevAeifjUBKzDEY4qZbb+qTP+30BIoEs7nMVjitptv6kz8E+goEs7idQSFAM4bTzoC2pBBbfKvbwXTMqfwVs1x3r7/XtPBx3QkKj26Hwvhuf2+hUUnlX0FHF0a3+XJP6+Gp85Wwdei/8SDX08VkX7NxhZdQ6ACUKCo5xqOkitqkNuLi95hTqbElJbjZw+9rrScrIhMkwslZ+kE97X2cgIP6sRAMVzTw0PmqP09/2dcMTUeVNX8/f9CW09s9o32YCrudooqXmkhOUQIhMkrUQLSq0AAVySx+FoO+2nla0Vfz05Zs7F0fiq6soWV73k7eWvkZjaZrmfT0L5U34/0dS/D07Z1F4f2SLRrrodMYapk3svnp4/exx1+hcTSzilJctfD7XIV6iaaujyWmnZgB5fnpQE1JTwVPimPTWR4xUZku24l2qlWKrdYgeHBPlSyQu3kRWgDRQPhIPoQKlMNcyFSVOE1x1sfh6PzzV+Czfgjto9H4mt8kHbi8l5gFVwT6doJ/DGT8PuehDoDEP5pRXi/QtLPWoXT1HfGXl9y0vw/W3Tj5r7kS2a6qfS2Fn+63areenmcdXofF0/237Hf+/IELjgJ6ifcbHzBrvUlNXi7rkefKMoO0lZ816FKXCVGUhNrAD1JMmDfTpboi3vL1IwsnHv8Afvh23NqA1TPK9vMC59RVnmZXSKlm5tH5618JjKvW15z4vyWS8kfoGCpdVh4Q4Lzeb8yOyscvC41rFpZS9kEZSYKZNykz7WUqAmR3jIrTD1oxjsyKYmjKUtqIrsTAqSkIy95RJCReLCAJPIc6xrzU53RrQg4QtIbUIsawNzlAFAFAFAM4bTzoC2gCgCgIPm1XU5LRvxKuEXqhSqPN3ZZZaBQDGF40BdQHFJBrrw2NrYd/A8uD099hyYrA0MSv8RZ8Vr77cipTR4V9Dh+mqE1/ifC/FeK9T5vEdB14P/D+JeD8/R9xzszy+Fdb6Swq/wBReZyLovGP/Tfl9zoaNc1TprDR+W77Fb62Omn0FipfNaPff6X+pINCvOq9O1H/AJcUu3P7ep6VHoCks6km+zJerF3NTXl1sZXrfPNvlovBZHrUMFQo/wCXBLnv8XmRrmOk6jUeNAajmFUEJWdFH/x63qSL52KKgkCK0p1Z03eDafIpUpQqrZmk1zzIFoV6tHpuvBWmlLyfll5HkVugsPN3g3HzXn9yDiIGta1OnZyi1GFm997+iMqXQEIzUpTbs9LW9WL14J74UA7sb9O3+99xqSJaC2I9tX7x+JoSiuoAUAUAUAzhtPOgLaAKAKArxGlAK0AUAxheNAXUAUAUAUAUAUAm5qfGgI0B1Go8aA3EOpW2EKcKSkngVAg6acqkrazuQ+Ttfrx/DVQm74B8na/Xj+Gqgu+Bw4dr9eP4aqC74FDjDJ/+SP4S6C74EPkjP+JH8JdBd8A+SM/4kfwl0F3wLsIhltaV9vmy3gNqBPmaEO73GY4qSTzJPrUFiNAFAFAFAM4bTzoC2gCgCgK8RpQCtAFAMYXjQF1AFAFAFAFAFAJuanxoCNAdRqPGgHaAKAKAqxOnnQC1AFAFAFAFAFAFAFAf/9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxIREhISEhMWFRUXGBcZGRcYFxgYGxoaFhgYGRgeGBggHSggGxolGxUXITEiJSkrLi4wFyAzODMtNygtLisBCgoKDg0OGxAQGy8lHyYtKy8tLS8vLS01LS8tLS0tLS0vLS0tLS0tLS0tNS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAL8BCAMBEQACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAYDBQcCAQj/xABEEAACAQIDBQUDCAcIAgMAAAABAgMAEQQSIQUGMUFREyJhcYEHMpEUI0JSobHB0RYzU2JygpIkQ1SissLh8GPSFZPx/8QAGgEBAAMBAQEAAAAAAAAAAAAAAAIDBAUBBv/EADMRAAIBAgQCCAYDAQADAAAAAAABAgMRBBIhMUFRBRMiYXGBkbEUMlKh0fAjQuHBFSQz/9oADAMBAAIRAxEAPwDuNAKAUAoBQCgFAKAUAoBQCgFAKA8SzKguzBR1JAr1JvY8bS3NbLvJg144qH/7FP3GrVh6r/q/QpeJor+y9TF+luB/xMX9Ve/C1vpZ58XR+pEybbOGRgrzxKxAYBnVSQeBFzqDUFSm1dRfoTlWpxdnJLzJcUyuLqwYdQQfuqDTW5Ymnse68PRQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoCNj8fFAheWRUXqxt6DqfAVKEJTdoq5CdSMFeTsioY3f/OSuCgabl2j9xL+HM8RoSp1rdHA21qyt3bswS6QzaUo379kU/eHejaGcpJNk0Byxd0C/wC8O8fiRW6hhqFrpX8TnYjF4hOzdvAryxTTtcLJK3UBnP4mtV4QXBfYx2qVHxf3J8O62Nbhh5P5gF/1EVW8VRX9ixYOs/6mb9Dcf+wP9cf/ALVH4yj9XuT+Br/T90brb2wsTLgsK5hftobwsoGYmMaxnS9wBp5ms9GvTjWkk9Hr58TViMPUnQi2u0tH4cCntFNA1yskTdSGQ/ga3XhPk/uc21Sm+KNzs7fXHQ2tMXH1ZBnv6nvfbVFTBUZ8LeGhpp4+vDjfxLjsf2mxtZcTEYz9dO8vmV94emasFXo2S1g7nRo9KwlpNWLvgNoRTrnhkWReqm9vA9D4GufOEoO0lY6cKkZq8Xck1EmKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKA+MQNTwoChbz+0VI7x4QCRuch9wfwj6Z8eHnXSw/R7l2qmi5HKxPSUY9mnq+fAomEx74jEZsQJMSzAgAd5gT9VeFuOlrC97aV0Z01ThaFonLhVlUqXneRcNnbtYyXvTSDDggCyWMlrWIuLKoJJOl7ZuQAFYZ4ilHSKv47HRp4atLWTy+5v8HuthY7Ex9qwsM0pMh04aHQegrNLE1JcbeGhqhhaUeF/HU3CgAWAsOg0qjc0bCgKltbaOLjkxMsTxGKK3zTXZ2yopcqFFwLk8TyNaYRovLGV7v9RlnKus042yr8alp2XI7xr2ihXZQSoNwGte1/Cs80k9NTTTba1DqCLEXHQ6/ZRHjXM0e0d08HNe8QQ/Wj7h+A0PqK0QxVWHH1M1TCUZ7r0K5LufPhSz4fJOpFijgBrAggC/dOoB5HuitaxUKqtPTvRj+CnSbcLSXJkDBKokJgkfCYlb90rlBUXNmXhoDxN75L2uxtObeXtrNErhZS7DcZeFv390LPu37Q0ciLFZUa9hKt+zbxN9Vv14eVZK+AlFZqeq5cTZh+koyeWpo+fAvitfUcK5x1T7QCgFAKAUAoBQCgFAKAUAoBQCgFAKAUBhxmKSJGkkYKii5Y8AKlGLk7R3IznGKzSehx/fHfOTGExx3SDpwL+L+H7vxvy7mFwcaSzS1l7Hz2Mx0qryx0j7kXdjdKXGWc/Nw398jU9Qg5+fD7qnXxUaWm7K8Ngp1dXojqGx9iwYRcsKAdWOrN/E34cK49WtOo7yZ3KNCFJWijUb37ckiaOCEEyPrccbXsAvUk/d41ow1GMk5y2RmxeIlBqEN2VX9JsXlzZmy3tfMLXte178bC9bPhqV7W1MHxdW176GZN4sarNfOTHqykjTUDvC+guQPWo/D0WvHYmsTXT8Ny0S4/tRHIuZQyA2vwNzf7RxrGoZbxZudTOlJcUYAxswvo1yw5MTxuOfrUrIjcskTWCnyrI0bEzJiBr4HX415HYlLcxVIifCaA1+1tkQ4lcsqAkcGGjL/C3Ly4VbTqzpu8WU1aMKi7SOabybrS4S7DvxfXA1Hg45efD7q61DExqabM4uJwcqWq1RN3O3zkwZEcl3g6cWTxTw/d+FudeKwcavajpL3LcHjpUnllrH2Ov4PFJMiyRsGRhcMOY/7yrhyi4vLLc+hhNTWaOxnqJIUAoBQCgFAKAUAoBQCgFAKAUAoDHPMqKzuQqqCSToABqSTXqTbsjxtJXZzbebHw7UyrFjkiC8IZlaNS31jJwJ6C2nrXVw8J4bWUL961+xx8TUhitI1Ldz0+5i3c9nz9pnxQUxrbKqNmEniSOCfafLjKvj1a1Pf2IYfo1qV6m3udBVQAAAABoANAAOgrmPU6yVj7QGv2mB2mEPPt1/0SV5J6HsUrmDEb17PsBHisL7wY5mW1r961j7/Q/GvLT31JXhtoYdubawmJwmK+TzRSP2YLBCC1rgDNb4V52lue9l3sNsC0lv3R95rZS2MNX5iDVhUWOPgPIVke5sWxnn0VQeI+41GO5OWyNXjdorCfnCFW1yxPAfnpwo5WYUbor+D36heYoylE4K5P8AqH0R8bc6scJxipSWjKo1ISk4Rd2uBag19RqDzrwkQ8RtGAFkeSMHgVZhz5EGpKMt0iLcdmc/3p3cVQcRhSHh+kqm+TqQea/d5cOnhsTm7E9zj4vCZe3Db2Nzu/ttdmYXCCQEjEPJI/VE0VSo8dG8daorUXiKk7f1svFmmhXWFpQzf2u33I6VBMrqrqQysAQRqCDqCK5TTTszsxaaujJXh6KAUAoBQCgFAKAUAoBQCgFAKA5b7Td5s7HBxHuKfnSPpMOC+S8/HyrsYDDWXWS8jh9JYq76qPn+DVbi7tfKn7WUfMoeH12GuX+Ec/h5XYvE9Wssd39jPgcL1jzS2X3OsKbcNPKuNud9abHvtuoBqNj3MfO6eZH217qeaGu2qtpMKP8Azr/okrxvQ9irM53g9z9oRoqnBxNYcWeMk8eebx+yujHGwUUrvZbeBzJ4Co5t9nVt635+BOwuwcTBHjpZ4EhVoFUBWUi4cE6Am1ZcTXjVta+nM14TDypZs1tbbF/ca1WWHmw6V6DNGMozHj9EfjUXroSWmpgdibniakROW7zHGYmaQPGfmgt1TvBAy5xc82sdTW3DUaatOo1d7IwYutVd6dJOy3f7sR8XgVOGw6x4aRZ8xDyXuHzXyhRfy5C1udao1oyqSUppxtt7mOdCUacXGDUr7m63MnxkTmBkJQZSyMcpQObZkvy0uR8KwV6UIWlTd4s6OHrTneNVWkvubLHYLBnF4jtxH2jojKZXyRquXKSLEFnuvAdOIqfWV+riqd7a7EOrw/WydW19NzabrYVUw0aIcyEvlJFsys7FSR4qRVdeTc25b6exbh4RVNKO2vpfT7FV9puzmWVJFA7FUWJQBYJkvYW6G5t5Vt6PqJxae97+Jz+kqbUlJbJW8CX7Md5cjDBynusfmieTHivkeI8fOq8fhrrrI+ZZ0birPqpeX4Oo1yDuCgFAKAUAoBQCgFAKAUAoBQGk3v2z8kw7MusrkJEOJLtw08NT6Ac60Yaj1s7PZavwM2KrdVTut3ovE43gdkTT4hISCHc3LNr3TqXv9IWub867s60IQclsv2x85ChOpUUXu/252jAYNII0ijFkQWA/E+JOpPjXBnNzk5M+khBQiox2MrMALk2HU1EkVfG7QnInnWbIIy3Zw5AVkSPiXa17vY2sRYWrTDqrxg9b7vlf8GWarWlPa2y5pfksWFxKyIrqbhgD8RfXxrO1Z2NKd0mSMQgYIxAJGo8CNLjobE1FciTfE89q3U/GvbI8uzxKvaAowzA8VOoPmKWQuzKMMx5W86ZkMjMkeDN9bWrxz5ElDmeJ4HJva/lRSSPJRkRWBHHSpogc723t/sMVjFVA4coL5rWKxKp5G9jf4VsiqM4wzTs1+TFJ1oTnlhdS/B5xe2I0jiZGV2Rozlvxy8fKstFwdR5nZO+prrqapRcVdq2hsN0NrfKMVM5AQmJQFzXvlY35DrWir1caahCV9WZqXWyqOc45dEWXG7LgmIaWJHIFgWFzbjb7TVUKs4K0XYtnShN3krmw2dEqe6AFRdANALCwAqqo29+JbTSW2yIePwqzI8cgurix/MeIOvpVkJODTXArnBTTUuJyDaeCfDTNGSQyHRhpccVYdOR8K7lOaqQufO1KcqU7cjtO523PlmGSQ++O7IP3hz8iLH18K4GKo9VUceHA+mwlfrqalx4m8rOaRQCgFAKAUAoBQCgFAKAUBzTeXGDE45iSOywgI48ZOLH0y69MnUiurQh1dHvl7HGxE+srN8Ie5N3BwRZZMY470pKoNe7Gp4C9yASOp90VDGTSaprZb+JZgYNp1ZbvbwLbWI3mi3xmdYUMZ7xljA8b3Fqvw8Izk1LazM+JqShFOO90V99oYtlKNGDmBB0toe6efjb1q5YekndSKHi6zVnFfvmT9zJ5DJOj6BUhyqLWAOe32AV5iKcYxTXFu57has5yalwSt9y3rqhHQ3rFxN62PcOFvq2nhRy5HqhzJaoBwFV7k0rHqh6KAUB5dAdCL0ueNXNbitmLqwVT1uAT/wA1ZGV9yuUGtiEcOn1F/pFWFVwsSjgoHkAKA9V6eEj3Y/Fj9g/5qO8ie0fEjVMrKh7QtmZ41nUd6PRvFCdPgx/zGtuCqWlkfE5+PpZo51w9jV+zPa/YYoRMe5MMvhnGqH71/mq7H0s9PMt17FPRtbJVyvZ+/A7HXCPohQCgFAKAUAoBQCgFAKAibXxogglmP0EZrdSBoPU2HrU6cM81HmV1Z5IOXJHGoUZolVbGTEMAz3BzNI7XFrfRCi+psWGgJvXcbSm29o8PA+fSbgkt5cfFnUpJosJCgY5Y0CoNCeAsNAPCuNKV22zuwhlSiuBB/SvCftf8j/8ArUcyJZWYdrAY/Dn5M4JV1IJDKLrra5Fxo3G1X4erGErvYz4mlKcLLfcqx2Njgf1MnmJI7fHPXQ66jz+zOZ1Ffk/Vfksm6Wx5YO1eawZwgCg5iAmbieF+9wF+HGsmJqxnZR4G3C0Z07ynxsW3BxczzrFJ8DoQXElVAmKAUAoBQCgFAQcZg7m6+o/GrIztoyqcOKI3ycD3nUeWpqWbkiGXmz5eMcmbz0Fe2kOyiNtHHoil3IREHw/M0SseNuTNJsHHT4hnmYBIDpGpHeNj71/H/wDOFz7Ft6iSS04m1xMCyIyN7rAqfIi1WRk4u6KpRUk0zjcqPBKRezxva/RkOhHqL13U1OPcz51p0596Z+gNk40TwxTDg6K1ulxqPQ6V8zUhkm4vgfW0p54KXNEuoExQCgFAKAUAoBQCgFAU/wBqOJK4MRrxlkRLeAu/3qB61u6PjermfBM5/SUmqOVcWkaDYkPaY6BdckETOFJDFCfmwpIJFx3SOJtbU8tFSVqMnxbt/wBMtGN68Vwiv8NjvZNJLL8lUoFyCS5BvdcxOovyHSuXJ8DrxXEndrLm4LfN+0P7Vf8Awdf+8qiTNduu8kUxw5KlWUy3F73YLbU25eFTiyE1xLZUys9wpmIFeN2R7FXZshVRcKAUBUJd+CuI+S/IMWZbFwAIdY1bIXHzvu3t468K0LD9nNmVvP8ABDPraxL3e3zwuLsnaRxzF5FELSKZD2bMtwvHUKWGnCozoTjrbTmeqSZs4du4V5jhlxERmF7xCRS4tx7t73HMVB05KOa2h7dGxqB6KA+EUBpsVFkYjly8q0Rd0ZpqzMBNSIFJxGOXGTfPlkw8Z7sdmu7DS7C2n4cOtZKmJpxlaTLG1BW4mzxW1xmBikyKuQBShysC3f0C37qgW1X1qccfh1o/+6GeWZ6p/wC8zfRyBgGHAi45cavi8yTRMqG0QsWMxAYHJNCGNiF/cbU90DQk348OdjvjeVKNt0zBO0a0r7Nf4Wf2ZTk4Rom96GV4yDx45vvYj0rJj4rrcy4pM29HSfVZXwbRbqxG8UAoBQCgFAKAUAoBQHPvabd58BEBe7OxFib6pbTK3IN9E8eBrp4DswnLw/d17nJ6S7U6cfH/AJ3P2PW6MZOKxrnXL2UYPkpLCw0GoGgsK8xD/igvFnuGX8s34Iz7d2FiJp+1ilRBlCj3w1tb3I63PpWFxudFSsQ/0ex/H5WP65et/v1rzIe5yTsbYWJhnWWSVHGUqffLWtpYnpYeleqNjyUk0WWpFZMwC6E+lQmWQXElVAsFAKAr8mxpDtRMZdeyXCtCRc5s7Sh+FrZbDjf0q3rF1WTje/2I27Vyt4bcaZIcGoEIli2h8pkcE3MXaO1g2W5bKUFjYd3jpV3xEW3vZxt5kOr28THsLcTEQTxCQpJBFO86SdtIsl2zFbxZMua7WY5rEXpPERlF23atsFTaZ0ishaKAUBA2qmgbxt8aspvWxVVWlzWE1cUFaxuBT5UoZu693N9Be5OW9xa9gL351xsTSiq+r31/w8SWbUj7Vw6nsjZEdiylIyGAAawa4J43ty92qJwTa4N6WR7NFpRbADoAPhX0CVlY8KpvlDefBn6xdDoTe+WwsCCb5iLXsb66Vtwz7E15mHFL+SD8jZ+zaS0+OThfspMtsuUsGLC1zwLAelU41diD8UX9Hvt1F4Mv1c46goBQCgFAKAUAoBQCgOUe11/7TCOkV/i7flXZ6N/+b8ThdLP+SPgT/Zd+pnJ4mQfYo/Oq+kPnS7i3o19h+Jd0jJ8utc9ux0krnrtAvu6nqfwFeWvue3S2Pl1bj3T9lNUeaMxyREa8uo4VJNM8asTcH7o9arnuWw2IG9e0nwuDxOIjALxRO6hgSCVFxcAg29a9pRU5qL4nsnZFS2fv1NHNEmMfCyRyYeScvhs+aERpnPaoWbQjQW4nStEsOnFuF73trxK1Ud9TYYf2kYQrI0qywZIu3AkCEvGWCgrkdu9mZRlax7w8ag8LPhrrY9VREgb7IoVpsJi4AZYoryxqAO2vkYsHIy3FjYkqSLjWvOofBp7/AGJZhit+oFdo0imlkE7YdEjVSZZI1DS9ndh3UuAzG2vWiw8mrvRWv4cvU8zo121t7pi6BBJh0fB4yVhJCO2jeCwUhGOU21IF8raa2qcKKtrrql3ankpM9Re0BIo4kaHFYmQYSHEyPHFEO46XLsvaWQ6XKi410vR4ZtvVJXaHWWRLxPtBw4J7KHEYhVhSeRokUiKOVc6F8zA3K96wvp5VFYaXFpa21PXURY9j7QXEwQ4hAQsqK6hrXAcAi9iRfXkapnFxk4vgSTue9or823p99ew+YjU+U0tXmYrW9MTZ1e3dygX8bk2NcnpGMsylwsRZqtnLeWMfvr94rFQV6sV3o8LuTX0h6VjfYH+yleImW3PXlpcX1HUVrwv9r8jHjL9i3Mlbjqq7QxCooVTCCAFCe66qTlHDW/T8TXi23Qi3vctwdlXkltY6HXNOqKAUAoBQCgFAKAUAoDlvtWwrvi8OEUszR5Qqi5JDMdAPOux0dJRpyb5nE6Ug5VIqKu2jebh7JOEikSZlMhZWMSsCUuthnI4E2PwrNjKqqyTjtz5mnBUepi4yeu9uXiWLET6EngATYeFZdIq5rbNEN6IDyk/pH51k+Opd5DOj3PvDEhyukqnoyWPwJqTxtOOjT9A5W3Juy9qrKC0eYAGxuPC/C9W0qsKyuj2MuRu8I914W8qSVmXxd0R9ubNXFYebDuSqyoyEra4DCxtfS9ewm4SUlwPWrqxoYtwcIjMUUokkBw80aBVWVSPeYAXEl9cy2NWvEze/B3XcRyIw4X2ewCGWCWWWaOSMRgMsKlApBUhkjBLggG7XvYXBr14h5lJKz8x1atYw7e3ZxPySeBJJMc04CH5RMsYiCqcjoFjsWD5WPM2417TqxzqTWW3Lj9zyUdLEmDcWMYbBxiV458NmZcRHbP2koPbHvhgVck3BHSvHiHmk7aPh7HqhojNLuWj5e0xE8jCDEQF3ZWZhifeJOXiPogaAC1qiq7WyW6foMmh7we5sUYe0khz4SPCG+X3I1Khhp7/ePh4UlXk/W57kVrFW2/uNOto8EjZTho8O0gxfY9oI0KL8oi7I5wFt7pBIuOBq+niIvWfO+1/TUrlC+xf93tnHDYXD4ctmMUUcZbhcooBIHpWWpLNJy5lqVkSsWBkNzYdfWvI76HkrW1NNPAU46jkRwNXxkmZpRaKrhN3JEkndpAwkVgOOpY3Bfyt41VUouUZLmiU5pq1jLgdhvHIjllIBvYX6eVY6OBnCopNrQqsbwmumCt78wE/I1KmzzADkTwGnT3uNa8JJdtrgjJjIvsJ8WZfZ7h8uNnNv7hCffsS5VrjOS4FhwbXy4VDGSvRj4v8AdNPQngo2rSfcv3XU6PXMOsKAUAoBQCgFAKAUAoCle0zas2GSJocql86NJbvqO6QEbkDrfyFq34ClCpJqfDgc3pGtOlFOHHS/ErfswxXzuIUkkuqvcm5JViCSeZ+crX0hHsxaMXRs7yknxL7i/wBW/wDC33GuTP5X4HXZSNjYSUskqRdoquBxA71r2FzxF7g8L2rh0oSupJXKoJ72JW0sDM6paF7IJWLO6MxUMM1yLaKftY1OpCTS0fHclKLfA2G536uT+P8A2itvR/yS8TyGxa9nPqR61smuJfTfAnVWWlH9p2MaM4BRJiI0ecrJ8nLiRl7NjZQurG4GljWnDRTzaLbj4ldTgaXC7e2jhcO7KsjrJjYYcN8uVllKSCzZ7WYDPazMCbE6HhVrp05yt3NuxFOSX5Je1d8sfE2LCjCf2GOJpw/aAzM6B27DvdxbGwzZrm1RhQpvLv2tu7xPXJ3JeG3txeJnl7AYSKGF4FdcQzrK/bKjGxBsnv2W4bMRUXRhGKve7vt3HuZsj7O34xk2I7mHVoPlLYcoqS9ooUlTI0t+zuLZilrgc9K9lQgo6vW1/wDLb+Z4pu5gwu++0CsweGIYjsmkiwpimRjaREus5cxzqFYnuWJNgPCTw9PSz0vvp7bo8zytoWfcrbkmLSbtXQyRyZWVYZYGS6qwDxyEkNqdQbWtVFamoNW28U/Ysi7lkqkkQdrSWUDqfu/6KsprW5VVeljXQ4krpxXmp4Va4plKk0e2gDi8fqh4jy6ivMzWkj1xT1j6HlcGQLuQg8eJ8hTPy1GTjLQfKUT9Wuv1m1PoOVMrfzDOl8qKXvbiO0xeGVmHdV3uxsAWBy65WA1Qcj5Vvw8ctKTXcc7EyzVop8Lm09mUJ7XHSN9ZEvcHVc2bUKoP0dbCqcc1lhFd7/dy/o5PNUk+aRfq5x1BQCgFAKAUAoBQCgFAVL2n4PtMCzDjG6P6e4fse/pW3ATy1kuehg6Sp5qDfLU59uZnhxEMxFo3bsybi/fuF0ve2ZRra2ldPFZZwceK1ORglKFRSez09f8ATp+PkVY3LEAZWFyQNbGuJP5Wd5lK2XtqOFMpQOc+e/aFdLWtYffXFpSlBWcWQi2lsSJN4oyCOztdJFv2x/vCCDw5W4c6k6ja+V8efE9zdxO3OnXI65luW0Fxc90cBWzAJqDvzPIppFljfKQRyrc1cknZm3jcMARVDVjQncwYrAxytGzorNG2ZCRqrWtcdDYkV6pNbCwxuAimCCVFcI6uuYXs6aqw8RRSa2DRD2ju3g8RIss+GikkW1ndFY2BuBc8QDyNSjVnFWT0DSYxu7eDmmWeXDRPKtrOyKW7vu687cr8KKpNLKnoLI+HdrB9v8p+TRdve/aZFzXta9+tufGnWzy5b6CyI8O5ezkEirgoAJBZx2a6gEMBw4XUHTmB0qTrVH/ZnmVGw2RsfD4RDHh4UiUm5CKBc9T1OlQlOU3eTuepWJ1RPTRY+fOxI4DQVphGyMtSV2RSakVhWINxoaC9g7Em5Nz417YN3PNDwpGJnz4vETZiqR2S6khiIyrOFsNdRY2I0ccb2relanGNtX/39+xz271ZTvotPQuvszwpTBByLGV3kOlueUachZb+tYMdK9Wy4JI6PR8LUcz4tstdYzcKAUAoBQCgFAKAUAoCPtDCLNFJE3B1ZT5MCPxqUJOMlJcCM4KcXF8Ti+ADZJsI9w6P3TdbKykjS+o79vduTm4ca707ZlUWzX7+s+cp3tKk90/39R0TBPHjcPG8iKwYAlWF7Ot1bQ8wcwrlVaeWbidmjUzQUh+j+E/w8X9IqvKi3Mz5/wDAYT/Dxf0imVHmZ8yRhNgQoweOBFYcGCgEXFjY+Rrzso97TNgYAPecDwGtMzeyGVLdmSHFKmgBtzJ/KvHFs9U1HRGwVgRcVUXXPtAKAUAoBQCgNdtTFW7g4nifCracb6lNWdtEaSWYZlTMqlubEAADiTfp05m1K1ZQVr6v9uUJXdjT7x4hkYLHMWAPvKQL6KdcunOubia87K0uPDy5Cas7IxbOjd1VnlmHaMUTK1wCBqX8LlemlzyqqnOpJXcpa6LU9jG61IcWLlVyjSPxKmzAkEHSxa62zAX04XqzC4qcKqU3dba3K5Lh7G92jjDBA0jkFlXjawL8BYcgWrvQhnmkiupPq6bk+BzzD4syRLho1PaySAFib3LkDQi1rmwIIN7cbaV05Qyyzy2SOVGpmgqcd2/c7ns/CLDFHEvBFVR5KLfhXz05OUnJ8T6eEFCKiuBIqJIUAoBQCgFAKAUAoBQCgOXe0DA/JcYmKA+bmsHFrjMpGa48QFYeKk8q6+Dn1lJ0+K2OJjodVWVRbPczboYvspDCxGSW7oQcwDi+ZQ2Y5sygMDfqONwPMTHNHMt1v4fuhPCyyyy8Ht4/upcKwm8zYTiW+qCajLax7De5ikmY8Sakoo8cm9yOcQl7Zlv0uKllfIhmXMCZT9IfEUs+QujPh8UV903HSoyhfclGdtjYw45W46Hx/OqnBouVRMkg1AsPtAKAxyzqvvED/vSvUm9jxyS3NZi9ok6LoOvP/iro07blEqt9jDi9Ujfwyn04V7HRtEZapMqm0dmvJOSbKrEAMzAD3eZ5DQ8vvrlYuhN1XJ7aa+RWld2Iv/xcpQZVuMxIN1GhC2PHwNV/C1ZU1lXHu5LvPLGSDCzxqcspQ5vcVyDfKTmCg6jLpf0qKo1I9m9ny8iSule58h2OxdbMpUWJZSGAvY2v18OVSoYRzmmnot2eSVjV7+7UzMuHU6L3n/iI7o9Ab+o6V9dg6dlnZysdVu8i8zP7LNkdriDOw7kI08XbQfAXPqKj0jVywyLd+xPouhmqZ3svc65XEPoBQCgFAKAUAoBQCgFAKAUBqt59jrjMPJCdCdUPRx7p8uR8CauoVnSqKRRiaKrU3BnGcRtSVEWB1tJC+jEnMhQ6ADqDccxa2mlz3o0ouWdbNe585KtOMVBrVP0sdL3d2yuLhEg0YaOvRvyPEf8AFcmvRdKVvQ7OHrqrDMjdDSM/vG3oKz/2NO0SLItwQdQQRU1uQexxHCwhmVSwUEgFjwHia+hk7Js+Zis0rN2Jk+zEUE9tG1lJ0IuSCtltfibn+k1Wqrb+VlsqSS+ZGw3DjvjEOW9lc3uBl7tr+OpA/mqrGP8AiZZgVesjqBrkHcPcDNcBSQT415K27PYt3siTicawNlbQaX01PM1CMFa7JyqNOyNfJtccDMv9QFRz0VxXqQc3zMBx8X7RP6h+dS6+l9S9SNz1HMre6wbyINTjOMvldzwmwd6N16WYfcfsrx6STLFrFoiGrNyo+UB8pYGt29tRcNEXPvHRF6sfwHE1bRpZ5WWxTXqqlC5zBVeaQAXeSRvVmY/iTXY0hHuRw0pTlzbO77sbHXB4dIRYkaufrOfeP4DwAr5yvWdWbkfVYeiqNNQXn4m1qkvFAKAUAoBQCgFAKAUAoBQCgOde07dnMDjIhqB86BzA4P6DQ+FjyNdTAYm38UvL8HI6Swt11sfP8lE2Dth8JKJF1B0deTL+fQ/810q1FVI2ZyaFZ0pXR2jEPoi9ALjmCdTfx4VwI8WfSyeyImIlyKWPLyH36V7KSirsgUltz8OCAXmubgDNDclRc/Aa1uWPqNXy7GB9G0k0s259/Q3D/Wm5fSh58PjXn/kJ8l++Z7/4yn9T/fIl7I2LBhXE6vJYBrlmiy2PdJPPQ9OlQli5V45UvQnTwdOi86kWqs5qJMPcQvzbRfLmag9XYmuyrkSrCsoeKkAlykXLOQFF9e9w086+edKU5ysuL9xGDlsTNuYpSFYo6gEi7KFsp9xABxtlbXjrVtShOWy9iyVOT4Gx3X92TzH3GtXRvyy8UUlhwkwVrngQQfI10ZK6JwlZ6mT5Kre5ID4N3TXmdrdHuRPZmGXCuvFT58R8RUlNMi4SXAg43FpCjSSGyj/th1NWQg5OyKpzUFdnMNt7VfEyF20A0Vfqj8+prr0qSpxsjh16zqyuy++zHdjKBjJRqR80DyB4v6jQeFzzFc3H4m/8cfP8HX6Nwtl1svL8nRa5Z1xQCgFAKAUAoBQCgFAKAUAoBQHwi+hoDnG1NwsmNgeEf2dpAXX9nl7xH8BCkDoTbpXVp469GSl81tO849Xo+1eMofLfXuK4d7JExk86nNHI5uh4FR3UI6MFA1rV8LGVKMXukYnjJRrSmtU2XzAbSixMReIhhYgqeINuDCuZVpSg8skdalVhVV4mNsGCFBB0yEaNcFOBvmvflfmNKrp3grLlYslGMlZnsw+B4Ee6eBN/rdeHSvLE7nkwDXTiST3TY3Fjpm5jj1pGOV3RGys0Sdmw2VI+AHdF73yjQcSTwqbk3eT3IxilaK2JmOfvkWsF0A8BXkFoSqPU0O8krLGpUlTnHAkcmrHj5SjTTTtr+StmuXYCOqSGVs2WN/1Tmxkaxs1+XG/OufCMkrqTV7cCyKaWjPc27SN70rtq/GGQ+55nn9lWdv636Eu1zMIgME8aK7EHIT3WTieBU8fOoUrwrRinu13FUlZllrvET5XoMGN2yuFTO7lRyA1LHoF51KFF1HZIhOv1Su2U7Gb7DEEjE4SKWO/dF2Rx/OOfkBW6OCcNYSaZz549VNKkE16M3m7e6WCxeTEpHPHGG/VyFSr2+qfeK35nja1Zq+KrUrwbTfNcDVh8HRq2qJNLk+J0ZRYVyzsH2gFAKAUAoBQCgFAKAUAoBQCgFAKA+ML6GgOV75bhNEWmwilo+LRjVk/h+svhxHjy7OFxyl2am/M4WM6Oce3S25FLwGOkgcSRMVYdOY6EcCPA10JwjNWkcynUlTd4svuxN9IpbLPaJ/rfQPr9H108a5lXByjrHVHWo46EtJ6P7FoDAgEG4PAishtvcUB8NASZu+gf6S6N5cjUF2XYm+1G5W95w5RFSNpO9c5baWB4+d/sqjF0XVgormRSvxNOuMxwAURzgAKALDgpuo9KxrCV1pmJ2f1Ho4/H/Un59PpcfjT4Wv8AUNfqMay4ppEkkgmYqV5C9lPCvYYSqqinJ3tYi433kW5mAFzoOZP4110VFZ2zvhFHdYbSP1+gPX6Xp8a10sJKWstEYq2NjHSOrKPjsbJMxeRizH7PADkK6MIRgrROZOpKbvIu25m4TSlZsWpWPisR0Z/4/qr4cT4c+disco9mnvzOng+jnLt1duR1KOMKAqgAAWAAsABwAHSuO3d3Z3EraI9UPRQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUBUt59xYMXeSP5mY/SA7rH99eviNfOtuHxs6Wj1RgxOAhW7S0Zy7bm7+IwbWmjIHJxqh8m/A2PhXYo4inVXZfkcKthalF9peZi2btifD/AKqQgfV4qf5TpUp0YT+ZEadepT+VlnwO/vATRfzRn/afzrHPA/S/U3Q6R+tehu8NvXhH/vcp6OCv22t9tZ5YWquBqji6MuJttn7XgzXEsbKdDZ1Oh9aonSnbZl9OtC+6PeJdFYjOpHI5hqOVI3a2PZWTtciS7RhX3pYx5uo/GpqnN7JlbqQW7Rr8TvThE/vcx6KC322t9tWxw1R8CqWKpR4mjx2/PKGL1c/7R+daIYL6n6GWfSH0r1K1tHa80/6yQkfV4L/SNPWtcKUIfKjFUrzqfMzPsTd7E4s2hjJHNzog82/AXPhUauIp0vmfkSo4WrW+VaczqO7G40GEtI/z0o+kR3VP7i9fE6+VcfEY2dXRaI7uGwEKOr1ZbKxG8UAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoDzJGGBDAEHiCLg+YonbVHjSasyp7Y9nuEmu0YMDfue76odPhattLH1Yb6+P5MFbo6jPbR934KdtH2bYuO5iKTDwORvg2n+at8OkaUvm0OdU6Lqx+VpmkGxcTh5A02FlKrqRkJU6ad6xW17davdanUjaMkZ1h6lOV5wZmfGYFrZoGQ93MBf+bL3xYeYJtcaaERUK62lf98CeehLeNv3xPitgLLdeWtjKLnNrYG9gRYA30Fybmwp/P+2H/r8f+npcRgAe7FIxueGoI5d0vr4fb0rxxrtatfvkM2HT0T/fMiQbBxMrHssPMVJNiUIFr6XYgC9WuvTiu1JFSw1Wb7MWb/Z3s2xcljKUhHic7fBdP81Zp9I0o/Ldmqn0VVl8zS+5cdj+z3Bw2aQGdv3/AHfRBoR53rBVx9Wei08PydGj0bRhq9X3/gtkcYUBVAAGgAFgPIVibvqzekloj1Q9FAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAeHiVuIB8wDRNo8aT3MXyKL9mn9I/KpZ5czzJHkZUiVeAA8gBUW7nqSWx7oeigFAKAUAoBQCgFAKAUAoBQCgFAf/9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUTExMWFhUWGBoYGBgYGR0fHRgbHxobGh8eGh0bHyggGB8lHRsdITEhJSorLi4uHR8zODMsNygtLisBCgoKDg0OGxAQGzIlICYtLS01Mi4tLS0vLS0tLS0tLS8tNS0tLS0tLy8vLS0tLS0tLy0vLS8tLS0tLS0tLS0tLf/AABEIALcBEwMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAFBgMEAAIHAQj/xAA8EAACAQIEBAUDAgUCBQUBAAABAhEDIQAEEjEFQVFhBhMicYEykaFCsRRSwdHwB+EVI2Jy8RYzQ4Kyov/EABoBAAMBAQEBAAAAAAAAAAAAAAIDBAEABQb/xAAvEQACAgICAQMDAwMEAwAAAAABAgARAyESMUEEIlETYXEyobFCgZEUwdHxBSPw/9oADAMBAAIRAxEAPwCfLrI+hD3LSPiN/wAYO1aKhSEsTzn/AD7YXKeY0JLAiBaBb/bGvAmrPSV6p1SLx/X3x87mTiLWep/47Lly27HzGPKZ7QreY2hUBYk3sN46/wC+FSrxerXrebQK01HpXWDBB3LQDJO/4xPn+II1QUXuD6T2J2H2/pizS4ZojZk3ExO+1sAMrInX/U9j6KM5JgnM8Kr06i1qboHBJIUQrSb/AJnHQchmqb018+nDEDURBHyMAMvT8w7gWmTaQDiz/HoBebcuwvYiR840epYm6iM2DER7j15jOeGpEo0ob6Z9PyMU6uYCtHpQwYhZ/EXwJ4bxOmKbmk8sFaLnSGufU0aQBIxW4/4iajTWpUXUhgFlXmRPW3UTiourdCjPEVXs1NqxqM5JqgW3K/8A5UQPkn74JZDhFStNZm9DCFZjLNBINgAALDCFX8e5dqiooZZKglhYSQJ+Jx0DNeJKarpUzpAFgYAvcdYjG4sI6y9fzGnNnsFe+tATUqEJonfSWQtYMeV8DhxMaDYgzBBFx1B9sW/4g5gU7WUyCTMW/riankKYc7Cd/kG/2x2UWfb1H4MpQHl3LGQzQIB+MMOUGpQRhIz9L+HQVQf+WzabnY8j7HbF/wAO+KERvLqGFY2b+U9+xw707/Sen8zPUYjlTkm4Y8Y8P15SoQDqQa1gXty7yJHzjlq5yVuTHQ9cdf8AF1QrkqxUSSkAaombWPI9IxyjiHAaigVaq6gPSxBMf/ewveJ54b6nAztaiJ9L6/D6dCuU/sT/ABKbZtZGprEgfe2HLJfSZkaR6f7YWspwFGnUhNNgrRBENsSDykYaKFOI06ha2rmOR748rLaj8dy7PjXOmuiLH8wb/wCmzUeS4VibKQd/+4Wj4xRreGM7RLFXTc6ZLER7xA9sPGSTVpYiBG3OZ641zOad3amttABb5EgDFaPadzwMhYmnnJG8UVqLVKddFSk0qQDGk3BKjf3AxrlNF30rTpqomoJIM39I/VIvbB3N+FDUzFV6wDKSCBp3EXHKPed8BOLs5K66flIVikqL6EgxDAC0gC5xYgFA/MrwOjLrxDOVzC+W+Zf/ANpBCgCSYv8A126zilwDi/8AEsxZSsv6R0ECAT1gT84t06anJCm3afvJthr4NwahWyATLFVq0yWVt/8Amc9XUEfgjClXmD+Znq/TjTD9VRB8X5h8qiCmToYlQs2U7/bCzkKzuQ7P6VN/+t/7DF3jFbNVKzpmBpqU502gRP5nr2xXTKsvpvp6gReNh1Pth+NeK/eCHyFQMh6k9fPMOUKbWFz7c+0Y2HCi8MxKMRKIwI1CLST9OJMnmPKqIrMqsSCwME2NtidI54NZ/iFNxp1q6kqur+WTbnyPTG38Rgo7iwc4ikqSGNwPcje/2xAa5TkGAmwgW5Yaqvh6mrEmA46gb+3P354WVzNMVGWIJYyNI077jqdscrqeosOGNAy5w7iZo6rehwNSzv3nke+Lh0vek1ypOkQuoA7jkCOYHIyOeB7ZMkt9Nh0jnvEy2+2CWQyRCagxEHoREXBHfl84xq7hcDeu5UqUWDaz6SbkXJm21vbElakJiCN7TuNv98Wc3l2INRF0geq5lWP6gNOw5xNo6Yo1dFRgovI9XLSexO39ccHE7mokX8AvNzPx/fGY1bh6raWt7YzB2YWpaocTdlKmoSNJAkmJiBPyRhxySVajU0URRUBmafrbktv0jc/GBnDfAY1et28oQdNpboJ5Dvh2y+VVFCKulVEADpjyMuRT+met6b030hR/aU8jw5KbM0S7EySJJ9ugx6KWk6GICsYUdCeRPfp198XKtcKDyAFzhW43mGqoRMTIWNx0O+/PErEauejjUtct5iq1GspZbT8W5H+mGJaVHMU/TohhsN52IeL9iMCqCNVywFf/ANwLBPMxs0cibSOs4h8N02pVKuoDS5BBHYX+5J+3fBLSnj4isiclvzK5y9TL1kL0z5SgghRIk7QBsPeMHeI0aWaotRYRTcbnSI2gpc+rvGK/G+KushQzIQPSq6iTe3bbnbAevWHk0/MyxFJSCbaiIMgASIE7n4iMOTiDq9Tz/UK+iYr8Q8CNl69FgXroXHpFM6hzGojl9tjjomS8P1mUiKdMMpiQS3TeTb5xSyniNWJOl1j0rtrI9msonDnwjjeVIYLVWacBix3O0gmzXBEi1sWYqyNTHqRZnZB1FU0q2TPqhktJExf3FvzjzL58O31A2J5iIFgbczgn4546hpeXRZWZhNiCCL7gTJkbYG8Ly8KPTpJEleh5++Js9I3FdgSz0xGVeTjc94sxrZd6JEatJveIYGxF+WOe5jhefpsVVSykny9HrkdOo+QMdWalI2xXq5eBaxi0csEpfzuPHECl1FzwnkapGnMvU1KJ8pyYE81E6eu3fG/iGhorQBqWAwVSAQl7kEyYg4JZJn1hjyII/wCoQ6kdrn8Ym4rw9KrU2qUwxSSJ5T1H6vnBY8lnQ3/El9V6LFkKnLvj+/5/3gjhXGnPpVTpmxIJt3IwdybedrYEjyzpUMIm0kiYtP7YMZAKRAi3LpjfNZYbjfHLj1TbEblzcjaalLh9RtahdOm5M+3L5xeVCDBbYTJ/zYd8LtTNeXqVmiJIaYMf0I/titkMvma5IdyKZgwNyJIEgi07xjMdVVST1JRTzI7g6rxSrWzmmlUU02KqWImW2OgWm3uMNWY4XQCFKi6iZ+ozO9oFtsS5fgFCmyOFjyh6Ry2iT1OJ8opY+ZIMiwjkffDx0BIsWWm/9eh5+8RG8O1molUIp6LB2WbC1huTgXw7OPQqs1NxY6Kn1QbEgxyuSOoNtsdIzNcKArMDLQVBiO+AniihQpUHdUpaiAAGIEkkbndusY7GxU0JVkfmbI/4ih4p41rioEVmkE2up6Ejlyj3xWzWeudNiRc7mDyExA9oxRWvSYyreWf5XNmnbS26+zffGucZ0fSwuTJdjsD06jFPmJ5AyI8GpVmL6AI3aYA9++K706VAaVMknmNrciRfFyrmAsEtqOkECPTHICNjGJKQQ6taaVIB67didoONJImVNMpng6qK8siDSrJIdVnnNqgHe4HPHmepGm0MJSNaVP5riCOY/oRGJPIpNTdkBUgxfZrTIFzFuvXElAfxCNRsTTl6TEXB/UkxeSCQOuB5C9TBrqQoQ0MAWg3G/tb3xA+cWjVVa2vS31CNxeCNwb/tg9waq2gOYX0k7fUeZtc3xX44i1VCFAWU2iJjsd1mZM43s7hHHe/MPZLMU/JpooBRlkERAk7/ADfFzPcCo11BiGI+ob2mx9sJORDZMhK5HkP9Okz5bGTE7icOr8S8sEBTEzDEAxtqM8icLKkHUkKZAxqD6nhtpPpB9mgfnGYXP+M8SFi5+FUj4MXxmGU3yJReX4E6ejEN3OPc8JW3L84G8JzFapUdnACAALbcneL9hJ9sQ+KqrCmUQklrNFoU7gfF/tjwatKPRn1IU8wPMqZrjdMk05mxE8p6W3xd4fwijrDOZZohSducDmcJnDuGw2tQXKn3IP8A1DcYYOEV2y9CpUZNdRm1Ekwz7AA2MDoP23wSooP/ADGZbUUv7RkzWdopNtjcxihneKqv1Eg/pH83tgTmarVIZxpNjp5LzjucXuJUqdTLUqplZ0gNF11Dv3AxwPMn4iigQD5MpZnilrC+0b48yeeqNTJpt6gYABH27G/PGZX/AJbeVVAv9LcmvH/1Mn8jEtPhOmsKtMkGRKAwrwR9XLa04LiILASOurOpNaqVJGlYJViDuG5xhfHC6nmaaZ0AAksCdj+//jHRK9CjWBSog1RsfqHcdfcYCZjgDI4q0ahkCNB2I5g84Pzhq2vRkOfGr4zQ3B3h3LOruWIIUA+rmZ6n7xzwz8O47SO4tEyJt2MgQcKqqX0eZTNNlPqhpDD+ZSLHuu+DC5VaommwYA8jYH4w/Ghf3SdVbEADCua8SIPpUled4+2K1fjtOCyGQIBtETMb+2K78KtG+KPG8zTyeXclAajEFZO8dRyUTJPPbnhxQxquITp5oh9KAMyqFgnmWYmfadsMVOhO98c78K5gkaiZLEknqTcnDxk88VWYmSB+Yn43wnC4VyD1GeoxkqKhDPZZvLJWZW9v86YC5bxECNJcHoZB+8YNcD4m7AiooJDG42icJ/iTKLQqsvkI1PdWWzAHke464sUpk6nnZFfE25frku8DTtuRMfFpwf4ZTCBOhHMRjm9Gm1evTpB28lTLEnlYwYO3LHSqlQCCT6SIHQD+2EMiqbWR+qyM9AwVxHja1nahSMhfrIO/YYgHHKdJWpoTrAgCLe08owpeIPFVOlmKlKgw8wtNR4FjEQveLdsD+D5lq1QohBMTJPz74A8hutyn02JOPJzQh16ruId9VRiTPIEAkT1tGEvi2ZapUHm1A5XZQxhRF45ztvjMxnswM09ARR0DSxff47HqN8UKDUw/rpq+kkEXAa/VSJAxThQjuF6jKjP7PE2orP0qasTECCL95JA+MEaWbZ6WkUS0GFDekqeekm8dRiI1fWWpIiS0fU0RG9yT9sS13GqZJC9B13Pxyw7R7iKmjVTTDa1KkxbkPUDYx0xvT8winpEhh6jvpG5sPn7HFEpUIIN15gzpNza47Tz3x5lKVU6lYaad2G0Rz7x7Y1lhK0uVUklV9XYc+Ww/riMJU1Bl9LKwM7aSOnUfjEGqxNErO4b6QwG4PQxGPVzKEQW0kfqI3Np+N8DU7UPVOJrpOpRMg6RtPUdpxbPEqcM4KARz0n8g+rClWz6hNO56/wBoGBmVy1QkeWYDeq9gRvtzxvATQ9dR74AiVHDoAQkEnlJmCJ6Wxd4qXpv5kyAN9zvFxEkE37d7gjuEZCpSSZAJAnRygd+fsOWLVfiRKaFOokx6pAUdT02wsjcaNjcH5rOVEcrJsbQLRvaLYzE3lBbfxBHOBA3v07zj3GUIH048ZastNVRFAAB0qOn+HAbxBmGpoG+p3JAnr7Yl4PRqanZ2Bci3RF6L/fnibNUg1UVCZWmpUd2NyelrR3J6Y8b2+dz6VTRgrhfCmA82sxNQmQBAj3jb2wVp0ywk30/vilWeozaEDaedRjAF9hN2+PuMSvWSn6S4DHm0gf7fJwLm/EZd9mbPRk72mT37DBvh6CDTdFVIsDeMUuCZMyX1q45aYMH46Yl4rSBGl/pO/tN/xhuHGVHI9SD1Obk301jAOCUHA1KsDboLYHZmvlS+imdTJf0zpHuRYnFalwZKhldvx8YM5XhFGmhCqO5O/wB8PB5aqecx49sTFXxNlWdVcE0zI0Gbg/5ywK4P4oqavLrrDKYLQREczy/yb4ekyVJoJWSNi24Hzi3U4bSI+kY5MRo3OT1BQe6LLcH82rqVtCRqJUglpmw6QefP8hTzuVzOWquUeGm7gAyOUgjb74eVp+S8KfSeXT2+f3OB3HUFRlIMcmtuP7jAhuJ1oy1GGRd7ESuIeMOJ0iVKKbWZKJPzzg9iMDqVOvmKFerWFR6jIdwZtZQBFt7ADDbmcmRL0PVpAJYkiG6Cx5RbG+TzVWpRasoAFrfzCFj2uT9sUPnNUe4KYFslToiL/gvJZsqNVFlA5v6Z9gb/AIx0DLZdgAGKjnaThUznGM0CB6VHIgSf/wCpH4xGMlUeS1Vz7sb+w2GEGnPIR/AqAreI253iKohUV9pssCT3gz98LOU4+rOQTMkQTfaZAviLI8JLMQzEgDYk3+NsDuJrQomGpNqixUx7diR3w7CQGv4kXqwVWh57hfhtBxX10GMLU9a29YjYHkB/bDLxjPVv4ap5rIoAkwOmwJJixgdzgBwLi9NKMeoSxJgDW2wAtZbAXnCP/qL4lr16gowaVARppg/VH6nP6j22GHqvNu54zqxNw3wLwPlqjB3fzDvuAD7gYbs5wahl6U0xSokfqgD7Hr/kY5DwIhSDBB5EWIw55sro1EmQNR6nuL4w435bNw1wltky5wzhQzlZHzADMqXkQzILCSGmZ5xzw0f+mKNwctRIIgeiCB/3D1fMzhH8C8YVM/T1n01Qack7FiCtzuJAHzjrvEnr0nXRTV6ZgXOn1dzBtpkz2w76ZNbjCwXQE5f4p8DFKb1aNQqim6katIO5DDcDveOeF7hOSc6dJUqN5k6pixi6yIM7e+PoSEemwGxU3tsSV5WO2OC8OyhSqoRzpvLLFwAVDCfjBkECcnuMmz+RZZFMgi+49QvyAnX/ALHFQJACl5ItJEWvIg7b/GCebyrtswYWiQQRyvyP2GBC1ndirTABBsDPzvgbJEYVAmFdLWVbm4UCeluZ52ONfN8pSzIoSTzuPeN8RoSIDTq21QSAPeLdb4mUvBUAHn7xeTPScEIJMiqVKCMrHUC+xCmCYmYAkf74hqZ5V1ammDtNiBf4ti3UrU0ADWZhIM7W5nacVM1lqbaWMkkG7bA8ot0GNEwxn/jQaYmPqEEHeeR+D+2L3AvDTZlw5laUmbQWIN9M7gndtumL3g7watVFq11hQBoTqv8A1djvH/jHScvTVRCiOWEs/hZSq6tpTyvCFRFRQFVRAA5YzBgAYzC/pib9Vpy+vw3zGEmy3I/zniwtOTpUbbdB/fF6nkncfyjcTznHmU4YQSC5nfHlMrN+J6i51SwT7v8AMjyvpc60mNmn+mJ8wiVCIpz7/wBcWFyonf7iZ/bHueqhKc/BgbThq4zXxJ2zLd7Jk/DssEUAADfbFLPjW6oQbmLexPxti/lDCD2GNQrSaigG0ATigj214kvM8y0s8PydLLUlQQFH7kk/knE1fS0GSe0/0wv8b4Y1ekr+YRXpy9IgkKrcpHMcp9/bC4niHM11WjWpoj/qenqQgg3iGIP+Wxq0BcRkPmMmYDVXJQldEjcwfgbnlfa+NMrw7MIjM9YurmVDOFKruACSC3K+NaFTaCVUr9zN+c85+d8IfijIP5q1g0VQwGqmTvyFjP06fT/fEyNzdgxq5PjylcmqP5jDnKVSSWqVDBkSxEGZi2JuKZipCNTAYavWs30xuvdTBI6TipxDjDU0p+akMem+nq3S/LElCsHAKgGIIP8AUYWSykEi572DIuVPboy7kcwKmTrmkJJNQRESwUC826X2wvjiAoUqeWJkoqlzykiYB5x/4wWrwmUryqgw5Ggbzzjmx588IHE8x5mZqAMVhvpjoBFwOmK8ajIK8RJyHExbzcP/AMVrE3JtDbd4v2wwZGuCowl5DI1BdahJ6H+g5b4v5fNlDpJjtjWFaELCbuz3GUZnS4jn/gwJzwV6gEDp6ptcYp5jPTYXOC1POKlKo9SEOkMTvsLna14OMVfmB6lhxlnK8OVYMYVPHeS1gBEl1uAo6404JxgVX1K1ZQHCmWlXBO8H6T1A64deK8H0rrBhN2uZbmADy5/fDkxsr38TyzlBFCckyOeCNpqrpOxn/LYM0c2MwWCEqgA1sNvnBPinAqNVmdi2tiNVxbla34wN4dk1oO8Qy2EEwZvuNjy3xZYImKCO4G4jk6urSptPpMQIiZnHUvBn+ombWmKWYVKnliBVvqEDdhs1ucj84R+IO7IpCBoMkqQQPidudumPMmMxRDKjqwYzHNf72i2NJNTqFx88S/6qBhUopQNMERrJGpgf5QkgD5m+wwocMTN1P+ZSoVWElQoBiOR1Gw/2w4eFPByg/wARmgGZoIpxN+ReefbYfs/0EmwgDCWy2dSnH6cgWdRB4R4Kq1NLZl9Fv/bQyfljIH598NWT8E5RQf8AlAzuWLMT9zhjoUlAxlXNKPfA78mHrpRFqp4LypgeUABtBYfscDq/+m1Bn1LVrLH6QykflST98N9OtquSIxaBAEnfHC/mc4+ROeZj/TbfRmCOgamDF5sdQj3xJwXwEtNg1dxVYGQIhR3IvqP4x0CcVq7Y4k/MxQL6nuWy0WPxiYLjWm0DGlSuBucCAAJp5EyfHmKP8bjMbc36Zihw7jprorgRIB327fGLVXMx6tQB7nfCH4PyVV6UMHXSzLAkbG8x3thvyPDkpEkjeLtuT84jyUGIjVQEWJboZjmZJPNRYD3NsWauYWopRNRa36SIBPXbbFDMmo/pRSBzm0/2H74K8Cp2vuSSduVotjkYHUF0ZRyMnqjQknkMBaecq+WpBUlhMAm3v+2D3FF9MdTGFLNZk03NJVZiYiDcGbR8nbDCB1EWauHOH1G0Q9mG+AnFqxpVdS09QOxAmCesfvi7lKVRCFexY33JPzg1R8tCzVI0hCSTyA3ONCWeJicm13OfcU4jpILBjzlhA9lG/wAnG/Bq4r1DAKGC+lv5x6QQedjB9h0xZ4tn6HmM+hjSIsReOthcDnifhFFGOundYibgmYNpv0vhJxp4m/6QKl+YN4wgZvXJYjbmI3HYf3xQ4YVo1ArvBqHSi997f5zwT8V8YXLoj6fMqNZFLRIiSSegsPkYWvBaPWr1M1XgimsL0BN7DlC//qcMTEWUk9R2FhhIH9Ucq9daZVWYS+w64HZ/hKyzoAGIiCLTPWJwFzPGUNUmvQ81BA9J9SA3259eX7YZcvxbI6fRXKxsKsiO0sLfnGNidNrKl9QmT25IAzGf8gaY9fO3P+2IclmBUJGaQLN1ZeXv0wZz1Si9yFJiQbTHY9MEuE+H1fS9QTPqVTyBtf7TGFg/bcDLgy87UioMynBtTr5Ssyi5YD0x0JO2KfiPKVKTFWRiGB0tuoXuBz2x1DJ5WAAAABsBtilx7gdPMUmB9LxZxYjnB6r2xRj3+qC+Orruc0pImWyfmlQXqXH3tHxfBGvxFnoUlJLU90PQx6Q0dAfxgf40pENTpD0hEgA7WgD8Tihk8xopCmpLzEhhz3gDpffDgpPukooGjJHzzltMLEG88/a2NsmlQfQoJJubbA8gJ364r1OHAlaihvSpkeqBzkmekfbFmlTKiQsRuQfkWiPzh0ETfOgEyyg7dj7W3v1w4+H/AAogKuQCv1AdTaL81AHz7YW/DedUVkapTVoLGInlY8tsdKy3iOiyyCJ98KZv6SalWHFy9wFwpl8sRdox7UrKkmYGAHEPFdFFJLqANySMKPGfEdTMUpouEUyQSCSygEki/Y/GMAH9MewrbmNfHvFaUl+sL3J/bv2wr0/FGphdmLG0A7dBIge+FTL8F87Q2YFR6pb1MPUqgbmdgCAdufK2D+WJoMgRAy/pDRPuTNxccueNKjqKTN9tR6yOeIjXCdEmT8n+gwS/4gSQZ/z+mOc1PENQA66YgTdWBgcuh9rYt8N8QKRIYH5/fAgERhdWnQFzc7nGj5oYVk4uD1xay+bm5O/LcnHEzgtw/VzHpxBSqFrg7dcVUyFSrGolFmTO8Ys1aCUwQPzgZuhqTGuf5h+MZgM1ZemPMHBlSpxSkG0msJHQMfyQB+cWhwvMN610kRKlrj3AFtucnCrxLgAdxUFWoum4VIueUkgzvtho4dnK+VUACU3KHYGL6el/7xiBFx9mUZXyr1PMpk8zLfxC03vazbdwTG/QYvcPc0yZRUSAFCjnJmwHt+cb0PEtHMALJpVDFm2a+ysLGduR7Y1HFGLGmKYBG09BFzym+2DKoptYl/rH25BX5ll6oqkaTZbzGB5y6jMyQJ0g/nF+lQbX6j6SDYWv8fOPc5lhFi3vJxpJ+IilGrg3MZ5HJdWkUagRh0JAkjk0ar+xxnivIDMZfSCJkEHpe/4wucOy+foO5CJVo1H1NoILbR6QxEHaRHLEPGvFdahpAy/lMxgGoDLTYCmJAEblrxHfDgpuRkse4HreFMzRYstSmVMyNRWw7E3J5fM4zN8aejl6dGkYJmXKtZegJ6THtg5wbKVcwoqspLkAa36C0gC7djz64G8X4ZTq1lpmpUqsGBI9ITe8ACSIsb9usZzXlvqMT6lcRBZ4nTrVMtSeG00jTZjcagLG+8leWMz9dEppl6AJRWJqED6pvftMC/TBvxJ4Xp5amtYPDk2RafK5JUA2Ci8x++FWoxZoIYyFuVA9MWFjz+98VKg1XUxnJu5sKokKF0zc6jYfPYftg7R4PSqUwkjWNMNa4awmd7T9h8iFYLyJIUCRYk77SRud7TihnOI1qdRChJJJLWNyIPLf6uVt++NKcupqvx7jDw3hgGZGXuyUoe9gOgF7iCPx0x0tEgA8hb+2OV+CuL+Zm6hcnWVWZtsTyx1GlmwRFiNiMRZBWSjL8bcsYYf/AHiXDmQAb7fjlinUzIIgHlgfqSjZJ0yTBMxJvc7jA3OZwICwaI5Hn84B3s0IzGmrM947SyzgGshciQCrFWufkNHcdcLPEKSggo40kgX+sE9R+r3H2G2B/G+NEsI5D9+3O374jVyVR1B1c53BttijBzH4k3qRj8dwtxJGywlx9U2mx7NzmBiBayEKKaQzGbuQoFjdZjYdsbDOZhrfVcGCqsREGQSpIO+I6FMqYZXQFri3wL7bjnyjD/zJRN+HZgjMUjZiag1CIMG1pAmBv846K3AstVUzSUE8wIOErwjkUOa82QwUMUHO4CyeliRh44I92Rjdf25fe2FZP1Sz0/6SZzbM8KoLVaUUuC0SCZg9CIU85i9x3xIuQCLBAiwtCwAZEBT15d8FfF2UCZkMgnzASbkQZF7QIJi5wDRg3qOloaWlmAGkQBBEbgzbY+0sBsSZxxYiXhBbQbk85K3B6qbR8T0vGPdAuhHP6RcC0kSRO3SNyMQVqyjUwQaTsRBLbzCzq2H7XjA5M4ml2VX0qNTzBOqecwV/2OxEY6oNwlVyyFGgtJJCjcAyBtcj3PUi1o0TJUgwOj1fUSCRt3B9V+t+2B+TzDkhgAFB3YyRuIiLEmw9+84L0adMgPrUsG9KgG0bSoAncze18cdTgblvhyIa6odSqQDcmLxB3MdMdIyeWp0hCJB66bn53xyYVGLt6QFYXudyLQdO1+fMnkMH+FcbNEupdmEDqb8/cmxOAYVKMeS9GP1bNADADO5ksb7YC5zxANMkkKR9Ujn898LPFOLVq8qgamoMfTvP6psD8fnAC2MczIq33GWtxnLBiDUuN4k/tjMIr5cMSXoVWbYlVJBi0ggxyxmGfTEn+u06H/G0aLEVaygwYtJU8jA3+cXqvGRWyz1EQgaTpJEE94BthFr8KdGAdWZywUWtJtf746LkODinSFNjq1rz5m84k4BRQMMZnZw+Qa+Ip0s8hUqFiRef2xZ8P+IQa6ZatJLHTTqTcWJ0v1ECx/ffE/EPCFYIzoykgiF/6SYueo9sD6/CUy8f/Lmj9CqCdHcgbfNzgbYaaep6j1Xp82I8e/4M6DXaGUWIv7i35xRzWYgkz6YP364p8JyObVQKxNQkAhogrbYxZh+ffGmfy1W0xE35W/reMEVa5444/Mp5XxDlxCh4IMEtKgcrk9MFM1VpVKUMqOhgwwDD3vb5wq8a4OKgLIBJ+ocniLHoe/8AgEnNVHZaSjyyTDQbgDe34wdAgFYG7po5cVBq0/Ko1NJJ9UdP5TGwPbpizwXg1PL0vSPU31MYk/PIdALYUOBcZrDU0KyyxUGxgbXHWJm++NuG+PVzTL5tMUQt19WobC5MCPt1vjQrG/tCZhr7zfivhDNVMzUzAripq+lWlSgkQBcgiOVtyd8As5Rr0j60K6YBGmwvqERZryd7/jHTctmwRIIIPMG3xgN44qocuVddbEgJ1B5kdLfvhyZSTRiildTnmYqkj6SB/MT0mYHU3++NKeYLLUOvTqXpbVawi87/AGxVz6+kRpMi45i5EW27jF7IKyFYIixIBuBa8HfFHiLvcBcNLUmDCS4M2H1A/wCftjo+S45TOW841kDatJplhr6TG8d8Kw0sxkCINgIi1jO4uJ+9sW+B+Dkzms+YaarBuNTNqmekXGE5URttH4XdNJuW854qpm2sT0mfxhd4t4gqRCqbwAx2+2/3jE2c4GuVzD0wAQrQCY1FbEExbngiMmjjSYYHfsdwfe2BXHjXfca2bK1gagng2SeolVnuw9fIAAXsOXO2CGXowIZj1kQInacH/CFMGtUTc21WtefvYYUBknNMKWcEO6VBBJhCRFhIBGCQklhF5aCqfMLrmRAdamlwfSpvNo9RXlz/AKYmzDs7amjURpENIIvcKT357YqL5gQ01ZVRjG11Ecpvy7n5xD/AE+pxZD6SRe56m0n/AC5wdRVxn8FkmoWF5EExECbjpM/NsEfEGcqZc6mMkk6GAItc6G5E26z/AF9yCrQyisDqYDWTzYm5+f7YXPEHi2lXpimgdnZl3UgLfeWEWE254TXJupaD9PHs7ld+N5p/MepTE7AI8+kdesmbgg4qrUqVNKpUDg3ckQsaiNmJb1XETsDsMeNl6lhTqm5BYaWHRRcqCBa8X9hj18s2pm1RJKnVbUTsIA9V7/e9sOAAkZJOzLxy9Km1JlKU6qatOkyo3E6F7ETO8e+IncwvqIXWD6mMmYEmQINp5na+I8nkkXSoqpqY/SxBLEA2GkRYE6RIvtzxJUpFnVWDtDXqCwHPTBJm9rX/AGGTpecDWNDFg6zJExMfQbBY7XNpO+Iq2WKi7QLCGknnEnrfci5vyjGCoEbY7RGwHqgR1ncnv95s3mwaRfVPl7KJnqTb4HMWnAi4eqg/N8T0aQxApgtIvJNrGBLb7ATy23kyatpZgiqWaQu5vsTcxyuJuD3xn8SigMwQmADr079J0iTbqIMW3xZ8tGIYIVAIMXuRyMWgi1iDaMaepy9x18N+DqqMtZ2R2aCdaklR0W9jHMzhxqZIRaxxmWzS6FCi2kQOgjEhJPPAUIws1/EoeX1xmLRTqMe4GoznFrMUAKuipSYOIK1ACUcAcyLBh3jtgmvqokiQySw525j7f0wazKAj3GAWSzQEGbEx87HC8yBD9pImTmK8zXhWWNZQ4lpuNZgR/NpG46TGJszkTTECtQpgySQAsnn+qfmcAuN1SKzjUdIvBJ0zY3H6sJfiTxLSphQKZqFpMyoFjzgHSPjrgcaj9IH7xLZjypZf8T51awNCk7MoYsz6mhm5adRnSDjnnHsxmKJWqtaqq1FBKh2A1A6XEA9b/OGKl4lyrylRWpn+YHUu/wD0gft8nF7/AIUrUmY1Ayqwq02MHSGUKwMctmH+2Hq3E7EwkaBuz/iZ4Y8Rl/LpVFKtoEsf1dDHIxv3GGDMcNBqGuBcIVI67QfcRH/jCdn6YEFTc2kdMNPhLjfmA0qkLUWwJP1jr/3dR89cKcf1CVAEaO5FlKWmmSBsjGAJP02A6ntgd4a8HfTUrgpa9MH6v+7oO0/2w2FqdNyqmWYzpFyPtyxV4zxM0EDMjeowoiNRgn9UWgTOMxsy2B5hOoOzCOb8qnT1GEVRytA+Mcwz/iapUqu1NQdMLTVwWaJ3Ancx06YOUeH5riTI1QstAmfQRpA+bueUxAxIfCa0swXQtTpCYBaX6WI2BF5NxOKEAUEtEliTSxfrIldtZMAKDpgXb6jOkxcEge3zi5l8qTZiAyr+oTHpmCOZi2M4zk6RYaAEAJUm94ja/fEmS8trLIOw2A6CSOv+dmA6neZGvDNaEawGM/SNj7f74I+FK3k5xU1DQ9MoINrXm/cfnFepTOn6jLAkMu+8HfciRtO+IPCuVqDNUzUcNAbkQZKn7ffA5NqY3FpxD3jTh5YiskSBpcRMjkRfe8fbC5SqKikm0gAGd2/od7YaOI16wrFFp6qekHVNgbypnfA6rwtiwIYJzIsRFxfrf354nxFq4sP7yjKq8uSn+0i8LVn/AIpiRCsvTnb+g2xSz7OMzXKyoNRwpjSBLGT3uMXKdGpS1NSGp4MEwAOUwDftbnJwH4bUrXDoJEC8yfffp0w5RstEt0F/MmBVY/UTuSSZJksQe/3++PTmAFFKT6hYMfbpyFtsbP5rMPUoVrTIhZte0WxWem1EOdRLSTJkkmIn29sOUxDD/EYeD8Pq1aTEuwW5BgR+Y/yL4X+GUGYuFbTBKHUsFiPURc6VgEGSRvzxe4T4mamCggjeftNukzgp4a4jpaodIAZ9RG/6QD+BhJtSZUoXIo31AVRjTMMpWAdZ9MLEi0NzEjUDz7WgbibEgUlD29ZvCry53tzO+L/H8pTNdFDELVdQoVRaYEGeQmR79sFOLeChSpGplmYtuVMSR8CI5xHXnjQy6MWcT2QINpZn9QRJFvV/9YU2iAIPqMjqcXmqlYJ9K1IbVKwZYzAudM/zRMjmTgAten5jOKRTzGJYSGUC8gEm558ueLWXpUyGNVxJt6yRCqTpA1XYgk7x2wVRdz2vX1gyQF5wdKm4uWj6vVAPL07zgcHqKqFEVkLSCv6o3m0gkLzsb9bWFpo9I+YqUlRgYUxrjUBq/m3mf7Yyo1N2GhDCaoBiJGlSY2sYuL7xgoPcIZ1su5Q1QAjghiRcC+8G3qAE4s+GuBtXqaVLrSUAEG1hux5y0QAeRPbA/h2WpswqMCVSCRpI1PAIMbkKIjUOY3Iw6eDs1UOYYKpNPZjHpHpBmeZm33wtuqjsfdx5ydEKAJNhHU/74tqeWxxXANxf4xbpiRgUE3IfM0g48xuW7E/b++MwVQYmHilemZeqn/ab8up/fFIZqpULeWJJMk8gff8AtfEFKhRqU3ZqupwpPtA3C/8AnEvB89oZQSGDATANrd4g/jHnNkFAGB/pMnHkxr7CLni2kfSoqE6gdY2gz03A998JVfKEHHRP9Rlg03X9Uj7R/fHP8zUbc4swA1PLaw5+JFRyBdgirLloA/35RvhjydRUHloZRBAcn/3D+sqOSgkAdoxWpUhl6TPUs7r6p3VDsg/6m3botrScAstxBmLybWCjYDew2m8H3jDyvMRiry0Y7cOcVElaMkMQF1TqI7acO/BeD/8AL8yulOkQJPqkAdSSAB/l8LvhrjXDspllcVQ9SPUBdy25EH6b/HfCp4l8S1uIulJiadBnCrSB3JMS5/UecbD84QMNkkz03zWAFFf7mdGqcdSQMqVqW+sA6Pgz6/iB3wl598wuYNbOHzE9IU6ZgE3CKPpMCOt+c4l/01qVKS1MpW9DSfKJ5xOpQdj1AmYnDTxrK1WoOKUamUjT/MAQSu3OMcBwar0Zn6lvzJv+IaaaFWUqyyNMWEwBA22P2wscQr1cwreSRAfSSxIB6wefSRzBGB9RP4agtEKVqOSWhTqBMk23mMVaeeNOgtJEJqiwpwZAA+sg3jqeuOx4t/YTC1Sl4iL+QiIPUlTlEGzA2/M4h8O1HDGmLtzibYK0uF1XVFqjSZLt+o3YkQRvY3OLg4GimzVbiJ2jlNhvEYqNVUWAS1ytx/iKhbKitpJMNccoiAF5RN++PeDALTWuzlisEqBJA7sNyLmJwN/4FW1Fax1L9QjYDvJsRa19+eN89NFECOSSQg3jtEbDGV4m2e44CujoriSH2i8HvAxqpKDeT1H49rYC8OzzQS6GoTFgYFwIAvg3TuBMbXAM8p5YxhCU/MzL1SNiPVy6YHcXym7qSHIBhd726X298X8zWCsAo1bCca57NBmVLk7ixBgSbdNsZU26ilTZXBpwdCiCXJ0xzjVdvv16Y2zdEVgVUkjSBqG1iNunLDHl1R3d/SWEKATZiRJJHMwfyPgG2fioabUxFypAtYwTa0m3cfGNBgmUMtwwgyWXawNiwsOQggdLTgrw8ikTqa7H6TyA77cxinw3iIbMEWspsfcRP2/bF+pQAUkrJYwwI5g9/wDLY5hejOQ8TYmcXdWqUSBdaiX7ah/bD1k6uoR2GOd031Aq0diD9r4Y/DvFWYQYlTBwhh4noYnBgTxVlBTr2Uw3rAVZtIkGJ3aY2ibc8BMzRWFR4hTOrVznUYB+kEHl7YdfFvDnrAPT+pVgTzk37ffCRwTw5WrvB/5K6tJeoNztCj9Zn4vvyw5WFbkmXEeWh3CFDOUmAXUtQQxAaIVQdzc9vsNxYTPWYkgoCCRcmZgWgH6T29/h24N/p7lqSjVrqGdRJbnM20xHsPmcEa/g2iZgsJ/6p6jnMbnbrzwJceJowt5iVwbg9TNGuyv6VKgqRuYuZM/YR/Z34RnKdJfKoISF+onkWvJPM4JcD8OUcsrLSDKHMtLFrx1OCK8OAWFAAHKN5/znhTBidSlGxqtETagxNzt0xMlXvbEFGlFtu2I87mAiXOCBiiATMqZwycZjmfEv9RMvTquku2kxKiRPY9tse4Pg3xM+pjEqZgrTuSRG4I29+nzhj4MQ7Kw+cUa+SJUgmWkr6QvI6pO9tM2ImQekHXhtV0N9gsgyIK79thNwItjzz6b+8PPkOTqWv9RXUZdGNir9Oxt2wmcMy600GazEAG9Gmd26OR06Dmb7C7LxZFrhKlUa1Vj5dMk6ajRYv1T2udtpxy6txmpWzWquSQWIZRuBsdug5doxdhQ1Rnjti90s8b4m1UljJ3hRfvfqepxtwmrSddBcIVk7GWO/TkYHtgvwzgPk13QSykBl7g3gfj3wwV/CJcaiihgPSRZh/f8AGHHKo1HJiIio9AkguDpkqZiZIBAEdNzyv7YtVOD0wy1/MMpDhRa49VulxipT4dmqhaitJ3aSC7kgDaSZEA/Mxh/ynAlo5d9cMz02Ejn6ZjTsACLD5xztWptgbgzxFXSsaTZaoGaoVJ0t9EX1nmu0dZjBPIeIa6BxVUMEt5gIEx/N1tzHUdcQcKy9JB6DIIkhoIHZosvflJOCC5Wm48siFvI21EEkGRuP7nCOK8ePiUC5GwLOakrJievSxPK/TE3mIDNtex5kdFmfx2x7WpclUC0bkW9h9v8AfFTySqhWO09yRyvztgpvczK1/URMty6Cb/GIs3myuuW0wJvPK5MffFinl6bgFrXmQCP/ADhG4jXZqh3Ik+o6jME2OqY+MMUAxTEiMebzQbYiCBeInfbry74qVKwaxFhfbuZ+MViVAAU7bf3nnOPQx0tAuRv0Pb74OgBNFkz3gCAtoBhSxdhEgxHa245c8MdOVBLEQBZiNuYG9zhOreaPXS9MG0DmIB22BtNrx97K5yo1gha6sZcgW589ViL4ypl1DH8SzWS4Mka7bQDpiZPPEOfXT9UFiAdUTEQZ6sZi/fA3NPUqFVLadLarBoMRAm2vY2G2LD5N3e7Dy7brqIt3YW7/AIxk6amvURgdfl6iBKwwCi3qNiCQZjcWxUdDVhAxcEyQBHPeRcRtcRz7Yu5uRVb6GBSAwaTI3EfpJH7TjXJMUGkFhM20jv23gjrttvjgJpMh/wCHigRURQ4mAQYJP8rTv3brte2N85nTWZFINJTIYj1GRfStiI6t7DF2nTSnTDufULu7AExO1pgX2H9sA6uZJZvLRmGoaGuDEEaSpIsIn3EnfGjuCepZq1lZvKR5VATJsBAtfftirwXiRWrJjSWKhhME7x7cpx4eDVKhDNpEDnA59Yjn+MRZsUqdMqYapJ0wBPL8SB839tIVtTAzL7p0ynnFakSL225zi3luJ0EAU6TFx2PbvjnHCuLVadJWqEK07NuR3/zbBPLeLcs/1SDe+k39rYnOIg3L09UhFdR7bxFQkQY+d/7Yu0eP0zscIaZ7L1bKynl3HwbjHpo0+Ri0SDgSDcdyUidCp8ZT+YY2fjlP+YffHJuJ8Xp01hSKj3gKSfuRP2wHqcerQdAXYnY8uskYMY2MnfNjBnaxxZDfUI98cz/1M8aapy1Br/8AyMp+kdJHPrG2Emv4lzZ9PmaZH6QASPfcfvgSGgDt/m+Gpho2ZPl9SGFLIS8WxmNzTm84zD9SSdqyG4Qayzs3lwwAUhQWGkgCZb2uIx7mqQp/8yvdPQBYElm322iY+DG+PMZiYDcfkYiSrwx6mltQYMJgqBI0yBO4E8thAib4sZ7hlLQwCAAj1ra7ATe3qsd97DGYzAeYwdQbkMmFHl/qpQQetMk6R7g29o6YN083YRsduZ/O2PcZhLGo3iCZ5XzIVdTC3Qcz3wAyebhnNQ6vMJAUbIACYv2BBPP8Y9xmHILW4jKOx9pXbMrThSLbd/gxaw/fBPK5lXQNAuJ2gRy9rf1xmMwRHthKfdUt0qQRTLMRciZJme5sBf8A3xVOn1MJuBbf37n5xmMwAhmT0qQNJt9O5+OX4xzvinEhTZ6TpqWAVvvMwe1x+MZjMOQbk7k1LeVEorbWED8csTFoEgc/vba/tjMZgowdSOgPLHqDzIvqBFxtyNza2JKCOx0SwB3HpIFrR02P+RjMZjINTzKVhP1a2VoIiBuf2P3xayVZK8QD6SRbae4PTHmMx1TLkuYrKhYBAxUazYDSsRKmZJ3N+/bECuzOGo+pgJKWUDkJk31AAmO/zmMxx7mgyjX4icw1SmqimU9TmeYJECDe4me2BuRr6XZvqYDT09W4IgjqdzB+MZjMHF/BhzhvnMFqMw08gB9xfYTPXEh4HTM1ACzEyNTG02gRy98ZjMB11GVyG5HVKPTYhYAtaAQF785wtPnFBZIBg2MXj35YzGYcRJ7lmjlllkJ1VNAeIsJjnzMNPbvy0qcNZmBd99l3AO1p2xmMwsncaosTTM0BTQeo22PPft84ipcRGmHhjG+ntseuMxmCAsQWNHUHjRubiOnPt995xHVyhA1arDqLyfYnGYzGwJsiW+me84zGYzA3Muf/2Q==</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMQERUREhMSFhUXFhcVFhcVFRUYFxYXFRYXFxYYFxgYHiggGxolHRUVITEiJSktLjIuGB8zODMsNygtLisBCgoKDg0OGxAQGi0lICYtLS0tLS0tLS8vLTAtLS0tLS0tLy0tLS0wLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIALcBEwMBEQACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABAUCAwYBBwj/xAA+EAACAQMDAQUEBgoBBAMAAAABAhEAAyEEEjFBBSJRYXEGEzKBQlKRobHBFCMzYnKCstHh8DRDkqLCBxVU/8QAGwEBAAMBAQEBAAAAAAAAAAAAAAECAwQFBgf/xAA3EQACAQIEAwYEBQQDAQEAAAAAAQIDEQQSITEFQVETIjJhcfCBkaGxM0LB0eEUI1JiBiTxghX/2gAMAwEAAhEDEQA/ANtd584KkCgFQBQCgFSBUAUAoBUgVAFAKAVIFAbxpvh3MqbvgDmC5OBtXmCSBuMLnmo9DWNGUlc0UMhQCpAqAKAUAqQKgCgFAKkCgFQBQCgFSBUAUAoBQCgFAKAUAoBQCgFAKAUBnctFY3Aic5+ylyWmtzChBtt2SQWwqD4nYwo9T1PkJPlTyLwpynsRtV2otqBYG4kftXXjMH3ds4BBBy09MCa0jTv4jqjSjDXdlXqC119/ednJJ5JLfSHj1EeTJ4VqrJWNHqXQub1DkqW4ubTMPzMjHeENjElh0rnaszlrws7mNQYCgFAKAUBss2i5getc+KxVPDU+0qPTY3w+HniJ9nT3MDW8WpJNbGLTTszypIFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCpAqAbrGmZoxAM94jGASc+MA1Ddi0YtkqLVoc72IIxI24aGGIghkxng1XVmncj5s1Xbj32gL4mAB3RMmW8M9cDyq1kit5VHZI03StpHuELcKqGWG/VlT8TkrlgsiQCMbs4qyV3Y0p0lmaluU2p1z3/jadslAAAqj6SqowPhnHVD9at1FR2Om99Dy1p8bbh29VUZcnGAPoyIAJ6i2QDRvoEup4uokG2oCq0YHU/R3NyQZjoBuBgbaW5i/I3dkPtYlyFtsNrM0gSMhgOSVbJgYBcYqtRXWm5VwzKzLF1KkgiCDBHmOaxOBqzszygFAKkGdkgMCwkTn0rDEwqTpSjSdpW0fmaUZRjUUpq6vqi7taEWbyvI92Zkz3drKcz4ZFfEVOK1MXhJ4Sqn2itay1bT2a6+Z9MsDCjWjiaLtHmuia3XkeWdAlzUCCGWCxIyDHGeJkj7KsuJV8Nw2dKonGWijyeu+m+i2fmVqYWlWxcK0NVu+l1t5alV2hb23CPn/f75r6TgdftcFHqtPlt9LHk8XpdnipW2dn8/5I9eueaKAUAoBQCgFAKAVIFQBQCgFSBUAUAoBUgztWy5CqJJqG7EpNuyJf6GqiXYg4MQRI7h7vUna3gM+hqt29jTIktTDU6w3CAqhR0C8y0zBAGDuOOKKNisqmbY03wlkE3SSw/6SEb88bzxbEwMycjGZq6i5bGsKHOXyKvW9pPeTYAEQGdiSFYGACxJliCRk9HBERW0YKLOjRKy0JXYtxihBAO3cyboh1P7W3B+IRLEDj9ZNUqrW5Sadsy3Rz3aQOivbbG5RAe3cJ3OVPG3EAqVKzG7db571bQfaRuy2ZWvE9sak3DIWJySD3VP0gWOFzEEnhrZqWrElhdKCGEXC3Jgi2G6wDlp3TmBDkQYqivsToYah2ukOSWY904kz0wPEZgdRcFSkloHqW+nbdbEkb0hXAMkLxbJIxOChg42ictWElZnPXh+b5ntVOYUAqQSuztOlxtrNtJ+HwJ8J8a8riuKxOGpKrQgpJeLe9v26nbgaVCrPJVbV9rW/U6LRaA/s7hDLb+ERiTnPjA4r4LF8UU5yr0o5Jz3afzt0vzdz6ang8kFTcs0VsmvlfrbkS76xzbBA6qe8PuFeXF3/Nr5ndHomQD2bbuPvclgeMwCeSG869bD8YxOFoOjRstd7a/D2zjxOApV6iqTWqVrX0Oe1pG8wAAMACvvODqp/SRlUbcndtvzf7HzPE8v9TKMFZKy08l+5or0zgFSBQCoAoBQCgFSBQCoAoBQCgFAKAUB6jQZxjxyPvpuE7En9GYlTcJUOQNzZIDH4iJmOSPGDHBqL9DTI3Zy2fMrtR2wVYpbU2gCyOcG91VhuHwkGcLGVgkzW0aa3ev2OuEVDYrbNltxESBhswsHHxHAB6E/uVo2rEpGzctpsbbhHVgRbIYdFOSCG6xhjjFRq0TojD3j+8DKWLSGQxJMZXHlBkcYcVNlaxHMsu2tCt+1O0kqDdtqrieB76zuEyRtkdZtrEbqxhJxlb35MzissnDrqv2OOGoNwe6wFJBRVwgeIEfxBtu45hkJPdrqtbUvfkSuzSbeLrbLbQYYd4kyVYJ0EkyTAh3521Etdgl1LTT64EFUlFPdecuI+ufIiSBAO1h1qjiWubuzZtvuIhBKXJ42nDKPrMIBAEmUU9arNJqxGW6sy1uLBiQRggjggiVYeRBB+dYHBKLi7MxoQKACjaSuwdd2ILoBF3kgETzAxnz4r8w468G63/U21zW2v5e7H2HD1iOy/vfDr8SzrwjuIV+0Fb918HyboRXRCTa819jSLuvQqdX2OoUvuCwTM+M/fX0/D+P4zNGhGGfZJc7ev7nj4vhuFd6km4878tfL9iibyzX3cHJxTkrPpvY+XmkpNRd11PKsVFAKkCoAoBQCpAqAKAUAoBQCgFAbrOmLDdIVZje5hZPAB6t5CT5UuXhTlPYit2uinbYEk8XbgEg4gomQoOBJk96e6RWip/5fI6oU4x831IfZmpb33eLN7zuuTJbx3nrKnvHy94KvOKylpRzXTNftLpBbP6TD7gRbuIuAXAhXZvAhQsAZZFMjdUUZX7pWDutd1oyrHa5uKN8dyAAmFCnAMeRYLPMOnhWuSz0L3uiyt2QU3OYgSBHeZTkwvQCd2Yw78xVL66E+o/SJQoo2gSfFmHLBm68bowJV8ZpbW4voT/Z1zO04XcGQyB+sWO6pPJYALjMqh61nWXMq45vhqUftDp109wPaQAXZdSc7Gnv27Y4WCwg5IFxSCIrWlJyVmyFJNKSKp7bXjvEszSbhP1uS7k8Bp3Enxu+FaJpaB66kkXFtRcB3v8LjOwETBJ5ckKeIG62cndUavTYnYshqzfUNklYTaI7o4UKBgD6OMYt+NVyqJN7l1oZNvYxG9JIXr7snIPQbWaY5h+AFrCa1ujGvC6v0M6ocoqQZI5UggkEcEYIrOpTjUi4TV090yYycXeLsy27P7XutcRTD5jiGiM8ek/KvmOKcBwNOhOtG8LK+j0vy0fy3PZwXEsRKpGk7O757nUK0iRxX581Y+kNGvH6s/KPWRWlJ98vDxFb2xoDdLEE92DHmRzHyr2eEcUeBlfKmpb9bLp8zjxmCjiqai3Zq9unxOauIVMHmv0jD4inXpqpTd0z4+tRnRm4TVmjGtjIVIFQBQCgFAKkCoAoBQCgFAKA91epSwF7vvHZQwBkW1BJGYy7SpEYExkzVowcjpp0o2UnqVHaGre8wd2mRCgYVPFUAwokiI6Mh5raMUlY3Z7e04HfuGJ5QfFu6yPoAzuzmHMAxRPkibHmo1BZZACjhgOpGQznliYnPVXgCaJWDZZ6MC9YK3Adse6fxKcI6+LIVAnoUt+NZT7sroyn3Wp8tmcpqCdJea2ol0JUuYlgR9AZCKysIOWi4CCIiuld+NzRvK9DRpzcW4TbO76ct8JU53XJwAZO6T1uCal2tqRrfQureotqw2ncwhhM7Vz9rkFSDwJQ8hqzs2tS2iMtQzMwYTn4Qv0c/AkcQcAD9w9aLREMudZpBqrW1wNzZAVlG3UKD3SYO0OGggjAuD6tYKWSWntfwUSUZ2ez+5xP6WTNs9y2eVAICkGQzA5ZlIk7pP7Uda67cy1+RlY0xQ/rZtoZUyJcgR8C8sQVBBwpNsZ71G77BLqbbGvOnci2sDKvmXdTiA30QREbY5tyTUOOZai9mXfZdq4XD2gG2w244t7WH0ycBWVjjmHIGRWU2rak+pb3lAYhTKyYPiOnNYI4JJJ6GFCBQErs3VC1c94QTAMDjJEc/M15/FMHPGYd0Iytdq78lqdOErxoVe0avYuOyO1HuXGELEbgo9RME9cz/AGr5LjXBKGDwsZwbbvZt/qvfxPcwHEKmJrOM7JW0/wDSzu69PBiRnaFMz+E/OvnqWBqSSldRT0u2l/P0PVnUytpJt25L2iu1LXdnvlYqW+iCCBHAPQmK9bDf0dOvHD1IqcOcmmm781zUV9dzmqRr1aMpxbjNbK99uT5Xf02KDUahrhlo+QA/CvvMHgKGETVFWv5t/c+XxGLq4i3aO9vI1V2HMKAUAoBQCgFAKkCoAoBQCgFAR+0tF7+1tBIdJuIRMkR+sQRkllUED6yKMSavCWVnRQl+VlBou2I7ij4oi4YD7volYwgO4LjIDiWMV0OHM6FLkStARdkKRGNxbAQ5hnn4ckzPQuBVZaBakhHS2SPiOVYsO6ueQpyxUrOedrCM1DuydEe6XUOl4EhmOVZRksvDKvyGPNUNJRTiQ1fRm/2s7NQqLuWa0qh9sRctuf1bbuirvAJgmH6bZGdCbvl6lY2Xce69/Q5a5qmuJswoSXVQIEctOZYjLSSTi6Jrpy2dyb3VjPTaY7e+xt8vbxLsYyEXrIXDGAWtjPeo3roErlpoO0g4NpBtJ4MyzYiN3QMMQABm2TNUlC2rJT5Fh2K/eIMC22CxICqwyhk9ZMR9Vz4VnUWnmVlDMrEP2p04tN+kKg3OxFwsAQl0CSQkRLAF+9OVuQBVqMsyyvkRGWaN+fMpBbuagjaHuXcBgJdzGFbxMBds+KIfpVrpH0LayOr7F9jPeJuvMjOoj3KPyMRvceEsIXptG5SteLxDjdLBzjGcZZX+a2iN6OHdWLcGm1yuT7hIAtxtVJAQDaqZzC9DPJ5PWuuE41IqcXdPW/U82o53tPlyNdWMxQGW0xMGJiYxPhPjQeZjUgk9nan3VxX6CZ9CCK87imDeLws6K3e3qnc6cHXVGtGb25+hL7O7T23iWPcfDeXgfl+ZrycfwJTwEaUPHBXT69V8eXwO+jxN/wBW6j8MvouXyMLmqa1cYAypjcvTjnyOOarg+HUsfw+CqK0ldKXNa/VeRti8ZPC46UoO6dm18PuQLjSSYielfR0KTp04wbvZWu+Z4taoqlRzStd3sY1qZigFSBUAVIFQBQCpAoBQCgFAKA9ViCCDBGQfAjioCdjm/aLs+3aue9iUu7mW2O6qsI94rN0WXJAGdtzkba6aU3JW6HcmpJSK3V6xni5IUSZUCFVuS2394CSTkkXRWiSWhLbZbad5UNeOxsLHLtjuNt6SFiTAJSRO6Ko97ItyuyTcvysINoACkA95l4G5uvReg/Z4qqWuouWXY7lrRVlDBJEHh7bz7y35xuJx9G4fq1lUVndGU01aa5fY5jtG0NFe225LCHS64B7pEqVTKyIIJM5R4Ck10RfaRuy90tUQmts7ym4lu+MksIOZY9VKxuP1UP0qvdJajXkbrot2yHEOxztQxbVvpLuGWgsIiBD2zuMVVXehLsiz/TTfAckTwQBChuTCjAVp3Y+sw+jVcuXQXudDdse8shNQGBddriQLg2QbV2DO1uPiGdrdGrnvllePvyMpSUJ367ow01pLSlLKhFODGWf+N+W4GMDGAKhycndmE6rlotEbLJYMCk7p7scz0isa8aUqUlVtltrfaxFNzUl2fi5WLL2kA96ON2xd0eOfyj7q8L/jDf8ASSX5c7y36f8Ap6PFrdsutlf1KtELGACT4DJr6K55aV9ib+iC2A1zMgwMwDs3LJHJyBGPnVc19jXJl8RLtaW5rGNuxb7gb4iNoXmJPTDcZ4wBkVVtQ1bLqMqrtBaFdr9E9hzbuCGHgQRHQgirxkpK6MqlOUHlkR6sUFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQHmp7PGostaJALMvuyeBdEwT+6QSh8nnpSM8sr/M3ouyd+f3ONs6lbRKqCJwz3B30P1gnCsrAnq3duQRMV2NNnRe2hq09pi7KQx5FzIkCcksTEgqDuJiUX61S2rELctNFrFstsfbdYYkT7qDiATBcEEQcDKfEM1RxcttCyaRNW+63VYHcwI24wwPA2jhWDHujo7DpVbJqwe5O9oOz0u2t3fm2puoF2lzbOblsngMhXdwYNu4IO6sacnGVvftmcFlbg/VHJjUl1NkAKpMqicFgIAJOWJAgE9RbiAa6stncve6sTuwewbmqx3UtNxcfCbhPwDl5BKwOA4nK1z4rFQw8HUld25JXf0LQhmajdK/U6u12R+gHaincebrQWaJykYt/E3He7xzBrz8JxOjj4Z6Utt1s16+7FMVCrQeVq3n1NddZwk7Q9lvdG74U5LtgR5eP4V5GP41h8K+zXfnyjHV/Hp9/I7cNgKlZZn3Y9WSjrbWnxYG9+Dcb/wBf9+2vOXD8bxFqeNlkhyhH9fd/Q6XiaGFVsOs0v8n+hU3bhYlmJJOSTX0tKlClBQgrJbI8uc5Tk5Sd2zdoEuG4BaUs+doAk5BE/KrStbUmmpOSy7nW6D2VAPvNY8nn3an+oj8BAxzXPKtyiehSwV9aj+Bb39cttdiAIo4VYED8v95rFRctTu7sdEcJ7QXy99iYwFAjw2g5+2uynHLGx4+LlmqldWhzCoAqQStB2fcvtttqT4nhR6mquSRenTlN2ijr+yfZi3ahrkXH8/gHoOvz+ysZVGz0aWEjHWWrJPavYFrUZjY/1lH9Q4P4+dRGbRerhoVPJnHdqdi3dPlhK9HXK/PwPrW0ZJnnVaE6e+xXVcxFAKAVAFSBUAVIFAKAlaXSbssQo+/4d/gcRGQDzxVXLoaRhfcj3AATHEmODj1GKkze5s1AiE+qM/xHLf2/lqF1Lz0tHoc97TaJAw1R3Q7bXVYH60CSxboGC7uCSyPxNdNGTaynVCSlG5SanUG4gEBQsAomBgbUbxZhGzcxJxbzmtUrMs3dGa6TdbDuQoAEdWdCYBRcSAWiSQIdc92jlZ2RNtLlhoe0ty+7UbYBgnLuhywZo6SWgACGeZ2zVHHW4uXvYLvtYAGEPvFY8K2AUJOJYQY8UOO9WNVIzqJ5cy5Gqx2Np7Tm4qlzO5FcDZa6hQs9+DgFsQq90xNHUk1YpKuvyom3bhYyxJPn+Hp5Vnsc8m5O7Lvsy29/T3LZzBHuyejeE+Ax/wB1fIcVq0OH8RpV4aXvnS5rrbq/0PawcKmJws6ctbWyt9TX7qxpvji7c+qPhU+f+fsrbtuIcU/CXZUur8T9P4+bM8mGwfj78+nJe/aIOu7QuXj3jjoowo+XX517GA4VhsEv7a73OT1b/b4HFiMZVrvvPTotiOtrqcCprcRhGWSks8ui/c78LwWrUh2tdqnDrLf5fuewvmazzcRnqlGJvk4NT0cpz81p+xP7FIF2VJBg1KeMTtWy26omK4c+9hnJS6Pp78zo9V2vnaJLQpIBlu9O0t1AMHPkc4NdCppbkZr68jWuja9Bc7RzA+L0ngefXwPWr7alL8kc/wC0NjZfYTyqn/xA/KtoSUloeXi42qFbVzmFAZWllgPMfjUPYmOrR9H0d9UAQKFA42iB9lcp7qioqyJwNCRQGt2HHPlQWPnnb9lU1FxVAUAiAOBKqTHzJrohseNiIpVGkV9WMRUgUAoBQCgNtmwWk8AAmTOYDHHie63ljmobsTGNydc93ZJAhyCQfHG3IMd3hxHOeog1TWRq8sPMiB3ukW1BMwAigmdogSByYHNW0WpTvS7qMdTpnstsuKyMOhEH1HiPOpTT2IlGUHZqzNJM5qSp5csrcRrTmFcQT9UgyjjzVgD5wR1onld0aUp5Za7HIOw0txreyXUlHLAdDB92pwOm1jP/AEiIrrtnVzr8LNFm1ce9tUNdc5gSTcDDJPUKytz0D/u1LaS6Ea3Ou0HscbAGoun3kHcqowKgA4N1hz1lVxlu9BivHfG8LOu8MpWl5q1/S/vobToVIU+1SuvL9SZculoGAB8KgAKvoowK6zzZTcndnlu2WMKCSeAMmqVasKUHOo0kubEISm8sVdlqnZiWgG1DR4W1PePrH5fbXztTjGIxknS4dC/Wb2Xp7+B6ccDToJTxMv8A5W/v3c1aztdmGy2PdoMALyfU/wBvvrowXAqVKfbYh9pU6vb4L9/hYyr8RnNZKSyx6Lf5leiTxXqYnF08Orz35LmyuB4dWxkmqa0W7ey99DKQvGTXD2eKxf4jyQ6c379o9XtsDw7Siu1qf5Pwr0/j5mDNPNejQw1OgstNW+542KxtfFSzVpX+y9EYgjiuhxaVzkLDsT9r/KfyrCt4TswX4vwZ1unsALvMDAJJgcCM/wCazlNJ6HoqOmuxHvdqBlYaco7j60/aB1/Coyu/fKdqnF9lZs5HW3HZybpYt1n/AHj0rpikloeTUc3Lv7mmrFBQGdn4l9R+NQ9iY7o7yuU94yS8UyD8ulATw8igPKA4P2l/5Vz+X+ha6IeE8fE/isrKuYCgFAKAUBJ0yqBuaOWHQlYXukJPeyeuO6aq7l42tdnup1zONvCgkgY67p+0MZHFFGwnUb0LfsX2Su34a5NpPEjvn0Xp6n76znWS2Oijg5z1eiO57M7Ks6VYtqB9Zjlj6t+XFcspuW56lKjCmrRRWe01+1e090AK5RSQ0TtYeB6Hxq1JtSRTFRTpNs+cV3HhioBD7R7Ht6hluO7KQNrhV71wLhCCcKQsqSZwqQDFaQqOKskdMascve3JloLbX3dtQicEDlslu+xy2WJg4E4AqjberMp1ZS05E7sjVPbuKFJhmAK9DJjjx868jjGCoYjDSlUSTim1Lmra7/odGBxFSlVio7NpNE7VdigXHZmW3amQeuQCQo9ZH5V42E/5DJ4anSpxdSta1uWmzb9P/Ud9bhiVWU5NRh729/A03O1EtApp12+Ltlj9v5/YK6qXBq2KkqvEZ5ukF4V78vmzGeOp0Vkwsbf7Pd+/aKt3LGSSSeSTJNfRU6cKcVCCSS2SPLlJyd5O7MauQbW+ERx1ryKKjLH1O03Vsvp5e+p9HinOPCKXY+Ft57dfPyv+hodwvNe3CnKbtFHzbdiJd1JPGB99ehSwkY6y1ZRyZDuagL1zXU0mrMoW/ZWsYKtwc5Hrkj8q8XE0oqbjyOmjVlB5kTu0O0rl899sdFGFHy6+prCMFHY0q151PEyIrQZBg+Iq5km07osbfaCuNt9dw6MPiH+/7NZuDWsTqjiIzWWqr+fMw1HZpA32zvTy5HqKlVOTKzw7SzQd0QK0OYzs/EvqPxqHsTHdHeVynvGL8H0oCxt8D0FAe0BwftL/AMq5/L/QtdEPCePifxX75FZVzAUAoBUAUAoD6F7MdlaW2Aw710ZJuRI/gXgeuTXFOq5aHtUcLCnruyy7a7fs6VNztMmFC5LMQSAPOAfsrM6W7HFaztjV9oHbbm1amMckebDM+Q9CaskVuTbHZ66bRXrYaSEafh5ZiYxxkxEmrQ8aMq+lGV+hyddp4YoBQEvQ9mveyoherHA/zXmY/i2Gwek3eXKK1f8AHxOvDYKrX1irLq9icNRZ037P9Zc+ufhHp/j7a8l4TH8V1xL7Ol/it36/z8jsVbD4P8Lvz68l6e/iVmq1T3TudiT9w9B0r38JgqGEhkoxt936vmedWxFStLNN3NNdRiKAUBD7Q7S9xtHRpzzER0+dI8Po4qalUvePTR/M7cNxHEYaEoU2rS3TV16+pEfUAjdMz1mvdjFRVlseY731Ij6qTEwOZ+zgdTmsa9WULKEbt+9TajSjO7k7JEdVJjdz99bRvbXcyla+mx0PZoi0vz/E15OJ/FZeOxJrAsKAUBu0uoa20qfUdD5EVEkmtS9OpKDvEk9tWgt3GJAYjwJmfwqtN3ibYuKjU0Idn4l9R+NXexzx3R3lcp7xi/B9KAsbfA9BQHtAcH7S/wDKufy/0LXRDwnj4n8V++SKyrGAoBQCpAoAaA7KzyK80+jHbVmwVRr8HbNxUALMxt23LbUHx90tjIqYkMiPqHvK6WWRAAy7VeLjDubWDj4R8Y2jy7wrhxvEIYOce2hLK/zJaLy9/UrD+6n2LTkuRz+pZ1JRpWWLlI2ruZixIUYySTPnXr4erRrQU6LTXVHjV3VUstS68jRXQYG3TaZrh2opJ8unqelc2KxlHCwz1pJL7+i5mtGjUrSywVyz/RbOnzdPvLn1F4H8X+fsNfP/ANbj+J6YRdnT/wA3u/T+Pmj0uww+E1rPNL/FbfH+fkRNd2m93BO1eirgfPxr08BwfD4PvJZp85PV/wAe9TkxOOq19HpHoiFXrHGKAUAoBQFF7ULPu4/f/wDWu3Bc/h+oKvRju+U16CM5bnQ6DsElBfvuLFk5DNm5cHP6tPMdfnkVzTxPeyU1ml9F6s2hQ7uao7L6v0NertW7zKNNaZLagjfcMtcJPxN5+Qx6VVVHST7SV30XIrUcJO0FZfcn6a1sULMx19TNcFSpnk5EJWNtUJFAbtLpHuGFE+J6D1NVcktzSnSnUdoonAWtPn9pcHh8Kn/f9FZ96fkjo/tUP9pfYr790uxZjk1qkkrI5Zzc3dnln4l/iH40exEd0d5XKe8YvwfSgLG3wP8AegoD0mgOD9pf+Vc/l/oWuiHhPHxP4rKyrmAoBQCgFASdPo9w3Mdq+J6+lcGJxuSXZ01ml06eprCndXeiLK120FI7rMB1kSaijQrON6rV/I7I45R0auiH2r2m18jG1QIA59STHp9lddOmonNXxMqr6LoQVJBkEgjgjkVecIzTjJXT5MwTad0Wdvtpo23ES4P3hn7ePurwKv8Ax2ip58NOVN/6vT5fyelDic7ZasVNefv9DL/7Kz/+ZJ/ix/TVP/yOIPR4yVvTX7k/1uG37BfP+DXf7ZuEbUC218EEH7f7RW2H/wCP4eE+0rN1JdZO/wBP3uUq8SqyjlglFeRT6jUqnOT4da9xtLQ5KVGVTX6lfd1rmYIH5fOspOTVk7HpUMPSpzi5RzJPVPmeL2ky85HWcffUqTRSrhacm3FWLOxdDqGHBrVO55k4OEsrJFvTu2QrEeQNWszJ1IrdoxuWyvxAj1BH41BMZKWzMaFiD2t2Pe1Cq1pd2ySRMTMcE4JxxXThpKL1KTqwho2UujsEjYqHdwwIiCImZ4r0XUjFXbIkrsvNP2cXK+8JuMAFVckAAQFA8AK8+piuUNEXUW3rqXVnRKgVrnwngA4gOitkc4ae74VxOV9jZQS1ka9XqQyqgEBS3HB3GeIHl0HpUxXMrOSasiPbtljCgk+AqW7FYxcnZIsV0KWhuvNnoi8n1/351nnctInUqMKetV/A06rtFmG1QETwX8zUxppaspUxEpLLHReREt2yxCqCSeABJPoBWhzpN6I6bsr2TLQ187R9RTk/xHp8vurKVTod1LBt6z+R1FrRW1T3YRQn1YEep8T51ldncqcUrJaGq9ouq/YfyqC5CuqQCCOlAT7fA9B+FAZAUBwPtVcC6m6zEADbJJgfAtbxaUTycRFyrNIqdLqFuKHQyDMH0MflV076oxnBweVm2pKCgFAKAn9oglUI+DaI8jXkcOcY1KkZeO/0N62qTWxAr1zAUAoBQCgMLy3CItLufoJAnxicT61WTsrmtCCnUUWcte1AW8xuhwwx3gV2j6rL9pBOM1SU1JKy/k9aEMmiNxuloC5PSOJ8o59KqWFu1OSZ8PD5UBKtX2tkFTEcCBk+JHWo1zJpktU5U5QlBO9teat0fmWem9pLpIR39CAJHritlVlszyq3DaKTlBfAu9Nrrj9wqLgPQgfj/etVJvTc8upRpx7yeUnrp7IYKVUOfoyT5+lXtE5nUrOLabt1KvtDWOxKHuqDG0Yx5+P4VnKT2OyjSgkpbvqRbKAsoJgEgE+AJiao2dKV2Tf0pLY/ViWkHcehEcEZKkbsY58qpZvc1zxj4SFcuFjJNXWhk22TLHZhjfdOxfP4j6D/AH0qjqconRDDO2ao7IzudohBtsLtHVj8R/3/AGKhQvrItLEKKy0lbz5lcxkySSfE1ocjbbuzypBe+yblXcgwdo/Gsqux24HxM7CzrQcNg+PT/FYnpEqgIXaPa9nT7BduIpd1toCcu7EAKo5JkjigMNe0jPnQG5DC/L8hQHEe1H/yXp9MTasReu8SD+qU+bD4vQfbUXB8t7X7Xvau4bl59xJmAIUdBAHkKi5CilqjqfZv/jJ/N/Ua6afhPJxf4rLOtDnFAIoBFASNNq2THK9QeK48TgoV+9tJbNGkKjj6G46dLubZ2t9U/lXIsRXwuldZo/5L9ffzL5IT8Oj6ES7aKmGEGvSpVoVY5oO6MXFx0ZhFakCgEUBK7M/ap6/kazq+Bm+F/GiXXbPY1nUrF1JImGGGXI4P5cVxKTWx7jRy/tL7P3NIo9wrNbNsbnWGug53blAHc4wuPEda3pVUpKTWxnOGlkcro9WkbQNvWOZ8dpq9yuxvMkTwCds+JiYniY6DNQDdatheKkhokWe0bloEJcYZk5gT50heCsmRiadPESUpwjoktF0/Un9na/3meGBmc5/eHzrWMrnl4jDqntsX2sJewHuCH3QDEEj0+37K2lrG7PMpWjWcYbFXFZnYZWrZYhRyTA+dQ3YmMXJpIs3uW9N3UAe4OWPCnyrJJz1ex2OUKGkVeXUrr99rhliSfw9B0rVJLY5JzlN3kzXFSVEUAoC89lvjf+EfjWVXY7cD4pHR1iekb9ITkSY8KAqO3NbotNeTUajYL23YjbS9wICSdoHwiSZbE8Z4qARvaz2x0mjQbrgdyJW3bgsQRifqj1pcHyP2o9utVrpQt7uz0toYkfvnlvwqLg5eoBN0l2RB5H4UJO+9m/8AjJ/N/Ua6qXhPHxf4rLOK0OcRQCgFAKACoauCZa1sjbcG5fvFebV4faXaYd5ZfRm0aulp6oXNEGG60dw8OoqKfEHB5MTHK+vJh0rq8NSIyxg49a9OMlJXTuYtW3PAKNpbgl2dCY3Odi+fPyrzq3EI37Ois8vLY2jSe8tCcvbIWFgsoxJPe/z86mjh61m6rV+i5HVDG5dN19S2s9oLfkqCAoC5iTxmOgq04OO53Ua8at2iDd9mNNfu72SGySVJUMcxvA+Lp5+dQpNGrij597Q6O/YYG/b3KO6Cv7IicbRHcP7pjkxNdEavdyr1MXDW5HXU7/hBM4ggjPgR1PpUg6nsP2Iu3ofUE206L9MjyU4X1MnyFZSqW2LKHU6HtTS2NELa2rSz3oJySRtyxOSeP8VthpbtnlcUpuTik7LW5RanUNcMsZ/Aegrdtvc4oU4wVomqoLm3SXdjq/gZ+XWqyV1YvTnkmpE3tDREk3bfeRu9jkE84qkJ8mdFai23OGqZW1qcgoBQCgLz2V+N/wCEfjWVXY7sD4pHR1ieibtN19KA+Q9o9narXdq3U2OP1ptyQdtuyjbUycfCAR4kz1qoOG7Yt7dReUcLcdR6KxA/CoBDoBQFj2P2VdvsDbXAOWOFHz6/KrRi5bGdSrGmu8z6H2bpPc21tzMTmI5M/nXVGOVWPIrVO0m5EqrGYoBQCgFAKAUBlbcqZBg+VUqU41I5ZK6JTad0WWn7RBxcA9Yx8xXh4jhc4d6g/hz+DOmFdPSRlfuXFyioR4qPyrOhTw1R5aspKXSTJnKcfCkVl66zHvEk+f8Aavdo0qVKNqaSRzSlJvUys6Zn4B9en21Sti6NFXlL9yY05S2RMtlLBmSz+RgCuHPicX4Vkh15v37ZtFxou99SZo/aHbl0kgGNpgH1nj1rt/p/M6IcQdu8tSzhbi5AZWGRgggnIrnasz0YtSV0e9g9haex+st2lDEnOTtHgk/CPIRUuTZNkWOv7Qt2BLtnoBlj6D8+KmMHLYzq1oU13mcd212odSwO3aFkKOTmOfsFdlOnkR5GIruq1pYiabSNc+EHxPpngdeDx4VZySMYwctjTViooDdptS1sypjxHQ+oqsop7l6dSUHeLJ3vLV/4v1b+I+Enz/351naUNtUdOalW37siHq9C9r4hjoRwa0jNMwqUZ099upHqxkKA36MXNw91u3eX5+XrVZWtqaUlNy7m50qdpi2At5l39doOPWsMt9j0+2UElUevkW+juKQWkbYmZER61U3zK17lZ2n7TokiyA7fWI7o/Nvw9a0jT6nHVxiWkNT8+drNN+6Tybjk+pYmsXudcXdJmnT6drh2opJ8vzqCx0XY3YAndcUs04TpHic8escVaKbehnUnGK7zsdpaSFAAAgcDgelda2PFk7u5nUkCgFAKAUAoBQCgFAKA26fUMnwn5dPsrmxGFpV1aa+PMvCpKOxZ2teHESFbzyK8Otw6VCWazlHy0Z0xrKStsyPqvf8ABmP3ePuz9tdmFWA3ja/+2/10M6na8yGthjwrfYa9N4iktXJfNGOWXQkW9DA3XDtH3muGpxHM8mHWZ/RGio21nobF7S93i0AB55n1rShhKl3OtNtvktkXjiXT0p7Et/aNwmxFCnq3P/aP7zXRGgk9TaePk1aKsVIV7jE5Y8kk/iTW2iOLvTZKs2Lab/ekErswCDMySBBzwBORmobb2LqMVfMa9Rr2YbR3VmYEYJJYwYwJbjyFFEiVRvRaIiVczFAKAUBL0naDWxt+Jfqtx8vCqSgmb08RKGm66G4vpnyQ6HyyPzqvfXmaZsPLdNADTL1uN5cf2p/cY/665tnl7tMxstKLa+XJ+f8AvrUqnzZWeJdstNWRX1ocxkHMFZMHJE4J8xUE3drGNSQchY9lGu3XuXjtQuxCj4iJPXoK51Sbep6MsXGMUo6s6Oz2ZaRQqKFA8ME+p61q6cehyrE1E73JVu2FEAQKslbYxlJyd2ZVJAoBQCgFAKgCgFSBQCoAoBUgVAN1rUuvDH8fxrnqYShUd5QReNSUdmZnX3D9L7h/asVw3DL8n1Zbtp9TQ7kmSST512QhGCtFWXkZtt7nirJgZJwB41Yglroyq73GO8BkRIXcskcg5GDOOlVzX2NMlldmd7Xxi2IHeHAjaSDEegAM89Zoo9SZVOUSCc1YyPKkCgFQBQCpAoBUAUAoBUgVAFAKAVIFAKgCgFSBQCgFAKAUAoBQCgFAKAUAoBQGdp9rBhyCCPkZqGSnZ3Pb94udzGTx8hwKJWEpNu7NdSQKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUB/9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxASEhISExMTFhUWFh4WGBgVGBcYGhUXGB4YGBsXGxoZHSogHRolGxcZIjMjJykrLi4uFyAzODctNykuLisBCgoKDg0OGxAQGzIlICYyLTAtLy0vLS0wMC0vLy8tLzUtLS0vLysvLystLS0tLS0tLS0vLS0tLS0tLS0tLS0tLf/AABEIAL0BCwMBEQACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABgIDBAUHAQj/xABTEAACAQIDBAQGDAkKBQUBAAABAgMAEQQSIQUGEzEiQVFhBxQycYGxFhcjM1Ryc5GSk7PTJDRCUlWCocHUNWJ0lKKywtHj8FOjtNLhFUNEg4Ql/8QAGwEBAAIDAQEAAAAAAAAAAAAAAAIDAQQFBgf/xAA/EQACAQICBQkIAQMDAwUAAAAAAQIDEQQhEhMxQVEFFDNhcZGx0fAGIjJSgaHB4SM0QvE1cqIkYtIVgpKywv/aAAwDAQACEQMRAD8A7jQCgIpvBtbEviDhMK4iyIrzTFA5XPfJHGrdHPZSxLAgArob6W06emVVaugaPamKlw5iE21sYvGkEaHJhLFzyGmHsvp0q10YLaylV5vYi0u0TlVjtnErmQyAMMGrFACxOU4e/JWPoNNTDiNdU4FeCxrTKjx7ZxJDhWH4mDaS4S4OHuCSrCx1upHVRUYPeHWmtqEeNzZcu25jmbKtjgTmbToj3DnqNO8U1MOI11TgUPj5BCs52pj8jvkUCLCl2fMUyqq4ckm6n0C9NTC1xrp3tZFyHFSNkB2tjEZyQqSphI3JBK2yPhweam3bbSmphxGvnwL+DE0oJi2tiXANiU8TYA9mkFZVCD2Mw8RNbUZHiOM/SeM+jhP4es83iY5zIeI4z9J4z6OE/h6c3iOcyMfHriIY5JpNqY0JGpdjkwhsqi5Nhh7nSsOhFK5lYibdkjCw21C4J/8AV8YlpOERMmFiYPZWy5ZMODydTflrWFShxMutU4HuH2nn5baxGshiAbxNSZFbIVAaC5N7W7bi3OipQ4h1qi3BdpFjGE2xiXDuYwU8SYBlRpSGIg6PQUnWmqhxGuqcC6uLJXMNtT5bM174K1ktnPvHJcy37Mw7aamHEa+pwKX2hZzGdtyhwQpUtgQwYnKBbgXvfSmphxGuqbbGx8Rxn6Txv0cJ/D1Lm8SPOZcB4jjP0njPo4T+HpzeI5zLgPEcZ+k8Z9HCfw9ObxHOZcDzxHGfpPGfRwn8PTm8RzmXAeI4z9J4z6OE/h6c3iOcy4A4LF/pPGfRwn8PTm8RzmXA08G2CyGU7WxqRCxEkseGijcMSAUd8MAwNjy7jyIqGqhtuT11S9rF/F45ow5O2MSSkZlKr4mWKKucsFEFz0ddO2sujBbzCrze42CYTFkAjaeNsRfycJ1//nqXN4kecy4HviOM/SeM+jhP4enN4jnMuA8Rxn6Txn0cJ/D05vEc5lwHimOGqbTxN+riR4V19IEKm3mIPeKc3jxHOZcDe7p7akxCyxzKq4iB+HKEvka4DJKl9cjKeR1BDDW161ZRcXZm3CSkro3tRJCgFAKAUBBd4JDg8XNPKreLYhUJlUFhDKgKESW1VGUJZ+QIN7aVsUKijkzWxFNyzRiYiHBbRVSJUmSMuCI3VlPEjaMq1r/kvcWsb2ratGZq3lAxYdy4FaA8WciBFRFJQjoK6X8i4JEhvlIBsOysapZGda8xh9z40aFuPiDwliSx4VnGHLmLNaO+gcjQi9he51oqSW8Oq3fIqk3PgK4ZOJMFw6oqgFLNw2V1Zrp5d0AJWxIJFNUsjGtefWZcu78RgSAPIvDfiI4K51cszX1XKR02FiCLGs6tWsY1jvc10O5EC8AcacrCQVU8LKWErT3tw7Lq5Xo5eiAOqo6lZEtc88jabu7DTBoyI8jhmzdPLZbALZVRVVRpewHMmpxhokZz0jbZqlYhcZqWFzE2rglxEMsDkhZUZGK2uAwsbXBF9eysON1YzGVnc1GP3OwkgjCrwgmcWjWKziTLnzK6MpJyLra+lQdJMmqskXsNu1Cj5s8jANMwRsmVfGCDIBZQ1rgkXNxc91ZVNGHUfrqMKHcjDBAjSTOAAgzFAeGsMmHVOgg0CSNrzJtcmsKiiWufrvKJNxYGTJxpxdXRmUQKWSVY0ZTaKx0iXW2bvtpWNShrnfYZk26kDFiWku3E60/92SOY/k9TRgDuJ586lq0Y1rJBmqdiu55mpYXGalhcZqWFxmpYXPG10PXSwuR1N01CRxjE4kLEQYPejwAFdMq3j6QyOV6eY2AqvVdZZrc72LDbjYc/+7PlEXCVboQimHxc5SULDo9K17ZtbU1KM65+u8lEYsAOwAfNVliq5VmpYXGalhcwtp7Xw+HAaaRUzaKDqznsRR0mOo0AJ1qMpKO0lGLlkkbDcrCS/hGLljaI4hlyRuLOsMa2QuPyXYs7ZeoFQdQa0Kk9KVzo0oaEbEnqssFAKAUAoBQHPt3mzRvMfKnmklJtbRnYIP1Y1Rf1a6NCNoI5mIleozZ5qusU3GalgYuCxokMq9cchQ/MrA/Mw+Y1GMrtrgTnBxUW96uu9rxTMrNUrEBmpYDNSwGaljFxmpYXNVvDvDBg0Dy3JbRVUXZiOfcB3mqq1WNJXkbGGw1TET0KauyDY3wmzknhQxqOrOWc/sK1z5cot/BE70PZ/RSdaolfL6mubwibQP5UQ8yD95qj/wBRqcDeXs3R3zZSnhB2j+fGfPGv7qzHlCq3ayI1fZ/DU4ubk7IyIPCbi1NnWBu6xU/sb91XxxlXfE5tXkvCJ2jVs+tMl27m/cGJdYmVopG0AJzKx7A2mvnFbNDFwqvR2M0sZyXXw0dOWceKJXetuxzBelgL0sBelgL0sCl5ABckAdp0oZKr0sYuL0sLi9LC4zVmwuM1LC5q9vzcMQTjyocTCwPdJIsLj0xyuPTVGIjeBfh5WqI6FXOOmKAUAoBQCgFAc53WP4LD5j/eaupRXuI5FZ/yM2marbFVxmpYXITu1tgHH4lb9GYnL5472t50zfMK5GExOliqkOOz6ZHruVuTHT5Jw1a2aVn2Tbku55fUm2auvY8jcXpYXF6WFxelhcXpYXID4VVBGG87/wCCuZyo9GCdt56P2apOriZRUrZbV62HPOAeo1xlOG5tHsp4XEq2lGM7fR9zTX3KDCeynu/Mvv5GG6620ZfRxf8A+hwm7Ke6v7l9/Iw9dJW1Mvrof+RY4658muYc9OXprbjTnb4jgVsXhtY06KvfO/kr3JFujEBjcN1+6D1GsYKaddJI2+XcNUhgXOcr5rJKy/Lf27DtOavR2PAXGalhcZqxYXIvvbvtFgGiQxSSmS59zI6IHrPd3VTVrKm0i+lQdRNkT2z4UZGnXxJM0CLeRpEaxJ/KOUFlRdO82NUTxTv7uw2KeE933tpE9sbwttF74vFpCsYsiwxSsrnnmAJBvy1a3KtepVlPabNOlGGwwZN79oNFwzjJMsbBlBJDtY6dIAk252ZvnprZ2tcaqF72JLtTwn45YkRHwrOydKSJZCyk8rh1ChvMDy6qseJnaxUsLC9zTbJ38xOGlMolmnLRlWWdiUDkg51UN1W7uvt0hCtKLvcnOhCStaxkYjwi4+R0labIqjLw4SV11Icq1w/mJI06r3rMq8273MRw9NK1jsW6u8EWNw6Soylsq8RVv0HIBK610Kc1ONznVYOErM93pP4P/wDfh/8AqIajX6NksO/5EdJrlnWFAKAUAoBQCgOa7sH8Fh8x/vNXWodGjjV+kkbS9WlRpN7NsDDwkA+6OCqDrHa3oH7SK08diVQpN73s9dR2OQ+TJcoYuNO3urOT6v3s/wAHNcFiWikSReaMGHfbq9PL015WhVdKoprcfWuUMHHF4WeHe9WXU93c7HYYJ1dVdTdWAYeY6ivaxakro+HSi4txltRcvUrGLi9LC4vSwuL0sLkE8KB0w3nf/BXI5X6Ndp6n2Sf/AFkv9rIHXnz6OKA9FDDV1YwFw2WYFV6JU5iesnWui62lSctjPFR5NdHlCFFRco5ZtZNWz6v2SPdX8cw3yg9RqHJ39Qjq+0/+ny7UdhvXqT5hcXoLmo3nV3h4ayNHxGylkNmtlZrBuq9hr2XrWxUnGGRs4SKlUzIBJuQrMHZ58wFgRKosOwWjAA1PLtrmHVLB8HuHHwj0PF+8CgPY9wcOpBAxNwbjpwnUeegD7g4ckkjE3JuelBz9FAVR7iQrmy+NjMLNaSEXHYbcx3UBb9r7D9mJ+nDQHp8HeH6uN6ZE/choDe7r7FfA3EMsiq7LdGKSKxJAv5AINtOdXUakoySW8or04yi29xKt6D7gPl8P/wBRDW/iOjZzsP0qOm1yjsCgFAKAUAoBQHMd2j+DReY/3mrsUOjRxMQ/5Zdpm43GLFG8jnoqLn/Id5OnpqdScYRcpbEYo0p1qkaVNXlJ2XazlW1NoSYiRpH5nkOpR1KO4f8AmvGYrEyxFRzl9FwR9q5J5Lp8nYdUobf7nxflw6jEBqhqx0ITUr9Tt67zom42Oz4fIecbZf1TqP3j0V6rkqtrKCT2rLyPkntVg+bcoSa2T95fXb97v6kizV07Hm7jNSwuM1LC4zUsLkH8J2ow3nf/AAVyeVpONOLXE9P7LUoVcVKM1daPqz2oglu+uBpxe2Pdl+j33Nq0ejqvsklLyl9z0X7qfx9f2MpYxb4P6SX5Yp/H1/Yf9Z/2f8jyx7fmFNKC2LvflYxqsVL4qiX+2P5k5eBtd1h+GYb5Qeo1u8nzbrxWxHC9osLGngZTbcpXWbd+5bF9Ejr2avUWPm9xmpYXLc8SupVhcH9neOw99YlFSVmSjNxd0Q3auCmcKyTtEy9FtTlNtDp1G9cSUdFtHdjLSima5MFjOrHJ89/XUSRkrs7aHwtfoA/uoC4MFj/hSfVL/lQA4HH/AAtfqloCg7Mx3XjP+WKAoOyMYf8A5p+jb1NQEn2PD0tdcirYnrY5gSe/o/2q3sHBNuTNDHVGkooubzH3AfLwfbw1s4no2amGf8qOoVyDtCgFAKAUAoBQHLt2z+DReY/3mrtYfo4nCxHSy7TRb/442jhHX029Gij57n0CuTy1W0YRpLfm/oey9icCqleeJl/YrLtfkvEh0UbMwVQSzGwA5knQAV5ptJXew+kVasKUHObsltJVvfux4rh8K4GtuHLb883cH9rC/wDNWuZgOUFiatSO5Zx7Ml5P6s85yPyg6uKqRl/fmu1bv/j/APUxNyMZkxGQ8pFK/rDpD9/z16zkaro1nDivuvTNL21wmswka62wefZL92Og5q9RY+X3GalhcZqWFxmpYXIT4Sjph/1/8Fcblno49p6z2Q/rJf7SD150+kigFAKA2m7H43h/lB6jW9yb/URPO+1H+ny7UdavXrT5ZcZqC4zUsLmi2hDdpU/O6Q7sw5/SBNcjFx0anadnBz0qXYW4crKrZQLi/IaVrG0XaAUAoCmSJWFmAI7CAR+2gMTEYSMZAEQEuLEKARl6fMDsWgN1skdFz+c5/sgL61NdbBxtTvxOPjZXq24f5LW8h9xHy8H28NTxPRMrwvSxOp1xjuCgFAKAUAoBQHKt3T+DReY/3mruYdfxROBiX/LLtIpvyp8YB6jGLegtevO8uRarRfV+T6T7Czi8JVjvUvFK3gzdeCzZSvJJiGF+H0U7mYat5wLD9Y14jlzEOFONKP8Adt7F+/A3PaLEy0o0Fstd9e5d1mTjefZ3jGFmitqVuvx16S/2gK4WAr6jEQnuvZ9jyZ5/D1nQqxqLc7+u1ZHFtkSETwEf8RPmLAeo19FwV44mHaj2fLyjPkytfZot/lHVL17ex8QuL0sLi9LC4vSwuQrwkHTD+d/8NcfliN6cVfeep9lKjp4qUlFvLdtt+ewhQNeclCUdqPpFHE0q3Ryv1b12ravqKiXigFEm8kRnOMFpSdl1my3ZP4Xh/lB6jXS5Oho4iN9vA8p7R4pVsDLVpuN172xfTj27Os6vmr1dj5pcZqWFxelhc1O38VHCBNIwVACGP9pfU3z1oY+GSkdHk+fvOJzqfwlKrERYclLkgu9ibkk6AG3PtrmHVJNuxvTDjQQoKSKLlGIOnap6xfzUBvqAUBHN5974cGcljJKRfKDYKOrMerzWoDQYTwkIzrxoCqj8pWzFb6XykC+l+ugOnbJlVoY2Ughlz3GoObpH9pru0I2px7Dz+IlerLtMfeI+4j5eD7eGo4romSwnTROr1xDvCgFAKAUAoBQHJ93j+Dx+n+81d7DL+KPYeexL/ll2mLvVsszxhlF3TUD84Hmvn0v6K0+VMG8RS934lmvyjuezPLC5Oxf8nwTyl1cH9N/U2YXg62+mHkeGUhUkIIY6BXGmvYCOvqsK+bcsYKdaClBe9Hd1eaPoPLmClWUcRS97LO2eW1NcdpOt4d5cPhoi2dWcjoIpBLHq5cl7T++wrgYPk+rXqJNNR3t+tvV+DzeFwtTEz0Kavxe5dvrsOYbobOZ5VkPkR637W6h+/wBA7a+o8j4WVSrrmsl4/o6HthynTw+EWBpv3pWv1RXHrdu65Pc1epsfL7nl6WFxelhcXpYXIb4RD+L/AK/+GuLy30ce09d7G/1kv9v5IYRXnIzlHYz6JWwtGq7zim+O/v2i1S1nFLuKuZJfDUkv/dfxuKaz/tQ5o99WfevIWo6stnhkZjgKCek1pPjJuXjc2W7f41h/lB6jW3yZ/UxOR7U/6dLtR1O9exsfKLjNSwuM1LC5z/wxzuMPAovlaQlvOo6IPzk+iudyg3opHR5OScpM1+yMDEkKBVUgqCTYHMSNSa5Z1zR7OgWLa0KRaAyKCqkiwcdJdOqxNWUUnUSfEqrycacmuB2LxGPsP03/AO6uzzWl8pxOd1vmPfEY+w/Tf/upzWl8o53W+Y4xgIll2jiOLqVdyA2uqtYDXnYequJNWk0d2m7xT6jdby4aNsPIWAuoup6wer5+VRJkg8Ec7tgmDclmZU8xCsR9Jj89dfANum+04vKCSqrsJJvAfcl+Xg+3iq3F9EyrB9NH1uOtVwzvigFAKAUAoBQHIt32/B0HYWU9xV2Uj0EEV38LnSiedxWVaXabG9X2Ne5pdr7vRTEupyOeZAuG7yO3vrmYzkqliHpL3ZcV+Uek5H9qMXydHVfHDg93Y93ZmjAwu6Cg3kkzDsUZb+kk1q0eQacZXqSv1bDq4z26xVSGjQpqD430n9Mku9MksESooVAFUcgK7kIRgtGKsjxNSrOpJzm7t7W82y5epWIXF6WFxelhcXpYXNJvRsY4lFysA6XIB5Ne1wT1HQa1oY/B85p6Kdmjrcjcqvk7Ea2108n2HP8AFYZ42KSKVYdR9Y7R3ivJV8PUoytNWPquB5Uw2NjpUZfTf3FmqToigFZSbdkV1KkKcdKbsuLJRuvu/NxEncZFU5gD5TejqGvXrXoOTeTakJqrPLqPn/tH7RUMTSeGoK63y8ic5q9DY8PcXpYxcXpYXNXvHsaPGQNC+muZWGpRhyI+cjzE1TWoqrHRZdQrulPSRzY7sbZw94oumnUVZLW7s+o81ciWCrJ2tc7UcdRau3Ykm4+5b4eTxnEsGm1yqDmyX5sW62tcd1zz6t3C4NwenPaaOLxqqLQhs4k5vXQsc24vSwuc/wB89yJZJjisIQJCbsl8t2/OU8rnrBrm4rBuT04dx1MJjlGOhU+jNDHujtbEsEnORAbksyEehUOp89asMFVk7NWNuePoxV07nUNjbNjwsKQR3yoOZ5sTqWPeTXYpUlTioo4lWq6knJlG3T7mg7Z8OB5+PFVWMyoyLsFnXj63HXa4J6EUAoBQCgFAKA4/vRMuy8ROsobgzO0+HKjMWZzmlhHYwkYsL6ZZO4108FiEo6D27jlY3CSnNTjv2kQxO/GKY+5xxRj+fmkb02KgftroqNaXBffyKVhKa2tv7eZj+zHH9sH1bfeU1dX5l3fslzajwff+h7Mcf2wfVt95TV1fmXd+xzajwff+h7Mcf2wfVt95TV1fmXd+xzajwff+h7Mcf2wfVt95TV1fmXd+xzajwff+h7Mcf2wfVt95TV1fmXd+xzajwff+iuLfXGg9IQOOzK6ftzH1U0Kq3p/Rr8sw8LSey69dhKd395osVdLGOUC5RiDcfnIR5Q+YjrFIzu9GSs/Ww1K2HlTz2rj5m2xOKSNWd2CqouWY2Aqcmoq7KIpydksyHbU3yw8vRGGMyfnSERjzqCC3psKoknWVtC668vNnQpYepTelp2fUaKbG4c8sMyfFxBP96I1pz5Jpy/sS7G/I7VHlflCkrKs32q/5La4qEc4ZD3Gdf3Q1BcjUl/b/AMn/AOJbLl3lFq2t/wCK8zZYDeGGE3TBLm/OaYs3oJj09FblHCKl8EIr6vyOTiZ18S71arfb/k2Ps8b4MPrj93WxarwXe/I1OZr5vt+x7PG+DD64/d0tV4LvfkOZr5vt+zz2et8GHom1/bGKfy8F3/oczXzfb9m92JvJBirquZZALmN7BrdosSGHeD57UjUTei1Z8H6z+hr1aE6ebzXFG3zVZYouaDbO92HgYxgNLIOapay/GY6A92p7qqdTPRirv1tfpmzSw05rSeS6zVDfxvgw+u/06ytbwXe/Iu5mvm+37Hs8b4MPrv8ATparwXe/IczXzfb9j2eN8GH13+nS1Xgu9+Q5mvm+37Hs8b4MPrv9OlqvBd78hzNfN9v2PZ43wYfXf6dLVeC735Dma+b7fsezxvgw+u/06Wq8F3vyHM1832/Zm7E3xwkuJw/jiPDGkgkzA50zprHmYWKqGsfJtcC5FaeMVR07NW7M1+u42cLQVKppXv8AY7tG4YBlIIIuCDcEHkQeyuMdUqoBQCgFAKAUB8y75bwPj8ZLOWvGGMcC9SxKbAjve2c+cDkBXd5PoKFPTe1+Bp153lYq9imL4UctoyZFV0iDgzujkKriIalST++tnnFPSa4b93eV6DtctLuvtAl1GEnJTygEa63Fx+ys84pZe8jGrlwPG3ax4EhOFntF750D0LKH1/VYHzGmvpZe8s9g0JcD0bsY+6r4rPd1LKMjaqLXP7Rz7RTnFK19JDQlwM1NxtoFUYRjKwQk3PQ4jMgDi1wVKnNYG2lQ53Sva/H7esjOrkYcu6+OU/i8rDiGIMqMVZ1JWym2oupsamsRSf8AcuJjQlwMbGbFxUIcywSoEy5sykZc9wl/OQQPMalGrCVtF3MOLW1GCpYMrIxV1IKsOat/l1EdYrFanpx69z6wrbHse032/bEYuXDCeWaKBgLyCMXltdj7mqghb5RfrDd1aeE06y06maWzzJSo06L9xWZewu6ytDh2afLPigxw8IjLB8jZLNJeylj3WHXWxLENSkkso7Xf8GVTuk77TJj8HeOZiofDW0s/FORiztFlBy3zB1ykW5kc6g8bSS3931M6mR5H4PMaWy58NyQg8XRuIXCqpy6teNhbzVl42na+e/dw/wAjUyPIPB7j34YHBu1rrxOlFmQyLxABpdQeWajxtJX2923dkY1UjJm8HzpA0r4iJGRXLq2i9CQR2Vr31vzIGpA67iKxqc9FRve3hcy6Vle5RtHwdYtJHWNo2UMcgdgsjopRHkCC4yKzgHW/dypDGwaTf67PqHRluNdtbc/E4YMZHw9lRn6Mt82R+GyLdRdw3MVbTxMJuyT7vqRlTaI9dgQysVdTdWHNW7f/AB11ZUpqatv3PgQy2PYTXaWMZdl4fGJjJzPO/B4ZTD5UdM3FOkYbKAptrfpp31yadfETq6pvtyLHg8Oo6Wj92R/dnYYxDShpOFHDE08r5S5yra9luCzEntrpTkqMUora7JdZiK0nmbMblTSLxcPJHJEwLRliY5JI1KK8nDINlR3Ck36ri9xePOoxejNWe/er9vWZ1Taui9P4OsctulhmuypZZSTdpBDyy8ldgD2d/KorG0nx7uq/gZdGSPF8HmOJsGw1tAH4vRZyzRiJTluXzIwta3fWee0+vu+t+wxqpF3DeDvFZc8zxxhoXlWxzWKKGyvoFAte5Ba1uVReNhe0c87f4M6p2uyvGeD2RRLkxELmKVkkYnJHGiR8Rnc3JUjQFbHmNaRxqdrxeay4vO2Rl0WYeK3CxsaSu5gHDDsV4nSZI8pZ1GWxWzqef5Q69KnHGU5NJXz6uJF0pIj+0cG0MrxMyMUNi0bZkOgOjdY1rYhJTipL7kGrOx0jwJbyuJG2dIxKFTJh7/kZfLiH82xDAdVm7q4WOw6pTvHYzcoz0lZnY60S4UAoBQCgLOMPub/FPqNAfJeD97T4o9Qr0+H6KPYvA50/iZL8FvvLH4u/i+GaaBBEkzqxfhLcZNGtfKSuYC9iarlhIyutJ2edt1ySqtWL6eEPErlCRQKiBVRfdDkRI3iVbl7nRybnW9qi8FB5tu77ONzKrNF1PCFKMOU4ScfP0X6WVE4C4e4GbWSynnca1jmUdO98v3fuGtduv9WLkXhOxSvnEEGt2ce62d2yAuenysg6PLnWHgINWu/sNdLgYXs8xB8qHDtpHYWkUK0LySowCv2ysLcrAemfM4bm9/DekvwY1j8PsZI8JWLuG4UGfMpLWk6So7SIls9gAznUakWvUeY09l39uwzrpGl2lvLLPFwnSP3qKLMM+bLAXZTq1rnOb6ea1XQoRhLST3t95BzurGni8pfOPXVz2EUZG2GJxOKJ5nEzE+cyvWrgegj9fEtrfGzMwG8+Ohi4MU7pGCSFGXokm5yki63OtgRVsqFOctKSzIKckrJl6XfDaLMXOIe/R5KgHubZ1NgtgQ5J5annesLDUkraPjvM6yXEvYPfbHxxuiy6sFAcqudFQuQq6WFzI2pBOuhFRlhKUmm19PXYZVWSRZj3w2gBGoxDWj0UFUbqyjNmU5rKbdK9qk8NSd3o7e0xrJcSlt7doG98Q5zBlNwhuJCGYWK9ZA81tLU5tS+Xx3GNOXEqffHaJDKcS9mbMdEve4Ohy3AJUEqNDbUc6c1o/KZ1kuJj4jePGOrI87FXDKwITUO3EYeT1vrUlQpp3S9bDDnJ5XNVVpEvsx4EK30GIxJA7Lx4G/8Avvrm0l/1k+zyL5dEvXEubL2nPhpBLBIUexFxY3B5ggggjuI6q35wjNaMldFKbWaNlJvjtFlZTiXIY5jon802BC6L0V6IsDblVaw1FZ6JLWS4iHe/HK6OZi+Vw+VgtmtIJyDYA2MigmxHoo8NSatb1a3gNZIuyb77RMjyDEMpfTKqplUAswCqQQCCxs3la86wsJRslojWSve5jy72Y9k4ZxD5MhS1kF1ZchuQtySulzr31JYeknfRzMacrWuXDvltEtmOJa97nox2Y5chzDLZrrpreo81o2to+JnWS4lmbejHPmzYhzmDhrhdRLlzjyeRyL5sotapLD0lsjw+2wxpy4mvx2MkmkeWVi8jm7MbC50HUAOQFWRiorRjsMNtu7N34Nz/AP1cB8o4/wCTLWhyn0S7fwy7D/EfSNcM3BQCgFAKAs433uT4p9RoD5LwfvafFHqFenw/RR7F4HOn8TL1XES5hoGkdI0BZnYKoHWzGwHzmsNpK7BtJd3MRciPhzlQS3i7iTJl5hhob87WvexteqlXhvy7ciWg92ZV7FMdwmm4D5RYkWObKVZs4HWtlOvmrHOKWlo3M6uVr2KE3Yx5IUYWa5XNbKfJOl/n0tz1FZ5xS26SMaEuBqSKuInlAVxeUvnHrrD2BF/a34xif6RN9q9auB6CPreWVvjZi1tlZ6LdZsOs2vYdtuugOgxboxTYh4jhzBAjNw545S7YiPMqq9jnDAhg5KqoF7Ei1c54lxhpaV3vTWzw7C/Vpu1sijBbpYIl4L4iSTJCxdTGBGJJMpZQfyVUEtmvpytzrMsTUylklnx3L1YyqcdhjSbo4SOIyvNMVWPPdDEOPdY2zQ3BsilypvfUeipLE1HLRSW3ry27SLpxSu2RTa+EEM88KtmEcrxhvzgrFQdO0CtunLSgpcUVSVm0YlTMCgLp95i+XxH2eBrnUv6yfZ5F8uiXriWq6JQKAkuw9mq+FMiYYYmTisjqZGTgxhFKsMrC2YlumbgZLVrValp2ctFW4Xu/W4sjG62XNxtLc3B4ZQ7yzMAACoKauZEjvmKLeM573A5A2JveqIYqpN2SXpX7ybpRRexe5GFMr2aeMFyOGTFeFC8wGIa+pw4Ea/zukNaxHFz0Vsffnsy7c+wOlG5HN5djQQKpieRjxDG4codRHFJmXKBZfdCNb+TWzRqym/eW6/3a/BXOKWwj9bBAUBI/Bx/KuA+Uf7GWudyn0S7fwy/D/EfSNcM3BQCgFAKAs433uT4p9RoD5LwfvafFHqFenw/RR7F4HOn8TL1XETLwJmjeOaNWuh4qNlJHuRzM3YVW2vZ11CWjJOL7O8yr7Ub7Y+9kkcjDDYTDq8pBsnjBZn1Nh7rcr0j7n5PLQ2qiphlJe/J2XZ5fcnGo75IxIN7pVZ34cDMzK6k5/c3SIwKygPY9Bjo1xc37qm8Mmkrv078OJjWsuzb6zHlHh192E7W4hzTcRJWc3c2zNGt1GgA0tzrCwsVvey27Za3DrGtZHpJczM2lySTbtJvWwlZWIFNAVxeUvnHrrD2BF/a34xif6RN9q9auB6CPreWVvjZi1tlZvt3N3PGwp4qJfExQHOyLdZL3K5iMzi2iDU1RWr6t7L5N9346ycIaR7DufMUWVpIEiZBIHYvYxlUZmAWMscpkVCLXzNblc0eJinopO+z69/VfsGre0ysfuSySOoxGHCqxtxDLmCGY4dWYJEQM0mml+dzYXqEMWmk7P7cL8eBnVZ2R4u4WKJKl8OHW3EUtJeIFXcFiIyDdUPkljqNKc8ha+f2z+/iNUzE2lurNBG8jSYdsgzFUZ2bJxeAHByBcpfqzXseQ1AnDERm7JP0r8eBhwaNFV5AUBdPvMXy+I+zwNc6l/WT7PIvl0S9cS1XRKDN2NghPiIYS2USSKma17ZiBe3pqFSehBy4GYq7sbn2FyskbJLA5Kl5CHDJGgeRTJnTMCiiO7W1BYCxqnnUU2mn1dy88ieqdio7lsIixngV0LcUNxMsQCwEISIyTJedRZbr31jnS0rWdt2zPb17MhqsrlI3Gnvbi4UDiCAtmlsJyyx8E2ivmzMNQCv8AOrPO48Hsvu2bb7f2NU3wPG3InVBI8uFReHxGzNJeNbKwzBYyTcOPJzDttTncG7JN7t3mY1bSuaHH4RoZZIXtmjdo2sbjMhKmx7Lir4yUoqS3kGrOxYqQJH4OP5VwHyj/AGMtc7lPol2/hl+H+I+ka4ZuCgFAKAUBZxvvcnxT6jQHyXg/e0+KPUK9Ph+ij2LwOdP4mXquIkl2bvQIcOkITpLHiFz5ELB5vIKMdQoPlDr761p4fTm5N719tv6LI1LK3abxd8cLFO5RWEYKMDAqHiMeLJOh4lisbSSjUdUCi1Uc1nKCvt6/ols32X3J6xJmGm+kREoeNyuUBECRWdBCYzDIeYTiHiXFz+ypc1d1Z+PG919MjGtXA3WN3wwUTrlPGJVjmWMMIVZ1YQAEx3TKMvP8lbg3IqmOFqSWeX5y27ybqxTIjvDvCmJiWMIRkdCl1QBEWJY3UZddZBmrco0HCV7+r38CmU9JWI9WwQK4vKXzj11h7Ai/tb8YxP8ASJvtXrVwPQR9byyt8bMWtsrNtu9hsVPIsOGazhuOovl90iBKsP5+th56pqyhBaU+z6MlFNuyNxhsFtURxSQ9EYeHKojJuI5RFOxIbQsfGUJH83kMoJqlKhdqW97+KuvwySU7ZbvX5LLw7ajdpyuKDqMhbLc2d8+W1jf3Rg3LQkHTSsp4eS0bq3r8C1RO5l4nGbaWJIeFKni44hcZ2ci0i3Ys7Ai3EuoHUbjSoRjhnJyvty8P0ZbqWtwNLtz/ANQj6OK4y8RSLPpmUPxCNNLCQhrdRIq+lqnnC2XlbwIS0ltNNVxEUBdPvMXy+I+zwNc6l/WT7PIvl0S9cS1XRKC5h52jZXRirKQysOYI1BHfWGlJWYvYlEOx9oxoydDJJhwoJYm0M3ExLKlhzPAfMCDa/fetV1aMnfg/urL85FmjNL12jaOz9tkNBIuIdU9xIFmU+R0cw5+ShuepQTypCeGXvKy3hqpsZk4DaW24WaUxzSFbQ+6hyFYsgFlVlzsXZBchr3FRlTw0lo3S35evIypVFma/EQ7Y4Tq64jhRpla4Fglg1iR5S5QD12A7qsTw+kmrXZFqdrPYR7ETM7M7kszEszHmzE3JPeTWwkkrIhe5brIJH4OP5VwHyj/Yy1zuU+iXb+GX4f4j6Rrhm4KAUAoBQFnG+9yfFPqNAfJeD97T4o9Qr0+H6KPYvA50/iZeq4iSXc7FYNBiFxQTLIYkBIuydJryL8U5WPaARWtiI1HZw3X9fUsg453JBip9ky2DDClRLmYkyRvwy+I6MZjIvzjuDfotfqFtaKrx47O3PLbf6ll4Mwtl7P2biFiCxxCaROhEsmKZjPknLRyqGLLACIrMtmIv0jrayc60G7t2W+y2ZbOvb5GEoO1tpm4rZWxI3aN8gZZlWQcaYFBmjzKoLXaPKXudWBv0hYCq41MTJXXDLJdfr8GWqaIVtngFomgVVDQozorOwSU3zqDIxbqHMnnW9T0rPS4vu+hTK18jX1YRK4vKXzj11h7Ai/tb8YxP9Im+1etXA9BH1vLK3xsxa2ysytnY+SBmaOwZo2jvrdQ4sWUgizDmD1GoTgpqz7TKdnckeJ3kx8sck8mGR4XPSfhyrHmth1BzK4As2GjNr2uWHWANdUKUWoqWa61ff1dbJuUnnb1l5Huxd4Mcz8SLDiRjPI4eNHYxmUpLMiDNlNxGp6YJAvrroq0aaVpStkvtkvSMxnLcjzaO/Ohiw0Yjg4YVVzyoQ3uhLgxygkHinosWGgPdSGE3zd39OriurqMSqbkaPa+2ZcT5YQe6yy9AEdKcoXGrHQFBb03Jq+nSUNnUu4i5XNdVhEUBdPvMXy+I+zwNc6l/WT7PIvl0S9cS1XRKBQEnwe8uPmHAjjWS+oRY5GKgQHDEizXAyNc9Wax01B1ZUKUfebt3cb+P2LFOTy9bLFMm8OJefL4tFxDJKXiCzXkedBHMGBfMpKryXLlN6yqMFC+lllnllbNbjGk29hs598ZYo1Z8PkxOVDCxVlRcOJIpVUBnu6EwgXIvqTm6qqjhVJ2Urx39tmuHX+ibqNLNZmnxO988mmWOwDgZmnlIEsfCbpyys3k6jXQ92lXLDRX24LY77kQ1jZH62CAoCR+Dj+VcB8o/2Mtc7lPol2/hl+H+I+ka4ZuCgFAKAUBZxvvcnxT6jQHyXg/e0+KPUK9Ph+ij2LwOdP4mXquIigJwu6cUuGgaOOVXZAzM4lDSOYJZgsasvDlVmjAHDbMARcEmtHnEozaby+nFLPevqW6u8U/Wwy49zsJHGBOJDISsdzcZHmbDKrMuYWMZmOnX1g2tUOdVJS93Zt7r+NiapR3mh2nuwuGgMkzTI9lCx8MDpu2KVc2YgquXDBr2J6fKtiFd1JWja3b/ALfMqcLLP1t8iNVskBQFcXlL5x66w9gRf2t+MYn+kTfavWrgegj63llb42YtbZWKAl+xd6MNFDAskckrxFbXWMZFEvEYLIDmZbE9BgRmbnyrTqYecpNp2T7eFtn5RZGoki8d8YI4GggWcHg8JXYRqSbKMzBWPZ31HmspT0ptbb7zOsSVkU7T3vh4cy4ZJUeVnbM6xdHiyI7ILE9HKrLfnr1VmGGlpJzs0rcdyDqK2RDK3SoUAoC6feYvl8R9nga51L+sn2eRfLol64lquiUCgNtu1tOPDyO0hbK8ZQhUjlDAsrZXSQgFejfQgggd9U1qbnGy49a8CUWk8yRwb34JGzrBMrXKhegwCcd5wcxbNms+W3VbnWs8LUas2vSsWKpFZ29XLU+90EvEaVJiwDiLSMi0uHSCzEm4CupcWv5VSWGlGyjbdfbud/0YdRP11Ec2/tRsTiJZiTZnbICFBSPMxRLLpoDatmlTVOCivTISlpO5rqsIigJH4OP5VwHyj/Yy1zuU+iXb+GX4f4j6Rrhm4KAUAoBQFnG+9yfFPqNAfJeD97T4o9Qr0+H6KPYvA50/iZeq4iZuxtnnETLFmCAhmZiL5VRWdjYak5VOnWahUnoR0jMVd2Nq27LtGs0EyPDwzNmk9yaJFaRXZku1gHiIupNyydtVa9J6Mlnsyzvs89/WS1beaKk3Hxd8rGBLvkBeSwcsQqZbKbhyTlPXlblasc7p7rv6etm8apno3IxhRZXMKKycQtI5GUEKwzdE6kMOV+w2OlY53Tvoq/0M6qW00GNwrxSSRPYNGxRrG4zKSDY9YuK2IyUkmt5W1bIs1IFcXlL5x66w9gRf2t+MYn+kTfavWrgegj63llb42YtbZWZmxnhXEQNOLwiVDILXugYZrjrFuY6xUKik4PR22yMxtdXJhG2AkCDHS4WSQZiZIM0YsWj4SHhIoK6S5tLojCxBtWm9bG+qTS4PPjfb9LcWW+6/iaPdnbEwUpgRYVaaaAzZGfEcOMo0cRF42LlHtPICT/wxex1Tq1I3beSdt19735ZZLvChF7Nv1PcVhdiRh7BGZHmFmmmBLIZ8iEK2sZtEAwsT1sbmsRliW19Ny6vvt8g1TRENuCATvwLcKylQCxAJRSwBYlrByw1J5VuUtLRWltKpWvkYFWGBQF0+8xfL4j7PA1zqX9ZPs8i+XRL1xLVdEoFAS/ZWKwww0al8MEEUwnikQcWWds/BZWy5rAmLUMMoVr9+pUjPTbs75Wa2Jb/zuzLYtaJkyYPZBMzIoaOKEzXWSa7SK7IYDmItGxePIwGYqlybk1BSr5J7W7bFstt7VnczambDEbD2XC0RmSNVkWRog0mJTiIPFsjSlmBWSzTeTZCdNbWqtVq8k9F7LXyXXs6tnWZ0YJ5+thG94U2cIrYYKHVo7EPKzOrI5kzZzl6LBBoq862aLraXv7M+H0K5aNsiN1skBQEj8HH8q4D5R/sZa53KfRLt/DL8P8R9I1wzcFAKAUAoC3OmZWXtBHzi1AfJeHjKqFYWZegwPUy9Ej5wa9NhpJ0YtcEc+orSZcq8gXsHi5InWSNirqbqw6jy69DoSLHneoyipKz2BO2aNi+82NN/drArlKqkaqUAdQmULlyWkfo2tdibX1qvUU+Hj63EtORnbO30xEMgkCI2WGOFFYuVQQ+Q1s2rXudfzja1VzwsZK197feSVVpmtbb+KKZDJpkCHoR5igtZWfLmYAKALnS1W6mF728SOnLiYOJxDyO0jnM7sWY6asTcnTTnViSirIi3ctVkFUZ1HnFYYRlbbjK4rFqea4mYH6xz6iD6a1MA70I/XxLa3xsw63Co2u6+EhlxUaThjFlkZwhs1o4pJND23QVVWlKMG47cvFIlBJvMlQ3RwLRIUkZgIwWmS5zsnjPEZFJAykwWF+rXrrU5zUUs19O61+8s1cXsKI/B/CwUieXpyIq2hZgqycHSRlBRHyzaXYA2HO+meeyW5ZJ7+3ZvtkNSuJVszcrDPGmIDzNGc3RdMuZbSqDnQlQweO+XMTbmBfXE8XNScbK/+OPkI0k1c0G9u7wwZgAaRhIha8icM3FgbIekBc9Y8xNbGHra2/V9SE4aNjQVsEBQGVLh3XDYeQjoviMSFPmTBj1xv9E1zKUlz2fZ5GxJfxIxa6ZrigJ/szdjZ8iQ3ZjM+GicxZm0LtHmmuPySJAoXtBrnzxFVN8LvP8ABcqcbFsbjYd3yrNKpFmYcPN0XSaRUiykuz+425Em/XbXPO5pXsvTSz3bxqlcYfcXDmVIeNiSzK8mkBXLGknC1QjiZ8zLcZNNToOR4uejpWW5bd9r9n3CpIbT3IjSGaRWkzQw5jZDldkMgZy7HKt8q9AG/YDSGLbkk978vVw6aSuQSt8pFASXwZxltrYGwvZnY9wEUgv85Hz1zeU3/Eu38Mvw/wAR9H1xDcFAKAUAoBQHEfCtuPLDNLjsOheGU55kQXaGQ+VIANSjHpHsJJ5HTo4LFql7k9ngUVqWlmtpzhGBFwQR3V201JXRptWPayBQCgFAKAUBItyN0J9pSgKCuGVhxZuogHWOM/lOeVxovM62B5mMxkYxcIPPw/ZsUqTbuyT+GHdCSKZ9oQqWhkAM4UXMTqAvFt+YVAv2EXPOtXA4pUnoy2P7MsrU9LNHNgb6iu5tNMEVkHhUdgpcDKOVv9/7J+elwCo/3/vuHzUuD2gFAZmx9lT4uZcPh0zSN9GNeRkc9Sj5zyFzWricTGjHr3Isp03N9R27b/g+jk2VHgYSBJh7SQu2maYZsxa3U+ZwezNfqrgQqyjPT3m64pqxwieJ43eKRGjkQ5XRtGU/5dhGhHKvR0a8KsbxNCcHF2ZRVxE8yjspcAKOylwe2/359D+ygPAAKXB7QHjuALk2FRlJRV3sCTeSOz+B7c6TDhsbiEKSSLkiRvKjiNmLMOp2IGnMBRfUkDz+MxGunlsWw3qVPQR06tQtFAKAUAoBQCgIxtbwf7KxLF5MKmYm5aMvEWPeYmW/pqUZyj8LsYaT2mD7VOxvg7/1jE/eVPX1PmfezGhHgPap2N8Hf+sYn7ymvqfM+9jQjwHtU7G+Dv8A1jE/eU19T5n3saEeA9qnY3wd/wCsYn7ymvqfM+9jQjwHtU7G+Dv/AFjE/eU19T5n3saEeBdw3gw2MjBhhQ3dJJNIv0XcqfmrDqzas5PvCilsRLIIURQiKqqosFUAADsAGgFVkisi+hoCEbZ8Fey52LqkmHYm5OHYKCfiMGQehaup16lP4XYjKEZbUaz2l8D8Kx30oPuas57X+bwI6mHAe0vgfhWO+lB9zTntf5vAamHAe0vgfhWO+lB9zTntf5vAamHAe0vgfhWO+lB9zTntf5vAamHAe0vgfhWO+lB9zTntf5vAamHArh8DOzwQWnxjj80vEAfSkQb5jR42u/7vAaqHAmuwdgYXBR8PDRLGp1NrlmPazG7Me8k1rNtu7LDZ1gGj3k3SwOPA8YhDMNFdSUkXzOtjbu5VKMpRd4uxhpPaRF/AxgCTbEY0DsDwm3drET85rY57X+bwIamHA89pfA/Csd9KD7mnPa/zeA1MOA9pfA/Csd9KD7mnPa/zeA1MOA9pfA/Csd9KD7mnPa/zeA1MOA9pfA/Csd9KD7mnPa/zeA1MOA9pfA/Csd9KD7mnPa/zeA1MOBvt3fBzs3BssixtLKvKSds5U9qiwRT3hQapqVp1PjdyUYqOxEtqskKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgFAKAUAoBQCgP//Z</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUSEBMVFRUWFRYVFRcXFhYWFhUVFRgWFxcSFRUYHSggGBolGxUWITEhJSkrLi4uGB8zODUsNygtLisBCgoKDg0OGxAQGy0lICUtKy4tLzAtLS0tLS0yLS0tKy4tLS0tLS0tLS0tLS0tLS0tLS8tLS0tLS0tLS0tLS0tLf/AABEIAL0BCwMBEQACEQEDEQH/xAAbAAACAwEBAQAAAAAAAAAAAAADBAABBQIGB//EAD4QAAIBAwIEBAMFBgUDBQAAAAECAwAREgQhBRMxQQYiUWEycYEUI0KRsVJiocHR8AczcpLhFRayQ4LC0vH/xAAbAQACAwEBAQAAAAAAAAAAAAAAAQIDBAUGB//EAD0RAAEEAAQDBgQEBAUEAwAAAAEAAgMRBBIhMQVBURMiYXGBkaGx0fAGMsHhFEJS8SMzNIKyFVOS0iRicv/aAAwDAQACEQMRAD8A+301FShJVahClCFVNCq1CSFz0uq5C7Biu/xBbZW+VxU8jqJrbdRzNsC911PKqC7kAXVbn1YhVH1JApNaXGgm5waLK7IpJrkihKkNnXILcZEEgdyBYE29LkfnUwDV8lAkXXNDdKYKRCXkjqYKqLUIipKKqhJShC8v4+0Msy6Pkoz4cQ00j474xqXyc+wuKg8beasjIF30Xqamq1VCEGXVxrfJ1Fsb3PTM4pf5nYUK1kMj6ytJu69BZ9hqUehVKqEKUIUNCEroOJQzgmGRXCmxx7GhaMRhZsOQJWlt7WjtMoYISMmBIHchbXIHtcfnQqgxxaXAaCrPnt8l3QoKUIUoQh6idUUs5sBa537kAdPcihTjjdI7K0WfsotCgqoQpQhShC26yLeqvQkpehCuhCq1CFTjY29DTG6Dsvn/AA1J4EhaNGZRBLKhIJxdkAdCP9ahrfvGu/MYpXPDjRzAHxF6H209FwYRLC1paLGUkeBrUe+vqtHU6h5tNKGkkblTxOGwCM8IKHOwUbAhyCP2RWdjGxzNIAGZpG9gO1038h6rQ9zpIXAknK4G6okaa7eZ06I2q4tKj8uPmMM9O6nFmP2YheY7Ei5JNxvvv7VBmHY5uZ1DRw3/AJuQ+9FOTEPa7K2zq07fy6Xf3a6+1ahY+ZJKwDzNGSI1JhSNpBku25bFRuD1pdnE5+VrRo0HfckD5WSjPKGZnOOriNtgCddudBVwrVs82meXLJ9PJG11ItKjqXVgB5dgT2onjDY5Gs2Dgd+RGnmiGQukjc/ctI25gi/JelZa5trokIbx1IFQIQGhFTDlAtCEY6laiWrgrTUaWH4o459kGnITPn6qHTfFjjzcvP0N7Y9Pek40m1t2tqpKCqhC8f4k0cjy6hlaQAR6U2UCz2la97gm67kW+t6F6Xhs8bIomkAnNJqeXdHjz219FT8b1Niq5lo01Su3L25ql2hHw2Jwj7beYX60Jjh+GJDjVOMZAzfymg/n1PnpouU4trUvzDcXeK4j+EqY2+0ED9x226eT50rTdgsC+sgo6OrNveYZPcDXfVHh4lqXESRyNczyxM7xi/LsXjkK2A+AXG1qFU/CYaMvfI0UGNcAHaZrpwuyd9+a2+GatptPkwGeLo4HaRLowA/1A/nTXKxULYMTlb+WwR/+TRHwXm+HcQmXSwrA7mQPBG6vCQsYYMhFyoyAax6np70l3MRhoX4uR0zQG09wIdZcQQepqxfJE1Mk8sunTMrKsmpgkdQAcVCOHHZSyKv+6moRMghhlflthEb2g9TYrxok+yo+IJrREs4KLDzAI75vmRqA5xOIRVvtb4h7UWn/ANMhDn6Agl2U5qoVcda65ia1vZO6XieoErNKRyRqmgAxAOL3McmXpdkX6mkssuEwxhDYx3+zD9+Y0cK9CVz/ANTk+zzFWkbUhWZkKMBEA5BCeXG4U7dcsb70J/wkX8RGHBoisAGxbtL11vU77VdLP4xrpX04UyM5OnyXli4mkDnLI49FVQTa17k+lC2YPDRMxBcGgU+jm/lbWla/zE6b9Oq9tG9wD6gH86a8s5uUkdFdCSlCFKELZrKtyuhCqhCuhCgpIV0JqUIUoQpQhShClCS5IpoXBFNRKE4qYUCgsKkFEoTVJQKyuOcHi1IiE1xyp450scfvIycQfUbkW96CLSBI2WgakoKqEK6EKUIUoQpQhVQhXQhVQhXQhUaEK6EKUIVUIUoQrC36UJ0u+SaWYJ5StYVlWxUzUwEiVmcd1jRwkxmzFkRT+yZGVMt/S9604aIPkAdtqfYWs2JlLYyW76D3NWs3ScZEOSFdU7czAK/Ld8sMyFIbcW33PfatMmGMlOBaBV2LAq66eizsxQjtpDibqjRN1fX1T3/cUIeVDkOShdjYWsACVAve4yA3tvcdjVH8FJla7+o0Ff8AxkeZzf6RZQx4qgxRiJPOrsAFDECNir/CT0sTcbWFS/6fLmIFaUPcaffVR/j4socb1v4boc/iDl6l42DOhELKVtZEeylye4yddqk3B54Q4aHvepGtewKTsXkmLTqO76A6X7kJrVeIY42cMr4pmMwBizxrm0a73ytfrtsd9qqZg3vAIIs1p4E0D96qyTGMYTYNC9epAsgenor1vHVQSYrkYzEGyIVRzdwzPvioHU2ojwhcW2d78Tp4aJyYoNDqG1eA18dUSPjUZnGnscygc7qVBIyxuDe9t72tuN96icK8Rdryuvv7tMYlpl7LnV/f3ST4xqJPtUUatKF5bOREFJJDoPPkPhsT+dW4djewc4gXYGt9DtXNVTuf27WAmqJ0rqN75JuLVytq5IxjykjS/wC1k+RDX9PKRaqnRsEAf/MSfKgrWyPM5Z/KAPOzf0Sem4yywyzz2wErLHjYEgO0YQ3Nr3HU26+1XPwwdI2OPehftdqlmJIjdJJtZA96r90zDxRZGQRqzZRrKTsAiPfHK53Jsdh6Gq3YcsBLjsSPMjdWNnDyA0bgHyB2SfB9VI5mDqQFmkCkkXFiLJYeg73q3ERsaG5TuB/dVQPe4uzDYn+yfas4VxXkf8QtFLKui5KM+HEdLI+IJxjUvk7AfhFxc9utJ3JNhAvyXqDViqWfxzVtFBJInxAWW+4DMQoY+wJv9KFqwMDZsQyN2xOvkBZ96WRpuKjTs6ONVIwaNLPy3Jdw5BQhtg2PQ7DbpvSXSlwZxLWvYY2inGxmGgIBuxuL33Ou+ifHiGHmmI5KVi5rEgDEBQxVhfJWCsDuPbrTWM8Mm7ISiiC7KK56kAg7EEjr47IEfiuAoj4yfecwKoUM148br5SbmzX29D0tQrncGnD3Mtvdy2bod66Oo8K9Qga3xKIpzs0kbaeOZcbWVMpM5ST2tht8qFbDwkzYcbNcHuabvU0Kb73qtDUcdjSQoVeynEuAMOZgZBH1vfEX6W7XoWOPh0kkYeCLOtc6vLfSr8b50uNRx9ArFVJKxRS2OwCzGwLEXsF6sbGw9aFKPhj3OaHEAFzm9dWjkNLvZuup6LpOOx86KAj7yRA+xVlW4ZgMgd9lbcC3T1FCieHSdi+cflaa1BBOoG3LcaHXfolvEM8gmgjRplDLKzckIXJTl2+MWt5jQr+HRxmCWR4aSC0DNda3e3PRNtrJTqxEoXlrErvf4ruZAGB9igFv3vahZxBEMH2rrzFxA6aZbHxu/BLafi7qNTLNjyopGVLbNdGKFDc2JJCkH972oV0mBY4wxRXncATe2oBv01vyTWl4ysvK5SM3MTM/CMEDYksb2O97WvexoVMuAdFn7RwGU1z1NXpp03uqtccE1M0k2oRlOCS2Ull8vkjsgUdjcte/f8kTSsxeGiZDC5h1LddDrqdb8NvTovQx6Ud6gXrEI+qOEFQtTpXahOlOZSpGZDZqkAokoOp06yIUcXVhYj/kdDU2Pcxwc3cKD2B7S12xSel4PCjAoWuJOZu5Y5FCm5O/QmrXYt0ltNbV5a3yVbMKxlEXve/Oq5oh4ZHnIxytKuMiXGDXGOXS4NvQ0u3flaP6djzCfYMzOP8AVuOR5K9PwqJcCS7lEeNciPge11NgOgFh8zQ/EPddULIOnUJthY2ibNAjXoUKLgcQVlYu2USQkki+Md8SCB8W43/dFSdi3kgihRJ9TuoNwzACDZsBvoNvVETgMNyXLvkrAhm2ydcHkCgWDsOp9zUTi5KAFCq5dDYHkFMYWPUus+Z6iifMqo/DsKghXlDNbJ8/MxXKxa4sdmI6Wt8qDjZCRYFDYVoPvdDcHGAaJs7m9SmdLwaON1eMsuMaxlQRi6oLLlcXuL9iOgqt+Je9pa6jZvyvelYzDMY4ObYoV5gbWuuIcJSV1ctIjKCoMblCVYglSR2uBSixDo2loAIPUWnLh2yODiSCOhpKxcJYaqSUvJiyJiQ9vNeQFSoFmCgi2QPXvVrsQOwayhYJ5ctPnzpVDDnt3Ps1Q589flytA4f4fHKljmLkPI9rvey8wskijoGOxO1TlxhztewDQDl4UR1pQiwgyOa+9SefjYPS+adPBlJVuZLkFVWIfEyBSSA+IHcnpbrVP8SaIyit9tvJXfwwsGze2+9dUSDhaI7upb7w5Fb+UNYAsB2JsL1F07nNDSNvdNsDWuLgd/ZGbTVAPUyxef8AFnGPsY05wz5+rh0vxY483Lz9De2PT3qWdR7O1rNFUg5QLUvqdMrqyOAVYEMD0IPUVK0Mc6Nwew0RqFl6bw/DGclzuXRyS7MS0YYLu1zazEflTWuXiU8gyuqqI0AGhonbyRm4UhlaW7AuuEi7YOLEAsLXvY9iO1CqGMkEIi07psHmOen7hC0nAo4+Vu7ckvy8iPKHUKV2AuLD50KybiMsmfQDPWar1IN3v+yHB4chW4OTAwtp9yNomYtiLDtewPoBQpv4pO4gih3g/wD3AAX67+quHw/EGDM0jkbkM3lZ8OXzCoAGeG1/570JP4nM5pa0BvkNQLzUDrpev7Ien8MwoPK0oYqFz5hzspUpfsccAALWtf1oU5OLzSHvBtWTVaa3fjrZJ13R9NwOKNo3jLqY0EexBzQEkB7j1JO1vyoVUnEZZWPY8A5jfkfDXoOd+6LxLhSTFGZpFZMgrRuUNntkLjscRQq8NjHwNc1oBDqsEWNNvmlP+kN9r5ucmHKA+O3mVtlIHxLYk733vektP8c3+D7LK28x5ciNT4G9NK02QtBwHbUJMZGWR3td9ijhWL4jYPlfe3amp4jiWsTogAWgctiLFWdarla0Y/DykIWlmBVcMw4RnQm4RioAtfpaxqt8jWCyVXHi3kupjaJuqsA1uLJ9bsLV03CkjmeZS4MgGS5HAkADPH9qyqL+3ubwJtRdO50TYiBTdjWvWr6WSnaSpUoQpQhASplVhClksR6Xsfa/Q/K/61nnmdEWk/lJo+F7HyvQ+YPIq2NgeCOe4/VEaStNKm0CPdm+n6Vkh/z5fNvyVz9Y2evzRmIAJPQCrppWxML3bBQYwucGhdxXsMuvf29qjCZDGDJ+bnXLw9Nr5pvDcxy7IlWJKUIVg0k7XV6KTtXnSpO1M6KRmXJenSWZcmU08qWYrgzGnlCWYobSn1qQaFEuKyOPcIi1QiExYcmeLUJiQPvIicQbg3BuQR708oKQcQny9SpQtck01G1zQkqZwCASATsBfqbXsPXYE/ShC6tQhco4YXUgjfcbjY2P8QRQhUrgkgEEqbMB2JAax9DYg/UUIXdqEKWoQqoQpQhF0MeW57GxHv8A0rHBiC9lO/MNHefh4HceBWl0IDrGx1H34bFNaz4f/cn/AJLWfHf5X+5n/Nq0Qfn9D8iik1sVCFzbtiOgHm+Z6Afr+VZxKXTdm3YDveZ2HtqfCuqsygMzHnt+qJetNKu1L0Ui0qk4vbv6Hv7j1qsTxmQx3Tuh0vxHUeSMjg3Ny+9+i51LLY36W3qU/ZiJ3bVlrW9qUWF2cZN+SzJOIHoo+pry2I/Epb3MO2wNMztz40K+PsupHw2+9IfQKl4lIPT8qwD8Q40GzlPp+60f9Ph8fdNwcQVyA+xuCPQntXXwnGYMW5sc4ymwR/STy+OovmBqskuDfEC6PUV6rRzr0lLmrhZwb23t37fQ96pinjlJDDdc+Xodj41srHxuYO9+6wvFmj1cyKNHOYWCykkW8xK2RDfpvffsbGriFAEc0GLU8VPmZIAMohgBdsTKRMwbmgbRjyjqb36+SiinoutRLxJJpuWsbxNLHysiLrEBAJCbuOt5rDthfe4BKRYR+ES60vnqVC3iZSqlcBIshKsQHYglGUbX+Fr/AIaKSJCU0eu4nYGWFMsEuFMYXmYNkou5OGYF2uTYgBepBRTJCDFxHijMQYogAyK1wAcTGxZo/vSG8+HfYG3mIIDopW1bK690gRphaUouS3B+8sLi67db9NqyY7FtwkJkdvyHU/e6tw8Jnkyjbn5JbhXEiSUkNySSp9z+H+lcbg3FnSPMMx1JJB/T6e3Rb8fggxvaRjQb/X6rTL16ilxbXkf8RNJLKmj5SM+HENNI+IJxjUvdyB+EEjeovGynGdT5L0XMqSKQJ9Qb4p8R/JR6mubjMXJnGHw+sh58mjqf0H2dUGHbl7WX8o9yeiBo9SwAzJKk7N6G/Q+1cvhmOmhjacQbY4kB25abqj4HkeXy2YvDRvcREKcNx1FckXW6QyNE4coY2LbAG4ZSpXfpsetemIXJCy+HeGBE8b893MeG7AMzYLIl2c3NyJDc/OwF9ohtKRdfJUPClr4aiVbySykAn4peaD0I2CyKoHpGO9GVLN4JiHw6Fimi5r3mjWNpRYSXSMRCTId8QPrf1p5dEi7XZcf9sG0gGoccwsTZVBXJlYhT1Fyu5JJOwvYWpZU83gg/9nswbPUyXYzX7oRKyMGKMbFhyx1uPMRbpSyp5vBepYAC5v8A332qM07Ym5nXXldefgkyIvNBGijBtbpTbI17Q5psHmn2dGiq1erSI7bsQBYdNuhP51wuIcSgwchdu8gCh8L6b+a6EGHfK2tm9fos5+LyHpiPp/WuC/8AEOLce7lHpfzK2jARDeyuouLt+IAj22NX4f8AEkzT/jNBHhofp8lXJw5hHcNLR0sikXQ3uST63PrXpsBLBLFnhNgkk9bPX72qtFzZ2va6n/YXckwXr1PQdSfkKvmxEcVZjqdgNSfIb/eqgyNz9v2Xd6vUEi4B2O9E0EcrcrxY+9R0PiFWyRzDbSs/XTXOI6L/ABNeK/EGMJkGFaTlZV+J8TzofG13OHwgN7UjU/ALJm4iiyCI5ZnHEW+LIkXB7hbXPoK4jMM98faCqF34V9eXVby4A0nKzqSTh4ijSGIZZjLIW+EKQLn0DXuPWtD8M9sfaGqNV439OfRRDhdL0GilzXFt8f4jtf1r1/BphjsP2U2pZ47jlfXpR6WVx8a0wSZ2aX8Dzrom869IGgCguYXWueZTpLMuJ5yqswFyFJsNybC9gO9FIzLzo8TzEI32aRR95mrhs9lvGwwVrAlZOu/l7kgGFqdDqi8Q8SPFyj9nkPNjV7ebJGYqOUbKRludr9R260yaSDb5oZ8TvgzjSzEhcsLMGYl8LDJQNl87EkWBFsuxm8EZfFehvU1Ws7jMQxy3uCAN9t/avOfiHDMMPbG7FAa6eOi63CpnCTs+Rs+KzuHxBnAPTfpt0Fee4Th2T4prH7anQ1tsurjpXRQlzd9F6EV9DGgXlCsPxZxz7IkJwz52pi0/xY483Lz9De2PT3pONKcbbKaD01blXQalpunlKHofgH1/U1yeDUcE0Hq7/kVrxwPbk+XyTa11rWTIq1aO0biMgOUYIT0DlSFJt2vaokoyLEbhevJV+ehdUkQEeQESchtxyyLgxSKCRsHU72IMdVLKE1xXSa8vFyJUC2RZCQLZgOWfAqfITjsDc2AGO5oJKMoVx6DiOFjNEHsnmBBHlmycW5QBLQ2XLYAj4d70ZilkC9OIxSzFGULsKKLKMoS+qZYlZ1FidrdiT3tXLxr48FE+dgonlyJOxra+p3IWmEGZwYdv0815TiPEki80pbzZG9ibkb47fiPYd7V4aOGXEuJBs3rZ68/Ic+i7dhopMqdqznRSSk3EUWQRHLM44i3xBiRcHuFtc+gt61ezDPdGZBVC78K+vLqolwBpaWj1PLa/b8Xy9fpWrhWNOFxAd/KdHeXX0+qpxMAlYRz5LcSMDcdT1PUn619Aiw8cZLmjU7k6k+vToNguA+RzhR2+C7vV6gkVLdwPzP8ASqI34ouGdjQPBxJ9sg+aThFXdcb8h9Vjk+Z/9bfrXzriN/xcl/1O+ZXpoB/hMroPksrScVEmplhWKT7o4vJdMA5VXxxyz3DCxtY2NRkw5ZC2QuHe1A1urrpXxUhJbi2tkWXSTliBLaNnDnrzFAteND0xJHXqASPSw2aENBLO8BXgehPiPjQQQb3T5Te+9Zb0pWWnOHnzH5V6T8MF38Q+v6fjYr9Vy+KV2bb6/oU5dvQfmf6V6rtMb/22f+Z/9FycsH9R/wDEf+y7rcs6lCFdCFRF+vz+vrQhXQhVQhJcY/y/qK4n4g/0Z8wulwr/AFHoVncJ/wA0fI/pXnOA/wCub5H5LrcT/wBM70+a37V75eXWR4n4PHqY4+aWHJninTEgeeM7A3G4ORFqi4WrofzIayVG1syIqyUrTyqtE/lH1/U1yuDH/wCG3zd/yK04sf4p9Pkm1krqLNlRUekllRVehKkVWoSpEVqEqRA1CjS5LvfZVt/qI/8AjWR7sSHHKxpHi4j4ZT81YBHWpPt+6T4wx5a3sPNvY3HQ97VxPxAZP4VmcAHNrRsbGtaHyWvAhvaGui81xjXJp4zNJkQpUALuzM7BVUD1LMBXlsPE6Z/Ztrnv4Cyuo5+RtlLBJpQWjZoklAyWRWWWEjytyxewJA+QPmF71oDoYyA9uYt2ojK7mL8viNDShq7Uc1qNGDbrt71hBVtqSnyn5UBA3W+jNitgD5Re5I3t8q+mNdiBGzI1p0F24jX0aV5pwjzuzEjU7C/1CvN/2V/3H/60Z8Z/22f+Z/8ARKof6j7D6oZNutbnvaxpc40BzKyBpcaCx9euD5fhf9a8Lx7C5Zu3Z+V+oPjz9916Ph8uaLsz+Zunp96Lw/HOE6yaV8Igj2nVdSjqqvp5InEcDoDkzhym5FgVuCL2qnDYjDxMGZ1juktIunAiyDtRF/JTkY9xOnXXw6JGbhfEpuY+Dw8xtHgBIvMjWEtHIW3sGIcvtfYDvtVzcRg46bYdWe9NDeo+VfsoFkrrO2y9b4bhliWWGXMrHMwhdyWLwtZ08xN2K5FN/wBmuVjHMkLZGVZAsDk7Y6eO/qtMQIBB5fJel0AAGR/F0r1P4fgbhoe2lIBkIAvoNvUn9FyOIvMj8jBeXU/fgnK9QuSpQhShClCFKEKUIUoQl9fAXTFbXuDvXO4rhH4rDmOOrsHVbMFO2GXO7aildBw90cM1rb9Ce4+VcjhnBsRhsSJXltC9ienkt2M4hFNCWNu9PmtUV6hcdeP/AMT9LI8Ol5SM2Gv0zviCcUXO7tb8IJXf5VW9XwfnXYnpLo5ERZ6EZUSKWwtWHh2Hfh8OI37i/iSVZMQ95cEdJ62qnKjpPSSpHSahRpGSahIhGWWhQIRFkoUUQSU6USga2zqVG7DcD5Vy+KQNxULoGkZx3gPL5XstGGcY3h522XkvEeZgISETgsoliNrvET94EDEDMDcAnt614fCU2XvOyEXR6O5X4dV2JLy6C/ovGTwcRWNooY9RaWGWKAM+8CiXJTM4Y4vyyQDcn4RfrXYa7Bl4c9ze6QXUPzaUcora9T6lZiJaoA6g14eacjj16TSapjPgs+nIg3YNFLGiz+Vb5FSQduhRrdTVJOFdG2EZbLXd7xBOXXlfxsdApDtA4u13GnzXuI4+Y4QdL3Y+w61i4dg3YmdsfLn4Dn9FfPKIYy8+nmvQrID0r6PFLHILYQa005eC8w9rmnvBXerFFL8ve539PQfSs5wjHSZ5Dm6A7DyG1+JsqXbENyt069T6/oqmjVgQ3T+96niYYpYi2X8vP6+iUMj43hzN1lPw913jOQ9DsfyNeOxH4fm/PAczTqOTvjX3yXdj4nEe7KMp9wuRDL+x/f51hHBMaTXZn4fVXnG4YC86Zh0B/wDVPyUdPqa6+E/D7IyDinb6ADrXM/fnyWKbiRIIgG25P0R4xi2B3B6VdhGHBYw4KTvRv2v78CD10KrmIng7dujm7/fxTCJbubenpXoYcOIbDXHLyB1ryO9eF0OVLmSSZ9wL69fPkuq0KpShClCFKEK6EKWoTpWBQnSsCladLq1Fopeb8fca+y6ePyZ87URafrbHMls+m9gnT3qDjQWjDD/ECwRPUV2ciIs9CjkRFnoSLUZJ6FAtR01FCiWo6aihQIR0noUSEwk9OlWQjJNQoFF5l+9qrljMjcocR5b+Xh5jVDXZTdWiIwA22/vrUWRxYeM5QABqf1JPPxJUXF0jtdSs+eLNiY9j39D7n0NeNxEX/U8S44ZldTdX4npfTfquwx4w0QEp++iC0Mo/Bf5Gs7+B4xprIT5EFTbjMO7+ZWmhlbrZR/fYVow34fxUh7wyjx+g/ZQk4hAwd3UrT0WnRBZd/U9yRXrOHYSDDx1DrqbPMkaH26LjYqeSV9v9AivGDuNj6j+frV02Ea92dpLXf1Df15EeBBVTJi0ZTqOh+9PREvWpVIdNQXEi3sO3f+lZMVE6bLHXdOrvIfy/7jvyoEc1dE8Mt3Pl9fT5rutapXKHc/T9KywuJmkBO2X5K54HZsPn81brcW/v51ZPCJoyw+/Q8iPEHVQjeWODh99QllJZx+6N/nXm4nyYzibMw/yx3uli7rzJ0XWe1sGENfzHTyP7JqvVLjKUIV0IUtQnSu1CdK7UrTpSladK6LUqWZwniEkskyuIwI3wAR2Z9id5LqALgXAF+tRtSyrTvTRS854+4bHPpQZMvuZop0sbedWxAPqLOdqi7ZacIy5mj76rxo1FQXeyLsaii1HIntUgQIQSQ6hhcAbG2+zHvf8AKi1UBd+C4WakHhBYjJPUrVZYmEnpqstTEc9NVlqYSemqiExHNTVZCYSWhVkIwJYWAJ+W+1crjQecG4MBN1t0vVXYSu1BK705sPnT4NhWw4VrubgHH12HoPjahjJC+Ujpoiu+31H6iteOcWxW013mf8gqIQC+j0PyKKGrYs6pRY+x6/P1rI2J0c5c38rt/Bw5+o0PiB1KtLw6MA7jbxHT0RAa1qlXQhc0KKlCFKEKAVBrGtcXDc7qRcSADyS+vmkRQ0UZkOaZKLZYE+ZkDMoLD3PqbG1iPJA0UogC7Vee8HcYi5EMbu/NZYR52MpleSPIvGwZ2KXV281sVNyFUg1RC1rXOcRqa86G1+5WiYOcBWwXqa1LGhayAvGyKxUspAYEqQexuNx8xvSKY3WT4OhwhKFZUYPuJpFeRrolpGCnyZAXxO97k3JuYt2Vjxqt6naQCHNMFtfvWDG8RhwmXtL1uqHT+60wYV815eS7VwRcVphmZMwPjNgqDonMOVw1VFutJ0lNceimI9QqLb0F/fA6hMM7qyZteU1qREeSaE2O/wAcbE262Gzntc7b1ZeqWVPNrRzREEcnEMW8oRQcrbkgsfKdlBtte16LTyryH+LkMj6WAxqzBNbA74/hQBxk3tkV/MVF+yvw7CZW11C8kspJsOp2FQXpC1OpARKIjixvbyyJY+wf4b0Ko1kzfp+ib4rqC85XEqVsmJIYrj2LAnIj19qhJII2F55KEUdMUR9mbsDYfTasJeQ5kfM6n5lMtV52Vff9K0xy5pXgbD5qBYjRMS2Kgk+g3NXCVojzuNDqVU5idkidAC62B9wd/pVOHx+HxDi2N1kef6qp0ZC7jmrYqXNWpHGOUHOQNz+yQeoAAvcG4PX0NO9VncNaQn1sca8yZwiAgFiGIBNyLlVNr2sL9SVAuSAWXUqnBI8S00mp1PIcFIdNKrsrRgh/IMeYGkGYZhKFKqLDFwwKutUkkqIC9DDZQFF7KABkzO1h0u7ksx9yTWPhGNdioS5wogkfqp4yERvodEcNeulJG2QZXDTQ+xsfFZAS02EUGrFWuwaFFdA0JK6EK6ElKEKUIUoQpSIvQp7LzHGuDSo51GkbBimEmKqWWPIuZYkCEu92LNGP80pGCfLZsMcUsXdJscjz8j5cjzG+q29qyTwPTl6Lb0GvZxeSB4WuRgxRyB2a8ZI3BHyII3tc1ScVhilETrsi9BdeYGvwQME9zS9uyfFdFr2uGZpsLMWEGisHi2oMGqikJtG6lJCTGkYCm6l3YZFgXYgZDbKwJ6InVTA0W5HKrC6kMN9wQRsbHce4otMNS2rjJN+wBrz3GsFLiHh4/K1rjfjvVegXSwcrYxXMkKtIBa4v7+nzp8Dhj7ETNsHUEXoa511pSxZdmyn06ohbf5103OyT5XbPHxH1HyVAbbb6Lgvt7isud/ZOA/PEfcbj3arQwZvArF8XWMIkP4HUk7GwY2vY7HzY7EN6W3uOiyRsjA9uxFhVOYW7o2r0wmk0+oiZDgT5yLko1r4kC+9iNiBvve1qmjIsn/Eri3I0YGOXOmihG9sbkvkfX/Ltb3pOOi0YY9nM0+Ne+i8bwKeEShtQxCqMlsCbuLFQ1gfLfrtUF3p2PLKYNf0WhwWcS6iWZxuA0oFyQu+5yIIsAe6m+w2oVMzMkbWDy+/7oGjYlHlA88j8uMfvPuxFumxrm4uQOmbGfytBe7yGw99fRXFoGnRP6qHzxaVOwyc/z/U/UVhw2JpkuOk8mj78dPQqsDTMhc4PIzD/AC4x/Bdh+ZrUwOgw7WH87z8Tv7BJzaC1PC88juwDWQeZthuT0F7X9fyrNxtkMcTSW246DU8udXSrc2kfi/E0kjTBgfMSR3FrjcfWjg+Blw87zIOQF8taOnsq3C0Hhyhjk4cxgjMoASo9SPT3r0VrNIK0G60dRrBI6oreRdgdt+wJuF3sAN/z70ws+QgXST1Wu5jLBowHc5LMssaOislwU1ETeYRBkfzLYMQuLkjFqpJQ1pc40AspJcaC2YNOEARBiik2ALWuepAZmIG2wubCw7Vyp+OYdjCIe847aGr9f0WlmDcfzaBGz3rRwTCPw+H/AMTQuN106KnGPD36bBGRq7CwkI6NQqyEVTTUV2DQkrvQkuqElKEKwKELoLStSpdhKVpgLoLStTDV5Lxvw/J4pJpphpwSrRIIMMyPIzc5SpYk2DMQqWBFjvVT97V7NqW3wWdXQMl8GVXS974sNr39revzPWuTwx0rZ54n8iCP91/fmteJa1zGOHSvZC8S8LGp07xgAuAWivbaQAgdRaxuVN9iGIOxrsErMGJbw7rS8YQowwAGYBET7sLRFt2Ata4AX02tQCpBq0dQ+x/KudxaYR4R56ivfRacPHcgQ4TZar4NEY8G2+dn32+Ctn70hVSvt/GruJNJw7nN3b3h5t1+OyIm07z0XBk3v7VXmrFskbs9pB9KI+BKsDO4R0KDNuhUdSDbpsex3BGxt2NLhcjDG6NpByucBryux6ch5JyMJNrP8Na1pNOjOzM92Vy+OWQJ6hDiNrGw7EV0gq2NsLL/AMRdIk2jJe/3Uscq2NvMGx39RZ2oK04eAPlaD1v2XzjmVFd/Ktbh2oePTzuqkrJaAtZrLcFm8wNr7psb3v7G4s8jGuka0nUa/fxXo+AaZOXDIrhsFkYC1vPIQovvsRuvvXkOIzydpKxzSMxaL/8Aq0E6ee/hzVMxNlvWl19mdRq5ursSiY7kKFG/z3X/AG0hOx/8NAdGii69LN/387SsEtbyWPqm5Wnij/FKOa/+noi/z+ldvDkz4uSU7M7jfP8AmP6KYGZ5PTT6ra8HPeLUW62H/i1qw8b/AM6G9v3CqmFELAimr0abmL1CTDTReXLmSAEFgyMoIIYYlSrAA/ErXuxHS9NYC3tHa7D1+/UIMEkaAmSWNG5bMnN8sWfLzVWkby3xOVid7HriwFcjnaAddfL+9eizTzAW0bpjRzst5HUJLJkTYEYRM7Oi4GR1RmyMjKpsC4HUG6kw7JmZJBY6aqqBhHfW9JoJBFzGbcXzW4GNrWB9W8w2+lKDC4eE/wCGwA9a1990nyFxolLRPWxUOamo3pqkhMI1NVEI6mmoEIqmhRXVCSJahJWBQil0opKQCIBSTpB1mujhCmVgodwi3B3Ygm23QWUkk7AAk1ElTARwwIuNwen9aSmAga9EaN1kUOpFmUgEMD2INZsXOIYXSEXQV8Ued4avGcBeSHVGLVTSufKEfKXkuzlxG7jJgZpFMl8iiAqoRGxDBQyNkYJG7HVSc0tdlK9kzVoUw1eS1y/ZNS+oaWKGGXDMtd5ZXGVoUXqW9CCdjjhtlSUg2tVuTPcD8/SvPfiInsmdLPy0/VbsM2iVyZK7mHLTEzLtQr2UcmqE0tLExGaJ0YNEjf7+Ksa2ja4aasbOGxgxOebLB79PbkraOqGZq2Q4eOG8gqzZ808lpaCFELMoN26kknuTYXOw36CrkhEBqvK/4oK76WIRhmx1MTPjc2UBxdgO1yv8KCCoOHfZX9QXiWNuu1C9EKOyc1PE2kjSMrGAlvMq4u1gQMzfzWBNtu5pUq2whry6zr7ei0+C8Vhi086Ol5DjjuwzsbqDY7Ytvta4rkY7BzzYqJ7Hd0Xe2mmvLXMNNdlTNE90jSDp8v7rSn1cZ0kMcc5DTF1YvbYuwMjSEC4sfKCOz3rDHDIMbJJJHYYGkV4A5Q3lqNSORFKprXCVxLdq/akr4xTDUWyB8iAKL3VQLAN8zkflWvgcmfDXR/MdepJvT4eqeG1Yt3winJ0ks8mwYFhfuqggH6km30rBxZ/b4tkLNSNPUn9Aqp9XhoWT4V05eQkqpRUbPK9unYi1iPi6rsp3F69QSlinBra5n7+91fE+J8+Ust8fhjG1wg6Cw2B3vYdzQoxw5G0d+a9Fw7hK81RNE+WnbJHdXjZTaNhJBKApMZZpFKBmHluwGVhz+JYmTDw9pHWhF30P70uVceIeQRR5VzSEjFXYHszD+JrbBL2kTX9QD8FqcxbvBeIoFMcoFmYNkQD0vcNft7gX6+txcVjljN2EafT4BXXLlt8BYAE/MA/x71IFUHVXE9SVLgm42pqlwTCNTVRCMppqBRKFFHFJC6tQmulFJMIep1SRqzOwAVcm7kL64jc+nuaiVMBeKQTcQ1G0oEKI6yGPN9PKjyeVB5l5epVB8VyykXIXYNDdWgUvaaPTJDGkUS4pGqoi7nFVFgLnfoKakAudSLqRWPHwGfDvjbuRp57rTAcjw4rzvHUUJzx5HiR1eVQvPXTEEyLA7+RHyCeZrBVzNx1rl8JxzHMGHfo9ulda/XqFfioSDnGxTPApl5CqrSMU8r80uZs8VdudmAQ5zy9LMpGxFu61VQiwlfE2nMsDqvxAZLsGvbcridmuOx2Jte4uKavLLCBwbi4lRVY/eqq8xTswv0d1AGBYeYKQDv0FjWbFYZmJiMb/AOx6q+E+6dkmHa9ZeHYbE4cdnI4Fo23v+3yWjLeqVk1AHU1ufMxm5WWfGwQaOOvQan780BtUewrM7Fn+ULlS8aedI2156pPW60qOu56f1rVw+CXFyd490b8vRcXHcXxDW6vNnatPksZpGPUk/MmvXNY1uwXmHzSSfncT5klcVJVKUiAd1JrnN1aaQZNLG3xIp+gv+dVOw0Tt2hdCDjGPg/y5nD1JHsbCAPDySfBdfe9x9b/yrlY6LC4cW4kE7Df7916Xh34s4iTUjWvHMnun3GnwSWt8NTx3KgSD934v9p/leuO3ERuO9ea9hheP4Wag/uHx29/rSBoeIhJS88QnO1xIWBBXYfw2sQelVzYYvjyROLPKvv2IXWLA5gyGh4LU4nx7Ua37tIyEUZcuMFjZfxMR1A27AdPas2C4ZFhTnu3dT+iqbEyLVx9SuNeTDGkAeN1cCVmRw4YtYoQpF4iq7dmN27ECuiq4++4vIIrTXTz8/ltzTfhzqXwBdGjaMtnZmDhREuBFmZ3j8xDAWII3vQsfEZHRsBafAjz+S9D4b4eI0SRVWKMjmEBsvKFKRoWMUZJUM5YsuWXUlsq4XGcU3s/4ZurnVp637mlgwMdNLuugWRPqw8juOjMSPlfauxhYjFCxh3AAXQLUzBLWgLM9q3eGS811EjbBbKCcQcR5ULdhsBf2prJI2hotDiEYRgAuIIuD5gGF9iAxJG1r1JpWUi1zE1TVLgmo2pqlwTCGhVlEvTUU0KEl0KSa7FRUgvIeIfDkuodpNNKmMxXmEsRiVHLZhirCZcARymxUMSbgm4gQrWr0nDtDHBGI4hZQWO5ZizOSzOzMSzMWJJJJO9CmNUVmoVrQgu9JXNalNQqMCHUMpBDKQCGUixVgdiCCRb3rLLg4pHiQjvDYjQ/v6rQ28uXksXguheAzKzko0l4w2GQIyDuBH5VRvKVG72F2NyFXLxEYkRiTDnVpsjqPLn91qjCxkE5tk7M9qvwGMGKhEg32I6H71W0MpIIiRjyqFuSbAdSSWPz3Zj9TWl8jWCyqp8RFhm2725lBknJ9hWCTEOdoNAvO4riks2je6PDf1KFWdc1B1GpVOvX0/vpW/CcPmxJtopvX6dVnnxLIhrv0WRLIWNz/AH7V7GCBkDBGwaBcGSR0jszlxVygpQhShClCFo8Kb4h8jXnOPxm2P8x+v1XV4a7RzfVP15xdRJcR4XFMPvF37MNmH17/ACNWslczZbsHxHEYQ/4btOh1Ht9NV5mbQajQyCaBjZTcOADbobOhuCNvcbDpW6Odr9Oa9fg+K4bHt7KQU48jz8j9nzWlwXRJKsnENe10yJAufMQbetyL+ULft6VyuIYyXtRhcN+Y7np9jUlbnnJUMf397kqanj8EwkiImjiePFYw33KsAFDNFFg5FrnDmFCxuRvdelhonxxNbIbcOf8Adc3EcLkcS8Osnr9UvxHjkkxKglYhYJGAqgKuyghdugG3QdqTMLE2Qygd48zqfTp6LdFhxEwN5oMMlaUOatHTyU1me1aWml6WqQWV7V6fQBZosRYODcsQXd3OZxFjsCAN/wBaLorC8UUvEasCpeE3G1NZ3BNRmmqiEUGmoJoUKCIgpFSCx/F3Fvs8GQkKNcNcIshWNGVpHMRIZkx8rFQSud7bXqBKtaLSngng32eDJlweQsxRTII0Uu7IEidjyjiwut9jtewFkArN1vs1JWNCC70K9oQJHpK9rUrJJQtLWIDgkXFco8SDMWYJBQqweul/X2WhraQeJs4H3aFmsT6AfU9fkKwcAxGGjzds8NDnAAc/YXQ1Gp0WLH4meKM9gzM6vQeJ2vyGqxNFNmtybtff+X0rv8YiMc40ptCv19bXicNiXYgF8jrdev6enwTFclaEDWz4Lt1Ow/rXR4ZgxiZqd+Uan6evyWXFz9lHY3Oyxya9oAAKC4BN6lVTQpQhShClCFKEI+ikxce+351g4nD2uGcOY1Hp+y04OTJMPHRbNeIXoFKEIunhzONwNu/6VRiJxAzORa04XDnESZAa5pbxHwOSXTRQQBVxkBI6KBZrn5Ate1YMHjomYuSeQ6EGuvLTz5L2mCldE1vbWTVE769fhuvGeIuGx6aYRRyGSygvcC6se23tY27Xr0HD8U/Exdo9ta6eIXUieZG2RSSjetqZCbiehUuCfgkprO9q0tPJTWZ7VtcK1eDhrm3RrEi49DYi42BtcXtUljlZYW9xFAArKreYlnZhuWbcXYeUbH4R0ptKxUgxGrAqXBNRmmqHBHBoVdJwU1Uq1GoEaM7ZWUXOKs7W9kQFm+QBqJVjV4OKVOK6sOqF9PE7JIspjeO8RlW3J5vlLllN2ivZQQ3aq9yrwKC96xpqbQhO1JXtCXkektDGpWV6FpY1KSPSWlraS8/ERCLsCQT27e9YcXwkcRIYxwDwL16cwubxLisWBALwSTyHLxWPruOSPcL5F9up+Z/pXU4b+FsJhSHyd9467DyH1v0Xjcf+IsTiLbH3G+G58z9KWYjEG4NjXo5I2SNyvFjxXAa9zTbTSZj1chIUEXPsK5cvDMFG0yOboPErazF4h5DAdT5KptNKTcgn6g1PD8QwLW5YyGjyIUZcNiCbcLS7oR1BHzroRzRyC2OB8jayvY5n5hS5qxRUoQpQhShClCFaneouFghNpogrfBvuK+euaWnKdwvTggiwpUU1YNBF6FMEg2E3HxBgLEXPY/19a5snDInPzA0OY+nRdWPi8rWFrhZ5H69V5DxPwbK88Y83WQftfvj39fWu7hpQ0Bh25Lp8F4wQ4QTnQ7E8j0PgeXTy28vG1bV60hNRNSVTgnoHoVDgtLTvUlmeFp6d6YWR7V6rhknMhZCfMtgPL+G5Ki4tfzX+I2G1GxWCRtOQ1BBIOxBsfmKsBVDwmYzUlmcEcGmq1oCmqQs3xPxA6fSzTKHJVNsIzKylrKHwDLcLe53GwNQcaCtYLKQ8Gaf7nnOS8j+VpCZTzFjZgHHOGSgm5tuNxY2tUQrqW6xoVzQgSNSWhjUrK9JamNScr0lqY1LyPYXqEjwxtlV4nENgjL3eniVkcTN0JPqP1pcIkJxgJ5g/L9l4Hib3Sxue7ewVl6eLJgvSvT4vEjDxGQi6XDgiMrwwJ4cNHdj/AArgu4/JyYPcn6LpDhrObimItMq7gb+vU1zcRxDETinu06DQLXFhoo9WjVGrEr0nxRhiB3J/Su5wJjjO5w2A+ey5/EXARgc7WXXqlxlKEKUIUoQpQhShCb0erx2b4f0/4rkcS4YMQO0j0f8AP9/H3W7C4sx9123yWqK8iQQaK7alJClCFKELxniXhfKfmIPI53H7LenyPX8/aujBLmFHcL3PA+I/xEfZSHvt+I+o5+nisuNquXbITkLUKlwWjp3prO8LU0z01keFu8J1fLa5uQQQVBsGuNgfa9qksUrLWi1ycwhRSduuP0Y9akFkcEeI1MLM8IwNNUrUFBVQXiPFfFoJ5dNAJXW8hcPFKkUyypIY4sEmIWVGZZhsGvjsD1qtxtXsFL2EEQRFQFiFVVBZizEKALsx3Y7bk9aFY0Ll2pLQwJaRqS1Mak5npLUxqWJoWhJah7n2Fc7ESZnUNgvKcUxXbS5Rs3T15n9EnrnAQ377D5mr+FxOfim5eWp8v32XDxjw2E3z0WdoTaRfqPzBr03FWZsI/wBD7ELkYI1O375LYrxK9ApQhK6vWBNhuf0+ddbh/C3Yjvv0b8T5fVYsVjBF3W6n5LMkkLG7G9erhgjhZkjFBcaSR0jsziuKtUFKEKUIUoQpQhShCJBHkwX1qjFTiCJ0hF0rIYzI8MHNbaLYADsLflXhJZDI8vO5JK9Gxoa0NHJXVakpQhShCDrdKsqNG3Rhb5HsR7g71Nji11hX4bEPw8rZWbj7I9V8+liZGZG6qSD9O/y711AQRYX0qKVs0bZGbEWjwtQhwWhp2oWd4WnpmqSyvC1tM1SWR4XrNfqPKCCvnAyHU2YK37RsBiAAQPYUgudSXiNWhUvCPUlRS1hSKpCx18OacS81VcHPm4CRxFzPMeZyr43u7Na1smJtc3qFK9q0nNCuaEvIaS0sCUmaktbAkpGpLW0IMz2FVyvyMJWbHT9hA5w32Hmfu0jXJXjFl8Tku1vQfxP9ivW8EhDIDJzcfgP3tcXiElyZeiDowM1v6/8A5/GtnEnOGFeW718OfwVGEAMzbWnqdUqjrc+n9a8vguHS4hwJFN5n6dV2J8UyIb2eiy31Dnqx/T+FesiwWHi/Iwe1n3K4r8RK/dxTmk0QsGfe+9u31ricQ4u8PMUOlaE878Fvw2CblD5NfBIzEZG3S+1d7Dh4iaJDbqF+a5spaXkt2tcVcoKUIXSqTsAT8qg+RkYzPIA8U2tc400WreJh1BH0qEeIik/I4HyIUnRPb+YELirlBShCtTbcVFzQ4FrhYKYJBsLR0utJ2YE+4F/zFeax3CGs70TgPAmvYn9fddbD44u0eD5gJ6uCRS6SlJClCFKELy3i7SWZZR+Lyt8xup/K4+grdhX2C1ev/DmKzMdAeWo8ufx+axIzWlekKegahUOC1NM1NZXha2lapLJIF6zTMW0wALXCnYKMSqt+InqQBe49T13o5rnPFOQYTVgVDwmQakqCFr0FUhctUVc0ILmorQwJaQ0lqYElMaS2MCUNC0JbVnoKxYs7Bef4282xnLUpDWylVuOt7VZwzDsnxGV+1ErzGLldHHbd1jsb7mvZtaGgNaKAXALi42VVSSUoQpQhEEzAYgm3pWd2FhdIJS0ZhzVomkDcgOiHWhVKUIUoQmNA1nHvtXO4rGH4V98tVqwTi2YeK2K8Uu+gy6VG6jf1G1b4OJYmHZ1jodf3WeTCRSbj2Sp4bv8AF/D/AJrqt48ctmPXz/ZYjw0Xo74I8WgQdd/n/SsM/GcRLo3ujw39/pS0x4CJm+vmmQK5TiXGzqVsArQKUkKUIUoQpQhZ/iCINp5L9lyHzXf+VvrV0BqQLpcIlMeNjrma9Dp+68THXRX0Ep2A0Kpy09MaayvWtpTUlketrTTNiFyON72ubXOxNvlTCxSAbp+GphZHpoVJZyv/2Q==</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUSExMWFhUVGBgVFxcXGBgWFxgXFxgXFxUXFxcYHSggGBolGxUVITEhJSkrLi4uGCEzODMtNygtLisBCgoKDg0OGhAQGy0lICYtLS0tLS0tLS0rLS0tLS0tLS0vLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLS0tLf/AABEIAOEA4AMBEQACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAEAQIDBQYAB//EADkQAAEDAgQDBgUDBAICAwAAAAEAAhEDIQQSMUEFUWETIjJxgZEGobHR8FLB8RQjQmJy4QeSFTNE/8QAGwEAAgMBAQEAAAAAAAAAAAAAAgMAAQQFBgf/xAAxEQACAgEEAQIFBAIBBQEAAAAAAQIRAwQSITFBE1EiYXGB8AUUMpGhwdEjQrHh8TP/2gAMAwEAAhEDEQA/AN5K8qeiElQlHSoXR0qiUdKhBCoQSVKLoVUUcFCHKEOUII5Wi0McEyJYLUC0wFyBKtNa4GeaI+wWmBmmiE0LrREzyIquHT4iJAtXCSnRM8kRnCdExC2iF+EtoiQIFUwc7KwRpwiJFCHDqFCdnChCemwQrLEqUQoUB1KQRFHqUr5+e2ElQlCypRDpVEOlSiHEqEQishyEhyhBVCHSqINKtFnJkSENVq0wAkRdmtcBEyVlBaYmSYx2GT4meRHUoW0TYiZAzsOnpiJDf6ZHYtkVXDokwWgF9FFYIO6gjsqiJ1FSwaIX0VZQrWWUII9tlZAQsVlHpBK8DR7c4FQgqlEOlVRDpUIKrfHZR0oNxQoKlkODShc4+SWiQUDE6LPLVx37UrAeRXRE4LRGW5Bp2IiQRyNMg7JK1YwJCigtcEZ5skbRWmJlmO7JORnkRVKFk2Ilg5opyFNHdlZELogqUUSYNAT6F0dg0QuoK7KB6tFEmUwc0UVg0NNFWQiq01CmBvpogTeyvC0e5oUFVRTOlSiHAqUXQqEEe1LySBYjkMPYtHNRSr7kYVRgkQufqHKEZOxErS5JqsbLDic5RVoXGyF2HtMrbj1E9+yuBiyU6I+xWv1BnqEraAWnHyLc2FUsOOR9l0MUBMsjC2YUclrjFCJZGPGDCfFCHNkdTAowHIGqYYhGgGCVaSamKaEbTRWAQ1aSJAtALmXRIohfTRA0QupK7KYx1BXZVEfYorKIn4eyuyqIm4RXZKNCSvFUe2OCsg5qEp34H02A7pGXK4rhASk0EUoCw5ZTlw2KnbJqjRqNdh9+qy45tva3w/zgWm+gVrb6LpVwPbVEjKR1S8meKe3yA5roPwtFcvUZJZODNkmdUpAGT/2fZFHUwUO+SRk2qBq+MEhrWm/TTz5BIWeXLQyGJ9tmfx2MxBcYFhMxaIP8LbjzLtvlnVw4tOoq+zsNxYizjmPQW+66GCOV3vboDJp4t3FUWNPjB2FvZdTHkUUZZaVBuH45PT0MrVHMZpaUsKHFAd06OQzSwUH0q4domqZmlCiXs5CYmKaBa+DlMTAYC/DkI7AoHqsRJlMAdTujBI6lJWmUC1G3gowWDPec0DRECEso2Q2XQPiWwiRT4KivxDKU3bYtyo0zV4mR7gflS96T5Ks7Kr3JkslY0pGaSS5AbQbSb3Z3C4uXI3l2+GZpP4hpPrP5KZsaklfzLI8hBWpZIyhcQtyaLGhSFiudN0/iMs5O6BcTxEA5WjpO/ty6pcp2vh/sbDT2rkVOIxz2kgEGdBuPM7oYYYySZthghNJhWEo2zEzmAmecWiErJNXSE5Jr+PVA1ZzmNqEiXQDAEyNwOZ/N02KjOUUuhsVGcopPgzlItc6Q3u75NyNf+13cWo9ONSOlkwtLvn5hNFrc8+Hzv7DyV5NZVOCFODUeeSfE4wNgB4ynYkD1lbsOpi/5rkxPDlf8RcHjTmgjMJ5j5OuP4XQbW3dFmJ7m9jXJe4LGA3gjohjmceLsB6e+WXuDxdk6GVmaeNLhFi2qCLrXGdmaUaGVaAItdMTFtFbiMNyRpgtFfXopiYDQI9yIEFq00SZTQLUARoFglXHFnkiUbB3NAmNx5cEUY0DKVlHWueaYLPS3UWhsb2PuvlsdVlll3P8Aj/4PYqbbvwNo0DPTzCZqNZBQbi+foFPIq4CKlFugtH55Ln4tTlVSl0/z6iYzfZHSpSVpzajbEOUqCXMgWHL6LBhySnLl99f2JTtkTHR+y15Yykkl9xjVhOVoBcTZJi3CNPx/kTcv4orquLc8w3utGs3Bv9dPJJyS3fy59jVHFGCuXLK6vWLXWBmIzAXEyYadOd0cIKS/1/yaoQUo8/1/yVvEMWQ7NHITY5pFjPRacWJVX4jXgxrbX4g3DYt1MF7iIytlsxY6ZZjkZH4UzxRyNRRmyYlkahFee/8Akq8ZxOpWGYENDR3m8jIOUG0ESPZacenhi48m3FpseF7Xy30/9lQ8mXtpdy5sDJg7En6LYq4c+Tc18Kc+RDSIAOYjQanTR3TkrU0+KAnXdAdek6ZJvrOk9RO616en0c7Pkq0GYTEEjV3LU6deq0Pb0jmvPL3NHgcTAEkn1QR7FTzXwXmC42wQJFjF5v8AJbI5VHhmR8stKnF2tAIvJWvBPe/h6EZkorkscDjQ4d2J3C082ZwogORglbjcMmJgtFLWopiYtohcFZQLXphGmU0VlTBZt0xSoW42AYrC5T0Rp2A1RWPcJg2RAnofbkfsV8z/AGsJO0++0ez9NMkqVtI1SMOmaclPoCMO7OFTznmiljb6qv8AJHH+ielWkDQQsOfTRTtW7FShTCaZzAysmSscouHsKfwvgSnQEz+Ba46iUl9C3kdUBcTqOkBuk5Y5cz5pHq+py+kaNPGNNyAGNysLWm4kGLnnbfnoj5ck35NDe6SlIq8TxHNlGSbgO5mDAnr9tVqhgcL5NuPT7bd/Qr63Exmd3GuOa9zG8npb6LRDDwuaNMdK3Fc0VOIrTIgjN4QbuHqtcY0b4Qqueu/YH/r+wGVxLyf8DuImPK0x0lH6Lyu48fMrMoTdrhiYXGFxILGNIvI6iwnU7fNTLi29NhqDq3YZQqnIR2knlyjlO6RKPxdGfKqbdDMTxD+3kcORB3HMe8eyOGL4t0Tz2oypJ2VzuJBosdOcLTHHOzm77RPQ4yXOFxcjyjew9PZakmkIcrdI0VB5aJJ8UE/boEE4vtjYp+Qj+qztyDUEEE7WjXqCnafJ6UrBnDfGmaPh9Q0yzvTOh8tQung1HqNpqjNlxqFcl8zH3mPNa9pn3BzRmCroNFVjMPCYmA0VlbDhGmDQMKWxRWCcMOAVdkoreJMEdEyIEjH4+k4mbwnozNM9Eq1JMcl84xY6W73PbxjXI1nL8907IopNsKQdAAAm/wCX1XFUpym8kVwZbbd0MoOvBv16J2aDrcv6+YU1xaLFjdLrhZJbpNMyNkeKrwYj+eSPlqg8cL5KvG0XObDTBPpoJJ6fwnYpRi7ZrxTjF3IHgMEvE7ze1pdqeYt6JvM3UGMtzdRZnqvEBqGREwf0ybz1g6LoRwvps6sdO+m/Yr69UhzXRpcWta2gnfYrTCKaaNUIpxasqamJcDcga3I5TrFzofJa444tGxRj4AsRTGeGm51OgdsRmi/eaPXyTotqPJcYqXI44p0mpplI1EanQ+e6pwT+H3CpKFNln21JzcwbDiJMGBfQCyx7Jp1fBxs+TInw+AHEUnPbnm03AbmhuknTl8xzWmG2L2nGzaac1uABTa5+WHA2MEAQZHMkkG/yWi3GNmWEcbntr+/zyWmG4a9paQwEEgNjW7pNuYaCbjZJ/cxYf7ZqdOjS4PhD3kx3jFzqT1gflkHrucqiJnifZfYbhrP/AK3AggSY1O08tdkSaboX8XRZYPB5qWR97+ojQ/RbdJNqSsRlVxC8IS2WVNj3HaZgdPXmOnv2t6U1D35MNccltgnENn1RsOJJiWBwkIUwmUeJZdNQpgsRcoygfEVuSJIpsqMUSfFpyTYimVOIa2NCSmIB0bSvSg7XuvmOl1O5U+lwevhOyFgvZb8jjt5Gtqgx+g06/suTCKjJ1ZnXY+m2IjdDmk52gJO+wqo/I0u/J0C5sYJu59ikt8kisNVznEDQCecut1UpJWzXtUYj3PaCJPeOgtJHP6lCk3ddAJNrjoq+K1Wu7jtfC3LbUQVr08ZR+Jfc26eEo/FH72U9TDghrSCTZuwIzTEgTN2n8K2xnTcjcsj3NplawOuwhxyjUREk6id9R6+a0yceJJmu4/ytA9HhJdYPyuuRABi240Tf3FPrgbk1FK64KGnXJztuTMFwFg0m2ltbLc4VTQePIk68oNbkIOVzi1rR55nEd3pvrzASKknyuX+WSWRt00rBc9QSQ0wCJnldwBG1rWtITah1ZicdttE7KFSoQ0GGzeY0F+hNpsrjFX8zDqZzT+Ho0uA+FGOlzHd6c0xeRqDO+luiJxcoUcmcIrJfz7NHg+DgvFu9BjMNt4MWC560s5ySuvkacuaKW5l1wPgRoySQSfpyXR0mhljds5mTURqkFVcGDUDouRcdAryYl6q478EjP4bAxVLHOaNbxytJCHTNersfuDqHxaAKdVjnHNIynKBf0I2jQr0+SG2FrwciMlKVFtQxpY3xEwYuNfVDjlHLBTj0w23DhllhcTm1VONDVKwTiVK8oosGSKTEdU1C2BPYjBZHUw8iUSZVFRjsPdMixUkapzyYvP5zXzeGKEXajR7FRXsStyiEnLLNkTdcAPc+RWuAt6+qCcJyaa4fRTTfItMk2j880zJi2O/f86JLglxegbOlz16e11zM8/i4QrH3uKbCN7zgbZTAvt0UyPhNHQyv4U15+R2L42xvdgEttJI8uW0q8eklLm+yY9FOXN9gVXENc+SBlAI0mDP+MctZB5+SescoKvI+OOUYVfJn+N4p5eYu5rjkkxpeQSf3XQ02KKjz15Ojp4Rjj+q5AKfEXOcSSJnVptfwjqB91oeCKVI0+lGMUl7FYBWdTrN7YtgwROU5nQQDyIIIJ6lav+nGcXtFTj6vH9NFXwYFpNAF0VCcwgcoJnWbC28LTnacfUfjozYcUcctvP3NNw3hz8zqID2kgiQTBJNpEa2/NFzs2aNKbo1TnCEVMsqmChz6eVwdB8XhOUQDPoNVljl4Ur4+Rn9VSVquRMMzsajQGhxtIJuLDWRC24su/l9GXLG4/CbLhwOew1vNrgrWoyZzMiW3k1OGZa62Yoqjk5aYW3RP3bY2uTMUvFqri4AGCL22XmNfrJyyqPTR0cEFttGT4rx6ph3NGIpM7IlzCQ9uZwMw4A3hrcsxOpnp3tBp8GWG3G3uVO/b8Zyc+ozxn/1IpK2u+17/ACDqtFwrU6jHEsLQ+RcZLFocL6z4hotstRk/bShNXK9v1AeOPqKcXx2FvxfaF1sukA6gbenVa9Lp/QxRiLyZPUk2W2EJaRyIkdeaKQyPBYYpstlLQ1mcxTLp6EsDdRKKyhwZYqyFZjKcpkWLki9osB1XzTUZ5xTcUeslJiupxfb5pePPLK6fZSlfA1g5p+SfsE37BuEA0j1XO1Ftp3yjNlvsr+L1BDiDe5B2Fo+yRBuWS2jVpou1wZ3E5gQTYncRfmPlK3Y6a4Orj2yTSKziGDzMaW3MgakSNxM289lqw5dsnZqw5mpNMK4XTAflfa0iSTtHqb+aVmk3G4idRJuO6JQY4O7Z7XPkttJMxPhFtdvZdHFXpqSR0MO1400vsQ4DDOL2taXAlpGYDNZ1hDR4jp8vVmSaa6LyyUcbb8EWIABInMXvJLQ3nEEHUW5boo2/sisC91X3Ca2MoteDBEBoHJoAEm4vckR/qUqOPI412A7jFqTXkKHxBSfUDgWjUAOm8An5kcpuEv8AZTjCmYXUYbbCsL8QNz5nmZjM039REnSNT9Uqeie3bH+xcorb8L6IqnGmveATBMbWgatIkxfda8GhkkIeeGNUa3gmNmGwe7YHnYfJdBYa8nPy5VLk09PEOyy0iQN90GX1Erg0vqYWot8oJo8RbEuIzDkduaHHq1JXPtewmWGn8PRVYyrndmkE3BjSNrriarFknP1G+Tbh2pbSi41wOjigW1BLg0tpuDnDI47wDDrgTK06D9UnpZfD03yuPAjWaOGoV+UuCr+DX1+9h6jSOxc5geCYGR0OYeepjpC9vJY8sVNdOmcHC5KO2S64NEMQwOAa4uJJF4N97fZO2uuStyTpF3gajXANdaAXA+WoPIpMk1yPi0+GWbRIIShxUYqldMTAaAqjAjAIahEQrRCvqiUwBluKcAHZfKZZ5Tm4p8nqHK3RznW/LwpCNT46X+yJcjGOutzScfmE0EsmCQZgErLKcVbYmVWrKKoHHXKIFheSdAbLPGl0dFOK6OZgxUiSCDOY2JmI5QPJR5XjuiPM8XQjsFTpQXA5SCC0nRx0MxIH5CKOWeTrsnrZMv8AHtFPi8VTFSoGMu1sMJNwR3S4Ty26+S248c3GLl9zfjx5HCO999/TuvuZfEOZ2oNnECXkaf6kkFdOG5Qfj2OgnfC4Htp5RD3C4Jbl3nSb2HeF+qtu+Ug4tybaXnz/APPkVOKb2cO1GuY789Voh8fBkyZpYrkyn4pii4gaCJG/8LXhxqKs5ubPJu2D4Ke1mpJgTcAi2kgiCNBFtdQnTrZ8IiCm8tTLnjFB7YqA2IiBo3aNd7kTGo1WbBKLe1jtRgklcfz5AWAruziXG1if5Wrg5bcqp+D0/wCGsSC3vG4HQT7WmUmcqQHTNBVqvjMA7rqLHfl01WHNjyNbkEmuiPDVyXCdBpHIjT5j5rEsTguREv5chlarbP8AptBvI3iN7hFki3C/YpUpFbULnHut7xd3QARsI8yuesTl0hsnRkeI8VxDKzmPa6mO0eadxDhnLbi+pEza/uvpH6dhitPCF8qKT+tHldXmkpv5tsbQ4s91VrnPM6SItreRqZMyum8a20cxZ5eom2eicPxoLA4GHDKHDaHNFvkFzpR5OzCdrg0XDqkhZ5o0wYPxCAVcS5FbWIlGgGVuIrQSmJAN0AVcWNEaiBuNBU/TJOvv+Ar49jk4/HR6mPuJhwLE/n31R6jLJXGJeS+kK+nqTb8sqx6iXEVyUpeETUyMrrbaocrvm+fYCSe5FfUpBsSYBtGs/llSk2nRpUnK6OdVFMF3i5Ae88i5RR3uuiKPqOujKY3E9s4m5c2ACTYEkl202H0XWxY/SVeDtYsfoquKZU8VwtR9TMLSCTrYg3E+V1swZIRjTH45KMNq/PYD4VhO1bY/3JcCLQQwEkg6kyN7+afmnsfy/wCRi1NK5r5X87r+iDijnU3itmLxVa1rmAiabg0tAynVpGonX5twtTjs6avn3MlywZm0m4t1/wC19yu4xhnsIpvJzOAdBBAaNiADedJI26rRgnGS3R6Q3K1m6f4inr4U5s0Enyt7LSsiqrMs9Hk4e1thxp5IdJ7RwiZjxchqTHt1S1Lc2vA3LheLa65ZfcOc3I5tSTmaQB4bi99dp99bLHlUtycfA1wUoJP7/wDorcFwl7ahIhzCbAnvAbXuT6rU9TGq8nFzaacZNvlf5NXgy5gtRJOhzVGhsRvAPLSEieqx+bMEk4+A5uOqMcS0kPNgAZaGwMwcSO8SY1jTdZv3s91x6M027JOHYoZhPj35eWnMqPJu5QyEd38ma3BFrwHWPURy0I0K0waqxMlzRR8c4xTw+TLTL6xcQxgJkGLOtIB0tCb+nfp89Vm3tVBeX5+hm1mrjhjtXMn/AIM9xPidTE1aTaoZkJdSLWCHF5EFxB0M3HkV7HFijitrt8nnsuV5Wr+gBjuAVMO6CQ6xPdm+Xxxba0krTDMpoyZtPKD5NHwDFOcJnWAfSI/ZZssUjdp5tqzf8HfZYMiOnjZBxd11IBSKbtCTCbQuyvxFiZTELZV5JkplizY1CHgQImZP36L4zteGTUndHrY3BuwZ7SNVphKEnwOi0+jg5W4QjKy6Cac5SeQWXK1vpCZVuRR8exYZlcxwvYjlJF+Q31hadJjcrUkdDRYnO1JFMeIkgUg0nSoSAe4P0gGZ7pF55Ld6CTc2/l9TasKUnP7fX5g1OqG1CASGf5aDvGxO0kSfqjcW4crk0STlDnskxmNe1geA95Lg1zssjK5wzOiLZWg/+qvFii5tOlx19ujJOocJcWqXsU2IwPZ1i8FwAdBAMBwjp/xK2LLux7fxG2D3tSvwBYviRa4mmCJuOQPVMx4U18TGZJpRUWrYHx2tnoF1chz/APBxM1J2aJN28+QutWjg/V24+vPsc/8AUfShgtra/CXv+dmWGIfaHOkQReRI0su3+3h5PPPVZH03/ZqMA7+ryOJOYHK9oAAaem2U6j22XFyw/btrx4PSabVx1ONN8Nd99+/3EpEuIBmZMFoi+zg6Jjp5blGkkrM+dzUtt8lxwOg4amIOkg6XPdFuQ9knLTlaRmc3t5Ze8V+JMPQIbUs+AcoaXS0kibTy6LPg/TtRqVuhyjFqtZhxPbPsXgXEaGJ7RzXGMhibPaRpLdpEkcwDyKXm0OTTy2ZVXsZMU4ZW3F8EbXOJLWsLhmiwkmRqDodrEocXHCBmmhfiY4mhRZ2TcjGuArGke+G2IIJ2Pev5Bdz9HwweSW+rqkn0c/Xyl6aS+7M7wsuxWKexgLX1X5wHaRu4kd7Mbusd7L1GKPo4UpeEcOalknx5NUeDlj6tKYd2XicMxJBJLyQZm0gmLrDrJyfp5I9KXP0NenwL4oPuh3A6Dqlctc45hlc14cH5pGR8ZtWOY4zyhafXhOFx+6ErBKOSn/Zqm8GpUKOpNwJAucpJgD5TySXllORpWGGOJbcHqlxPXpHySsiofjdkXFWEkwpBlzK6hRiSmNgJAmMo3JIsjiwZIosQ+CYsCnJCWzXU2FsDc/JfF8uRZG5HrpSUuSCCTrKa5uMVSG9I4MMxCpyi023yTcqssqVPunnBsVhlL4jHKVyMl8Q1ACWkhtQgRz/CCuxo4t01yjuaFXUlzEBwmJpNGSYflLRm2f3bku1HSwstM4Tk7ri/8D8uLLJ7q4vx7AWMpU2NDXPl0d4tAIB/U5oIMGbR7J+OU5StLj5jsc8km2lwCUcZUfSq0RRykAZHMnK8mRMnwmyfLFCM4zcr977X/IiSmsjb8fPj8soeI8XpiqXF8l0sdBJyuFjINxuLi8FbselnsqvmvmXDXYYNJv6/Ir8VxRpILBmg6nSLW6n2WnFpX/3cCc36ol/+at/PoqOI4h9R0uNhYDYeQ/fVdLTwhiVRRydVmyaie6b/AOER0mSJOibKYhQJKFfsnsrNElhBjQEA3BhJyQWSLi/JcZvFNTXg1xpB1QOIhpANgbA7XjrvtquK5OMaPUbFlal+f4sbj+LNoh2VwdUdcNMnLm/yJ5ARbUz7a9Hp8moaUuIrz7/I4P6lkx6a9vMn49vmzN4hrpDnyXPvJuTtsvV4oxhFRiqR4rLKU5OUnyGfDvE24euHvDy2HNLWamQQJBIFiVl/UtK9Vh2Rq77Zp0WdYJ7n1RtPh7i9PEBz2/2gDcOdDg/NYCdzLY6mF43W6PLpZqPb74/z/R39Nmx5k5Pg0GLxxqU5BPm2COWV3SCkSyOKsvLFS/iuDIYLjHZ4twZlaWnK2oRmLcsHLcwP0nyiNV77QSlm0kJZO2uTymqj6Wd7Wej4HF0sSyu4GbA5iC0Q4TryF9PRLyQaqLNOLLGVyRR16dNzGPeOzOYMzAhshsFwY6RANjYwANdZDTwljyOMeqFZsiyRW7g1neeKLS4WIcDE5wAYAMwLalXwrZo5dIO4XVzPc5BNUg4O2yau26FDGB4ggCYRqwHRmcfisxLRJWiMaVmeUrZnsS8zCekIb5NsMU6IXx3JpEncT2zxKx9ISP8AuFlnaBk+QujGo3/N0iV9CJ35OfVOaxspGKrkiitvJnfijhbajTmflOjZuRygWkHSNl09BqHBqlZ0tDqJQpRR5dxPEE5eyJcLsMDWCY+c+wXqMEO9/wBTu5MjcLh5BsRUxBczvHL/AJCAZvsP8hJPsnQWFJ8cmHP+4jKMk+PP1LvglUkVKOIGR72vYHQSC4+Fzdj5a/ILHqYpOOTFylzRN+acakqa/p/NGdxGEaysWOa0wfFBg216+cLfHLKWNST+wn0MSyVOP59hmOyNeGsaAWgl0C0mIBkbR80eJzcbkZNZHFCajjXXf1KrG+ILVCXBja5FpviyvdYdcD6Q3TEzNM03wpVBBYf8ZiTFjoZ9hH+o525f6jjae9eTs/pOpuDxeV/4/OAP4qYBXs2JY06zJuJ6aR6LofpErwd+Wcb9aiv3D+iExrM1MOBu0A/SV3YM8xlgVDH39Z/PdOX8rFv+NFhg6TqrK9FpAJy1AN3hskgc7hvt1WLUuMM0JyXyv2sZhvbx7D+C8frUKFWkHmHd1rdC3WSDrNzA29EOb9JwajJHI11y/n7WaI6zLiThHz/gDp4oNaRYtnMDHeje/wCaLrJKKME4ObN/wriraGGe0hz3PHZBtgAXAuAdmNjbUbzErhY9W9Rqmo/x/wCDW8Xp4eOwMYd1YhjZcymT/cAdlDT3YEkwxsGOa6qyRXXZzJ45S4Nxh6mYMAMNLQ0bloAAFzzH1bzXKzahxbVcnYx4k4mt4dSDG2EQPdBCcp9jdqj0Mq1ySnpAWC1KJdYyiTopqwTGYNrWkmB1Rxk2DKKSMhjnMDs0StUUzJJpOzUtK+S5raaR7loKogm02XNn8L5ETaiPaWtNj9kNSl4Be6XZJh4JndDO0gZ2kVvxMDkHdzEzA1Gl/Ww9lp0T+I1/p9OfLoweJ4fLczAM4MwbNBJ5+e0L0OPNTqXR33kfXgl4JwmrY1WkQ4DNu0aTpMCCbRpdDqNRj6g/H9mfNqFVJpkvG8KxtRgLg4ZTmNrAkZDtvBnlCXpsk5QfFc8f7C0+WUoNtVz/APSoxzW2uC7QaGNtDr+clsxOXPsaJQ9Tr+yqp4eH5QTJcT4iRJ116ne1wtUslxt+wj9pGKq/d92C8X4NnMiGkDT1vMDVMwaqlTMmb9NclujwyhxFBzIJi+l5st8ZKXRzsmOUK3DcM/YpqMUw/C1H0yKrIBFufI3B2sEU8ccsdsuhcMs8Ut0HTCxxFj6L21SXVS4uaeUgb7CQZHKI6BHBOGaLx8RqmHLUY54Jxy8yu0/zwOoPBpR/rH3XYgzgZYlU10HTotK5MbRaUGNc5r6Li2pTIdleQQ8TdoLRYWjrOyxamc2nDIri+LQzG4Q5JeOYUCKouD3XTqCR3RzdABGa+yH9Nzu3jf2Ka44f57DOC4QOzVCRnHdDYm9otz0Sf1jVzhWOPntjdPHdKvbkMxtXu06J8VRwedLhugmNyR7LH+l4/wCWV9JcE1k5JOMTVYbilGhhQwTmqzVeALvzGO/+khpj0XXwQc230JyZNmNJ9kvw9VL6hbDi2RGY8oygHr3FWoxxfAennPbR6eDlpwSJ0WaEV4NrfHIFh3XlNYtBQc49EPAfJT8Xw+a5KdjkKyRso62CD7HmnqVCHGy0a5fM5RPdNEtOuRoViy6eEnYuWNM7MlekkXtFZIuglT7KdMJdSNRhbvqN7+SyqXpzsRuUJ2ZvECm2oaZaO+ZuGiImJGrhbmupBzcVNPo6sN8oKafX1/EFY7EZKUC7nNgOJtZtiQ7U2S8UHLJz0mIxY3Od+E+jE4nAVamaXbQ158JJEiRrGa3T0Xcjmx46/wAo6M3cHFcMEGG7JgDmjKTdpF5gzB522TPU9SVp8m3FCEYqMQCpRIc5onKBIPUke3JOUk4p+QcilKX2Oc50iPEQZcZ01IA59flurSjXyE3kcqTS/OgbH4PNTJAdoCf9nbQduoTcOWp8itXpk8Lq2+/qUmEb32xYiASeY6fmi6NnmZCVSWl1O8TfptvsU2LMskDB3JPjITJFtw13dPutMGYsqsDrMyuPyWuLMTXgfQruaQQSI/hFOCmuSi+wTmVwQ5wnWD0Gl9vsuXOM9PNbVx7iNk7av6A2GoVu0LKNN4JAJkZN4JBMAbX6LRqY6fMk8jTr88GnA8kOfJKyjiMwlxlxbd7szgGSGxPhAk3OtwnY4QjGoLgCeVN0+wnC4cvdTpUiXufALiIDM2W0+pPSyLLl2JtgYsLyNHrPw3weDTaIysu46kkAQJ8/2XHjnnNu2duWnhBKjRYyjm7oWqHCM8lYE3DuZfZM3JgJNE73ECyFBMgfJF90XTBK8YctvlsmXYFUDhfPJI9sPBWeS5BFBSJxZKJWPWOUJC3EJwr5ISMkaEZI0gL4gwlPKXOZmB1tMGPO03un6PLkuk6H6PLNvanRnsXWY4MayXZtB4SItBbrFjc8l08cZRblLg6eGM4tuXFflheGxLgCxwA0bmiQbZcs8zIA2CVOCk9yE5MUW90Xfy/zZnPiKsZYKbYpAZoHeIcbbSTebT+y6Okjw9z5N+mhL+UnbKWsxz8okNDRB5TrFudlti4wvzY6ablaYziWAaIDT/cmWG4uIzRvPeHurw5Zct9eRGphCaS6l2vz/AXQxBrse0sh7O9mNhcQB/sL7x5JU4LFJO+GHgy7nymvBn8Y0NMkAnnYS62sbfZdLBJs5H6tGEZ2ly/JR46vJPNxv7QPkt0ejgyYPSdPpdNixMuCejULYO0/T+VohIRONlm6uDBEHqtkJHPywBazhNgJ5p+4RFMjY+/2RWmqCaDm1KhMlzj/AMifogjjhD+KSFzlapsvcFiy/KWMyuc6C6XRJGVrQOX38orJNRVsmPE5SSRuuEcOZRaA2DVdGd15J2Enl91wM+Z5ZWeh0+BYY0ejcFwxawOPKwTcUaVi8krZNWpyZWhMQ0MfTUslED6KKwaI3UbK7JQFibI4gMpZXinA9pQspbxoqhZQPEVQockTwlUPa/dYsuOlQLigim8OBa64KwtOMrQqUXF7omexPBTTrB5PdkX6AzMeq6WPVLJjcUdOGsWTE4+QTij25yxptINgDlIgZRNp8VzaU/AntUpfn+xunT2bpL/3/sqeIYepVz1AwAU7NJbBcy5BP6tDppJ1WzFKGOoX339R2Kfpqr5f3+xVcMxLmgs7MOzNzZDqHF3hGkae605scZPdur5jZJtbuvJPx/hIBpVHVHNeCBBa0eKAZAvbpYZvNVptQ2pQUbX1MMoepkjNSqvuVf8A8gHBwylpZDTcF5AdId/xggXlaHhcWubv+h+HUr4k1yn15+pn+J4wEwAO93pAIJF9Vvw42lyef1+WM8jcemUoF1s8HLbJjDRP+1vJRC2wuk3U2tfWfSyZGVC5IgdXdMAHmtEZiJQH0ja413WiMjLOLsIpYoC0JqmJlib5CMHRq1HS2w3J0AFoE6nok5tTHErY/DpfV4S+5reFUqNKI71Y6u3aTsAPDfzN1ys2onl76Orh0sMPXZ6R8H8OdUio/RoE8idz56occLCy5K4N80iIWkyjCFZQ2orIDPKIoCxNYhHFWA3RlsfjXF8FwhbIQSRjnN3Q6V4Sj34qqmQ6VHEoUJcyhwKxzjFlD2G6w5ccQX0XFFgcy9/28lyZNxlwc+bcJcGP+IuHObYmDmkEDuuGpBk67rtaTPGXR3NDqIy5Xt9ytxXE6OQ0qgLWPgEi8QYgQRAv16ytWPBk3b48tGj9vki1lTVr/ZVcX4xSDwwBkEAd6A4nTMHSCIA30PstmDTTcXJ2WqhUck6b8X/oBq0WjCVXF1Ws2me1gkajSHRdsgSL6haIzbzwSSjfH4vcy58ccOOVtvyvt4MBVx9QuzEw8Ag9ZMm3OfoF3FiilXg4H7nLKW5vlcfYHbiOvujcDO8iY+mJMqfIWyPE1LgbD36yiihbkS0yIkG2p6c7KyrEhxiDba590aYLoac159yU6MmJlFMXtPsmqQvaaPA1j2DYdOZxBHO5iOlvkudmTnlZuwTUMfsekfAfwY6tFRwLWDVx1J3Dfz7Io4kuwZ5nLo9boYdlJgpsENGn3PMpqFCgqyHZgoQZWrAaq0rKbKXiPFQ0Egx5p+PFbEzy7VZkOK8WfU0NvX3W7HijHs5+XNKXQHh6ZzAl3mjk+OAIrm2XS+fdH0kVVuIOQNsgoKVMoUFZJpFDmlY8qBaC6OJLYDTusEsafYiWJS5ZYva17S14kHY/sk45ThL4DGnKDuL5Rifi34Je9uajLhy/yGuo3AnZem0WolFJyOzpv1LHNenl4fv4PNsf8LPLg4eJpAvOW5Hi5XO3NdrF+oQSa8f5Gav9OhlayxfK/pr89i4wuHqYQxSd2jH5hld3rC5YCZG5MEe6yTyQ1Kuaprz/ALG4tJsTina7p3a+jMp8S4MZjXFs7rtgCPKLQuppMjpQfjyc79T0SxP1V5fkoHME2W22cOUFfAzKdCitCmn5JQ7Rrrg+4Kn0AY/Dsyk39FG7K4JnVoENAnX89lEUwN1QmT0+qYmC0G8M4RVrODWtJk7CZ5Qj3UDR7j8B/wDi7Jlq4oQB4ae56u/SOmvkhcvYiieptaGgNaAALAAQABoANkIRG9qtFENSdkRRA/Nsr4K5BsThHu39f+kUZpAyi2A1+GAzJnkDomrK/At4k+ykxuBa10lw8lojkbRnniSYP3G8pRcsH4UESvC7X5PoFoWULiy7HApLUyCylyhJkFlKeFsoUOSJ6WTKoLwRbPeXN1GDJBXRnzKVcFh2see3RY42pbkZNthFLGdFshrZQ6QuWGwTHcPpVjmLGhxvmAEnztdTL+pZJeEhuLPkxLanx7GZ+JuCueG9iGyxxcMsNIdECNjutOi1cYt+pfJ09JqUk97fPR5V8V4PEmRUpFgmTrB8idvdes0WXCv4SsrXPLqYKHFfIypwj26hdP1Is4jwTh2IRzVoRI5jC46H2VimGDBOdsoUWvCfgrF4gjsqL3zbMGnL6u8I91abKdHovw3/AOFXyHYl7Wf6t77vKfCPcolYLaPU+A/DGFwYijTAdpnPeefXbyEBWUWxdyVkI3KyhrjzUIQVqgHorSKYJVqOi38I0kC2wN/a84R/CC9wFiaNTd0jzTIyj4QuSl7lJi6Lp1WmEkZpxZAaUc/NFYFUTgrxVHvrHZlVF2KHKnEuxQULii9w4FC4l2OlBtLFBQPGiMnpzzXM1Onx+F/QmVBnbREXt5/Jcr0HJvwZ9m7sIGJ7pISHhalUhfpfFTAW1pNuv3Wx6WSXJocaQ2qZk2I+R9E/DpmpJPhhRXgEqcIwtQy+hSJ5ljZ94ldvCpx/7mVJMWn8HcPdrh2ehcPo5dTFOXuYskL7LDC/BPDh/wDlYfMuP1ctkZmOWMvMBwPCUr08NRaeYptn3iU5NCXFltnR2BQhcoShqsobnUIdCso4sV2URupDQ6KWSgTEdEaBYBXqko0kA2B1hzTEAwM0S490Jl12Lq+h7uDE6qvWRHhvsqV5U9oKFRBwVBDghZaQ4IGwkhULLHNKCV+CNErXrnZsUpc3yA0Gh7WiRBK5OzJOVSujLtlJ0yB+KnX0j6XW/FoUmmn/AGNjiroiLhtqt0YNNqXQyn5I5WpRQZLTKbFASD8OVpgZZllhytUDJMOpOWhGWSCWlMQpjgiBZzmyrBHCmFCDlChrnKyAtdytFMDqSjQLITT6K7Kob/SFym+ibbDKGEa3QIXNstRSHVgqRZhAF51yPW7RwagcwtgsIXNl7UKglkZdI6Uh5JF0KhnmklwShVn/AHMvJRyTLUS7ILKUtTKyqOla45nFE6OlPjl3LonY6U/HKuGDQ9hWmILDcPUWiBmmiyo1FpgZJoJZVkwCtCM0kFU6iNMS0FscjTFslRAiSoQQqFENRyhYO88yiBIXu5K7KGSoQlY5U2Wh7aiEshxFRGgTESvOUeuFBQuIViyqouzpVOFksWULxk3HSh9Iu0dKF4YksWUl6aJDpS5aePsWcCrjg9yqFlNjiKFDkxY+SmLmWiCAbCKT1pgZ5hTKhWiJlmEUKpnmtKMsi7wj2u80SESDG00aQtjnFECCVcWAVCgPG8WawdUcY2DKVFeeN2mUfpg7ybD40ESTqhaotMlOIMWVfUsHbiL3VlDnYpSiWNZjOqpxJY59a2qsoyy86evRyhGKqIcrKEVkFQkQ4IJBipbCOQss5WiHIkUciXYMjgnIUyWknRESCQnxMsyXC+JaUZpF1wzxe6MRIumoxTEqaKFFRX1VoplBxXX1T8fQqZVVNCmrsSw7hXhagn2Mh0WWG1KVIYJW8XuouiiNWUR0tVciohD9FSLZ/9k=</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEBUSEhMVFhUQGBgTGRUXGBcXFxgYFRcWFxcYGBgYHSggGBolHRYVITEhJykrLi4uFyIzODMtNygtLysBCgoKDg0OGxAQGzYmHyUuLS01Ly8tLS0vLS0rLy0tLS0tLy0wMi0tLS0tLS0tLS0tLS0tLS0tLS0tLS0rLS0tLf/AABEIALABHwMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAAAgUGAwQHAQj/xABDEAACAAQDAwgGCAQHAAMAAAABAgADERIEITEFQVEGEyIyYXGBkRYjUlOh0RQVQmKSscHhB1ST8BczY3LC0uKCorL/xAAaAQEAAwEBAQAAAAAAAAAAAAAAAQIDBAUG/8QAMhEAAgIBAgQDBgQHAAAAAAAAAAECEQMSIQQTQVExYaEUIlJxkfAFMrHBFSNTgaLR4f/aAAwDAQACEQMRAD8A7ciigyEe2DgIE0HdDQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CCwcBDQQAtg4CFmqKaCMkJO0MAepoO6GhU0HdDQAQQRhxk6xCd+g7zAC4nGKmuvAaxqHa33Pj+0RjtqSe0mFVgdCD3RWy1Er9bfc+P7QfW33Pj+0RkELFEn9bfc+P7QfW33Pj+0RkELFEn9bfc+P7R6u1hvXyNYi4IWKLFInq4qprGSK7h5xRgR49oiwq1RXjnEpkM9gggiSAggggAggggAggggAiM25t6RhEunPSvVUZu1PZX9dI28fi1kynmt1Zalz3KKxwba+0pmJnNOmGrOdNyruUdgjnz5+WtvEpOekvk/wDiiK9DDEji0wKfIKaecY/8Um/lR/V/8RzuMfPL7Q1pqNeEcXtOV9THmSOkf4pN/Kj+r/4g/wAUm/lR/V/8RzuE51a21FdKVzrSundnEe05e45kjo/+KTfyo/q/+IP8Um/lR/V/8Rzdp6CtWXKtcxlQVNfAgw4MPacvf0HMkdHlfxSz6WFy7JtT5FB+cW7k/wApsPjB6piHAqZbZOO2mhHaCY4XGXB4p5UxZktiroagjcf1HZF4cXNP3t0Ssj6n0RBEdyf2mMThpc8Zc4MxwYGjDwIMSMekmmrR0BCTtDDwk7QxIPU0HdDQqaDuhoAI0NsdQd/6GN+MWJk3qV4/nBgrkyWrAqwBVsiCKgg6gg6iKhsLY86VzASWZKlMROmqliXzTOR5MtyBWgDTdN2UXOYhU0IoRCxQsUjBS9pTHl840+WHaTzn+SKDmcS0+wLUKvOGSo1NADXWNXE4raEuSGmGeCZMmXd6sWT3eUlAK0ms17ZkAAodxjoMK6A6gHMHMVzGYPfWFgpGPO1OadZQn0cT2lmsnnlPqlkrNJNAuc56Ln1BUUMbOMkY8KWV53rMTPDBbGZJAabzFillyPqyTWtKbqxcIIWCnvI2krFkmTGIeYqrM5sIUXCURmtGrYgA5HLPdCI+JM7DSlmz1M9GM1ZzSzNQSpkh2mBUNArDnJQpoZikCkXOFCCtaCpyJpmQNBXxMLA0WDB/5a9wiFwmHLtTdvPARMtiZamwsAfZrn2CkSiGZ48DDjpGEFm+6v8A9jQ+Sggd9G+yRDypKroOGdSSaZZk5k9sWIMkEEeVgD2CPLoKwBHYvb2GlThImTlWY1tqGoJuNFplnU5RJRHYzYsmbPl4h1rMkq6KQSKX0qcs6jOh3XGNksya9JczUdYaagdb7WmegodYEbkRy8BOzsRT2QfAMpPwrHEY+g5xlTleSWVg6srKCK0PRb8/COHcoNizMJPMqYDTVH3Ou4jt4jcY8/jYO1IyyrqRkREnBTFlyqAXAlmyUWnm3oCR1ukwiYgjkjNxMk6IYS8RzYpzl9amrLoFoQOkcyTluBFctD5icPNvJCuc5lCGUEVWWqVJNaZMd5iagi/OfZE6iFmYWcSaipKzBXo6tzag+SsYJqTEJCkh3msACwIZWUqCADWii1j/ALYmo8hzn1Q1HirQAZmmVTr4w0EbWy9nTMRNWVKWrP5Ab2Y7lEZbtlTqn8LgfoAroZj07qgfmDFvjS2Ns5cPIlyU0lrSvE6s3iST4xux7WOOmCR1xVKghJ2hh4SdoYuSepoO6GhU0HdGvtHGCUl285AdvyiG6BnmzlUVYgd5pGt9aSfbHx+UVidOZzcxqTCRi8r6E0WWfjMO/WYd9DX8o1CMP70+X7RCwRHNZNEzTD+9Pl+0FMP70+X7RDQQ5rBM0w/vT5ftGWThpL5LNqeGVfKIGCHNfYFl+ql9o/CGTZabyTGrsXaJJ5tzU/ZO/uMTMbRaasgxhVRcqACI9sAzsWqArm4jO4afEgDu7aRu9Zvup35t+oA7xUnQrGSdNCqWOgixATZgUVJoI15ONVwabv7rERNmvOeg0HkB84lMJgwoy1474gkymYTpHlGjOEhqRJBrENHnOkaxtUhWlwBV+WvKv6FhwyWtNmNaitplQsxAzoBl3kRm5IcspGOW0dCcoq0on4oftL8RD8peTUjGS7Zq5itrjJ0J4Hh2HIxxfbGy8Rs7EgFirKb5c1cgwG8cDxHbvBzq20ZybTvodm2dybGHxEzEh2a+lVqTkqlRRaa0JyzqdKaRMbQ2dJxMuyaizEOY+akZg9oiE5Ccqlx0jpUE6VQTFG+ujr2H4GLAvRan2W01yPDsHjE0mi6pop0/+GeGJqs2co4VVviVrGL/AAwke/neSf8AWL7FA5dcpnDnDSWKhcpjjUk/ZB3Dj5RhPDiiraM56IK2aGM5G7OlG2ZjmBG7oEjvAUkRrejmy/56Z+Ef9IrsEc+mHw/qcvO8ixejmy/56Z+Ef9IPRzZf89M/CP8ApFTxWKKsqKtzuGIBNoAWlSzUNBUgZA6wjbUlAkM1CgYk0a3oCrgNSjEcBnE6I/D+pPMfwlylcndkg9LGzCOFAP8AhFp2RtLZeFW2Q6LXU0cs3+5iKmOTSNoK8wIA9St+aMABUgVqMq0PlG3FotQe0RzpR6HXxyswXv18m+USmFxcuat0t1ccVII+EcMja2dtCZIcTJTFWHkRwYbxGizvqi0eJd7o7fCTtDGhyf2suKkLNXI9Vl9lhqO7QjsMb87Qx0J2dadq0epoO6ILlG3TUbgK+Z/aJ1NB3RFcocMSocfZyPcd/wDfGK5F7pZEBEZyjx7SMM81KVWwVYEqgd1QzGA1VQxY6ZLqIk48Irkd8cyJK7M2w8qbLw8tvpLPa7TJjypfRZwlE5tArEdI+QzqIxytvz2+ivZISXiGdjWYxbmkU6eroXNQQOwCuZK2BcHLFtJaCypWiqLSdbcsvCH5hKKLVomaigotNLeHhE2gVAcrmmlbVCLdJeqTQzFXk4jEWTOhRTZJS5RpzmTZRnTlLiGMpTKky2mPIrdNJASdKeaQTzeTgSyN4zGcWUYSXSnNpQbrV4EcODMPEwzYZDqi50PVGq9U6ajdwibXYEZsTa7z3mKZdvMFkc1rSYsx1sGXsKj14TFiYjWwGDWUlqljVmdmY1ZmY1LMePwAAAoBGzFX5AyYZqOpG5h+cWfHY4S6ChJOlKZdpuIGu6vHgYgNk4YvNHBekfDT4xO4/CLMZa1BzzHAd6ka04amm+NsSdMhmbDMolhgejS6uYrXMk1zrrrnEHP2mJ3QNVNejvB4V3gxv7ZYS8PYuQNEHdv78h8YhNiSrppb2B8T/Zi0pPUkgialc3IlF5jBVXNmOQzyz8xG9hMVLmIHlurK2YYHIj+wYhuWUkts+eqqWJUUABJPTXQCKhMwbTcUHpMe+bh050yjLJUpOV6rQWjQHw4xnlzOEqS+9yjlTOkTMWisqE5vWmRIyFTUgUGXGM1wjkv1dN5hWMp7iJyUtatJeHly13byDSJPaGz5gnEJLcdCXYQrUEvmJnOgGlACxzG8mMlxUvh7epGs6NeOIj2sctTZzdXmmtsVqWtS44TM6a3U8Y3Z+AelObmWXE0VGbpNh5dCB7V1c9xiPbJVen7+g1+R0DETVVSzMAFFSToAOMV/ldsFMZh2lmlesj+y1Mj3bj2GIObgXum+rerHE1NpqaKhWvHpVI7YuspBzSUFBatBplQU1jbDmeRtNUSnZzPkHJwuExiyy7zJ7BpRfNJStvQLq+YpU5VAoI6hjXAlliaW0IOZ6VejkCCc6ClRWtI5Fy7wpkY0TUy52kwHg6EVP/5PjHVMBOXE4dGI6M5FbuqAfMH8ovjk7cWUxt24sfZe1peIQtLNQO48d6kjcd+6OM4iaXdmOrsWPeSSY7JsfZsuQGSWtBUdlRSugUDVm0r37hyzlPsw4fEuhHRYl0PFWNR5aeEUzJ0rMuJT0pkJPxctCA7qpbQMwBO7KuuohRjZZewMLsxTPdr5b+Ea+IkTPpCzADaqhcmC5l6tUEZigWIfB4BmBMu9X5t2BLTB/nTmYDM5GxRurUgnOMlFUYKKosGJwYcq1WVkqAymho1KjMEEGg1G6NUYGVfQO1z3uoDAgXEc4yggjMnfXrGmpjDJ2fMDLW4rQ5Ga1UYtWuXWypQbqdsYJezJyypYXJpKJQXkhnWYrMD2EL4XUiV8wl5khK2QiCiF16ITotTIMzjTTNm0oKGnCN+IU7Nmh+szBVFpvK9KjXXLTOrGvw3QjbMnAWqzFfV3C81a1GDZmtOkVNN9sQ1fUNX4snYIgpmzZ3SALUKqoJmEtVbND7BtNwOZqc84mcOpCKDSoUA0qRUDOhOdO+Iaoq4pdS/fwumm6em6iN49IfLyi+TtDFV/h1stpUhprChnkED7i1tPjUnupFqnaGOrGqijuwpqCs9TQd0ekVyMeJoO6FxE5UUsxoFzMXbrxNSIxmw86yyB90/oY0vqed7I8xGHHbemOaIbF7Ose8/KND6bN94/4m+cefPicd7ItuSv1RO9n4j5wfVE72fiPnEV9Mm+8f8AE3zg+mTfeP8Aib5xT2qHZkkr9UTvZ+I+cH1RO9n4j5xFfTJvvH/E3zg+mTfeP+JvnD2qHZglfqid7PxHzjLI2JMJ6RCjzPwiF+mTfeP+JvnGbD7VnIahyexjcPjEricd7pkFwwmFWWtqjvO898ekesBpopzpxK76dnHwO7V2TtNZw4Muq/qOyNoj1gNNVYVpwK77e3iO46j0YSjKNx8CpD8qCaIAD9o/lGvybXJid7fkBEjyidlkMVJBFMxkdRWIjkviiwa5iSG1JrlQRlqSy15E9C1LpDQqHKGjcgrmI5WJLmTEmS39W7qClG6KKjFjUinX7dIebytkrqk3IuCLVqthUGvS+8I09o8lZkyZNcTFAmmaRUHLnERR5WHzjDjuTM5ppAK2zTNJf2Q5lkClak9HujhlLiFdL5FLkTM7lHKUsGSaLcxVaX9MJ0KnPMjWnGGwG3FnTQiI1pQvcciCrlSpHhrWIyZyWcsx5xcySDabjWYrrea50AtiUwGzZqTVmPMDmxkbI1ze8U7Bp4ReMszlutidyWhJukPGOcco6yxzX+KMglZTAEkORkK5Mtf+Iiyfw+mE4GUGBBW5aHI0DtT4UiD5eY9k5sIxUliag0NAP3ESH8P8VNmCaZjswFgFxJp1q0r4RjsshjsshcJY9Y3aqmtO1t9M9BvPcN+rtrY8rFS7Jo0zVh1lPEH9I2Za+sY0+yorTgWOtufW4nuG+O5QbdXDKBS6Y3VX9T2fnGkmq3NJVW5S8byAxCn1bo69pKN4jMfGNb0Hxvsp+MRlxe38TMNTNYdiEoB+HXxjW+sZ/vpv9R/nHI3DscbWPsZPQfG+yn4xB6D432U/GIx/WM/303+o/wA4PrGf76b/AFH+cLh2IrH2Zk9B8b7KfjEHoPjfZT8YjH9Yz/fTf6j/ADg+sZ/vpv8AUf5wuHYVj8zKvIbGeyg73H6CJ/YfINUYPiGEwjOxa2V7Sc27qDxitjaU/wB9N/qP84ldl8q58sgTDzibwesO5t/jFoyx3ui0OWnujoYELO0MY8HikmosxDVWFQf0PAxknaGOs7T1NB3RX+VeIPQl7usfyH6xYE0HdFd5WSTcj7iCviMx+Z8o5uLvlOiUVXauNEiRMnMCRJRnIGptFaCNKTyhlWzGm+r5lyjZhwbUWYxUpW4ANnllQ1je2lglnymlOSFmChpStKgkZgjOlPGNLauwJc+lWeWBLmSbZdiqUmlSwIKmmaKcqcDUGkeXDRXvFhsTygkJ9pjSYso2o5o7GlK0oaakDOkNh9sy2NCQCXdVC3PVZblCzUXoC4EZ5VFKx62x1sCh5gInHEBhbcHZmYjNSCvSIpTSmdc4wSOTyS2LJMmqWDq4BSjh5kyZ0qplRpr0tprnWJ/l0BtncoZM0SwXVZkwL0BcwBaWJoW8qBmhuGlRXgY9blFh6oA93OOssWqxFWUuDWlCtBWorGhgeSii9ZjuZdxslgqFAEhcOrkhQ19gOVbRWtKxuSeTyKVYTpxZJizbiZdSVlczaRZbaUrkANaikS1ivxI3MmG27Ka0Oyq0wkKAWYUMxkllmtAW4rlWmdQK0jPs/a0ieaSpgagDZBh0SSKgkCuYIy0IpGjJ5Mylso80qol3IStswyWLy2fo1qGNeiQDQVBja2XsdJFtjObJSSBcQejLLEHIDpEsansGURJY6dEk5svEFJyMOIB7jkYs+1ccJTIaVI45CjZUraTnSuXs+Bquz5Jeaijew8hmfgIuuKwizOsMxoQSCK9qkGmQy7I7OC1aHRVmtiwJ0g0y5xdDqKj5xTOT+JsnlDlf+a/2fKL1KHQApSgtpSgFuVAOGUUPlRzMicXuJeocS11B4s2gHxzjbiGoOORvwBbtrYorg5zKSCspyCMiDaaEeNIrWz9sz0lSqTgUWY6u7esYjnFtLZ3WENS4aEiJDY+0JeJkUbNJgtZT8VNIl12PhmNxlLW4vv6xpU6/dXLTKE4Sm1KD2oo02QLbdxILKXW9piKoCqQFZmFyNW1hlTPQ1jNL2ziblueUA0vLqsnOWMaOwPQzFRuoDE59SYfpeqX1hBOuoJIpwzJOXGHGx5FQ3NLVVsGW6hWlNDkSIrycvxerIplZfbuJCr6wXATSwKLUFFRgOBGZoRqDGxM2ziAbAykq0zOigEJZQGpoB0jnrpE2Nh4cCnNigu3n7YAbfwAHhGR9lSTrLBzLb9TSv5DLsivIzfF6sUyuYnas9lmC+go5FAARZNVRQjsMWPGzbVzMYZ+AkAHoDMEHM/aNx38c4r/KXbSypZOp6qrxO4fONsOOcG3N34ErbxKbyuxvO4q0aShT/wCTZn4Ui6cjE5nB84R/mNdTjUhFHifzin7N2CcQeclsas3TD6i41JVtG35R0+XhwsoS1ApQSwCKjSmY4DXdpFoJuTZnGL1NibB2ks8OyilSCfK0Z0B+wdfPcOf7axZm4iY53sQOxVyHwEdPw2GSWCFFK65kk+Jzjlm1MOZc+Yh+yx8iag+REVz3SK57pGrGkdpLc/RNkmoeaaBFIW4jM1NBStBv743YjJ2xwROUTHVMSGuTokBnW1mUkVHGlaVjnVdTnVdTYXacklRzgq+mudSQO6tDTjTKNUbcls9sujj1XSuoDzrOMqjOiy2bLWHn7GRppmEnpqEIohyCsooxUsuTbiNO+uKXsEAgmbMYrZmbR/lpMRRRQBSkwnvAi3ulvdPcJt6XMly3Wl0yyqXCqhwW4Z0Ctp7J4QYfbqGy8Wc6JdBUE3TEL2kbqADPthJfJ5AFrMclAqAm0URJcyWqgKAKDnWbjWMy7GVSrK7go6uOr9iVzNuY0K18TD3CfdNzD4yXM6jBuiHy9kkgHzVvIxnjQ2PgeaViwAaY7OQDUKCxKoDwAPmTG/FHV7FH47Fv5AYs3TJR0oJg7DofzHlFxnaGKX/D/DEzJkzcFCeJNT+Q84uk7Qx2YfyHZh/KepoO6MWMwyzEKNofgdxEZU0HdDRo0mqZoUnHbKmSjmCy+0BUePCNKkdDjy0cI4ZcCm9mTZzyCLVtrlBIw/RPSf2Fpl/uO6K8/Ld65SUA7ST+kcObkYpaZZN/lY1I1oI2PTeZ7mX5mD03me5l+ZjHncN/U/xY1o14zSMM7miKT3D9d0N6bzPcy/Mx76cTfdJ5tErNwvWfoyNaLNsXZPMi5qF2y7AOAiViienM33SebQ8nl09elJUj7rEH4iO7H+JcJFaU/Rkai4TBa125utproG7cqDfovbFd5ZbA+kJeg9Ygy+8PZ7+ETOydsSsSpKHMdZDkw7xvHbEbjNozZeIElVqm7TTIgcd9BTIU30MdeTlZsW+6fbcHMcBtCZhZhIBtJoyHLT8mEdD2JygSatyNUbxvHYRujzlRyVSfV0oszj9lu/t7Ygtlcm2koWbKYxzodANBUefjHNwuPPhny3vHv9/oC/SccDvjYGIEUL6VOl6i74H5Qw28RqsweR/WPSJL02JHGNXEbQUb4pj8oK6JMPkP1jWfGz5mSgIOPWPmcvhAEvt7lEkpasczoo6zdw4dsUuSk7Gz7iO4fZRf7374mjyb52hYm6ubHMkbxFr2PshJS0UU4nee0mKNNsq02ZdibNWUgVd2/id5iXw63G/cOrpv1bx/KIXZ2KeZN5th0TquWQoSQRrQGimutd0S20dpy5I6RzOijU/IRa0kTaSN2K/yn5PfSBzkugmKKZ6MOB4HgY135UtXKWKdpJhfSiZ7tfMxnKcGqZnKUGqZTcVg5ks0mIyntH5HQxgi8nlO/u08zHnpK3uk+MYaI9zDRHuUeCLx6St7pPjB6St7pPjEaI9/QaI9yjwReV5SnfKWnYafpEzs3acqdkBRvZIFfDjFliT6krEn1OXUiT2XsCfPIopVd7sCB4e14R00IOAhouuHXVl1gXVmrszAJIlCWmi795J1J7YzztDDwk7Qx0JUdCVHqaDuhoVNB3Q0AER3KDaHMYd5g63VX/c2Q8tfCJGK1y+UnCqRosxSe6jD8yI5+Lm4YZSj4pEMoExyxLMSSxqSdSTGvIxUtyQjqxXUKwNO+mkZqxXcPsSYJUslmEz1atawW1OcEyaoZKE1pStT+cfIYoQmm5yp7FCxQk2aqgsxACgsSTQADUnsiBm4PF3MVJFBMVTzhoVuQSgATk1gbpNU3EmPcRsyYSxRZguk80tZxJUl2uuJY1NCpBz01yEaLhoWrmvT/YJ8GoqNDnCrNUsVBFygEjeA1aE99D5RCnDYmpyYkzGuPO0DSumZYQV9XT1YYgBjQ6xr4PZmIDIWvDASAz85UES1rMDAGrlmZlzy35b5XDQp3Nen39/2BOLtCUdJiZ0HWGrMVXzZWA7jGwDFewezZ4surX1Qdr86JKmVzBqfWOPzjHs/CTFaRIudbZQM4c4Wt5t1ZSCCQOcJYbuiDwpEy4bHvpl++33+wLbgMY8mYsxDQqfMbwewx1nCzlmS1caOoYdzCOPx1LkypGDkg+yD4GpHwIj0PwTJLVKHTxLRNtpBXq5j2Tuqcyp1GROWmQAtiIw+0ZU6dMkjJpdMiRnl0hlvU5GLBCLKUaKB3AR70lJtaX8/MsQs/ZwO6NKZsgcIs5SFMkRcFYXY44RtSdmAbonOZEMJcARRVUKraxL1oANbRWlTQDxMbqYUnr0p7A6u7rE5tvyyHSzBpWNsCPYAw4ucJaM5+yK99NBFBxE5nYsxqWNf77IufKBScM9OAPkwrHPNrpNaSyycneiBqgWBiFZ89SqksBvIEYZfGjHL40bEicri5GVhmKqQRkaHMdsZIqmD2NiJTc1SuHWYzBZL8xkySrTQPUIrCbVbs7gaHSMhwGKt6QmkmaTNtnlecl+ssEmjASQKyqgWk0OZ356V3M6Xcs8eExWJGBxq2KxZs8OWcTTS2VczqAaFiSQCaC4a8I1hsHElEWYZswBcIzgzzUzJTO04qS1BT1fCttdc4nSu40ruW2fOVFLOQqrqTkBujHisbKlf5kxUyZukQOilLjnuFRXvEVnGbMxky+4MbqqQJooR9IlsLUJtUiUpAJzqTXtabsjFMKG4q14sebfaszEyGtZmPSIlJM49agJhpXcnSizycQj1tZWtYoaEGjL1lPaK5iM8uYVIZTQjMGKjO2XMDGbOZ0FmLHOCaRzXPTmaWaBs+hYBStCBwETewEmcyHnV5ydSYykkhKqoCCulABXtJO+Iaoho6hs3Fc7KV/aGfeMj8RGzERyXUjDjtZiPOn6GJeOqLtHTF2ghJ2hh4SdoYkk9TQd0NCpoO6GgAjW2jg1nSmlNo4pXgdQfA0MbMERKKkmn4A5HtLAPImGXMFCNDuYcQd4jVjr2MwUuatsxAw7Rp2g6g90Qz8jcKTkHHYG+dY+czfg2RS/ltV5ldJzqCOh+heG/1PxD5QeheG/1PxD5Rl/B+I8vqRTOeQR0P0Lw3+p+IfKD0Lw3+p+IfKH8H4jy+opnPII6H6F4b/U/EPlGSTyPwqmpVm7GY0+FIL8H4jy+v/BpZS9gbHfEzAACEU9NtwHAfeMdRRAAABQAUA7BpCyJCooVFCqNABQeQjJHucFwUeGjXi34sslQQQQR2khBBBABBBBABBBBACzEDAqdGFD3GKLtPZ7SXtPVPVbcR84vkJOkq4tYAg7iKiKThqKThqOdQRcZnJ2QTkGHcx/WsL6NSPv+f7RlypGXKZUIIt/o3I+/5/tB6NyPv+f7RHKkOUyoQRb/AEbkff8AP9oPRqR9/wA/2ieVIcqRUI2MBg3muFUd53AcTFpTk5IG5j2FvlElh8OqC1FCjgP7ziVifUlYn1DDSAiKi6KKRlggjc3CEnaGHhJ2hgD1NB3Q0IjCgzEe3jiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaCFvHEQXjiIAaEnaGPbxxELNYU1EAf/2Q==</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxATEhUTExIVFRUXGB0XFhUYGBUYGBcYGBYXGBoYHSAYHiggGBolHxgWITEhJSkrLi4uFx8zODMtNygtLisBCgoKDg0OGxAQGzAmICUtLi0tMC0tLy8vMC0uNy0tLTUvMjUtLS8tLS8vLy0tLS02NS8tLS8tNS0tNS0tLS0tLf/AABEIAMEBBQMBIgACEQEDEQH/xAAcAAEAAgMBAQEAAAAAAAAAAAAABQYDBAcCAQj/xABAEAACAQIEBAMEBwYFBAMAAAABAhEAAwQSITEFBkFREyJhMnGBkQcjQlKSodEUscHS4fAWQ1NicjOCsvEVY3P/xAAaAQEAAgMBAAAAAAAAAAAAAAAAAwQBAgUG/8QALxEAAgIBAwMDAwIGAwAAAAAAAAECAxEEEiEFMUETIlFhcYEykRQVI7HB8WKh8P/aAAwDAQACEQMRAD8A7jSlKAUpSgFKUoBSlKAUpSgFKUoBSlKAUpSgFKUoBSlKAUpSgFKUoBSsV66qgsxAA1JPSqjZ50D4lLYCraLEFySSdwvQZZMVFO6EGlJ9yerT2WpuCzjuXFzAmqxiuPkXFOZQoJ8sxm2H8a2OZuMeGAigljqYjbtvoaqa8QRoBzySwIygwYU79RXK1+on6ijDx3x8lR2xTxk6VZeVB7ia91F8u4zxbCNlI0jVMg00kDt7vyqUrr1vMUyQUpStwKUpQClKUApSlAKUpQClKUApSlAVjmznXDYFgjrce4y5gqgRBJEljoNQe5qK5W+kmzibvhXU8FmaLRzZladApMCGJ26HbetX6TsDadma5bby2AVvpqbbZruVXXrbYiM3Q++uc8FwmDW7YdHxGJui5aYsqFbNo+IhJJO8e/pWGD9GUpSsgUpSgFKUoBSlKAUryzRXhMQpMAgmhhtIy0rQ4pxS3h0z3CY9AT+7aqpf57zNlVfDH3m8x+Q2/Oobb4V/qLFemusi5wi2kePpD4wyjwIChvMWkGROmkaVz3BXS962qmS1wKvckZT169de1WLmXib3LTNdObqPZ0Hw9NPjUfysrWnOIIClTmQkjKJUTpvoPdXLnbGyW99jq6Xqenp0TWMS54+X/gufN3DHSy+IjxGXUougCxB6eY7n41RrmKVLYAS4cjSyT0KkiSOkH8qseM5wuOsFrAzqQrnViVYiQCYB1U66dxFU3g3GHv4hiUhdJJyjbQyNR12HSpblBvdD8nlJpWPfH8nWPo+vq2HABadWyMxbKCTtI26fCetWquX4Pja2rgfOu+3mDFQRnEHYQQf+3vXQsTxK2tsXMwYGMsH2p7VNpdSnU3PjH9i5Bpx4N6lQvBuNeM7KRB3WPu+vrvU1Vuq2Nsd0exuKUpUgFKUoBSlKAUpSgFKUoBSlauIx9tNC0nsNT/SgKP8ASHh7xvq2Huhbow7Dwjvetkt4gE6MVEHKe8jUVzvCLxZ7dl7jizhlNsqpZLQdQywAF8zkgbHea6Bz/wAUWbbm0blgowuldLllgwFt1O6MCzDsZjqK5UvF8GqKEw1y9fCibt64WCFQJNtFmFWNJiIrL7GD9N0rmFvnfFNcD6ZQdUiFI/fPrXQODcUt4m2LiHSYI+6wiR+f51opJmzWDfpSlbGBSleWYVhtLuD1XwmsTXagOcuEXsVhzbs3mtPvEwr/AOxo1g+n51B/EwzgztZLXblu6CAwMEAEGeoB99RT4dgx80ZTuN9gfhvXJOD8fxGDdrN+2+WzOYgxcsxoMs6Ean3hjvoKs3GvpCt24CZLty5EQQ2vsRC7mR6VerktvtZSnHM0px+2PJ8wPNNu1icZhL5ZvEuwLrsWyKYhTm2QAk6dTU7c4BhBeuELmXQoMxKwyg6RuJneahOZOVHRvHADu6C5fIAkEAKTpuun5VBYjCY79nuNbNy2ioXJkqCEUmPvEb7Vy5WZtxKOT1NOnS0ynC3bxys/+5PXGsblxN20keUjyAAABlBEDtrWS7jQlv6xfL1EanXp3rY+jXgNm7hGxJKnEs/oSikhVXXUT7XxqS4jwwsWsvbmNCDsJEgz7iDp3qf+XRnFycsM8lqJp34SbWf3Kdb4ypRiLUNJZNQ0EzvoNCD+Va3CuIWVJMZbjGAUXyqSNSdf4VMYbhdlL7o4ECB1IICjcnpFb2J4RadYQDXbpXLssjXJwZPGiLeFwmaiAI4Fx3uKh+yd5UTJEE66xI3rfu8ahARcMDzFGzZQIgD5BRv2qt3nKwjAmDlmddNCfyrFi74yEgF9dV1EiTr8tKi2OTWT10ui01aNpfqx3+WdA5Q4iTirIAtQymck6nbSJ0B3HuOmtdNFck5WSyfDusCsQZEeUjSdta61bYEAgyDqD3FdHQyjtcV4PMQjJL3HqlKVfNhSlKAUpSgFKUoBSlKAVWeZyyDNbC52YLDmAJBM+7SrNVY5zSbMZQ/1i+VjlHXr939KyjDOe8w497b2WOLt5zcKGFmyqspBW59+22x7QD0qC/8AkBbweRsZh8OptkeDhrQe/dkEfWv9ievvqW5lUMLVsmw83QDh7WmYHoLh2uGND3A71G8K5WZrRKcOd7pDefFXRbQHWMltBmYxGrQJ61nwC3fRjwfD4m3ce+rObdwoEYnLESJA9o++dq6Fex1iwsAAKo9lQAABvtp8qof0K5lt4q24IZLqhgdwcvbvU9jlGZtJ1Ilthr071pwlkxKbNTFfSjhFxC4YWcQzsyqDlQL5yAG1aSus7dDVvx+OW0huOyqigl2YwFUAmdtelc8s4K215Lty3bY258I5WBT1bzlX20kaTW7w0MCfGuNfuMfE8be2/SFGq21giFHQk6mTXP8A5jW1wzfBZ+LcyYWwoe7dCIdA5BgmJgQJNZsBjrV60l604dHEqZ3/AK76elUbAc2WsbebDXcHc8ELmz3RlIIOhykeWTMEGakMdbtlbNtCRbtsfJubhZGXM2uoEk6gyWGogVFfbWl75Zl8G0OWkWv9tSYzCYJ+A71CY7jJdXRDDT03y+p6E/Oo/D4AeYsqwNdtREkERpWZh9WNIzEQI39fQ1xp6iTR0YUQi/kh+O8uJdRhaVFuXEys+sNlGYTHXcTvqK5nxTgzYTw3YDxAxzL0MGVI94j+5rtF+2Qyjodxt8fQ1o8b5fsYpSl0beyw0cHuD/7BqxpdZKt7Zds8icE/cu/grPKvOigOjMbiMptwdHQa5YHVdTp66dql8bx6xcQYW23iXr6eGFTUBnSNTsAJk9YBrmnMHA8RgLujaOCEuLEOoIkEGYI8sg/M1JfRXiLdvGG9dOa4qxaUzu5hiIEAgaT0zGvQaeLljY8pkGp1NezdOPuXx5+v+iycs8Ev4L27suCNFBVRl6GT5uh16ipbjPM1q0Wu3QVzRsJBIUA67DbrVmxSWsRaNzZs4B2DKGKiGHQwapX0mYC2nDruUazb1Jk63F+FdKcobMNco4FNdvqbk+GReFGIxiYjGW7Y8FXAGskgIM59QD27+la2F4m6NLar1G3y7GvPIfN7W7AwrgGxKyQPOi5wzwB7QYBhG+s+ldDu4bCXcS962ttgURgwAiSbgYx0bQT10rh20Rtm8cfJ62h1004trUk1w1+DnPHcRme2UUhQCTpEyQADp8a3MJwN3QFlI6gTHX0qd4kFfEOUZWIC7EHWNjFTWEtFRDb1ydTd6L2R8FSWqtjH04tpfBo8N4d4VsCIFXjlxj4Cg9CQPdP9Y+FQdjDPdIVRMdeg99WrCWAiBR0/P1qx0pWTtdnjH7lFszUpSu+ailKUApSvF24FBYmABJPoKA9UmqjxDmxiYsqAPvMNT8Olan+KMQeqj/t/U1YWmsayUZ9Qpi8ZL0KVHcH4kLyTpMAkAzE/+q2b2MRZDMoIAJE6wZjT1g/KoMNPBcUk1nwbFVfnNZskFQ/1iHKxgHzAb9u9ZOP8WvmxcOCCm6okZx06wOp9+lUnA8Zu3eFM99vFuC4c+fQyL+xiMukCO1OzwzCkpLKJflxRcuNbL2AVQstu0shDIElup1j41vYzFC02Qhi8TkUFjHfTQD1NV/6PuKPcxLqFRVFokIigDRk36kwTual+ZDihiClmZa2oYgDYM8anQbmk3hZNo9yGucyFb6XLdsISQH11uDYT00qwYjEBzmy79WOgnoKofHscj+ELdoWwpHvcmJJPw/Ordh5KggToNW226Co224Gkl7jYsWgBX1EVVCjQAQANIA6CqNZ5kxF+2zh/DCmGRAM07CSwMA+lTPAsQ3hM91ydTuZ0AE9K8tHp1kpYk/uWKoOx9uCwWShJIWW2zdY10ntOvwrOLClg2UZgCAeoBIJH5D5VU243dzxhwpk5TmUntEQRvJqc4bisW6EsiqRpIRtdBqMzVFfobFL29iS2r0+fBMPAQZtA5KqZE5oJgd9AT8K+kKVUdunr3HrWgmNvIq6hstzMwZQSRHTYJERIH2qzcAYuSt9ybh1HRWn4b79YNSvTpQioy58irVxziRv2sObmukDeNzr0/X0rcXAoD1PT8vTY1uBfsgRAEERWvj8UlpC7wvT1boIjc1MqIxRmVrfJH8Y5ewuJteHetyOj7OrbeU/ZO3oa4zzfybieHtnVma1MJfSQROyvHsnp2P5V1z/5XEXDKKqjbUSdNv7ivty3fuq1t7hZWBVlULsRHQTVjT6z0nhckEpKRzXgfPmS0fHcC4IiEbz5SsE5dye2kZfWo3iXOzYhsly2blknzoYUEegHUbiT0+NWJ/oqxLXCFKeH9l3MGPUCTNSuD+iBf8zE/BE/ix/hXoJWuyGH5/crQojGWUcs4xgLFi4tzCYjOrDNBDK9v/Y8iD/T3E7V3mG6QUtqyAnUFyREnKDsWiY1rtvAvo7wWGuLdU3HdZgsVjURsFFT2B4DhLLFrWHtIxMllRQZ98TVZVfPP18nQr1Vlaai+Gce5M5S4lcuC+FNr/fcGVSO2Xdh8PjXXMJwRABnOduu4E+7f862OI8TSyUDB2LkhQis5MCTtsK+HjWFEzftAglSC66MoJKnXcAGR6GsT0tU5KUoptEEpOTyzYt28rQBCRsIiZrYqLv8w4RACcRa1yxDA+24tqdOmZgJqTFTpY7Gp9pSlZApSlAKwYu0HRkOzCD8ax47iCWhLfIb1SObea7xtsthGAOjON1nSIHfaZrZqSjvx2Fey2xU7km/lmYcvq4zWrudSSJCltRuDGxHaKzYfld58xJHoMvznX5CqRy9xXF4e74ihgrt51I0aT2PXfUV1vhGOa6NQB2I2O361LDU2uGWsEGp6bpartkJKXnhmllw+AtNcdo077nfKs7n9K5Vxfma7fveP7DAkKB9lN1Hru0zXT+cyMqKwlGJDDTsO/WqZa4ThUM20JM+04Bj4EmT/eu1Ry01l2GmWtN1PSaLdGyGX2xxjDJnlPGXLlwBlIIXz9pIiPTeYqt888Lu2BiHw3mzaXresNlIIugD7YjXuPdVn4XjTaeYkHQ995n31ucTw+Ym8hzKdT3U9Z9K16hCyG2a5wUunXVWuUe2W3j4+xy36IOKMeIHOdDYeAIGua3qO5ia6Dx2zfuXSLT5B4a52LZQBmaJO8b7Vzvmfl9sNe/a8NKDNmOX/LfuP9p7epGxr3xHmq7i8gt4e490JDqgJWQSc2kwPeNKhjbGyG5FyUHGWD79IPFgq4bw3Vsp8yKuVR5QYnq0jevF/wCkJsipYs+aAMz6wewVfa+fwqA4pw7FupuXMgCicgMkfKZMetb3JOPsYbEZb6IwYjLfENkMxIP3D1I1Ee+I3Ytr28m9tVlWN8Wj3y1w3EJdVyRbU6PnE5lJ1BUa/OI3q1Y22quRbECNQDvIgwe3T9KtvFuCYZ7pvZjDifDWPajeexqHwos24U3AWOndfdO1cy+xqzJZfppxlp1KTx7voaXBry2rguG2G06kiNR5tAdRr0qxpzZaZggtMJIAaUCQSQGJJkbdqhsZwstJt5YO6kkR3GnTetzgXBTmklSxGkeyqjt3OtbQ1WF7TE9RW47vJ4wuLuX2ZivhrPlnePWOvzrbQHToazMOnr/YrLhcIztlX+/0qjLM58LlnLm90m0b+F4wxTIyZnBgawDB6mvtvhV684uXSNPZGuVR6A6k+vWpnh3DktDTVurf3sK3a6tehbX9V/glWccmlZ4dbXcSfXb5VuKgG2leLm6+/wDgay1errhDiKwbHyKwKfrT/wAF/wDJq2K1l/6rf8F/8nqUGzWrj+I2bIDXbioCcoLGJMEwO5gE/A1tVF8b4SMQbMuyi3cLnIzoxm1ctwGQgr7YPwoD3i+HWMQbVxwtxUlkBCupzKIbUHpqCO9Q68p4Zzd+udvI1g6p9WpzOF0XdfFJkyTIma1zyUogW3W2AzEMqHOgNwMmQzoQgW2SfsgViHJl0IyLet2w85vDtsuX6vICnm0MksZoDds8qWA/lvvnXKxAFoebxfFVmCqM3mQxmnrrVoFUz/BjZw4awhDo0JaIC5GuGACxB0cDXqCRFXNaA+0pSgFKUoCN4vw5bgk79xVYtcJvIWX6tlbQ5p6bEAaz8au7Edar/EOYLNpyqpnI3Oke6etWaZzxtSyUNTTUnvk8EB/h28SBmkToACAPcD+/U95q5cGwHg21WZMa/p+ZqN4fzNauMFylSdtoPyqZtYtCcoOsTHu3rW6U3+pEmljUsuDyaXMeE8Sy0CSvmHw3/Kao0xXTSKqHMvBck3bfsn2l+7PUelS6W1R9rKnUdNKX9SPjuQoapbl++RcC7q/lI6Gag1NS3LrfXoPU/uNXL0nWzmaSTjdH7mtiranMpEjUEHUEbfGtrgi27bJlVUVT7KgKPkK0nPmM9zPzoGIOleG3NS/J7m2lWQXyeeMcAwgF1ldiTMDZUn4agT1rlOM4K1nMC6taBEOAxZBO4XQCSYPzrt/CMmY59VZSpHv3qucY5XwwtOgvF2bTNoFUTv2J+NWYWOK38YfdGIXQtjL+JlJyXEUVzkbmYo6YbFaLK5GboDBCNP2CCIPr22ufFOWLIuO/iQjeZLa7yenoJrkuJ4U9kEXMuVSctxYaTplB1BCmN4ME1c+TOZz4gw2K0IIVGfTb/LeevYn3dqkthGUW4JPJDGy/St7crJNYe5aQgM4zdN4B23GlWDAYhFV3GrgHJr5ZIgAxrua0uJ8sWPFa4bmW23mFtR5p6j0E/vrxhMEQJnXt/fWqLi6Z8ckeqjRBR9FtvzkyWFuOQIljue7dSOwq4cPwa2lgb9T3/pWnwLBZRnI1O3oKlWSa6Wi0+1epLuyCK8s+19rGFg/D+IrJXQNjFc3X3/wNZaxXN19/8DWWtV3Zk18VjbVuPEuImY5VzMqyewnc15dgrs7EKoQSxIAEFiZ7b1Hcd4Tduur2/BJ8O5ZYXlLqFuFDmAHtEZPZMBgdxUFe5OxD+OHuoRczlRLwGdboDEAD769WPl32jYwXetbG8Rs2QDduJbBMAuyrJ3gTvVSblHEFh9airJJVWu+VT4w8Bf8A6/rFadNbQ02yzCcAMWAzkCy1w+VnU5XJyKCNYAIEbaUBPTXlLgIkEEdxqPyqntyricxPjLBJG9z2izN+0/8A7gECNtN+la+C5SvhnUlEth1ghnPiWw1lmSNlQ5X0+8T01IF2GISA2YZSYBkQSTAHvnSsgNUz/B1yQTcRiLivqXgrbuYd1X0g2mjsW99XMUB9pSlAKxYm8EUsdhWWsd60GBU7HesrGeTEs44Obc78x49RbbDqCC2Vrce0rTBzbrtv61rJmK5iI2EbmYJOvUafuqz8V4BcLDK3lGkNvHaY2r7b4MJHiHOV0W2ghR740+cetdBThFZRxZ022vEl28lc4eG8Rcu4IJ9ADqT2EVc8HbJxCn7qksPuzoqn/duTXxeHlQJy2lGsLE/oPfr8KiL/ADUtuUsWxAPtMT5j301PvJqKzdc/aixTs0sfey6ivNxAwIIkHQjvVX4bzgjGLy5D94SV+PUVZLGJVtj0n3g9R6VWnXKD5RdqurtXteSmcwcJ8Bgy+w23oe1R2GulGDDcGRV45iw3iWHAEkeYfDX901QLZroUT9SGGcPW1ejbmPbuTHEcMT9cgm2+v/Fj7SntrNaS1n4dxFrR01U7qdj+lSQwuHvCUYW7nY6A/Dv7vlXB1vS5xblXyeg0PVa7IqM+GRSXCKk+G4VLmdHgq6lR6E7H31o4nBvbMOseu4M9jXmxcjrXIjmuacl2L91e7FkO6Ifi3JpFl1e6pdhCqBI33Pu3qpcscCuNiWs3rLtcQZ51IhRsehUiCPdHpXTFWpDBXCpkVNVdy1jhkE9fbbap2c4IDBYfEw1xSWtr7QYnSPuz+6p7gyeKdoA9qpO5ae6MoAVDv0Bnf31v4PCrbXKo+PerENKpWKS/T/cxqbvXs3YSMyrFeqUrqER4PtD3H94r3Xg+0Pcf3ivdAYrm6+/+BrJNeXQHcTXjwF7VrzkyZZr7WNbQGwrJWVnyYFaPFOJLZC+R7ju2VLaZczEKzH2iFACqxkkbd63q0eJ8OS8FlnVkbMjo2VlOUqY6aqzCCDvWQaycyYUkAuUbyyjq6spZVYBgR5SA6TO2dZiRPheaMISIuSCpaQrHY2xERmJIuKRAIIk7Vj/wrhoAHievnYlhksoVYtJYEWLRM6kqddTWra5Kw/hhLjPcbIEZyR5gPD0ykEZR4SwNY331oDexHNOCRHbxQQgJIUMS0BicunmgKZjQRrFTFt5AI6ifnUA/J+GKqs3BlDBWD+YC5IfWOoZh7j7jU/bSAB2EfKgPVKUoBSlKA8MgO9RvFOL2sOIO/RRvW1xTF+FbZ4mNh6naub466zsWYyTvVnT0+py+xQ1uq9FYj3ZvcY5guXpUeVT8z+gqCJr3Xg10YxUVhHCsslN5kz4KuXALxCYaN8zL71kz8P0qH4FwQ3vMQcvQDSfUnoPzNWbCW0S4p0yp5QQNJOhA/wBoAPvM1U1Via2nU6dp5xlvZYiKpnMHAmtsblsSh1Kjdf6VbhiEP2h869hgaqVzlW8o6F9MLo7ZHLMRavMua1spGdQJaD1Hpp+Yr1gbGIdgMtwAzLsuVVAG5LACr/jOCWnOZZtt95DHzrUXlkfauM3v/qaxZXC2xWOcl9PBmm22ij0FVB/8sckPwTiNzRLsOjeXrt0Ouo7xXlsG2cqoJgkaa7GrRY4NaXpJ9a30tgbAD3VBraYXtNeDfQuyiLUuf8FewXBbkeaFHzP5VMWOH216SfWtsUNR16auHZEsuXk8WrgJIH2TH5A/xrJWjZxNtWuBnUHPsSB9hKz/ALba/wBRPxL+tWAZ6Vg/bbX+on4l/Wn7ba/1E/Ev60MHtgZkV9luw+f9Kx/ttr/UT8S/rT9ttf6ifiX9aYBkluw+f9KS3YfP+lY/221/qJ+Jf1p+22v9RPxL+tMGTIJ7D5/0r3WK3ibbGA6k9gQTXu68AnsJ+VDB6r4agOB83YXEpnVsm0AtbaZFs722Zf8ANtgiZBbUVn4TzFYvsyrmBVA5kaZWAIMiQd6ArC4Diliz4lt7j3LkTblnKFfFaW8ZnEsTbUhAggbjSNlb3FBfzkXSis2kWgrI16wYygT5bS3YOYyTvJyiyLxzCllQXQWaAAJ+0qsusQJDpE75hR+M2FRrlxsiq72ySCZa3mzezJiEZp6BSTtQFcTEcXPhsQ6yy5kyWdB4do6/7SzXgxzaZFgjrdRUJj+asFaS65uT4YbMqhixKByQumv/AE3E7DKZIipsUB9pSlAKUpQGpxLCeLbKbTsfUVReJcIvW91kdxrXRa8soPSp6r3X9ipqdJG7nszl1nhd5/ZQ+86D5mpTA8t65rpEfdHX0nt6Cau/7KOv5QP618vZUEgCaklqpS4RXh0+EPdLkiWPh24IyruQNGb009kbADfasHECVRJgEusgbCdIHoJA+FaOJ49YzF7jqqIZBY6u/SBuQN/fFV3ivPduT4aG4e7eVfgNSfjFU77IweGdvQ6W2+KlXHK/6LJhBmtsG1CjWWK6g9/snTeot+abdh1VLhug7rILW/QsPKfzrn+P4pdusS7GGM5QSFk9hW3w7hV1grFcqkxJ32Osdv6VFp7bLJbIrgt9Q6fp9LS7rpe7wlxydk4TxUXFVgZVvmp7Gpaq3ylg0WyoXsZ/5Ex/fvqxptViaxJo49MnKCbPVK+VhZbk6Mseqmf/ACrUkbM9fKwZbv3k/C381Mt37yfhb+agyZso7UyjsKw5bv3k/C381Mt37yfhb+ag3GbIOwpkHYVhy3fvJ+Fv5qZbv3k/C381BuM2QdhTIOwrDlu/eT8LfzUy3fvJ+Fv5qDcZsg7CmUdhWHLd+8n4W/mplu/eT8LfzUG4zBR2r5cSQR3EfMVjQXOpUj0Uj95NZ6BPJXbXKGHUL5rxK5fMX1Kp4ZVDp7I8NPXTfU1lw3KuESPq84AUBbkOAUACMJGjLGhEbmp2oPjfDLt6/YIMW0Dl/aIJm1lEK66kB4Osa6a0MmHB8qWrdxWD3CoynIzTmZMgQseoUW0gems04lynh76ulxrrI7tcNvMMgZwwYgR/vYiZgwRBAIhLeE4sxVWN5FBRgy/s4yFbGoA83iS5Mltvu7NWXLxlnAYsqM/nCjDwEFi+QFJJYhnFlWkT5tCBJoCXxXKeGuBgfEGZWQlXIJW4bpddOh8V/wAoggGrAKoscaCn2yQ4hFGGAKgXfKHYkqp+plipIJ7TF6FAfaUpQClKUApSlAfJqt818SyrkU+ZhHuHU1YLx0rn/Esxuvm3zH+lWtLWpSyzn9QucIbV5NHB8NF0kMMyhSxXvHSoK7y2paVYqp1y7kegJqz4S+1tg67j5Edq37mOstqcOM3WGj9wqzdRCyWZRyVNF1G/TQcarHEg+EcvJPkQEjUs2sDvJ2qfbAqVyIRcckTl1VRvv8q94HDNfbKRltjUqu39Se5q0YXCKghVAFQzmq+EsE0IT1Hum2/qzHwrCeGgUfE+u5/fW+BRVr7VNvLydOEVFYQpSlYNhSlKAUpSgFKUoBSlKAUpSgFKUoBSlKAUpSgFKUoBSlKAUpSgFKUoDHdFRfEeE27up0buP71qYrzkFbwm49iKypTWGij4nhNxDsSOhH96V7wvDHYwFPvIiKumQV9CirH8XLGCiumwznPBqcPwK21yj3k9zW7QUqq228s6MYqKwhSlKwbClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAfK+0pQHw0pSgP//Z</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMTEhUSEhMVFhUXFRgWGBgXGBgaGBgXFhYXGhgXFxcYHSggGBolHhcVIjEhJSkrLi4uFx8zODMsNygtLysBCgoKDg0OGxAQGi4mHSUtLy0tKystLS0tLS0tKy0tLS0tLS0tLTArLy0tLS0tLS0vLy0tLS0tLS0tLS0vLS0tLf/AABEIALEBHQMBIgACEQEDEQH/xAAcAAACAgMBAQAAAAAAAAAAAAAEBQMGAAECBwj/xABGEAACAQMDAgQEAQgIBAQHAAABAhEAAyEEEjEFQRMiUWEGMnGBkQcUI0Jyc7GzMzRSobLB4fAlNdHxFUOSwhdUYnSCw9L/xAAZAQADAQEBAAAAAAAAAAAAAAABAgMABAX/xAAuEQACAgICAQIDCAIDAAAAAAAAAQIREiEDMUEiURMyYTNxgZGhwdHwBEIjsfH/2gAMAwEAAhEDEQA/APEzTu/8L6iEe3auPbdFYMQBza8RpE+RYDEM0blE0kavRdxe21g2E/TLpLdxxfvLuZNH4lolAsFQvI43Aek0TCD8mZ/4npvrc/kvXuertjMV4Z+TIT1PTfW5/JuV7trLcDFK+w+BTds0O9uaNcVtLM1ZSoi42L3tQKHa3TPUaQiuBpTVFNE5QYGtvvUiVKbfau1sYo5C4kVpJNFKlcJboyzZJpZSGjElsJipBRCWYEVERFSstVBmkWi1t0Jp2osXKm+x0bbFb05JNbS3PNSlwooWGiV7gApLrysHuaI1etAFK7up/Gq8cX2S5JLoDv2ZrmxazkUTNdWLc10ZaOfFWNel2A3lPb8KbXtINoC0v6XbIIpxdHp6Vxzls7ILQvKhcDmt2x61K2nM1OtmKVsNAV22ZqNhTNbJauxpQK1hoS2reeKKFicUZ4UdqgvXtta7NVAN7TAUr1Viab3rp9KkXTCJNOpUI42VC9pZ7Uk6l05u2au2v05MqP7qBXReGJOSK6uPmrZy8nDlorel6OLeXyfSo797ODAHpTXV23uMZxUQ6eB/rV1O9y7IvjrUVo+fTXpGj6ldTRB7x1yA2QtlVuWmN3amwPs/Npt2QJ8zNJGF3ZI83Nel6X85TQLcuaXUtusAWVtXdaZTZAvXSLht27cCQgGZGFXNeeeiVz8l/wDzTTfW5/JuV77qCcDtXgf5Lv8Amml+tz+Tcr6FZanLsePQBfsDkVsWoohrdci3NZM1ENy3xUb2QaIah7jRTIRgVxIqa1aBrsJuNS+H6VRsmkcFY4FdW+a6M8GtqKAxOzYgVGqVLbXFSW1iluhqMtIaJtrXNsdzXbGKRsZIx7wFLtTqJODXerPYGhCKpBEpyB3UmtC3RO2utlWyJYg4FG6O3J9q3Y0m400sacLST5EPDjYZoUijwtA2jR9s4rms6DS2xzWPArN01zeFYxz48cV1bfcfYVoWKlYBRWMauLQJ00mTRQu0DrOoAYor6GdeSW6oUZoI6ndiuTeLd8elR2hBk9qZIWyZNMAZzXN7TBqy5qRBk0M3UQMKJNFKTA2kSt09R2BNK9R03MkkewFNbbmJJ96Gu35PlBYevH8aaMpIWSiz5n+F7Nh9XYTUmLJuKHPAjsCYMKTAJjAJr0pOmaNrYmxatWhb87u6gkbT50K3SRiCJzJAjtXkJr0gG3+Ym6hthFtWRZdtHfK2HFkpqf0q2tjO9w8sWE5wQKFbsLViH8lQ/wCK6X63P5NyvozwxXzn+Sw/8V0setz+Tcr6OS5HNS5Oy3H0c7K4a3HFTs3pXIE80iYzQK9uaGaxTQrWxammUqFcbFfgYxWhaNMWtVz4dNkLiBbfWpltYolLNYbdbI2IOLXpRNu3WKIruaDYUR3G9MULcUnvRZSo4pkxWBvbNcDTmjwlZPtTZCYoA8Kti3JokrJqW0kdqOQMSXTJAooJUdsRmujdqTdlkqJkxXZvUGLk1s0KNYfau1p7maBF+KiuaqjTBaGx1QFC3L5ND2DjNZeuen3o0azWo1W1aSAs7zRl/J9q5RwuRzVY6WiUtsMIW2M80BqNb6ZqO/cJqBLZ5oxiu2LKXhGmV37wKJ02mjgSfWubdv1NGC5AhfxoyfhGivLJhphgE5Fc3tVaTFRtadhj8eK6tdDHLGSanryx9+EfJxq+dJcXXGsT868O1pksuGt2lsBF04tNb8Z74UqzSYiSW4JqhmvRbF5run/M9VctPebTILdpN6XktqEvWre7abBchEO0gMQY3BsUwRL+Sf8A5rpfrc/kXK+jmsTXzj+So/8AFdL9bn8m5X0erGufl7LcfR0titm171oMa6qdlKNi1Ugt1grqaGRqI9ua5NqaIArqKbIWgU2yK52UWVqJxTJgaIilQMholTWsU1itAB3V2oo1rYqFlprFog2mtbDU5BraVrBRxZtVOixWNc9KjN2h2HSJDXJWufErResayUVw5qM3a2KxrOStRslEBZwBU40hiYNHIFA9q12oi7ZgVJprEZNFG3ilctjJCF7VaXSzTO7aqFmp1MRxAzpxWvCorbNSLp62RsQEWSaKs6WjFs1prgFK5tjKNGmFdLQz35qW3exmlpjWj49NehqiraGpZtMNTasWVuXWa9NsXdP+gYWiNt6+bahZU4bJUwWCX/4ddT/+Uf8A9Vv/APunY6L1/wAPwvAJTaqQU0hJVE2JLESSFwCTNVzj7iYS9hN+Sr/mul+tz+Tcr6NN08RXif5PPgnX6fqOnvXtMyW0L7mLIYm06jAYnkgV7Ywrm55LLR0cMfTs2LldLNCtIrLWpgweKkpIdxGatXVcIQRWLRAbqVXrmK0UrbRtMkauCK4UkVIINMpCuNEBQng10LVSNW1Bp8hKNC3WeBUoFaINGzUQPZFc+CKI21ogUbBQMyiom+lFso9KTdR67p7QdmupKGCqsC0zEbRnBmfSD6UyYrQSUrWz0qqWvi97lxtiLsAGCTJIJLENxkEYPp9qaW/iZAX3I0LB3LldrcEscTgmPTvWlLHTMoX0O1SK7CVvS31uIHQyD+I9j6Gt379u2AbjqgJgFiAJPAE96GQcQqygHHNGW3xFApr7SrPiJExO4RPETPNGhsTSJhaNPiqV8d6++iALdayvjou5GXc1o2iWORKkMCPsKa9d12ltOfzm7bUkAhbjmIwAQhMYMnA7VTPib4v6f4apbZCfFVzsQ8KSYwMzgfjRVraVmI+n6uz+ceEl6+7btouvee6LgZGllX5UhoIgV6HprXlWTuO0S39rHP3rxrQ/FOmU29qM1wXlfdsVVgNtwJkDZ/eSa9H6f8TedbdxYDbiCP1Qr7M+ueeMRgd1c5ZbjSDiq7LLbSpJrGIFQXL8U/YOjd25QdxvU1DqNUaCu6j1NUjElKYa12oW1FLxq1LBdwk8Anmur8L8zKJ48wp6Qtv2LDtrYFTeAfrXJUivKPStHG2uStSVomjZiFloW9Yo2KysEXpcK0fptRNR3LWD9Kpek+NkO4m3s28AtJb2Hlpo5PoV15PQ63FC9H1PiWleI3AGOYmjoqidom9M421y1v0rq5cVAWYgAck8Uj6n8WWLY8pLYHmEbVmI3EkeowKKjfQuVDee1TWlxmqQfjWLoTajgCSULDGMjcMR9SPftTfpHxVaeQ7ookw24RjswnymCPY5psJLszkn0WSa0xAEnA9TxVB+I/j8SbOkgcg32B2qcYVYO6eJMZ4nmqV1HX3boi69y4d0N4m4qvG1uYUx/Gqx42ybkker9U+KdLaE+KjmY2qwJmO8TVY1/wAfkqVtWWVty5JJgHIJUAHMce9eeOHZmXaAy5hZJz7GIGOf4Uf0/eFuXGe3bUQPMzSWUYVRH/an+FW+xc0ywa3441LEJIQkj5UKM0mBtLFo5H/XtVVvNcN47/m3ksWAk5LNJOQJJOIAp50roja5Q1wqFCvtUZZmYGIDD9n0oRNBZtXF8ZgUUwWLsFBB52r8xicHGO/doJedCzlXSv7jem6nasObd4XPKwUy4gHuY4Jgt8sYP3rWk1KWlfb5kZYRgYyDIBQkgFSWH0Puait9CS4yte3GT5T5Etm2DIGQOc+nHNM+l2lF24piyDMbV8hGRBcQFiZjhiK0owathjKV0g3p3UGtlVtEicFyCu5gsblkR/ZkZ5+9Q9WsHVE+LffehJZSVKKAOV29jAA9/Wam0Fnwwunt32c7QxKhlD2ycKMypgsdwzijtRrrYRLXhIpCbEG4gwMzgTuwc8wftUZwUZf8eynHKUl61TKVf0fhhLikvFxrZUKbbK6k4EyIMHirF0j4o1dmMEW8qofIMZxngSJ45oTXWLSMqbblwsXCvvdttxtp27V3HafNkdwccU1ZhpwQzkbshbYBcGMSZjaPN+FXk+PDcW3/AH6kFDmc1Ulj/foVz496q+sa0btrY6blxuhlO0qRI9zSfS/DV90327FxlzB2xOcwDkn6VbdN1HTI5a4t0wPP8gEmGB2k98cGpl+IEXdctXfLPc7WTsqgE47YEd+aMdLS0M6vb2VLQdAuFlPhjaczI/y/71butdWS04wxi5d8iJuYowJHHy+Z+SRxUev+JtLd0dwNuW+WXaWG1i4cSQwwY+sCKTjV2ktoSpIYwqhgd0QSWVRBjP3Y0HDN+oylj8pbrPx4rqWO1TjahMkk8gkGF/0NLbXxteuDcEtlBywLQpJICNuiCDgkT7e1c6nbXUG0ihZUeI0gbn7gOBiBEhZP+Qm0+jAtMN42xJRSFJX5tkx5Mx2qsfhKL1shL4rmt6H3VeuXRa3MwXzAEBokbjEOuRIE8ev34fqaEbCSbqSVb5pXcPlxL8nkj5eBNUG/1K8ALTAsrFQwJWCEgiWUTxGfYU96dq9tx9i7BL2x+ttiCQFPIMDPpUpR3ovF6HWs+IGuDeoC3JCySJhQQRt4k4kzwvep9T1lVAFxLTE5ktsGY+Xc309ao3VtW95pcAgpK7lDYWT+jYcnJgfwph1DV22W2LtpTAMZGJicA/QfamjBdAlN9nv4u47RVW1/x5p7VxrYBubZzbgjy8zMZn0ke9UXrPxPcvyXdUtsCvhbmA5BBfPMkenFJGu27aBt+1sxs9DgiRngxFcUOF1cjobV6PTtL+UCxcts4tOdsTwOeZJOPpBpVq/ygtO1NOFIbO95kZ7CI7V5jbuQ0SdszE81YtR5rtwqFKKFhtpCktbViC8bd3IAkZH1plxxy2jXrRZR8b6j+xZnbJ+YZ+54qNPja8oIbazEzO3AHoMif95NVK9rkZRulXO7cFiDmRB7A/T1ovpyoxAQoCB+tIBgQTuMfrew/hTPjjXRsn7lh1nxM2oNnba/SK8iWAUmREieDHFVm/oLi3WDAK0ztP447RUmttts3G4YDeZbe0ldp9VJJOJ9I55iuLemdWDFX8wBLcFgc+4BMinUYpaFyk3sb3C4JcsyIqWxG6PPEEqpwcqJyMUF0nr2pugi5eeLQZ7R3EZXEFpg4JH3NHaDR3HXOwopgIdzbZyTnknPPp7CutZ0G88FDbRZJiD378YPFTcopVdDVLsA1PW7t0bm8RmMQzTtnAExCgnt9vrXItAg/nA2soLNnMx8vHGBOO/aiOndOuu4S04uJIO0MQIEyf2gciTTLqXQUVA1wFQ2GyrLGfm3EkcCQI9jVXjFX/6TTk5VX8COz+bsdu64FXIwCDnIMZjMSJj0Nc3ynmYPca3lgrLGJMAEfMYgQaYWupWywcadJDeGvkbwwFAyoTOBBM8A96D6dq9MLjSXhFkkK0A+YAZaTPlIOOKaKbFk0uxr03TJcvksyi0B8qptyq+XcwwT8pjEx9K71Vhbbki07bm858Y7XheQN0jt2jHOKD1OrRFVrF3czEAkGYGD5gfMDkD8J4rq9c1IJ2wx2rnHLMeSIMbJMccetSaaY6kmS6DpttrjObRkARaDCNozLMXmc+n8azXdMW5u26Vba7ZMHI+UyZ8oPuOc0vZHEs+933bSFbb8wktIAzB70VoereFbCXFa2tzDbyzbecBjgYE/hTxcm6f6CyxSsj6To7ltQyXFO1lZWwSCIMKJO5Zj8M8UV1+bqoLxt3TJIQKFQYJYu4EZEkczP1obWLcQnw7YVH3x5M3AJJkx3xBEfSiRoSsupZrm2Gwyq3YQYUYA7TwMc00n5fYIU9INGjdytlAx8quN11CsE8Ru2wDPAJ713oXFu+lprKsCwDGd5VohSGAG09477TXHUP0DC6bik7Sds7wBMSSPcNxHNK9B1Hxm1As+KB4bxCkoWGQzKB5DAIDe5zkU3wm42mv3F+KlKqf1LBrk0jW437YXewWF2jmC6/Lnf78+tef9XuWRcJsu6iRO8BmLegMFsYjjH95+u+KtRqbSJbABKjxWAQBuwDN6kyYMdooi/wBCvXv6NCrEkFgV8PcORicyYkkcevKxWKHk1JiMdT1N1hZththYnaBBZoklhwokTkxJ9aMu3pj858RHWBDblYgHazEnLg7sD2xV56R0NrdpUKgQsl5B3E8kBTJn/pS4dC/O2P5xfdvDuQttSFVCk4YEHdzM1SKSYjk60ypdN6UiXSHko8hBcCm4CxBDswPqrdp7VOVtXXKPtKICS24gNEy5wJMH6YHaKt1z4T3ai1vebKIfKBDFsySy9sj0iKX3vhSzbF654h8Ii4CoVSf0ZYvtgHjYPxP2MpYp5X9K/gWrevxEmm6taW2923aVQVISQsEsYBAAJZ8cscZqr6t4FwSRsBRRyVYySIGfT/1e1PdT0myVUW721WWQu0+Ug7gZmJ4Hzd84yAl05O5SCzSp3EeUwYBuHBEkTkTzmim10CST7OrZuWk/8wTH6QnBgYBgzOO/oac2NTaY20/Ri4LksSBDAjORKljgDvihdRo7yEnUQLZxKgBUJHEntz+FS6LXeHcZbS22t7JAMMr7ACRt3bgYBMgiIHrlVGKdsLcmvSRddv6dbqyvmgRb2kzJPyydoiPXBpT1K2zuBZ3iXPExtnE/QDjtFPNdoyFS7etx5mDOIgKIIkyY+Uj3+9JLHWbRI2hxvnduz5iSAy58uTGBiB70aV6BtLff0HPQunNbsG5dRC2wIuFKoOYIkgv3ERwfpSyxpWYl2AG4DA5wO4JG08fjVm0uiS402x4S7AGG5iobkY5J4ntg+8ja/SbbjK7Lc7gCGCA9gcHPOaXhllG5Kn7f2w8qadRr72ITbIAZj8yyJB8w4xETXN11Q5IJP6oz+LfL27TTLW3Fa0iDT8k+Zrj7oDHABAJmDiI+tC68qgs2bWfKbjFACdz7TtYscKq455mhSW0UbfTFqoILTxmPb2Pr7U3tBlUrLIsbna4wCq3y7uPciM9xQmlvFyVDWwOYwqAZOYwD9aP/APCbFy4lx7ylD5ilpGYREYY/0mTPHc80kVasLYus6m0ZXaWwJYMsGTmZ+Xtn3ph1PqumIRLdmYXzszyS5HqOYOfT2FSaPp1oswNw+HvJ8okv2G0TnmPaR61L17ottBNl2ZgVU2jkyZAMj6HAzP1wy6tGrwzYClVRbi7biHiHEATO0wUbHP4UZpuoEKyI0qkqN4KzIg7mPlgQAAYIn7Uts6e1aAW75ri3CHIUhUkFSrT3H1zBpvptdp38S2+oUQPK7KpDng+GyrmN38KDjkzJ0jR+K3toq7EUxLEHcrcxBWAO/rTPpHWlvWw127cDs+0BUULBjILA4iDOBn6Ul0F7RbnlXulYIKg2wzEny7ZJJn689oom1pNKWulXZXYhzZY4BAHlLH6HIqsVxyjWO/cRuad2c6bqJt3PEsEIAzqpPmDqgAjarCD+NLeqanxka/ee5OAonbuef1fQZ5jkD3pdd6tYunwzae2s/IseUiJl+YxnE0V0ZdP+l2q25IZGbkggAn6DicfhS4tu2ZSilS0Pei6t1tDwbio8E+eQxkic7flwBn0ofU9eW6EXU2BCsYuWhtbcp+YLwfdZz9qU2dY2yXVlw0NABJz8s85/2Jppp7tlSXtoXwRscAkvwGJXCggk7RB4GKE16uvx8DRejLPTiGUaW3KQS7Mdu2RgneeZiQJGKc9FD27u1DauuVJZSQQigYzyD2nbGaq+ttPc04uFd5S4d1mJ8m0ks4mRG0c4haTWes3EdjaAU3BHhopAPBnaOTgGjlOSxfQuEIyyS2ehfEKeRWRHuO0k+CSGHlK7pg8TkxErxSLU6e549pA5KeVv7ZSJBZgQZMkjgjjilen1bMGW4jhSgV4WSmRBUSNhke8x711pdTqA0WheR3gHKSygwZEECQB3jOKMXhK6RpJyVWy86i0tx187ExPLbfrx9areoF86vwdpZFCwwXkAD5TgM5LHHGYjFH9NAVXm4zOBmX8oJAfaJ+YtjIjJGKi6a2ovXSRKW7W0jt+qu7cZkTJPrEd6pFp9IEk6I+qX3hrFtFVgQS7hkzmFUESY/DJpFrdFqNK6tZvBiQQGtSCTgsIBk5x7xR3UzbY3Wu3bjtJRLas0AzA2liTyCCZ7R2oHR3Li3GV0Vm9yW24APmM7cEGPrmkjJRlT6HpYv38Fr+EOnqBbD22LsrPcO6GUggbIBheRz7d6tZXaF8JAg3QVbEAzJn15MwZ/vqldH67F3wmO4LIEvKYMHcojdEYJnEcUw1FxL1wb71xhu4SCoB9oEAcQM1Rr2I34LW+zcAApgqYEzC9/sO1LtBp7wuPcuBCGLHeBtO0QUWBzHmE+3vRV7VBWC5lVnygksvqo5Pb8aKvqVSUUk7e0eUn9cj7zU5aCiPQpuZmOPLEehPf+NUn49Z7t/TaZCqKZgmQR4j+GpBHIjke9Xrp6n82UiZYKczwQI5/3mgfiPU2UZHubJtnahYSRdZZG318pk+0+lNqasC0eZ/EHw6dNdNpQ5HylnjawCq0qYjvxPNSWtLeY7UtEggQR8ueAxMA/KOMY71a9R1YMVsapDqNy7iyqphCYDBRyAQZOCI4xVaa64usLVhvBLEhSJMSR5ZGMCY94E1NtLZRK9EHV9WWS0HICA74Q7t8KVgt65Yg+9EfDz2YZLYC7kbLvI3TgY8wBAjvAY0ptaTUMHXwogE7Su2FBAZlUx5QCo9RXeg0xSWQpGIzDSBJheSPeg22m0akqTCuspcF1bbopZsFUbcoJwACSNueeKX6fSodqbIdTAC/PgSfqMx9Zq4N0r84th7oYXZUK0/qjM595E+opFrCi3tjDfcIG4wSVYCBB/XUj1AMCjKcpNNghxxgqRFc6kR4lsgCDkAd+NpJiIinmkARAWZ13MY2oG4Amdpx/3qr2NNubLKI9O8ExMRAOAfoeKc27i5L3XmcFTGOwkcxP2k1JqMvS/wBR2+iK9eQ7bt3xLoC7hb2NAPDbgTBjH1+1O+haTba33hbQESEQAQJlQe0iRkd6UaG3djat5WCky0FfKVIgE5JJAmMRNQdS1GosqtxiGtfKFtniTC7gQWzjt+FVSSBQT19LV4wwgQSrQAJESGIy/rmkB1t0ou5d1tWKxEqTmREe89q4udQdnXxLbAdyfmZCJAAHY8fhTmdPfRhbXw3ZYK7VBZYjO3MZoOXhj4K7QJotSEHlL7ykv4ihljdgEwfL98H61z07qDWblu8qyWdtswQSAVDFcBFn9bPGB+rS3pureytxSChaFzJ4nEEzBkciMURfsHIDwm1Wf0gAw0j5skYoNLt+DJusUEajX3Ltwi6SUPmO0KFlWP6qgbjuxkd6WvqLmzY5m2rsyYAMznPMcmK66SUAZmYIggBvUCcKPfcK51z7RgAzgA5I9M8Tj5RxQtgCtHqRYUajapuMDAb6iGjtiT9xj0b9E6kt7xGfT7CV+dD5XO4RIPoYzSbTaO88FV3XNoVNx4HdpOeD34x61YbNxxuIAgEGY9OyqYmDP4inU8WhHG7APijpoV96ja13LAd3EAwCcTg/Wai0Om8DxN42lrLRkdpkQRE544zTPpvUBdvquWLhivl+UiJz+rw0niaeazpdow164ERPMQIliO26cD6CncvX9AKCq32VW7rrQtW7G0JtYkn6geZsyxJA/CMUTpFdgLbKEs7Bugjc0wysrSfMfKZ5gCm2itJdvg3Ftm2jFU8ucCYgdsgZ+3eav8R6y9buv4clLhIG4QBgDapHJXHbE0Vp2+gNN/edbrFlXaxkmFYktIG7mB7TInsKl6dqbLuWMBoElNxLEDucCSJx/GtNaI062i4ChVBAAyRk7iR3/wA6ZWtNZ0yrmEQq7AggjzDjbySRHvn3qaeTZRpxSJdDbtXkNsXbmIDyAu7cp2sZMd2xGMc811b19qxaAUM9wRuO0QQJ2gt2HbilfUnOqRntB1HiBS3kUZHlVSTM8EgDAHNXP4Q0dtVyCLhBDKGJHCgmRyJMj0inx3Vi3q6Kml4hVRhDAkkkZ+TaGM4BA7DiKsWmvi3o9qkkuNqkc+xJI+9Z8QWnsuvgW2ukjJLSV7FmJBPpnNQdOstfDgBra2xO4rgSIAG4jIUT9DTv0+mJOLy3ISX7jb006sA20hS2VTB8zerEkmDyTS/U6C2qi0HnZuG+IJk9/UCTn/StaLT22HJ3Bzca48MTwvlHde8HuTHanXSOlG44LbCDuKMx2JKEfKok5n+5qVce7Y0pewt1OhuWmW2qJLpAUd9sTuAmW4JJPbtij+m9LvW4FyxcAJ8xUAAKDIIAYmTHoTx64jvpfZrqOSkXA82z8xJghS3ErmV/siRxVu0+ra3tXY123sS1tCsSriNzFvYeWCMkUJ8mqBDjrsX9H+LNMh8IC+5BCqzbWYgxJ85UAjjOSAOTir1fcBAU2lZDMYHyASYAHmOFH39q86t2tDe1Vx2010bSPmcSSABtKKTKnuW9Yq8aPV2b9jyrI3m0ymQQe4JGYAM/So/Er8B5QYbrdUqoLhMW0U3HnnA8q/Wf71HrXjqm9qLl3Uh1th2aX3BSAZwC0zHHbgRHFel67WW9rIxUNbVbrIqSQggFZBw0lfoMHmlfVeq6bbvcvsvICqkRChZJCRCkzyTMAik+NaSaDGFPRSU+FJG784nJJZMxE/rSMgj0qPqt027e6xr3LEjahDE+h8xPH27UPqPiW2APA0zbWLZuO0EuxObaGO/Y01+Feq3HvLbeCnZbMIAImTvO6McT61WMctGtLpiGz1TZbcvLX2dSLk+YAA/Ixky0kccGgtPqQcb4IOJUKRJ9RzV4+IekLuY+cW2MFUMC25BM5+YGJ5x6Zqs6LpQ3sTdUjdtHiBwx5KkAjn64HrxSfEaMo9j3o/xIqXba3TcbyskkjYCTjAzIj7zNMeqae07C8G23nI2GA4KggAMpIKQQeB6+uE/RejeLeK3bapah1Z0yGbEHIH0njJqzp0SzaUmzd8ZtysofbuBWZhhk4/VPJHvST5K87Kwh9NCvovwQ4veKzhbYYMsSx9RE4GPWmXXemtbu77NxVVxJDrPmBJJB9PNxTrSdRfT3c/prF1A+9ATtYY3bQCRIgH9ke9GanUpdAdNrDImAcjkfWqcfHKbyuiXI0lR5Ne1dww0gMo3Pv8pcIM7QABgduTHpNBnUFii2VVXdxufliVIxtkx9on6TR3T/AAnur47Eg7YOPIRlT7TmT71dLngadS3ktjucSY/vNPBOTsz0qKprLF/et65aM7VwR5ZVpWRiAMYn/QnofWdr3N6AkwV8JMRnygDPbvUGq63c1N3wbDC2oDNvY84AACg5+/rUPUOsbFtLcUfnAmIiFI8u4+h/3xRVXdmatUznrV/xrjlLBJQEMrhxtkcttwJzyRNK7YZkIW2TAAaEkCATA52g+g7Vq/1Euzi67gsTIB/R4iAUPIx60To/i1ktC2W2kHIC/MBjLCJmK3JFr5hYSi+jep0Ytqge7aLmItSJSeNx7c8e/wBqZ63T6fTolhgGufM7fMd3fYZgKPSYOfWk2o1Vq+ReulEUN5ghBvsuABBjGOY4PtTa8bZfdp03WXtkAkT8g3OxaZ/WzPpFRm2vlRQJsa+yEC2XCpBABJ8Q5E8/Q/7igNfqS1xLdotlwSnBIkEiYxUfVOkx4b2GBxzKlQCfrJ9foag0+lPjK9q6qHK7nE7Sohu4g47+tUVzpmcsEO72pXSwwGwuASGRfE7cEHOYx60Ppr76lD5yF82/aRudUMkZyoJK8ZzUOrRnHjXDudCUBz8xDKhWYhRuVvtTPpHR2s2WuxK7FGwGOSTJJ7me3ZaSldBt0Q6fW7SL4z4qpAx5QJYzEE8gTzEe1at9P1F24kjdpgXcqoCnc4OQziVAJ5MY9cGptJcs3rtq2FiXAYgMRtkCOyquJz3B+/fVbzqRZDt4Nt9hIwWWSE8y8zn8Kuksdk3ll9BfZ0Cm4qsxbaZKAgrJPkVdvM880ffS8LsGA9wwAMTA82DlgAI9IAiZoaz1hbdxUt2yWeTx5nBHl2qOABmecH1invwz07xLt+7vuXAsAM/KiTNuQASZxAzj3qdJqkUbrsW2ekpfttYJzbbcu2BaVj+sQozk8kAdp7080PVEtKBkiVlhxkETuMKoEAwCR5hHIFT6rrCaElEtpvYeaZjAnaM55P41WNd1prybDp7aodx+WAdwhoZyIkenPvWcqfpEptbBPiTqe+6r23OxpBIb39ZxOOP4046SbhuNo3Z/AAd9zCDcW6BABIOBJzP35pQr6e3Y81i3MKyqcsTkzuzBmB/0qG9qLluWvW2Vc/JcLBZGIndtExM+/FUlJQa3ZFKU00lX1ofX+k6YOUnyqRjHygfJK5aTJz6mob/X1LC2yps3FVx5gIHCgEj7e1Z0Xqtu8ipcuWwxdCCPmCiRJWO0jnn7CnFnpFiwN7lVY4kAST6AcsfpQ5Oao6VDcPC79TsrPVrrWzbFot5yY3AS5HKjGG4yTMD2pr8O/EyTct8Kim4Zb+jVSA25mMrEwAZ9B6Uu+OLlzw7exR4YuAtKywwQG9FGc/Wq6nwzeJu7bkKwBuHBEE7x5QZYSAfsKWEn2WlC7SPQeqWrGptjVWCHf5NyNEkjCsVzHAP2PamH5PbJXTsbkBbt0soVSBhVBO4kzkRP/wBJ9apHw5rdNoi1sNduq5IcOsKGErICiT35OJ9qvfRtXYt4tG2EYEhdzMFcEzBHzLGQMRn7M2nsm4taBOm22takWHnzbg5bzK9s43ByJGWXknI7CaVde6O7ixbVXe5ZFxLZgBeeGDHsFHr3+lXDV27Ii+53NPlDDAnsIyAfQzxUXWdVYFm3eusbRbKmCMNmXU8TA5gkwPWlcHJoLlWzzbquia5Ju+R1UeXbJgcYAEGDwBzSqx8Qtasn9AQwuAgkE7syJnIIgY+lW34i0wcBheDalAHCeGxRhubaCQeSDwcTiqlpD4uoRmvAsLgZkKeUlTIEqciQBBjtTS1onBxbtDjp3X01W+y5aw7LtG4mfEY+WJyAIyCe9DfDXUgpuLdsI5TcC+ANwMS08iR25ml/XtEj3rjK5a4zloWNoJM4PJGcVZ/hr4Mc22e64XcPKuTEkebn5uw+tcijDjm5N6fg6fVJUjjT665bkoCyjkdxOd0Rxn/Yo3/xTeC9sw23MjkAcgc+pxQui6A6XGCOxaTG4eU+57D7VZF+HnvIQzeCQsGFgGeYIM9vTvTv4coenvyFPkUvU9eDzPqD3RfDi55wRgSYJKxHtndRVnr72iQLj5PMsJI5mDn70Rr/AIbu6cFyyEOchZlVVl8xMY+aMdiaH1/R9PfbfY1CWsAMpysgcqZ/HmqQm41ROUVKwNbhO4sxMja0SDBGc9+3NQ63T7ypYu68RuJKjAGO494qGzfYsxcgDccR2kwaZW9M5AcIxBYBW2NBYnifWgtB7I9I66ZSyQ24zwd3A8rH++PekXiO1wKphSQoJxGYknnk/wB30qya7pjpYdcFy0wskjAkekxIx/aUHiKUaRTta5dJOxIHaJY4JmPX8aeqQLtnGo0U3fCtM1xwYaFJluSR7Ad/aiuk29qnciMAwJJI4OOTg5gfeuehdKuaiT5BbBl7jTJgZCAZc4AiRyKfaHohtsbhIAAMLtAE5ye096HJNNbf4A44U9IR9f0C/nLpaAFt3ZbbQR+ttO3MELzP3q3vdRD4Fu0rKF2gsYxAUCQCTld3f5h6GkOt6qFuMb9m3cIMgsp3Ajgqw4BwY4OKYdD0ovhbrXHTc+GYyWIYzGQUUZEyTJrJuuhq2Vv9PqLhUsLSqQZafDDgQoAHJIH4TVmPRrtpS7AGOCBGWPJt5YZ4J7T7Ud1Y7H3WQFYEYEQQRAafb17Sfei+lK1kr42psEFvEIUuzueZyR5oAHHsO1SeTd3r2Q6peCvdNS47raVfE3OsgCMbgCJ7LkiJJ9BVuboN9wN6hWJEy4hQrd0GGHaJmuuuXrF1FuW74t3QR508rQQZQ4wdu4CeKE+ItYBbW1a/Nryqqki+XY7pBkyBu7GZz/CsGmrYssr0ibqemTTWQltUN1hFxiQW42zMegHApBrVWzaa8rKbo3bbZA8RXMAFgRGQSZjtR9zpXiYu662I8+xLPkUwDC7jIGMULc6YguoTq0uW4IK7W3gHG1QTge4MiOK3HKcbyrYJJSoX9A014qbqWioYnxLqkbgAJK2z5dgLgAx2MU2ZLl8gLcdTtDBYgbdoyw3CYOC0mYme1ddL11tLm0hFsA4NtG3QMR5xJkLHzRk/SrYfi3QhN1tgWIiApknsCQOcipye6ijU/wDYon5syMgusN1xiqBg/KwSdoknke1WBfhsm2G8Rkczu2/KFE/rcQcAZ712vxIgKXGCC38oCiGAmCB6H2rrq/xOPDK2/NcBAAnAgzPmIk4GOc0zg/DQL2T6fp1nTsGYTt3AsWWQceUFh9QPvxSTXaF9SysNPss3dsEN+pIBLJHl8vPOCM0Fd6rev7SyeVQYBXy752nGS/P8fUVJ0nqFpWLam+WuFmDIVZEVh5Yc7ivm2p24I+lSfFism9jqW6RB074RBvbUZ0J3FAZKhQx2k3EPEAH1pxa6NqdM6G/ft3RtuFuZXbtEJicTmTmfau7XUP0ioSdMWyBIgRJdixJAAAyZzEfTrqz+YXBbcpbRpcFTuDbJZnjPyYjmTV3FOrQI6fdCPWDx2dBqiivtCqyx6ggkjE8c9q3a6LeRGBKDYsKHJ/SkDAmPKnB2jmAJ5rnWX11Mul8qybiLbuAQAMMjAeVpzt4/Cm3R/hi9dtWLqXFJV2eXJl1OdpaMjOCeI9qektICdq2BJ0K2zW7V9V8UruJB2ySTEbcEYiOeeah6mX095LYXag2wMnc244Y/KvHBonqnRtTpg95rTElPJsJuBAkl9xUYwTH7RpfY+IEu2LguIQ5UqoUSWcjlsSAYGYMR9qWPu1oyasK1HxObTq7qz2b24MDl7bbvNAzvWcgcj14res1aXAy2y1+2Cu9oJcKwwY5kfbjHpQuj6KsMpPjTtDIp4YQYX1GeD6TNGWLraVo0rG0748PaWO1FJZ8HzHn/AFqfNa+X+BoP3Feq0b24c3neHDrBO24igBSxBncMYqTTdEs3TuuOqETkBtoPKtAhrfuc1YtUdVqrQa6bQI8wKofEYQNrYBAyePY8TVeHTblpTcKuVZBufa0KWciJjPGfrSxcmrff99hcYp68gVzSPbukJaUhMSPMpH9tWmSuTkgV6H0bXolpEciSvHO2c/h71U/h27aa+7Xbty3+qrEiCVIAnccESvp2p7e09qzfktu8oLBQIMz+pnbkSQMQaTkjZTjqKLHb0XijyGJ7yfX+6g+t6LUgsBd8NdoQRliR34pj8PakXDKnbImOMDAMH/SiPiHqJtKquUXdMMwwDBgnOBiPvSRgoqvIzk2eWdC6Rq719GbxLqW7k+Zhtba3BUzH39KaarRWrLuu1QxYs4V2Ubjk89swMDg0zbqdsWFSzft3HWFZlc23IngmGBkk84zyKrfUulvYfezyLuQW858vMsrAE5/336ZRvp/p/wBnMsr67Kla/wDM+i/4jXtnSv6lb/dD/DWVlPEY8y6Z8ifuv/2Gld35Lv1t/wAVrKykn8w6+X++yLpp/wCr2f8A8v4tQg/W+/8A7KysqT7KeEKH5f6f9KGX+huftGsrKzAie7/RW/3a/wAWqbVfI37a/wCBKysrewPcH6P/AEqfv7Nb1P8AXLn/ANy/801uspl2bwWPqH9eu/uj/LWq7a+c/VaysoPsy6Ih/wC1v8RovRfO37dv/Ea3WU8ewS6Auo/L97n8Eri58w+ordZWj3+Ikv2La/8ATD963+BqcdD/AKtqf3lj/HarKyujx+f7E/8Ab8v3COjf1q9+6H+dKvi7m7+7P8DWVlL/AJX2f4A/x/mf3s8m1n9An7Tf5V6d8B/1NPq/81q3WUwx6Wnz/wC/akWn+e/+2n+G3WVlJMMejz3pvzfdKP1/9Cf2D/MNZWUnL5BxfP8Akas8aj9kf4RXpfQf6qn7I/jWqylh2xX9q/uX7nk3xr/Sa398v+A0t+EPnf6H+C1usoyLR7PXtb89r90v8Vqtflq/qlv9sf5VqsqM/tEMvlPKbnA/YX/FV46l8lj9ytZWV1cPZDl6Z//Z</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxMSEhUQEhIWFhUXGBkXGRcWFR0YFhgWGBUYGBcVFhgYHCggGCAmHhcYITEhJSktLi4uFx81OTMsNygtLisBCgoKDg0OGxAQGy0mICUvLS0tLy0tLS41LS8tLS0tLTU1LS0tLy0tLS0tLS0tLS0tLS0tLS0tLS8tLS8tLS0tLf/AABEIALcBEwMBIgACEQEDEQH/xAAcAAEAAQUBAQAAAAAAAAAAAAAABgIDBAUHAQj/xABEEAACAQIEBAQDAwkGBQUBAAABAhEAAwQSITEFBkFREyJhcQcygSNCkRQWUlNicqHR8DOSscHS4RWCk6KyJDRjwvEX/8QAGQEBAAMBAQAAAAAAAAAAAAAAAAIDBAEF/8QAJxEAAgIBBAEEAQUAAAAAAAAAAAECEQMEEiExQRQiUWETMnGBkfD/2gAMAwEAAhEDEQA/AO0UpSqioUpSgFKUoBSlKAUpSgFKUoBSlY+Pxi2bbXXMKo+pPQD1J0o3Qbrku3ryoMzsFHdiAPxNaxuZcKNPGH0Vj/ECoDxXiT4hy7n91fuqOw/n1rDrFLVO/ajFLVu/ajpP5zYX9cP7rf6afnNhf1w/ut/prm1Kj6qfwiHq5/COk/nNhf1w/ut/prIwvGsPcMJeQnsTlJ9g0TXLqV31UvhHVq5fCOwUqD8pcfZWFi60o2iMTqrdFnsdvQxU4rXjyKatGzHkU1aFKUqZMUpSgFKUoBSlKAUpSgFKUoBSlKAUrxq81oCqlU601oCqlUiaa0BVXk17VkiNf6igL1Kpt7CvWoD2lU601oD0mudcz8a/KLmVf7JD5f2jsXP+Xp71POIYTxrbWizKGEEqYP8AEbelQbinKt+1LJ9qv7I8wHqvX6TWbU72qXRm1O9qkuDRUpQ1gPPL2DwzXXW2glmMDt6k+g3qXcZ5XVcOPCE3LYkmNbg3afXqB9KyeV+C/k6Z2H2rgT+wN8nv3/2qR1uxadbfd5N+LTrb7u2cfpUg5w4P4NzxUH2dw/RX3I9jqR9fSo9WOcXF0zFODi6Z7U+5b5gV7JF5wr2wJZiBmXo2vXofX3qAUqWPI4O0Sx5HjdonWM5tUsLeGtm47EKC3lWToIG5/hUksghQGMtGpiAT1IHSobyPwwknEsNBKp77M302+pqaL61uwuUlukb8LlJbpAmk15cGlULvH9RVxcXaUqnWgKqVTrTWgKqVTrQzQFVKClAKUpQCKRSlAIpFKUAikUpQCKRSlAIpFKUAikUpQCKRSlAa7ifBLN/V0836a6N9T1+s1q+Ecpize8R3DquqCIObuw206euukVJaVB44t3RB4oN20IrX8U4vbsDz5if0VUk/jsPqazrtwKCzEBQCSSYAA3JJ2FRLG/EbCW3CLnuCYLoBkA6kSZb6DXpXZPjstjjnPiBquNczvfU2wqpbO4+ZjBkSTt9B9a0ddQ4fi8Pi7YvW8lxDIkrsRuCGEg+hpc4Hhm3sW/osf4RWaenlJ25WYsmlm3y+Tl9XsFhGu3FtJ8zGB6dyfQCT9Kn9zlPCnZGX2dv8yau8J5etYdzcQuSRHnIMCdYgDfT8KrWllfPRWtLK+ejYYTDLaRbafKogfzPqd/rV6KUrebxFIpSgEUilKARSKUoBFIpSgEUilKARSlKAUpSgFKUoBSlKAUpSgFKUoBShqDcd+JFixaJCsLpICI2VmOuphW6a9+lDqTfROCY1NaDiXMwU5LFs3T1aYtj6k+f6aetcv458ScRe+zFsiAJW2vUjds0yfQ7aVf4HxvFNcNtbQLQCPEuC2ADrn/syWHtGxquWSjTjwJ9tfsTq3xjGvMC0nYG2Sfr9rVi9xPiaDPOHf9nwmBP1D6f1pUO4vzjibLQr4csN4e46juJQrPtWJc+IWJ+7kA7wWP8A3MRUW5F6wx+EZPxD4xxG4iC4vh2JJuLbaUbYAM4jyiPkbSTMnSMbggtX7Qe2REajtWpfmbE45jhzeAttoxyov/KGA3Paav4jgxtlEwpFtwQrAsQjKT1GsEHtvMRtVOaSXDfJbj0+7mPRtuWeOHBYsOWIsuQtxYmR0YDeVJnTWJHWt5w7nvFHFveuWz+RsnlsgL4yOqiIbQNmYGZMCRtGsSfA4uyUvslkycmRnmZGadII23B0+tXeHcfF51tHDtbdmyyHDWw0wNTBg+386rlmzbU8STRrlptLKdZW0+jfv8ZT4z21wDECMivcyXiI1JXKynXYAk+/SWctc+4fF3PAINq8flVmDI+gJFtxuYIOUgN6aGuYccw6lcxAzLsY1HpWrwl9XBvNmtsFnxEABm0wksQZM6GTtprua0afUfmjaRk1Ogjhlt+emfR9Ki3LXOVi+bWGe6DiGQNopyv9mHMMBlDRMqDoVapTWg8uUXF0xSlKERSlKAUpSgFKUoBSlKAUpSgFKUoBSlKAUpSgFKUoBSlQnnfi2Jt3BZR/DtkDzKPO0g/e6ag7QdK6lZKMdzoyubuKsfFwaYhLGe2qi6Ea66PczhgyggW/Lkgkk+fbTXlNnlLE8PzXWs+KWOS3dUNdthI1uMY8m8BWAMz0k1kYrHYvCMVwjKBiLypDKCDdIjdiNSIBPtVWL5l4tg7osrftOx+74ZyiBqTB0FU793TNkcTiuDCwqBbRuWysTDXC2hY6lRoSzE9B3NYeC4Xi8a5NpWunVZEi2onXM50Ue56bGpD/AP0jFoym9g8Pd3PyZWEbtqpjbeak3A/ihZxStZuWblh8pZQgVwwGpC6Qp/eEa1GEaTdnNqh45IJzFya+Gtm6uItX8hHiqgKm2CYDQ3zLMAnTfbtrcLytexChjeS0hEgjzkk9AFgR6z+NT67euXA+nlYEFYBGU6EExrvrWs4jet2UzXrhBIkIozOR3gfKPU1CWVyfsLIt7W5dEM/4Y+BU23IIdj51kq06BdflMDr/ABrPw3NNyyoGjwRoRLRIBVWJ7D6e1ON8Hx2KS3dXC3EsuodNS5cFiAxyjQwJy9iDrVfBOScZbK3cTgbjYcnUj51gjzNbkOV76bT7HssSkm5K35RKGZqknS8MyOeeMul+0tu59mbOYKV0DOxBb1MAe31Na/hHFFtJbh0NxCLhJUHys/mhp0KaDXc6bDWVce4Jaxy28RauBjbBACEMjgkHKTPl2/reveA8qWbb/lT2UldSCfUH5Jy7gGSOk1TpsmJYVBuq4o06iM/yWl92WMdgWxdxLdmUS4ouEupBto3Rl79AOvtJqQ8J+G+BSGK3Gca5zedWnvCEL/CsfhPElvPiLtjKYbLps2Rcxgjcy59JrLwnMhZWC6aTm6DWD1rTp8cMULXky6nNkzzr4MnDchWbRLWb9622nhmVPhsohCvl6fxEjrWv5R+IV5MV+Q8ROYvc8NLuRVZLubL4dwLAKk/K4HUT6ecF53e6txHtEunyuNFboufsfUb9hUD+JFx2vJczqly4FZgAwCuoElXjuAepkn3M042tpCWObT3r9mfSNK0/J/EnxOCw+Iu5fEuW1Z8hlc0akRt7dDp0rcVMwilKUOClKUApSlAKUpQClKUApXjV5rQFVKpk0k0OlVKp1pJocKq8mvasnTU0Ol6uX/EnjzXMSMBZIHgqLlwkAhncAok7gBdTH6Q7V05W0k1y/i3A1xePu3xdKo5SMohj4aBInXQ6nodvaozbS4LsEU5ckLx/Fkui34zMl+0yXEEDwzkdQbaKD80y8mZiNdKvYa4Lz377v5iY+YeW0g1YHfV2X/p9dalWP5RwYAutZLmYN03GhT3CltR0mNTtWvxODt2sym0wgtoYhsz5iRBiC2widKxza8G2WeONdEP4rd1usfKATLT5YLmAmgnY6dY/HGwGDtAK7m7495vsrdnS4WbQBYMr80T6x3ra4fh1++z2bNnxbjTlJggEyYWfkAnVjtNdn5O5Ss4CyqqitegeJeyjO7SSdTrAJgDoAK1Y/wBNmbNkumaD4d8lPateLjwzXiysga/cYooUGHGYLMnVdRoN6m93hthspaxbbLoua2pyjssjT6VlCaNVlGZybANezVjbvV+hw1WN5dwt0OGw9sFwQXRFS55tyLigMD1kGuQ80/CTHBibGJbEWS5Phs7C4qlvKId8rwDqZG21dxM01pSJRnJHz1y7fucIxT4XFp4Stlcaq2QsPKzFCRBAgmdCvuR0dOAYW+DcBYC5r9m4Cz+ksAj17a1tPidg2u8OvIAYm2WK/MES4rE9dNNfSa+frHETY8lm7dSdfs7rLP7XlIFcbXTLccpSl7ezsd3gX5PYdLDliDm+0AUdN3JC9N/pXJ8ebuLe3bysVUmWAmHdiWkjQgTvsa3+A4bdv27fjPcuuxznxLjOqqYyABjEx5tdpFSJrtjCWSJVW7tsddgRuT0ipxxx7NUpzh7G7NHyBxzE8PxlvBsSLN28tt7bEMMzkILlvQEaldum47d9ri3J3MmGtXxcxNkNcaYxO5spJgZCPKI3ZSTqZ0rsdtto/odKjafRlzu5dF6lKp1oZyqlU60k0OlVKp1oZoCqlBShwUpSgFKUoBSlKAUpSgFeRXtKAw+LgeE0iRsR3BMEVBMXzRhcGCww1/N2UKR+LPtVXxD+INrDg4aypuXFdA7DS2kOCynq7RIgaA9ZEVXwvA2ccCxYNbicwg79Ndjv7RXPazTGM4JWuzC5Y4xa4hYKtcAIlms/fQs7gKTpOizm/aFYHF+a7GthrfiMIGa2Zj3Jj171JOOYvhnD8OyJaViATksqHuMepdht7sf5Vy48bwxU3zh7+Yy2gRUEfdBzTA0G1Z3jina/ov2vJ+o6Z8KsAsXsVszN4YXSVQBWk/vHX6VP6i/IHCrlmwbt4Bbl4IxRTIRQpyqT1PmMxUoq+KpGKdbqRS7gCSQBtJManYa1qOYLd27h2bC3HDjVcpIzgbge42Yb6awau8Q4Ot+/bu3Ya3aWUtn5fFJ/tGGxyqBE7Sa13Eua8MD4S3mVmOUOqyoY6KddxMdCD/ERm1TTIGo5BxGJe5ca5cYoqwUclmZzqILbQFPvPpWs/PLG+N0+bKLOQRJMZZ+aZ033qXcMxF5EutiMpI+0UoFllQDOfLEkggCdTP4aezwS5ZxF7iGIyAIXuIrOAHdpYCekAkD1A00qmKksaqzji/BGhicZexLLbu3Wuh2Hlc5RBgxsoUe0aV1fBJcCKLrK1yBmKiFJ6wD/AF6CobiubMNdd8Moe2jfNeslVaSAx0y67kHrvFSDgHCWw/y4l7tphIW5qQdCGVh0I6R2ruBJN07CNzXz78QsHbXi1y2lvVrlu486yCitEdF6RX0FXzxzjYzcVxjpcZl8WMx3kIua2s9FbMs9hWhuKVyNWm3b/b2TTBcQs4e0ZcG42pBEfQHSD2magPHuYS7vZQZbbgPLRmykTlAUaTAB16R3q2vClu3UWCTMwznLI+8delbm/wAo4TXPmDtqWV4g+g2/EGq/URlwrNmTC4ctqyP4e6ga2X8wlQRMSoaWE9NJr6S4ZjkxFq3iLRlLih1nQwwmD2NfOvEOXEtWbjJfzMqNAuba9FKkebtoda6d8G+aXxVg4Vrf/tktqLgACEEQtvKBowyn3A19ZQquDHmUu2dGpSlTMwpSlAKUJ61jYTH27pYW3DZTBgzE7e/uOxpaFoyaUpQClKUArA4rjLtpc1uwbo65Xgj/AJYJP0ms+lcatHGrRCL3Ot3XLaRfclo99qw7vNuKOzKv7qD/AO01nc93bWdUVF8X5mYbhY0UxuTvrtA71FK8/JOalW487LknGVbjY3ePYlt77/Qhf/ECp1yzxHx7CsTLr5G7yOv1EH6muaVvuTeIeFfyE+W7Cn977h/iR/zV3Dlany+zuDK1Pl9nQqUpXoHonzz8VuX79nG3MpPhXs15SNhJJcNHUNOp6EVrxxsZLf5PYthmHme4guOSAM3hofKBMiTJPYV174ocqPjbSXEvLaFrMbhfNlNqCW+UEyI2jqe1cp5YsWGbxDcXMDCoSAfQQdQPWqnA9GGWMopvvySPhdy8li5dxJGQjKWuGAFOkADyqJ6KBuaiV2/5fDC3SjEFDlIU5v0dAxmPYxp1pj+OXMTfFsGbc5UtrbVhvLELd8uY9ztO+9bTjOEtiMioYyR5MrqSfOqKoyneSNwCd6gsdMvlkqNHRfhPzFauWRgZi7aUvBuZiys5JyggFQpIGXXKCNan9cF5U4tbwvELOdERRKOVeSrXGADKwEkSIKliILdRXeqvXR5maKUvb0YXGLFt7Ti85S3BzMHKAD1Ox9jNc6scsWsQ5GGxiXADqrqUcAdYI1HqABU+47wZcUEt3HYW1JZlUwXOmUE9hqfwrExnLtpMNdtYayA7oVBnzGehdjMd9aqyYlN8opasjhtJYsNF04lbauXy3FZbSlcqqqAliAYOvlAB61m8xcEuYq2lwAi6hIa1IACwP7ITECNOpk+wjlzlnG2Fdzb8uRw5DqfsypDyJ7TU4t4TE4nCG3eYWLjQVa1vliQHHSeoB/DaoxipR2NP/fYu1VHPsPy1jGeBh7nuwy/izRNdO5dwl2zYS1eKkqIBVidJkAyBtMfStTynwTE4W4y3LoeyU0AJIzyNgR5dJ23qU13FgWN2mcijxhIIBj17eutfO+PxdxnuXHPi3CxkiCS2fLn8ukR0HQaV3PmrihwuEvYgFQyL5cx8udiFSZInzEaTrtXzli8UrLmunUMc0ZgwLNLyVXQdd9iN6snHdwa9PNwtoz8Zx7wlRUtgAuzFh/aMonKryTIGYnpqB6zh43mQXIUFgY7SQT6d6tX74uAiMsGIDffXynLIHQfUH0r23cCpFv7gGv3g2zAa6DXuf8qi9q4LnO1yy02IZxBctGhJWAR0O9dS+CeGvWfGBE2rxFwAD5CBAYn9oaRrsPWuaYa2Lr2lZwiu+TxGBCrLDM5BjQEz02r6G5Q4AcFZ8E3M+oPoIEaE6nSB9BUo3ZDNJKCRvKUpUzGK0PFearNqVT7V+ynyg+rfymt6ygggiQdCDsQdwa5nzBws4e6UHyHzIf2e3uNvw71RnnKCuJRnnKEbiU8U41exHztC/oLov1H3vrNecD4kcPdFwfLs47qd/qNx7eta+lYN7vdfJ5++V7r5OvWrgYBlMggEEbEHUGqqiPI3FSZwzdAWQ+n3l/jI+tS6vTxzU42epjmpxsUpSpkxWHxbHrYtNdbWNAO7HYf10msyozz8p8FCNhc1+qtFQyScYtohkk4wbRCb95nZncyzEknuTVulK8o8k9RSSABJJgAbknQAVteJcvX7Azlcy75k1yn16iO+3rW35I4TJ/KXGgkWx67M/wBNh9e1TOtWLT7o2zXi0+6NswOBcQ8ewl3rEN++ND+O/sRWfVmxhUQsUULmMtGgJ7xtPr1q9W2N1ybY2lyWMfaL2riKASyMoDfKSVIg+lfM9/h037qQ1sJcKsvVSrGUHbpqZ3Havp+oF8R+WHu/+rw9s3HgJctrALLrFxf0mBgEHp7QUrrg0YJRUql0cexfDLQBIB6mAZJgEnvt/U9AxBZ1OXPEyJ0gjWeuUduvvVp74cBkbSNuoJ6EdDNUqY+9JI11OnQEnSKgr8m3IotcFeOsNBlsiuBotseYyQYJAzfN83Q12Tk34j4e6iWMU62cQoRDm0t3GOnkYeUTppPX0rjmIw4fNduEMqaC2ghZCiJYsAADmGs/L3rDfiClZW2C2oIRgdGgKPL18p0/nViMkkn2fVtK5hyl8SUt2reGxqMty2FTxLcujKEUBm+8G1IMSPKYPSpBgviXw67e8BbzA7Z2tslsmYyhmA1PTTWhQ4tG85mcLg8SWiBYuzO0eG29bCwfKp30H+FRbnvmDCpgryNdRjdtvbVVIaS4KicswJO9aqz8WcGdFsYlgBoQianXywXkbDXbWg2tnQapuOFBZiABuSYA9yah3FviHYTDrew6+NcZgotklIncs0ECNNt5+tcm47zDiOIXXGJYQrDJZUQiTPyaks0SSxB000kArJLG32ZfxB5r/wCJ4rwrPinC27bBY8ge4CZuAH5p0UA66aDWtBZ4c1htcl615VcGGyhl6HdJMCSBBU1n8Q4i4tIhs5HtupF4NJhSSqkZQZIzTMiJPoWIxSPJtrEr0II3Gkbg6/KdiKjuZcopcFvEYUFQqBRqAGEPmgbnWBIG/eNZq1dwtrznOqsI8smST8ymAPTUTM+mty2vmEgAKTmHQawNImCZ2317VpeK4tWuNCwNhBECNtBAGgG/1qp43J8En0SHk/lm7xG4uHAbwUb7W7uEDI7L5WOpLJECdwYr6ORYAHYR+Fc5+C3BWs2Lt51YeIwVCwgtbUTmjQRmZgDGwro9Xoz5HzQrQ8S45GItYa2dS6i4ewn5B6nr2/w95o45+TrkQ/asNP2B+mf8v9qgvD8V4d5LrScrhj3OsnfrWbNmp7V/JizZ9r2r+Tq9a3mDhYxFop98eZD2bt7Hb/8AK1P57Wv1V3/t/wBVPz2s/qrv/b/qqby42qbJyy4pKmyEOpBIIggwQdwRoQa8rZcfxtq/d8W2jKWHmDRqw2YQT039q1wHQa150lTpHmyVOkbvk3DlsUrDZAWY+4KgfUn+BrolarlzhX5PZCn528zn16L7Db8e9bWvSwQ2RpnpYIbIUxSlKtLhNWMbhVu22tOJVhB7jsR6g6/SrzV5Jo1YqzlPEcE1m41p91O/Qjow9CKtWQpYByQsjMQJIHWB3qe828JN634iD7S2JH7S7lffqPw61z4GvMy49kqPLy4/xyrwT6zzXhEUIouBVAAGTYDYb1X+eOG/+T+5/vXPqVP1M/on6qf0dB/PHDf/ACf3P963tm6GUMNmAI06ESK5Ca6rgTFtCT91f/EVowZZTbs0afLLI3ZmTSapRtBPWvSa0Gk458TOQ3stf4lhoKEm7dt/KydXZfussySNDqd505tYxOYdhMlh8xOhJDdK+q5PauWc7fCvxWfE4NlViSxsFYDT8wtsvy9wpESdwKF0MnhnJLQU6uoKl0MMrmQudpbzSQYOhGuaakvBrwKutoIASCSVUtMQT2WNW+gGm1RbFB1drRRlZCAQ6wfMd2VtV0Iif0q2eEuzbKRLSIjSRMlWI11jX0rkui2JueJ2BdLLacHwzGcGdQhyprGvfUb6+tXCbGHJuLcfwrdpXcAkKZuK8ZSSc0ZdYB1C9DWnOOZbJuq3mBB0E+YnyZCTuB/nWLwXFl7oN0BmhsnlC5yh2YH3Yz666TUKdEr5Nla4Y1pLlwzosoGIHgMT5SqkkucoY6xAiRMgecDxSILb3VYPdEIQsywzZgyjddIMarnk6ljWXxfHZvE0+YDNOnlD52CntKxO8D8NRj2VwLAGUCERoglSVbwYXq06kdQZFdXK5OPjo2HBbL3hdv5SgLKyZfNbKn5l7TmW2MxmNR2jS8YcBtGAK3DnZCdM3mTI8SVAYkbRqI2rcWMVNoWrZhACfDY/LrsoEgwRqD19hMZ47f8AMUkanMwHeABP+P17VKPZyXRkY7GjEGbk5VAA1MCPlLAQBvGkidBuBVm19iVc+bKTqjRnWNyCCOoA01rEv3gUygRlAHuepOnc16Xe4uiz0JA9fLP8+sVOiFl0cYdpV3kTIDaH8R+FdR+FvJFrFm5i8Sha0hCW1kgO4hmY7FgvlXfUlwdqs/CLkI3HTH4i2DaU5rYYf2jwROU7qrSQSNSqkaTXcbagCAAB2AgVx/RCU/BVNa7jnFVw1o3CJJ0Ud2jr2Gk1n3NqxsXhluobTjMp0PcdiOxB61GV1x2UyunXZy7E4hrjNccyzGSf62HpVus7i/DHw9w221G6t0Ze/v3HSsCvJaafJ5Ek0+T2leUmuHD2pPyVwrO/5Q48qGF9X7/T/EjtWk4Vwy5iHyWxp95vuqO59fTrXTMJhxaRbaDyqIH+ZPqd/rWnT4tz3Po06bFue59GRNJoKVvPQE0pSgFKUoBUB5v4KbTm8g+zfUwNEY7z2B3HrI7VPq8YSIOoPQ7VXkxqaory41kVM5BSulXeWsKxk2QP3WZR+CmKt/mrhf1R/wCo/wDqrJ6Wf0Y/ST+Uc4autYIfZp+4v/iK1h5Vwn6o/wDUf/VW4RAAFGwAA9hoKvwYpQuzRgwyx3Z7Fe0pWg0ClKUBHObeSsLxHKb4dXUELcttlYSQdQZVthuDXIuaPh7jMI9y5bU3cOskXMwJW3ozm4ukaSIAM19AUoTjNo+SsUhFpso0VjLL+lm1M94IOnQ1rcDxBkPkyg7KSBK9DH7wkHvX1XxzlHB4tFt3rIhSSvhk2yM0ZoKRvlWfYVoLfwi4UCSbLt2But5d9QVIJPuTtXUT3o4y3EVdSx0JObMdQWIykajvPrWH4oKIZ1zBj31PnA6xAj2rtQ+EGByFTcvlo8rFlGUxAOVVAaN9d611v4MWluL/AOqY2hrBtjxSYOmcMABMH5eketRol+RHG8diisMmjSDoNyZzAj169z9KxsZg3uO1xbb5ZhiFJhiYhtNDMgA7x619C4j4UYEqvhm7bdVVQ4aZYb3GU6FiNOgHQCpVwHglrB2Ew1kHIhLAsczFmJZnJ7kk7R6VJMi5o+fuT/hXi8aQ93Nh7EtLMpDkhRkKo0ZgS240gPrMA9V5T+FmEwqEX1TEuWkFkIQAACMhYg6gmTPT6z6lGyvcylEAAUAAAQABAAGwA6VVSlcInlIr2lAYHGeFriLZttod1aNVbv7dxUBwOBKYu3ZuqPnAZTqCD/iDXTawcfwtLr2ruz22BB7qDJU+nbsfrVOXEpNNdlGXCpNSXZT/AMEw36i1/cFBwTDfqLX9wfyrYUqzZH4Ldkfgpt2woyqAANgBAHsBVVKVIkKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUApSlAKUpQClKUB//Z</t>
+    <t>https://i.pinimg.com/736x/96/2d/e8/962de80bed6f1a85602fb967b6c3023d.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/1c/c6/d3/1cc6d37bdfef75b9d3c964bf7ab795a6.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/d7/b7/66/d7b766e3211fa8f3446b148e4384d989.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/59/f5/8c/59f58cb4b65372369fdc55354986fd75.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/6b/da/59/6bda59316b8e60672c4e84c7b27bcff2.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/5a/dd/1b/5add1b25fe8789d551a699d6b7addfa8.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/d0/88/bc/d088bca34250412f5ed3775017c20273.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/21/cc/f6/21ccf6837c82a1137aac8e48d2a1ae18.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/85/62/b7/8562b746aa087ad29762abc63f37ebe9.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/9e/93/d8/9e93d858c9afd681c29a261e51a216b4.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/75/39/ad/7539ad0691dff2ce614046b9ad65c160.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/70/2d/cf/702dcf991165f1842a0eff318e27274e.jpg</t>
+  </si>
+  <si>
+    <t>https://i.pinimg.com/736x/7e/cc/a9/7ecca997160364967f4190484e985dff.jpg</t>
   </si>
 </sst>
 </file>
@@ -869,7 +848,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="E35" activeCellId="1" sqref="A11 E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,7 +898,7 @@
         <v>104</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,7 +918,7 @@
         <v>105</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,7 +938,7 @@
         <v>106</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -978,8 +957,8 @@
       <c r="E5" t="s">
         <v>107</v>
       </c>
-      <c r="F5" t="s">
-        <v>132</v>
+      <c r="F5" s="2" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,8 +997,8 @@
       <c r="E7" t="s">
         <v>109</v>
       </c>
-      <c r="F7" t="s">
-        <v>136</v>
+      <c r="F7" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,7 +1018,7 @@
         <v>110</v>
       </c>
       <c r="F8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,7 +1037,7 @@
       <c r="E9" t="s">
         <v>112</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1078,7 +1057,7 @@
       <c r="E10" t="s">
         <v>113</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="2" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1098,9 +1077,6 @@
       <c r="E11" t="s">
         <v>114</v>
       </c>
-      <c r="F11" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1118,9 +1094,6 @@
       <c r="E12" t="s">
         <v>115</v>
       </c>
-      <c r="F12" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1138,9 +1111,6 @@
       <c r="E13" t="s">
         <v>117</v>
       </c>
-      <c r="F13" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1158,9 +1128,6 @@
       <c r="E14" t="s">
         <v>118</v>
       </c>
-      <c r="F14" t="s">
-        <v>143</v>
-      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1178,9 +1145,6 @@
       <c r="E15" t="s">
         <v>119</v>
       </c>
-      <c r="F15" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1198,9 +1162,6 @@
       <c r="E16" t="s">
         <v>120</v>
       </c>
-      <c r="F16" t="s">
-        <v>145</v>
-      </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1218,9 +1179,6 @@
       <c r="E17" t="s">
         <v>121</v>
       </c>
-      <c r="F17" t="s">
-        <v>146</v>
-      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1239,7 +1197,7 @@
         <v>122</v>
       </c>
       <c r="F18" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1259,7 +1217,7 @@
         <v>123</v>
       </c>
       <c r="F19" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1279,7 +1237,7 @@
         <v>124</v>
       </c>
       <c r="F20" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1299,7 +1257,7 @@
         <v>125</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1319,7 +1277,7 @@
         <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1339,7 +1297,7 @@
         <v>127</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1359,7 +1317,7 @@
         <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1378,8 +1336,8 @@
       <c r="E25" t="s">
         <v>129</v>
       </c>
-      <c r="F25" t="s">
-        <v>154</v>
+      <c r="F25" s="2" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1399,7 +1357,7 @@
         <v>130</v>
       </c>
       <c r="F26" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1408,6 +1366,11 @@
     <hyperlink ref="F4" r:id="rId2" xr:uid="{6256E1D9-0D74-4BA7-8A86-A63B5DCABBCF}"/>
     <hyperlink ref="F3" r:id="rId3" xr:uid="{1BDAA662-1B5E-4A1A-B044-66D1A046A779}"/>
     <hyperlink ref="F2" r:id="rId4" xr:uid="{3C9215DA-6D76-412F-A0B9-7EBAD964DBF0}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{6BC2153E-AF11-461A-9EF7-E88910AE3518}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{61283AA4-E31B-4808-96DF-79DC9EAF1762}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{71E9BC0B-8E7F-4876-86B9-061BF575D3F0}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{A4EE7C0A-C9FE-4B1B-A14D-0411061406C7}"/>
+    <hyperlink ref="F25" r:id="rId9" xr:uid="{F622804B-C454-48E3-892B-8FAE6B328585}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Meger Hiếu Nghĩa Mới
</commit_message>
<xml_diff>
--- a/client/public/templates/environmentvocab.xlsx
+++ b/client/public/templates/environmentvocab.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ki2Nam3\CongNghePhanMemHuongDoiTuong\project\StudyToeicWeb\client\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tienanh\Desktop\StudyToeicWeb\client\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2DBBC2-77A7-4B86-875D-104C834BE135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFA6E2A-D74E-4DD3-9147-BA3EF6EB7638}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="148">
   <si>
     <t>content</t>
   </si>
@@ -425,9 +425,6 @@
   </si>
   <si>
     <t>https://encrypted-tbn0.gstatic.com/images?q=tbn:ANd9GcRS6p8Ex-T0G7QcHdbhvoL0MafS_BT3bd54Y1pQe6sACHOb_a4BCXmRqgo8yYTUnJ7KRNI&amp;usqp=CAU</t>
-  </si>
-  <si>
-    <t>data:image/jpeg;base64,/9j/4AAQSkZJRgABAQAAAQABAAD/2wCEAAkGBxISEhUSEhISFhUXFhgXGBgXGBgYGBgYFRgWGhcZGBYYHiggGhsmGxYVITEiJSkrLi4uGB8zODMtNygtLi0BCgoKDg0OGxAQGy0lICYwLy0tLS8tLS8vLS0rLS0tLS0tKy8tLS0tLy0vLS0tLS8tLS0vLS0tLS0tLS0tLS0tLf/AABEIAL4BCgMBEQACEQEDEQH/xAAbAAABBQEBAAAAAAAAAAAAAAAAAgMEBQYBB//EAD8QAAICAAQEBAQEBQEIAgMBAAECAxEABBIhBRMiMQZBUWEUIzJxgZGhsQczQlLwwRUkcoKy0eHxYqJDU4MW/8QAGgEAAgMBAQAAAAAAAAAAAAAAAAIBAwUEBv/EADoRAAIBAgQDBgUDBAAGAwAAAAABAgMRBBIhMRNBUQVhcYGh8CKRsdHhFDLBI0JS8SQ0Q1NysgYVM//aAAwDAQACEQMRAD8AYyeWG19vX0+/tjRk7GfGJf5DhpvSdr3B+24P3B/THLUq2eTm9jpp09M3LmaBOFWLqifL0PmPz/fGb/8AYxcoy6prwa9+p1/prXXRr5MXHwoALt9Kk/iAwH6nFNHtGLUL8otv6e/Esnh9ZW5tL+SpzvCj2/En0HqPc+X3xo0MTmUY/wBzV33JnLUo2u+S08WUWeytE0O2329vv/n274TT2OSUWtyjzEOHKmipzUWHTKpIp8wlHDFS0ZAmwjRfAj6h6jEFtmdwEBgA4GB7HAS00dwEHUFmrA9z2H5YAOYAAHAAYADAAYADABwMPXATZnSfcfmMAWYYCDqtXp+QP74AOpXnfY9vWtvwvAAnAAYADAAYADAAYADAB7VwnKN3HUPbv/6++OatNxV0r9x0UopuzdjY8Oyg0gfl6g+3t7Y8pjMXn+CDuuXKUWv496NGvCGTVrX0aLqHLYrhhpVHeW718xZTtsLbLbYeWCVtBVV1IGby2xGEhVlSk1Juz3a3fcunvwLNJW7tuniZfi3D63YhR6XX69z9h+ePTYes2lmWVclz8zPq01f4der5GWz8HoD+I0j8F740E7nFJFBnEw5Uykza4dFEyw8CcSaDPwaUifmyRwMJF1AJLLGGKixTbbHfz2xVWjeJ04aVpWPS87Kmal4zlpVghjy8MSLIsVsiyLIzuQN2YeQFdh98caWVRZ3u2plYv4S/PzEcmbIihaFVZIWd3M9VaKekKWFncVZOkA4tdfRaFXAXUpPDvh8QcdiyU2iURzkHbpcCMuhKm/8A4mt/TfDylenmQsYWnY3Xi7gk3EWggkiysKtnsxFHmY+uQJEuaKxvBpXuIRZ5ndQaxTCShd9xfKKkrFBkv4TxuZL4grLG6QkwwmUid2oowVzpC6ku+1knSBh3Xa5FXAXUTwn+EbSK3MzehzPLBGFhZ1JhL9bsG6A3Lbv22FkkDBKvbZAqKGuH/wAKxJFGzZ0LLLl5Jli5JIHJMYcGTXRAMii6B3sDY4HX12BUVbctPEnhOPNcPy2YWZY3g4THPyxHfMCxhmLOCACarzNm/vEZuM2u8Z07pIreIfwo5ce2cDTIcvzU5RCquZk0Aq5bq09Rrz0/02MSq/cJwV1G5P4VMGlQZxSY83Fld4tIPNigkL/zDVCYgLvZUbi9p4/cTwF1FyfwuQ5yLKxZ9GLCUyhoyssYhNauSWtlc/SxoVuCwIxCr6XsHAV9zNeO/Cv+z2i0ymWOeLmIWjaJx6q8bbg7r3o7kUKxZTqZ0JOnlaPW/E2QZzkomGRTJOcpzdSFp2k5oKoqrty3IjQk9tTE7DHLFpXetzpJGYGTWfic/Oy4fLwwxm8oxGVX5rixfzixYk6a+hQe2DWyDQwWd/hKyZcMmZuYJAzo0bCP57aKWbsxUhidroCwLGLv1CvsU8HTcnZH+G+VgzkCvnUnCziGeJoipLtDzFAGo2ptBfYau+xGIdVuOxKpJMxHjTLQ5biE6ZZ1ZFkcVy9KxkswaIK96tHbV2PcYuptuKuU1ElLQz2HKwwAGAAwAGAAwAGAD37gkIsdDA+oAH/ScZWN/a/hl4x3NHDX/wAl5myyaff8e+PMRvOs3K/mrPzO6bstLeWxZRLjdoU0ckmOMuOiUFYW5DzK4xcZFJXR0U3czXGCRuoUH17n88dnZidvhjHxzXfp+CMS1b4m/C1kYbidk9Rv8/8AU49FG/MypGfzYxYUspM6MMiiYxwnNrDmYJmBKxTRSMBVkRurECyBdD1ws1dNFlGVpJmqfx1ludxZ+XPWeSNYulLUojqeZ17C2Ha8c/Cdorod3FjqXj/xQyUkua1rnoopjAyvEVSUGGtaEq/SG0gWpshm7bHCcGStsTxYmHy3iaKPiy8QWOYxLNqCO5kl0aNG7uxLPW9Fva63xc4NwylamlO5tW/iVw9JIeVFnNEedmzTlhGS3PizIYKNYqpMwKB8gd7708GXMt40Sq8K+OspDHm4p/jUWfONmlbLsEfSWU8pmDgrYQA6T2Y7jY4edOTs10IVaJO4b/EfJcnlSrxFAmYmmQQzMDKkhkKJLNzRISOYCeruqmyNsK6Mr3VgVWNrCOGfxKysYyuqLM3Dk8xA9BGt52y7KVZpLZRyWsmjuNjvgdGTuCrRI4/iDlfg/h+XmNX+y/gr0pp5vL06vrvRfnV+2J4TzX77hxok/iv8UMo8TPHDmOfL8MJFbRy1GWk1nSwNkm2AsenbEKjK4OrE5xv+I3DpRKqwZtxLmocw4bQg+WkKEIyPqUgQqR/8vMA7RGjJcyXViSm/itkknyzLFmpEjEwaWXRzlWUgqidXWBSgliDSKbY2cCoSsyOLG6MD4741BmmiGXObZY4tBkzUrSSSMatqZ2CDYfTQJJ2FDF1OLitSupNN6Gk494x4XmJcpmeTnRmcscqASIgnLgmWRxQcksRrrtuRdYrjTmk1dWLOLDciZzxvl3PGCEm/39YhFap0mNHU8zr2+oVWrzw3Ddo9xHFjqXHGP4lZSWNZFTPGcLAvKMpTLqYZNbtSPTlga6lN6U2G+EVGSdtCXViNcU8d8MOajzkOVnaY5lJ5ZHWIOiJEsRjiIbf6QaJqy2++wqU7WbJdWJiPGXEMvmM3LPlVmVJWMhEunVzHJL1pJAWztvi6CaVmc9Rpu6KXDiCnIvYUPS7/AFwAcFYAOYADAAYADAB73wKrA1kn0Xc/jXbGXjIqUbXk+6JoYaTTvaK72bPJsB/7v9seWUeDWytW7r3fmd8viV73LOJ8bVGsrHLKI4z46Z1VYVIhZqTbGNjKt1Y6KcTNcZlFfSrfar/Ju+O/s+hopZIyXVfyn+Ba87aZmn0f4MRxJ1s7UfQqR+2PQQWmhlTepn82cWooZSZ04dFEyrmxDGgQ2wh0I5gAMABgAMABgAMABgAMAHSMAHMABgAMABgAMABgAMABgAMABgAMABgAMABgA9m4bn62FAe2w/8AP3OKKsHJWvYupySd2rmu4XngQCTt5e/v9sebxuDik5RVorbrKXLvt7XdrUqub4W7v0S+5dw5rGdmq0m4yW1k/Fq9h3FS1XMdOZ3r/NsWcepJ5YrXVea1YvDS1K3O54L59+xHrizDYaVSUZN2v+2S5Nbp+/5Q0pKKfO267uplOL5oMTvpb2+lh/n+DHpMPRUdbWlzts/fzM6tVb0vdd/Iy2dnPY/l/nbHekcTZS5p8MiqTKbNNvh0UN3ZXTHCsugiKcKWhgAMABgAMABgA6cAHMABgAMABgAMABgAMABgAMABgAMABgAXHKVujVgg/Y9xgJEYCAwAGAAwAej5TMV3/L1+/tiGrhGRfZbiddz9/wDP8/bFMqabUny2LozaVlzLvKcWrSCfMX9ybP6CvwxwSwSeW/8AlmfidaxO/hZCn42RRvsQf2vCRwKSut1PN78hnibu3WNiHxPiFllvY/ofL9Nvwx208PGN1bR6+ZzSrN2fNGczWdJ2O/8Anf2OOpI55SKnMz4dFTZH4dIvPTWgdbNqWRb6WrdyFJBohWIDEBfPBJfCLFrMkyVm+BZW2ZsylXIdUbxBGKtKOVHGWLI1IjWbWmof0lq+JJLYuVGDd7kZPDuSkLVmyAA2zPFZoQtrB2BCiVgV2JMbG1F6VdSS5e9SyNKBV8G4HBLl1leXS5kdeXzIkL6YmZFTVdFmXTqagLACmxcym07ExhFot28M5J10rmYxy13cSRWxM0xIcWQxEahdSkDYEagQMJxJX2HcItGd+FyvMzHXLyoktKaPXI4lij2Naap3ehZpfucWXlZCZY3ZoX8NZOFnJnSSoZCFMsVI3KzADEijL8xI9IQAgsCSRWqvPJ8veg2SKDMeGMmrEiZWB5pVVni09EuX0mzvo5csp06i1QnquwBVJdCXTiQ87wDJoGfn2o5jDTJFUmmKeTRGLZ0KtHHGWe9RkBHkGlTl0B04mc4pl1jmljR9aJI6q+x1KrEK1jbcAHb1xbF3RRJJPQjYkUMABgAMABgAMABgAMABgAMABgAMABgA7Yqq3vv/AKV/nfABzAAYADABscvmMMVpk6DM4UbMTYs8fXff9v8A3iLDZgkz37D9sGUnMJnztgb+Vf8Ab9bwWFciBLMTiSCLy2a8K6iiCg5FPmnIJB7jyxbyujnad7MsYOFwSZRpTIqyLHI+nUosq1AMGJJJHYAC773pDUym1Kx106cXC5zg/AspMEV8wyyGHmt1RhR80ppW/wCpVXmEEiwf6RbYWc5LkWwhGyLE8GyOYZEWSOEKD2ZNbgQ5A2zHZiGlzLeV6WFgAlVzSV375j5YuyIuW8M5RqDTkWICJObAIysh+dKEvUFQkLpJBB7+YEupLoRw4jfEeBZaGDMssgkkVUCgvGeWxkyhIoU0jFXnGoADSjWLsKKbbXvqDhFJjw8O5SRInMxivLxyOBokBEcEL5hwqWyH+ctN3l0gdzRnkm0M6cWQuAZDKNlnmm1Fhz1K8yMadMcTRFFI1F2LSANuOhtsTNyukhIRja4jxHwGDLxK8WYWYmRkNFaIVpBYUbrWhfMg6wdhWqYTbdmiJwSV0Z3FhSGAAwEm34twfKSM0nMhi+XfLjeCoBUxBkKswzFssajRTFXQkWQGojKS9+7HQ4xe4yvh3IM5Rc0RTOLaWGnCPmEVVYL0lzFEwY2AJhsdiZzz6EZIEHJ8Dy7y5hDPSxyKqNrhWkbmapm1GpFTSgKobOvatgWc3ZOxCpxuyxymSyMuecHQsMRy2hebEqMgaETGR2HzNi5NEE74VuSiMlFyIGY4HlPhWnjzFvpRhGZIiyaliJVxsXJLSi1quXuDZqVOV7NCuEbXRN4TwvIa4HllU9MLunMQJenJh0YNZstPKx3FclxX9sSlLVL3uMowOQeH8lMz1mQgV4QWMsCqea0Rk0RgDpVHfe9jEdjuFM8lyIyReoxl+BZKSFJlncFtfy3lgV9SrLURLActiUjIcgipaqwNUuck7WBQgMtkMo+azKl9KfGCGERyRqvLkfMdetgRy1EcY1DbrHtc3korwIyxbZbw+H8hGZQ08UgK9LNNFSHXEVXSrB2cpqOsUtEirukc5Pl71GUIr34DOa8NZKMP/vCsQjmzNEyp8nMaTSANKebGlBa+pdmH1CqSfL3oGSIzP4dyS2DmiCWKKObA9CpykzMm3Lblx9GxGsWTakznl0IdOHUyAxcc4YADABdQ5isWHKm0TI81iGh8w+uaxFiVIUc1iLE5hBzWJsK5WJsK2AR2OOac7F8VcUSI2Bb6GNE+St5E+xxRNucWluvUthaL12GfFmQXSjx0XNg6SDYUD0898VYHEycpQlsuveW4qhGyktzGM141DkSsbPhPA4Z8tlFICaxIZZQqagVlzNAu0tg6Ej6REdqN7455SakzrUYuKEZHw3lBOInlkkdESRgOWsZuWJWWy10FaRm86G3beXUla4qhFOxFy/h7Ly51IVmIikQvq6LSndCDvRrTq230ke7Cc7UbkOCciRkfC+WLIGnJZdHMj+WC7MkDlIyWGy82TVe9RNW+FdSVthuFE5wjhuWLZx2ZwiSSpoRlCGLRO8ZNkF6kii0i61BLvyJSlZBGMbsjca8NwQ5czR5nmHWAF6dg3ZGo7OFKt6EHt54aNRt2aFlTSjczOLSgMABgA45oE4CUruxt5v4esrSDnSVHd3lzq6ZXQnlrIXoqjOhAbWAR0mrpVa/Iv4K6gP4fm6M0opnU/wC7ksdFUERZCZGKnVS3pCtqIYacHG7g4K6le3hQLPloWlk0zqzahCVNqD0pG7BntgFBIW7BF4niaN9COErocz/hqFRr5zxoscZdWiGpZDHkdVgy9i2c1GyNOhhRoYFUe1vepLpIczPgZ1upWOksGDQlGCquYPNK6z8kmBQr31czyqmjjdwcFdR3i/g6OCJlMrGZTK9mPSCsUTvormGgVTUGonrAIUg0RqNsHTVrEfLeF4ny0cnMkDy6CjGP5YbTnC8Ybmbi4EtqtenbqoS6jUmugRpxcRGZ8H6c3FlRM7a1YlxCRQTVbIruoljpdQdW3F0LFGVU0uK6aTSHs34MSMW88opTZ5AKs6JmpJFRjKL0jKsvrqdbryVVb8huCuopPA1tp5715OuXZ0oy8sJauTz6IkMQBpOrVQwcXuDgrqOjwUkSyPPJKAIif5QFPbgGMiYrMU5ZDCwAXTc3eDi32J4cUrsY4h4KWBGkkzR0orMxSBmB0uEqNy6o7Wd1sFSK37gVW/IjhLqVviXw62UIp2kWt35TogJLadLNYdGCkqwPUAdhWHhPMVzhl2KPDlYYAJSS4a5S4jwmxNxMg4JsTcXKzvP98GgZWJ52C4ZC78NZoMTEe/df9R/r+eOHGKyzo7MP/iar/ZYlUow2YUf+498Y88Xw3mXI7lSzKxnDkFysiZeWVS7KXutKgWQosnuaY/p9+xYl4iDqQjotPuRClGnJRkyn8UcPVJNUdEFQzUbFktZ2+wx04Ks5w+LrYTFU1Gfw9LifDvBI8wk7ySGPlKrXSkEU7NYJB+mM0e19/IHqnJq1imEbplzmPCWUVzGcxKp1ALqERFPLLEhYhh/Yrmv6WGK1Vla9h3TjcZl8JQhHYZgkrDLIt8sLIY1jYSKwc6Ym1sAWo2lXZIE8V9A4SJHEfCeWhE0TTNzA9JqCB15aZ4nWoYjlyGCMg/Vuu2/VCqSethuHGwznPCmUjkVGzhpnhjVwq6bmM45pth8qolax/fV7WZVST5CcOPUovEHChl5SqkslgAmgdWiN2UjvY5g3oX+YDwlmQk45Ssw5WGAAwAcIwEo2fG/CZlkeaM0smt0MutpJX+ezmQCJeQ3yXBDDSGU0Su4pjUsrHTKDbumMf/4Ji5RZ4GKl9fS4pYmnRzbKAabLyADz6e14ON3C8N9SJw7woZZZYRJGGSZItW5RtaZhhQC2SxhUCyN2qiSKZ1LK5Cp35i/DvhX4iPns+mMGUEaW1DRDI4YdJ1AOFBAs713xE6ltAjTvuPSeB5IxrM0YVbdmRJSyAMgQ6VTUHOtDpoEDVv0NRxV0J4b6ljmPDEuYd0zOZjOYUBUVUbQpbNtF1aIwCGkMrEgXvqPphc6jstPwM4OW7IuR8Bnmxc2WPQzRBxHqZwZTHSjSpAsSDrPSPyuXW0dhVS2uyo4X4ZabLjMa0RCX1Wr7COKaUvsOoVA42veh608qlnYjht8yVxXwp8Ll5ZZHBdXUIEB06OZNGWJK1ZMNhQbAq+9BVUzSSRLpu253N+DGVJXE+XYxyNCQSY+uMoHXVKFUACRDZNfVuK3lVe4jhu25JbwhNIsTy5mAfLjAFl9CO6JCAYwQwJlG4NDfc4XiJN2RLpt7sQ3gnTGZDNGKDMGVZGDBXii06AmoU8jdVnZew74OLqHD03FZjwE6FqnhoNL/AEuGKQczmOI61E3Cw0jv0m6Oxxl0B0n1KPxDklgzM0KElUcqCe5A9dhiyDurlU1Z2RX4YQ6DgAUHxNyLCubguRlDm4LhlOGXBcMpN4Lm4o5Vkl5pCkEcsi7Hrfce1jHPiYVJ03GFtepdScYyvI9c4FxvJzAFJVBPk/Qb9OrY/gceLx+GxlK7cG13a/TU16NSjL+756GB8dwmaaWZdwraf+ROmx+IJ/E49J2T/Sw8IS3au/F6/jyM/FfHUk1t9iP4dzEcg0uyqw/uIAYe1/ti7FqcNYptdxZhcktG0io41kRHI+gdAYgHvX446sPUc6act7HPXhknJR2K6sXlIFR6YAuxyaVnZnYlmZizE7ksxskn1JN4ErA22IrAAAYCAwAGAAwAcY0CcBKV2aPjnCc1AX1zlgziBrkbUV1TLGJRZGk8iXbUwGn3BNcZRfIulGS5juf4FNl4pJZJnEiWw0s1GnyRVramBvOO24BBX3OIUlJ6L3r9iXBrmP5fwzmdOtcwROzOXAkI00uXI5kljr05prrV6Xuah1I9NP8Af2BQfXUjpwDOQoGGZSOKuaXEzoiqTGI32AJ164qKg9xemtpzxfIhU5LZjrcAza6WGbUaWPXzZAkbyrl2AD/UJHOZW6Wu5LEXRnj0Jyy6jS+Gs6mqpVVhGdaiVtSroSQxMFFklZQ1CxQYkgAnBxIdCOHJczmS4PmpYYZMvOzNyXPK5jCRVEssYWNfNWMSKFB3dgK88S5JNponLKysxPDPD2cl50MUqhYpOW45rCMuxK0ABRsqRZoH1OBzirNoVQlqrjg8L5yRBUqPGxZ9pHZToEmuTTp6qMUinSC1r2ogmOJHoTw5dRcPhnMASiXMKi6XaSpGYFk52hpQAQyk5eaiNR6brcWOa5L37ZKpvmxjM+Hs7EjI0g+SHZohKSY1USyatI6QG5DEUbvTdWMGeG5HDltcfi8L57UAsqg1KCRI+ldMghcMwFC2ddvINbaRvgzw6Bkl1M83EJvOaW9Qbd2+tQAG7/UAAL70BiyyK3KXUYkkLEsxJJNkk2SfUk98SK3cTgIDAAYADAAYADAAYALjw1mAJOW3Z+3/ABeX59vyxzYmLy5lyLaVm7M3uW4dYojbzGMKribGlTo3MT4q4ZHlJEjj1aqLkk3sTSKPLam98a2AxM8TBzltt9zjxVKNJqK33LDhDQTpTsgvZlJAP4X+hxViXVpSvFN99jpw0aVRWk0u65lZ4ChFjv2xqRknsZjTW41iSAwAGAAwAGAAwAGAAOAk0k/BuJyNTa3fWhr4iJm1iR0RiBJYIlkkXUfpZmBonFalBFzjPqMH4/N8wGQyBLV9U0QTzcgFnCsKy2q1sVCD2AOD4IkWnK+pOyuQ4kSsbyzRqiuN5VYoiWp+WH1csvCqB602qgHYDCycLXGUZ9TiZLi8PLS5o9ICRgzRqPmFgI1t6ZrRvl7sunsMTemwtUXMcyWS4qyQvFJOXp0RRIF0xKMuAQxYCizRKB3uNa3AqM0AUZ23ImQ+KTMJl5czPA0wjUFSsrVKESPWokGnoCdzqAC7dsM1Fq6REcylZsnZXJ5yNYvg5XnjWSTRGwWPRIj6BJyeadlkfWGvSrUWqyMK3F/uHtJbEbg0WfhXMZWHLIzrpdydPMjbSeU0b6wpYAlkrUbtl88TLI7NsWKkron57gOfyyKuXzMkoTXKyxOgWOuYrVUpLFjHP0heoKxq9SqqlB7oZxkloyl4lBno45HmlOnXypB8RG7FvmEoyK5NjmS2K21tdWcOsjdkVtTXMnSQ8QSKWabMyoIGLAc1JCZpGKOhCydLDmvrBtlEhtes4j4L2S3GtJLVklMlxS4j8S5ZpGUhZ0dlEvwzFyFcl7OYQkAErpBNWDiLw10JUZ23MnnclJEVEq6WZFkA1Kx0uNSk6SdJIINGjRG2+LU09iiSa3I+JFDAAYADAAYADAAYADABJ4fmhE4cxpJXk1199j3+94rq03UjlTa8CynNRd2rno/AvF0Mo643Q9jXWB+VH9MeXxnZNeP/AOck/R/b1NjD46k/3Jr1/PoUPiqD4l5JE3o9Huqiq/EC/vjU7O/4ejCEt+fi9fTY5MUuLUlKPl5GRy8xRgw/L1xryjdWOCLs7mtljhny7FWUtpsLY1A+W3fGSp1aVZJp2vvyNRxpTotpq9tr6mRmiKmiN8ayaaujKaa3EYkgMABgAMABgAMAACBuQCPMG6I8waINfYjAStzb8d4zxGScRLC6c1yoRokk50iSjdTJCuwKRKBpFCNSdyxNMYwtc6JSleyRQ5p88uuSRJlE8j62aLSHkZZo3FlaDFZZ1oV3at12dZXp0K7zV2TI87xSRiqpOz0VNZddekvIChYR6tHMWXputattqXaHGn7Y16nQUuZ4rIOYIZXDaZA4yiG2UFklDCL+ZTMRIOogk2cRaHthep0HcjmeKTS8lQbQrE6tBEI4hNJGo5kfKIC6ljP0mtNjzwNU0rkpzbsV2blz9LJJE6/DmLSxy6JytJ1xgkIKFyhqOxLqTdrhll5cxW5k/kcRgSOSJ2bVFzqjhkbTHLyswxdnhEbC+XqCswFFTtYK3g3ZjtTQjJ5HiZaVlgdeYpLh8uoRuXHI6gRmMqGIjcKVUbmrGrEtw2Fip6jWdzvEERnkJKtaSaoVIjdZJjofXHUcwMkjitwsy7i6AlB6IHnWo3xH/aEuqOWCQmRtZHwqKzOBZbojB103URubAa8CyLVfUhubJnFsrxM5YvMj8t2d3QQaG6SpaaXTEBZIW2Lajps7C8RFwzaDPO4jMub4pFUjJPHyQBqMCrpvkgFyY92+TALaz0qD33m0GRmqJFJnc/JKEDkERoI0AVECoCTQCADuzGzubw6ilsVSk3uRsSKGAAwAGAAwAGAAwAGAAwAT+C5rlyi/palP49j+B/1xTXhmg7bltGVpanoWWyePPVcQblLDmT8aZaOJkSNAt6nYgdyx239qbb3xp9mVZ1Yucn3LyODtGEaclCK735lNwvOcpwT9Pn/3x31qeeNjiozyyuzRcdykc0QkiKswO9EGgQbuvesZuFq1IVXCaaVjSxVKnOkpU2m78nsZJlINHuMa6dzJascwEC4YmYhVBJPkMRKSirsaMXJ2QvM5SSM06Mt9rGxr0PY4WFWE/wBruNUpTp/uVhnDlYYAOMLGAlOzNBxDjeaeRJniCvBKZr0Ps8jpJT6ydK6tJCjSOsnuxJrUY7dS1yl0Dis2aKLA2XVdcSPpjRzIYYeYsSsCzEKg1DtdBdRNA4IqK1Gk5vSxPzXiXiMUxWZQ7wOXIeMsoZFWLmWtULRiGBALSSHfWcKoQaugc5rRorzxLNA84RrUiRydKswCQJPk0vc6RXNG53IBw2WNrA5z3OZDjOZWZpFiV3bldJjc0cuU5TAKQbDRD2NNY9BxjawqlK+wNxvNNl1y2glGVUSlkBIVYlpQrBXsRxXYb1FXgyRTuDnJq1iTleO5qMI4ykZKwiMSGKazHCqxk3roUsWlitf1XiHCL5k55b2Iz8WzXz9UIJlchyY3tHkikhIWiKYpKwpr8qGJyR0BTnroLmzebzCyQtCPmu8xtHB1QRHWI9R0ghIyCANR+m96wJRWt/bC8pK1iVH4rzuoMsEerVpU8uQnWFVWFliWcqqA6iSAqgUBWI4ceoZ5dCHlfEOZy6heWgsSaWdGDAS8wPpYEWCXbY2LVTVqMTkiyOJJbobzHiaVo5YwkSLKzOwTmL1yaeY1cyjq0rYYECukLiVTRDqtlLhyoMABgA7WAArAAVgAKwAFYACsABWAB7KZl4m1oaYedA/uMJUpxqLLLYeFRwd4mx4D4qkbaREYj06TXr5j9sYmL7Jg9YSa9V/Br4XtOW0op+gjjOX+JZ2qtX035UKH7fqcW4T/AIanGHTf+RMQv1FSUuuxjXiYXYIo0fY+n32ONhST2Mpxa3Ljw3nDG+lgdDedbD7+2ObF0HUheO50YTEwpztJ6MsPEvB9WmSFQQQbIP2r/XHLgMRLWnV0a6nV2hRhaNSlqnzWpW8N8PSSHq6V9e5P2GOyvXVNaas4cPTVV72Ra/7PGVNagdgSao+e3c32xzQlLFRulzsdNRwwksrlyvsVPGppJmXoIVRQ3F79z+35Y6sPhXRT6s5cTj4VmuiIEHD5XOlUYn7bD7nsMWVKkaavN2EowdZ2hr75ljxLhMUEXVNqnJHQv0qPOz3/AG+2OKhiq1arpC0Or3fh7fiaOIwlChR+Kd6j5LZePteBTLsb/wA/TfGgZiZsMx4/mLq6Qxrp1UpZmUkgBdQ21BaHf0xSqKL+MVz+JmMwl5e3IbLleZISUfWSeaTq1W92b7D74bh/DYjja3JbeOJisqtGh5vMN2bUyNO1Am+kDMSLp9K3G9xwUHGIvDfFMkMKwiNSEVgp1MN2bMElwpqQVmHGk7bD1YGZU7u4KtZE6Lx/mRs0cJU3qpdJbUlHqHYmRpZTsbaZ/I1iHRQcYrc14lllzKZh1vQKCam07qVJF3RPc+RI3BG2JVO0bEOrd3LGTx1NrDrGFbma/wCY9V8Q+Y01ew1uwJ810jywvB9+ViXWG8r42mQJ8sFkWNQ2txsiwKSyg0zn4dCHO6350tS6KDjDmd8aMYwsUQQskyv1PpXmtm65S3SkLmQdW240gBdjCo66jOsuQjM+OJ3RlEaKWM3UpII5/Ps+uoHMSENf4dyZ4SF4xA454hbNIiyRLqRaDBj3qJWbT23WJRRv28gGjDK9BZVMysUlYcrCsABWAArABKMWGsU5jZPmMhIzxNHFGrRZVTOnc6ZMpzOWtUj6TmNbAGwg2+rVTlmtfH+Tqz09vA5l+FcN6S7gHXGHQT6kGo0yo4UFhRVi3YdQ1Ar1Q3Pl9AtT9sq+HZLKHaWtRnK/zaRY1AOrVpOqyCoNqN7sdw8s3LoJHJz6lwmR4dGk6rJG1mUK7MrMNPxHKVV0GgU5BLi+pyNiopPjbRYnTSeojOcL4cgflyKSFcg8wPVwShQikU5Myr6EalPTscCc3uD4auIk4VwwGuYd20jTLqAQlwsxPLHXQBMflt2ugXqEWpdSvyOSyr5Ql3AmVJSotV6rGkEAanJqhuavsASyu82bTYROGTV9S98McIywSN7RpXjZXRpAK+bAwIJW42CLL5eg3uzTiNIvPoupZh5xbShrLoauDg+UGnrJFC7ajVnU+ynqAqk77n0s4M68Ovr8/wDRvQpVOnv3zIXEshlWiZCoFCN9WoBtfKl1aRp6vmFFK+e2+1jv7Kle8l3L6X8N38jP7YVkoS739beO3qMJwTJI7FDrAjYLrYUbSYB6rd75PSaILE16a+abWvvYxFCknddPv+NCDwuIqulu2M3tPCTm1UorU1Ox8bGCdKu9Ovv3/Lk8BU9A7/lhcAliKfxvVaNcxu082Fq/01o9U+XeV03DGY2xJONmChTjaKsjz9RVass0ndioeBDu5oeg7nGdiO0nm4eGhnl6Lz9rvNXCdjrLxcXPJDp/c/L/AG+5Dk4ZV5cShF8/U4KfZ0ZVONiHmly6L38u4mt2tUhSdDCxyR5vm/t6vvKWbhZPdbxqWiYuaoncgzcIHoRiMiHWJmtyHLw1h23wrgy6OJi9yM0FdxhbFynfY5ysRYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMwcrBYMxYnLYa4mVmsznCci+qQFhpi5jCJ0K9KwKqkBPltJJI60bI0WRvihSmtPfM6ZQpvX6eRF4RksnyQZfqYaHPMUMpOYy9FEKkrUXMOrewGHns0nK+nvRiwjDLrv+UcbhuTjkyjJJrHMjM2sxlKtC9oOpQDrHUKIAIvzFKTTuDhBNWfiTZuFZOQs0siIdagCOXLfRaA9MUarfUxBAP0G+26KU0tF9R3GnJ6v1Qxw/J5Fo11Lp5gVWuZGkjY5kAkAx2umGmJqmFjajhm53096CxVO2unn3jJ4PFKuWkPSzkLMqlFoLpUMqgVHa7kt3bUarfDq6bXyKJSi1FrzLyHwvkwxqQ6RfZ1JvVsL09tHmLF3RNYhVJpbBKhTk9ZaeP46FnDwbKukf/wCPSq9mUtbS/MLdALnQTR3rSBQ7GHKd2t/9DRo07JrS3frvry6EoZGNYyQza77a1cAdO17Fu5Njt28sZGOwVGSz5beGnobXZ+MrR+DNfuevruRmy4PfHHSqLDpKHI761L9Q258xcOQU9sb1LFU6tsr1te3TxPO1cFUpXzLS9r9fAkLwz2xdmKcgjM8OKjUBddx7YycZTnRn+qo7r9y6r39/HawNSnXp/pK+z/a+j97fLZiYeHO+5GkennirhYnHa1nkp/4rd+P5+XMu4uF7P0oLPU/yey8Px8+Q83DPbGvRhClFQgrIxK06labnUd2WfB4YY0ZZADqeM0V1CkZTv+BfbEVMzehNJRimn3egDJZDp1RDbTqrm0eltXn61X4Yi9Xr9CctHS6+oiHK5FKkCKGGiv5hOoEatidxpuzVeQ9SN1HoCjRXxW+pX5jJcMFVADvv/N7GZL8/KLXW/wB8OnV6/Tp9yp08P/j9ev2Mhx7hMTSuYlAjJ6QNRA2F1qF1d96xfCTyrNuclSms7cNEUOZ4E6jUBtipYijKpwoyWboX/psRClxpxeT/AC8SCcoR3GLbiKN9jnw2C5OVkzhXBWnZkU0wRmAr6iCoC2SKst3wspqKuNGk5OxPHhCXlFy0YOoADXHp00S7tIXoKO217g9q3Tiq9h/08rXGF8LZg6aVOoIV+ZHTc0uEVTqpmJjcUPT3GG4kReDIW/hSZFlaTSgjQsOpSXIEZIUA2RUqEnysDv2jirSxPAlrcjr4dmK6gE/lGauYmvlquotovV9Nnt5HE51e3kLwpWv5k5vBs1IAUMjPoKao6V7lGkvrrV8ptq72PuvFQ/6eVl1I58LzBbOi6RiNaUqusr3IxbooRNsf3oGeJEjgS9+f2Gc34cniQu6qFFdnQmiSoYAEkqSNm7GxiVUi3ZEOjJK7IHw2HuJlYfDYLhlZcnLYS5fYvpuE5VV2lJ1IuwlRgH05gkmksi0g2IU/MO/pVml0LMkeojP8Py2qGNGAS3DOGVmpmqOR6UUKpihFgWPfEpy1YOMdEOPwbJdeiZj0FlLOiHVT0pQr1bxm6PaRNjuRGafNBkhyYQ8KybMw+bQkdR81N0V4VVv5X9SvK3/88TeYrUF/v8EyHgMCPFpbUCvWSVbffyApQfIGz615spSsxJQi5LXQmZjhKBvl/R5dQY9huaArv2PviVN21FlTSehIg4d7YHIlQJ0PD/bCuQ6gdlaJNmYE+g3P/jCVItwd02h6ckqitJJ9708yqkm9MeQqycZNP10Pa0YKUU1r4aiY5nAJUkX6Y2ew8qzOXPReX3/gxO31L4VD+3V+f2t6jUsjnu7H8Tj0qSXI8rml1DMcJmFHQzWqt0gtQfddVDYn0xEasetvwM6Uul/yNy8BzAomJlu6sHuEVwDXYkMAB3JsdxiVXg+fvYOBNcve5C+HzQ1aVzAKmm0iTpJ7Bq7H74fNT529BctTlf1JeWHEtLOqzEKQKaMksSSKUFbatJuu1b4SX6e6Tt8x4qvZtX07vwPxcczKrqmyblQAxYI6AKdgxJBFH12GEdGm3aMvVDxqz/ui/kyZlOO5WXbXyz6SDT/9vp/XFcqNSPK5ZGpCRYSZAEWNx64pzDuBCm4d7YZSFcCFJkyNq2xlY3sxVpOrSdp79348UbGA7VdCCo1o5qe3er/XwKnOcJVuw/z2w2Ex1Rf0sSrPr9/utBMb2dSf9bBu8Xy+32eq9Cmn4cV8tsapkp30Yvh6OjjlsVYkLYq9yPX3rCuzWo6unoT58lmwVgJJ5gIVbTdWJ70ekHc7n19DhU47jtS/aScxw7PsVDsLVkK9cStqUtyyKIJOpzR9X98QpQ5EuM3v/Ambh+a0P1x6GUsV+ShI+UDpQfTZMY6a1UL8sCcQcZWOpwnORaw5EY5LA6uW2pY4paRQTuaSRTW4BPkdzNFkZZL5e0djTOsiSxyl9Ss5A5eoFWzC7p3ckLIdRFktW5rB8F7P3sT8drp+9TmUy2akZlaVF0Poa+UeorP0le0i1zRRtQGPkNhuKWwJSbs371/JHz+QznLaSUkpsCdSkEFg6kUd11MCCNt6xKcb2RDjO12U/wANiy5XYPhsFwsXPw2EuWWD4bBcLB8NguFh7L8OLfbEit2LjLcOA8sGYTKWUGQ9sLmHUSwhyXthXIdRI+b4lFF0jrb0HYfdsWQpSlrsiudWMNN2VWYz0knc0P7V2H4+v446I04xOSdWUtxCRYlsQd5O2ODH0lUp5mr2+hpdmYh06uVO1/r+RGiu2PPutCkrJ2sel4cqrvLW4qHKlzSizV/5eNan25h2kpN356aHnsV2RVo3ktr6dX/os/8AaeYiH8pPpRbpztHWns9DsPQfnjphXwlZ2jU/jfxRy5q1Nft6enmVcnGZNCrUdKUa+qyYxEFJOr0hTtXnjvVGN768/W/3KOPLLbTl6W+yGE8QSo0jBIfmMGIpqBX+0BtrHn33O++JeHi0k29CViJJtpLX31GX8U5gSczTCTd0VegQZzsNdg3mH/JfTdlhoONtfdu7u+pDxVRO+nu/f3/QiZ3xVPJHJGUhAkVVYqHB6FKg/XV6TXatu14aOFhFpq+nh9iHipyTTtr4/coEhLGlF9h+ZofqcPUqwpq8nb8aiRTew/k+KTZZiIpDsSCvdLB3Gk7d/MfniuOSvFSto9updFuGxruEeKhMrB4SHUd1+hj+O6n23xk9o16eCim3dvZc/wDXeavZ+EqYyVoqyW75L89w1Pm3c7mh6DbHlK/aGIrPWVl0Wn5fmeuw/ZmGoLSN31ev4XkM45M0t7nbljtYSyg98aOE7VrUNH8Uej/hmXjexqGIV4rLLqv5XtkWTIlSHTyN/YjHqqNeFeCnB6M8jXoVMPUdOotV7uTo8tK8aTc0hldlQVGoBHLJLMWXvr/tb6dzidE7WI1auByWaB7ohWyBqiSuUxY0o2ADoewqxgvELSHZMjmAWQSBqDabEZDKtB7YnooKh0nzo7EXiLx3JtLYi6cyyNJYKvrBNRgnSjtIaq9Whntu51VZvDfCnYj4mrkvh+TnSgzKoiDOoLRXqV3VT9QJCysxFmgQTv5rJpkxTRFy/C8zGSigAsarVGSSqk6ls3QV26h5Md++GcoshRkiPnFlFxSH6SBRCkjSFAAarApV7GjV4lW3RDvsyH8Nhri2D4bBcLF58LhLllg+FwXCw7Bw+/tguKy1gyPtiHIhRJ8OTwrkMoj85jhQvIwVR5n9gPM+2CKcnaJMrRV2ZXifHnmtY7SP/wCzfcjsPYfrjup0FDV6s4amIctFoiFCmLGygmxJhGBMSPy3J81UWw9LHZfxIxnVO0acbpfN6J+D5+SZfDDye/59+JZQ5MabKm/Qn9yP/OMLEdsV5Nxg0l3L7/ZGhRwdNNOV/fgVOby0i2ShA9twPxGMJp31PX0KtGaSUlf5E/w/F0M/qaH2X/yT+WGgjg7Wl8ah0X1LJhhzJaIkuUQnURv9zjojiasY5U9Cpwi3exHzGRjb6kU/hv8Anh6eMxFP9k2vMrnTg90Qp+DQt/T+R9PIX2HsKx0U+1cVDaXv+fMqlRg+RXyeG4fVx7g/9xjsX/yDFL/F+X5RQ8LTEp4fiXcaiaI3I7nzFAUR6jFdbtrEVVZ2S7l6at3Q0aMY7Hc/BG5KugPYg9jf3G+M6jjq2Hl/Tk19PlsbuG7HjiqEKidtXm8E3t38unPxYhhCKFUUBjnr1515upUd2z1FChToQVOmrJHZHCgsSAB3JxXClOpJQgrt8iydSMIuU3ZLmSeEouZQtCyvp+pRs49CVO9HyONSp2RiaUfij6mVHtfDTlaMvS3vzGnSsZUlY1YyuPZE22k+e34+WNPsnEulWycpfXl9jK7awqq0M63jr5c/v5E9o5EFIQACW+lSQTVkEixekX9sepaTPIxbWhFklfUGLC6I3C1TXYqqN6j+eKp1aVOym0r9WX06NWpdwTdumvodWSQENq3BJBoGi1WRY2Ow39sWLK1oVtST1Ewl1GlSALutKm9mXexuKZhR23OJdmQroVzJNWvUdXrt/fzP+vfEWWwaijNLt1Dbt0rtsFobbAqACOx88FkF2MSQlu9fgAPO+wHviSBHwuJuFg+FwXCxe/Ce2K7llhUeRs4LkNFhFk/bEZiMpE4xmjFpRPrNHtdC6G3mTjK7Qx7otU6f7n727zW7NwEa151f2r36Eifia5bLrLmNnNgINmZgTsB9qs9saGCjVrQWffn3GfjpUaM5ZP28u/QwfEOJyZl9ch2/pUfSo9B7+p88bcKcaatEw51JVHeR2EYGQToRhGBbZXJMfqJUeimmP/E3cD2GPLY/tKEpZYWl3vZeC5vvfloaNCg0rvT6lrBGFFKAB6DGHUnKcs0ndnaopKyJCDCFiHlGAaxxhgBjLYBWNPiUVsYfEiMZbAIMviRGMtiRWVeaPUcUVP3HtOx/+Th5/wDsxl3ABJ7AWaF9vYd8EE5yUVu9DRnJRi5PZalIOKRysBICqXsbsH2kHb3vy/XHrI9lVsHSc6TvK2vVf+L+q5+h4XtHtKeLlaOkFsv5ff8AQlHhxhdZss7Ruu+xJDDzFG+/puPbFdDtaprCssyflb6e+ZlwqtMvDmxOdVKGO5C9rrcgHcWd6Pa/PGNi0p1HJK3v18T2nZVeUsPHNv8AxfQTl4zzE/41/wCoY5aSaqw8V9UadZqVGd+j+ho+LTJCN92PZfP7n0GPUYrHQw8ddXyXvZHksH2fUxMtNFzfvdmcVHlbYWfbsB/pjzknXxtXq/RL35s9RGOHwNLovVv+S1ymRIQAjfufxx6PAUuDh4we+78XqeZ7QrKtiJTW2y8EP/Ce2Oy5xWD4T2wXCwfCe2C4WD4T2wXCwfCe2C4WD4T2wXCxf/B4quWWH48pXliMxFh5MviLk2M5xo8jNCVlLKAGAFb0pAAJ2vVjAr3j2lGUttPla3o9TaovNgZQjvr9b+ux57xTiUuZlMsp37BfJB/aB/l497ShGEEobdeveeIqylObc9+nQIcSyEWGSjLsFHn/AJeOXFYiOHpOpLl69w8IucsqNLlssq1QF+vnjxOJx9fEN5paPlyNOnShDZExccReh5DiB0PIcA6HQ2Aa5xmwENjTHAKxlsSIxlzgEYy2JEYxK1ev4YZK4jKPMzZmWM8sLGSzLuGLBdRAY9tB0gNuD3G2NKnTwtKqlVbasnpa217d+unLxKpOTWhT53LZiGMOJCf7wQtqzbk3vqBJP5jGph32fiqzhKmr/wBr11S07rO38ltPH4yhBRp1GkuVl480VjcUm/8A2H8l/wC2NJ9i4B/9P1l9yyPbOP8A+4/lH7ECSQkkmrPsB+g2xowgoRUVsu9v1epxubnJye78F6LQsOF8QkWt7T+0/svoN+3bbGTj+z6U1eKtLr9+vu50UcPGo7y/2aJAslSISp8j57bbjzx5aXEoSdOevd9jdo1smha8LkkkddEdyg9vKx2b7djvitRfFXC1e6/PgaznB0W6jtF+/UtOPcHMMIkdi8rSDW3kOlth7WBv+3bFuLwvCpZ5PNJvV+T29+mhRgcXxa+SKywSdl5rf38yT4Qy4aJz566P20iv1LY6+yLKnJ87+ll+Tk7bu6sVyt631/gt2yeNbMY1g+DxNwsHweC4WD4PBcLB8HguFg+DwXCwfB4LhYveUMVXHsd5YwXCwmeREVnchVUFmJ7AAWSfwwJNuyBtJXZ4v4h8VPmcwZASIltY0P8Ab/cw/uNA+2w8t9b9BTlTUZrXe/R93vUzP11SNTNF6dOq7yqknDNeOqlS4ccpy16yqTzDsb4dopuaPhxWGIyvtdeVmv6QB6nHke1ak8XiVh6WuX68/lt8zQw6UIZnzEHPSyG9RjXyUVq/5m8j9v1x3YbsajTj/U+J+ny+5XPEyf7SVlmYMG1uT23Jr03H+uLa/Z2H4Ukopc7rciGInmWpfKceMNZMdVsQNcWGwE3OFsAXEM2AW42zYki5muK8ZfWyRFQFIBerNj6lAOx9L+/pj0XZ3Y8asFUq315d3J9Thr4nK7ITk+O30y0D5MNgT6Ef0+W/bv2xGO7EdJZ6Oq5rmvuLTxKlpLQnZ9SyOqkgkEWp0sLHkfJt9vwxi0Wo1IyktO9XX+updIz0DTxaY1aNYgSAzKC3bswRzXrfuLIxt1Y4WvmqNNz6J6eKcor5fJHP8a05FLJpJmd0Z6I0kMzKrEV37Dv5g1Vb+epGMoQpRpNJ63ukm14b+NvHwW927kGdgWJAABo0DdWNx+d/5vjUoZlC03drn17/AJe+QmnIjti0sRxJSDi5xjWjZnVSqOJccM4mIzbNS+Y9L2B/OseZ7RwDqq0V8S2fXuNFV4Rjmlq+S6lt8bJHKk8TaZIzY76WU/Ujgd1I/I0R2xk4OoqF48nv9/L8GLV7Tq1Kmeb06cl79T1bKzxcRytjYMNx5o6+R+x/Mexx11qca1Nx5M18Hisso1Ye+qK3guUaCQgj2Yeo/wA3H/nGdhoyoT+psYuca9P1RquWDjXuYtg5I9MTciwckemC4WDkj0wXCwckemC4WDkj0wXCwckemC4WHMQSGADzb+KfHiayUZ9GmI/NE/Zj/wAvvjSwNL/qPy+5xYubfwLzPO1hONNSM6VNjqwnE5kVOmyblcuzEKO52xVWqwpQc5bIaNNt2RpM7w1mSNV30EdzWwUi69e3648hgcbCGKnWqKylfv3dzunTbgooiIhBIPcGj+GPUU6sakFOOzOOUGnZkuIkdu/lhK1ONSDhLZkwvF3RfQ3Qv0GPCVadpyS2uzYi7pDwxXlGuKxOVjXCsRlYXEEYMrIuUed4tqDpErHpYaxtWxGoedD19sbGG7JneM6rSV1o+eu3mc0661SKHk0NKjsPLfyvHrlKKRmOLbGUWiGK2ti7Fit7seewPn5YqxLcoOEJWdn3O/LXl8hoQ1u0OR8VYaw8coRt0VXOtfTqJBoj3I9MZFTshyjGUJRclo9FZ+S5ryfU6FV11QvhvC8u0bOEOzE6nFv5GwY6o2L233xzYzFYunVVNtLRaR258pX9dAjCNiDPBrLISusyS6i7GwFAK9IoUQtaq2r1xfCcqajNJ5VGNklpdvXXXZva+pOUb4hwZ6BGouFFpppQFAsKb37+94uwvacFNp2yt/uvrrtdW09LEZSjMWN65KixpoTguWqI2qEEGga8j2wk4qUXHYdq6sWvBpXJZGs+YJN0PSzvXbGD2nhIU4xqR05Pv7zixVFJKSNn4K4wcrPTH5UhCt6A9lb/AEPt9sZ9CpZ2YuCqOlPK9n9T1holJ1VjrcE3c3VNpWHMMKGAAwAGAAwAGAAwAGACNxHNcqKSWr0IzV60LrDQjmkkQ3ZHi88ZkdpHNszFmPqSbONqLyqyOKUbu7BcoMTmFcEOplBgzCOCLXgOUHMJ9FP7jGV2xNugo9X9xqcEncV8RMb61G5GyjyPveK6XZmHcU2n8xnJoUmXP1MbLEkn7UO2O+ko01w4rRFco31ZOyeQ173Q/XHNjMbwPhSu38hoUcxNy2aV3KAG1vv7d8YNTByhTVRtWZ1KSbsTBHjmyDihHgyABjwZAOGPBkAbMQ9sTluLYYTJIptVUH2AGLalSpUWWcm13sXKlqkVPiFL5cX97XfoFodvP6hju7Mp5Zyq/wCK9/QrqK6sPNwWPp+rUoChgSDS3Xb7nFX6yreVrWk22rXWpHDRV8ZdVTkRgrRCnuNtIbYg3dVuffHTgsO6tXi1HfmFimj4ehIU/SSAa77n3xvVJuNNuO6RGU0MPCmj+h7GkDS9kagKBB/pBHlvjy9WrCrrKNnfddH1XP3ciyMvnMoDI9UBrbb8f/ePR4RtUYp9CxR0I7ZIY6cw6iho5EYXMPYfyOU0sGB7EX7gkCsc+MSnScX5eKVyupFONmXj5QY82omfkR6T4QzrSZcBtyh0E+tVR/IjHdTleJqUJuUNS7w5aGAAwAGAAwAGAAwAf//Z</t>
   </si>
   <si>
     <t>https://i.pinimg.com/736x/96/2d/e8/962de80bed6f1a85602fb967b6c3023d.jpg</t>
@@ -477,7 +474,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -485,7 +482,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -493,7 +490,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -559,9 +556,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -599,9 +596,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -634,9 +631,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -669,9 +683,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -847,18 +878,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" activeCellId="1" sqref="A11 E35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" customWidth="1"/>
-    <col min="4" max="4" width="42.7109375" customWidth="1"/>
-    <col min="5" max="5" width="88.85546875" customWidth="1"/>
-    <col min="6" max="6" width="41.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.296875" customWidth="1"/>
+    <col min="2" max="2" width="29.09765625" customWidth="1"/>
+    <col min="3" max="3" width="30.8984375" customWidth="1"/>
+    <col min="4" max="4" width="42.69921875" customWidth="1"/>
+    <col min="5" max="5" width="88.8984375" customWidth="1"/>
+    <col min="6" max="6" width="41.8984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -958,7 +989,7 @@
         <v>107</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -998,7 +1029,7 @@
         <v>109</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1014,11 +1045,8 @@
       <c r="D8" t="s">
         <v>85</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="F8" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,7 +1066,7 @@
         <v>112</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,7 +1086,7 @@
         <v>113</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,7 +1225,7 @@
         <v>122</v>
       </c>
       <c r="F18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1217,7 +1245,7 @@
         <v>123</v>
       </c>
       <c r="F19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1237,7 +1265,7 @@
         <v>124</v>
       </c>
       <c r="F20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1257,7 +1285,7 @@
         <v>125</v>
       </c>
       <c r="F21" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1277,7 +1305,7 @@
         <v>126</v>
       </c>
       <c r="F22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1297,7 +1325,7 @@
         <v>127</v>
       </c>
       <c r="F23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1317,7 +1345,7 @@
         <v>128</v>
       </c>
       <c r="F24" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1337,7 +1365,7 @@
         <v>129</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1357,7 +1385,7 @@
         <v>130</v>
       </c>
       <c r="F26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -1371,6 +1399,7 @@
     <hyperlink ref="F9" r:id="rId7" xr:uid="{71E9BC0B-8E7F-4876-86B9-061BF575D3F0}"/>
     <hyperlink ref="F10" r:id="rId8" xr:uid="{A4EE7C0A-C9FE-4B1B-A14D-0411061406C7}"/>
     <hyperlink ref="F25" r:id="rId9" xr:uid="{F622804B-C454-48E3-892B-8FAE6B328585}"/>
+    <hyperlink ref="E8" r:id="rId10" xr:uid="{ED87E29D-927F-42F0-A2A5-44FD621391E2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>